<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 36 new rows for week ending 2021-01-10 (total 36 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +469,724 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1042143</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Order 1042143 Swish +46736813550</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1042143</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Order 1042143 Swish +46736813550</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1042143</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Order 1042143 Swish +46736813550</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4042212</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Order 4042212 Swish +46736240489</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>493.75</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4042212</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Order 4042212 Swish +46736240489</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>59.25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>44200</v>
+      </c>
+      <c r="B7" t="n">
+        <v>4042212</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Order 4042212 Swish +46736240489</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>553</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>FACEBK XF4BLXWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>328</v>
+      </c>
+      <c r="F8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>FACEBK XF4BLXWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>82</v>
+      </c>
+      <c r="F9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>44201</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>FACEBK XF4BLXWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>44202</v>
+      </c>
+      <c r="B11" t="n">
+        <v>8062303</v>
+      </c>
+      <c r="C11" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Order 8062303 Swish +46737299838</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>643.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>44202</v>
+      </c>
+      <c r="B12" t="n">
+        <v>8062303</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Order 8062303 Swish +46737299838</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>77.25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>44202</v>
+      </c>
+      <c r="B13" t="n">
+        <v>8062303</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Order 8062303 Swish +46737299838</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>721</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5071909</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Order 5071909 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>538.39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5071909</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Order 5071909 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>64.61</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>44203</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5071909</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Order 5071909 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>603</v>
+      </c>
+      <c r="F16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>44204</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>9081316</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Order 9081316 Swish +46767627755</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>803.5700000000001</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>44204</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>9081316</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Order 9081316 Swish +46767627755</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>96.43000000000001</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>9081316</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Order 9081316 Swish +46767627755</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>900</v>
+      </c>
+      <c r="F19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>0081718</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Order 0081718 Swish +46736386982</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>564.29</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>0081718</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Order 0081718 Swish +46736386982</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>67.70999999999999</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>0081718</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Order 0081718 Swish +46736386982</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>632</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>0092025</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Order 0092025 Swish +46705757460</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>0092025</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Order 0092025 Swish +46705757460</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>44204</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>0092025</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Order 0092025 Swish +46705757460</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1092029</v>
+      </c>
+      <c r="C26" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Order 1092029 Swish +46725322220</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="n">
+        <v>806.25</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1092029</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Order 1092029 Swish +46725322220</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>44205</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1092029</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Order 1092029 Swish +46725322220</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>903</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B29" t="n">
+        <v>3101601</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Order 3101601 Swish +46709703734</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
+        <v>564.29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B30" t="n">
+        <v>3101601</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Order 3101601 Swish +46709703734</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="n">
+        <v>67.70999999999999</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B31" t="n">
+        <v>3101601</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Order 3101601 Swish +46709703734</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>632</v>
+      </c>
+      <c r="F31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>634.01</v>
+      </c>
+      <c r="F32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>158.5</v>
+      </c>
+      <c r="F33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="n">
+        <v>792.51</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>FACEBK A63N9ZJZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>410</v>
+      </c>
+      <c r="F35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>FACEBK A63N9ZJZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>44206</v>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>FACEBK A63N9ZJZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="n">
+        <v>410</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 27 new rows for week ending 2021-01-17 (total 63 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1187,6 +1187,522 @@
         <v>410</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>44207</v>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>SvE*LINDH BROS AB K0135</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>788.35</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>44207</v>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>SvE*LINDH BROS AB K0135</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>197.09</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>44207</v>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>SvE*LINDH BROS AB K0135</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr"/>
+      <c r="F40" t="n">
+        <v>985.4400000000001</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>44208</v>
+      </c>
+      <c r="B41" t="n">
+        <v>4121803</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Order 4121803 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="n">
+        <v>806.25</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>44208</v>
+      </c>
+      <c r="B42" t="n">
+        <v>4121803</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Order 4121803 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr"/>
+      <c r="F42" t="n">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>44208</v>
+      </c>
+      <c r="B43" t="n">
+        <v>4121803</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Order 4121803 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>903</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B44" t="n">
+        <v>6130504</v>
+      </c>
+      <c r="C44" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Order 6130504 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="n">
+        <v>1242.86</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B45" t="n">
+        <v>6130504</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Order 6130504 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="n">
+        <v>149.14</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B46" t="n">
+        <v>6130504</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Order 6130504 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1392</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B47" t="n">
+        <v>3131821</v>
+      </c>
+      <c r="C47" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Order 3131821 Swish +46738066249</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="n">
+        <v>398.21</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B48" t="n">
+        <v>3131821</v>
+      </c>
+      <c r="C48" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Order 3131821 Swish +46738066249</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr"/>
+      <c r="F48" t="n">
+        <v>47.79</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B49" t="n">
+        <v>3131821</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Order 3131821 Swish +46738066249</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>446</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B50" t="n">
+        <v>2131916</v>
+      </c>
+      <c r="C50" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Order 2131916 Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr"/>
+      <c r="F50" t="n">
+        <v>502.68</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B51" t="n">
+        <v>2131916</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Order 2131916 Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr"/>
+      <c r="F51" t="n">
+        <v>60.32</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>44209</v>
+      </c>
+      <c r="B52" t="n">
+        <v>2131916</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Order 2131916 Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>563</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>44210</v>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>MATVA.RLDEN VA.LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>30.84</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>44210</v>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>MATVA.RLDEN VA.LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>44210</v>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>MATVA.RLDEN VA.LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="n">
+        <v>34.54</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>44211</v>
+      </c>
+      <c r="B56" t="n">
+        <v>3152209</v>
+      </c>
+      <c r="C56" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Order 3152209 Swish +46722017122</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="n">
+        <v>398.21</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>44211</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3152209</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Order 3152209 Swish +46722017122</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="n">
+        <v>47.79</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>44211</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3152209</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Order 3152209 Swish +46722017122</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>446</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>44212</v>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>FRESH STOCKHOLM HÄSSEL K6885</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>172.66</v>
+      </c>
+      <c r="F59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>44212</v>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>FRESH STOCKHOLM HÄSSEL K6885</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>20.72</v>
+      </c>
+      <c r="F60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>44212</v>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>FRESH STOCKHOLM HÄSSEL K6885</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="n">
+        <v>193.38</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>44213</v>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>442.54</v>
+      </c>
+      <c r="F62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>44213</v>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>53.1</v>
+      </c>
+      <c r="F63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>44213</v>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="n">
+        <v>495.64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 15 new rows for week ending 2021-01-24 (total 78 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1703,6 +1703,286 @@
         <v>495.64</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>44216</v>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>1250</v>
+      </c>
+      <c r="F65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>44216</v>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" t="inlineStr"/>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>44216</v>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="n">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>44217</v>
+      </c>
+      <c r="B68" t="n">
+        <v>9211635</v>
+      </c>
+      <c r="C68" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Order 9211635 Swish +46707883566</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>1036.61</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>44217</v>
+      </c>
+      <c r="B69" t="n">
+        <v>9211635</v>
+      </c>
+      <c r="C69" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Order 9211635 Swish +46707883566</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="n">
+        <v>124.39</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>44217</v>
+      </c>
+      <c r="B70" t="n">
+        <v>9211635</v>
+      </c>
+      <c r="C70" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Order 9211635 Swish +46707883566</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>1161</v>
+      </c>
+      <c r="F70" t="inlineStr"/>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>44218</v>
+      </c>
+      <c r="B71" t="n">
+        <v>5222159</v>
+      </c>
+      <c r="C71" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Order 5222159 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="n">
+        <v>547.3200000000001</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>44218</v>
+      </c>
+      <c r="B72" t="n">
+        <v>5222159</v>
+      </c>
+      <c r="C72" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Order 5222159 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="n">
+        <v>65.68000000000001</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>44218</v>
+      </c>
+      <c r="B73" t="n">
+        <v>5222159</v>
+      </c>
+      <c r="C73" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Order 5222159 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>613</v>
+      </c>
+      <c r="F73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>44218</v>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>1529.97</v>
+      </c>
+      <c r="F74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>44218</v>
+      </c>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>183.59</v>
+      </c>
+      <c r="F75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>44218</v>
+      </c>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="n">
+        <v>1713.56</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>44219</v>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>OKQ8 K0135</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>764.26</v>
+      </c>
+      <c r="F77" t="inlineStr"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>44219</v>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>OKQ8 K0135</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>191.07</v>
+      </c>
+      <c r="F78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>44219</v>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>OKQ8 K0135</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="n">
+        <v>955.33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 24 new rows for week ending 2021-01-31 (total 102 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1983,6 +1983,480 @@
         <v>955.33</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>44221</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1252204</v>
+      </c>
+      <c r="C80" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Order 1252204 Swish +46730393329</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="n">
+        <v>502.68</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>44221</v>
+      </c>
+      <c r="B81" t="n">
+        <v>1252204</v>
+      </c>
+      <c r="C81" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Order 1252204 Swish +46730393329</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="n">
+        <v>60.32</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>44221</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1252204</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Order 1252204 Swish +46730393329</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>563</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>ELGIGANTEN STHL K0135</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>808.8</v>
+      </c>
+      <c r="F83" t="inlineStr"/>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>ELGIGANTEN STHL K0135</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>202.2</v>
+      </c>
+      <c r="F84" t="inlineStr"/>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>ELGIGANTEN STHL K0135</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="n">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B86" t="n">
+        <v>8261903</v>
+      </c>
+      <c r="C86" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Order 8261903 Swish +46733304498</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B87" t="n">
+        <v>8261903</v>
+      </c>
+      <c r="C87" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Order 8261903 Swish +46733304498</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>44222</v>
+      </c>
+      <c r="B88" t="n">
+        <v>8261903</v>
+      </c>
+      <c r="C88" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Order 8261903 Swish +46733304498</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>774</v>
+      </c>
+      <c r="F88" t="inlineStr"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B89" t="n">
+        <v>4311427</v>
+      </c>
+      <c r="C89" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Order 4311427 Swish +46727242898</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="n">
+        <v>806.25</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B90" t="n">
+        <v>4311427</v>
+      </c>
+      <c r="C90" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Order 4311427 Swish +46727242898</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="n">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B91" t="n">
+        <v>4311427</v>
+      </c>
+      <c r="C91" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Order 4311427 Swish +46727242898</t>
+        </is>
+      </c>
+      <c r="E91" t="n">
+        <v>903</v>
+      </c>
+      <c r="F91" t="inlineStr"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B92" t="n">
+        <v>5311815</v>
+      </c>
+      <c r="C92" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Order 5311815 Swish +46708751433</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B93" t="n">
+        <v>5311815</v>
+      </c>
+      <c r="C93" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Order 5311815 Swish +46708751433</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B94" t="n">
+        <v>5311815</v>
+      </c>
+      <c r="C94" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Order 5311815 Swish +46708751433</t>
+        </is>
+      </c>
+      <c r="E94" t="n">
+        <v>690</v>
+      </c>
+      <c r="F94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B95" t="n">
+        <v>2311908</v>
+      </c>
+      <c r="C95" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Order 2311908 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="n">
+        <v>739.29</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B96" t="n">
+        <v>2311908</v>
+      </c>
+      <c r="C96" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Order 2311908 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="n">
+        <v>88.70999999999999</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B97" t="n">
+        <v>2311908</v>
+      </c>
+      <c r="C97" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Order 2311908 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E97" t="n">
+        <v>828</v>
+      </c>
+      <c r="F97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B98" t="n">
+        <v>9311931</v>
+      </c>
+      <c r="C98" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Order 9311931 Swish +46706649892</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B99" t="n">
+        <v>9311931</v>
+      </c>
+      <c r="C99" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Order 9311931 Swish +46706649892</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B100" t="n">
+        <v>9311931</v>
+      </c>
+      <c r="C100" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Order 9311931 Swish +46706649892</t>
+        </is>
+      </c>
+      <c r="E100" t="n">
+        <v>774</v>
+      </c>
+      <c r="F100" t="inlineStr"/>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B101" t="n">
+        <v>3312155</v>
+      </c>
+      <c r="C101" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Order 3312155 Swish +46707676358</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="n">
+        <v>1106.25</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B102" t="n">
+        <v>3312155</v>
+      </c>
+      <c r="C102" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Order 3312155 Swish +46707676358</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="n">
+        <v>132.75</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>44227</v>
+      </c>
+      <c r="B103" t="n">
+        <v>3312155</v>
+      </c>
+      <c r="C103" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Order 3312155 Swish +46707676358</t>
+        </is>
+      </c>
+      <c r="E103" t="n">
+        <v>1239</v>
+      </c>
+      <c r="F103" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 36 new rows for week ending 2021-02-07 (total 138 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F103"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2457,6 +2457,700 @@
       </c>
       <c r="F103" t="inlineStr"/>
     </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B104" t="n">
+        <v>6021019</v>
+      </c>
+      <c r="C104" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Order  6021019 Swish +46707393913</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B105" t="n">
+        <v>6021019</v>
+      </c>
+      <c r="C105" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Order  6021019 Swish +46707393913</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B106" t="n">
+        <v>6021019</v>
+      </c>
+      <c r="C106" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Order  6021019 Swish +46707393913</t>
+        </is>
+      </c>
+      <c r="E106" t="n">
+        <v>474</v>
+      </c>
+      <c r="F106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B107" t="n">
+        <v>5021732</v>
+      </c>
+      <c r="C107" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Order 5021732 Swish +46764282407</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="n">
+        <v>801.79</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B108" t="n">
+        <v>5021732</v>
+      </c>
+      <c r="C108" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Order 5021732 Swish +46764282407</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="n">
+        <v>96.20999999999999</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B109" t="n">
+        <v>5021732</v>
+      </c>
+      <c r="C109" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Order 5021732 Swish +46764282407</t>
+        </is>
+      </c>
+      <c r="E109" t="n">
+        <v>898</v>
+      </c>
+      <c r="F109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B110" t="n">
+        <v>9021920</v>
+      </c>
+      <c r="C110" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Order 9021920 Swish +46704008971</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="n">
+        <v>655.36</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B111" t="n">
+        <v>9021920</v>
+      </c>
+      <c r="C111" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Order 9021920 Swish +46704008971</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="n">
+        <v>78.64</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>44229</v>
+      </c>
+      <c r="B112" t="n">
+        <v>9021920</v>
+      </c>
+      <c r="C112" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Order 9021920 Swish +46704008971</t>
+        </is>
+      </c>
+      <c r="E112" t="n">
+        <v>734</v>
+      </c>
+      <c r="F112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B113" t="n">
+        <v>6040901</v>
+      </c>
+      <c r="C113" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Order 6040901 Swish +46736813550</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B114" t="n">
+        <v>6040901</v>
+      </c>
+      <c r="C114" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Order 6040901 Swish +46736813550</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B115" t="n">
+        <v>6040901</v>
+      </c>
+      <c r="C115" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Order 6040901 Swish +46736813550</t>
+        </is>
+      </c>
+      <c r="E115" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E116" t="n">
+        <v>1196</v>
+      </c>
+      <c r="F116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E117" t="n">
+        <v>299</v>
+      </c>
+      <c r="F117" t="inlineStr"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B118" t="inlineStr"/>
+      <c r="C118" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="n">
+        <v>1495</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B119" t="inlineStr"/>
+      <c r="C119" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>FACEBK PR3NBYWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E119" t="n">
+        <v>257</v>
+      </c>
+      <c r="F119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B120" t="inlineStr"/>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>FACEBK PR3NBYWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E120" t="n">
+        <v>0</v>
+      </c>
+      <c r="F120" t="inlineStr"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>44231</v>
+      </c>
+      <c r="B121" t="inlineStr"/>
+      <c r="C121" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>FACEBK PR3NBYWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr"/>
+      <c r="F121" t="n">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B122" t="n">
+        <v>6051243</v>
+      </c>
+      <c r="C122" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Order 6051243 Swish +46705757460</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="n">
+        <v>1239.29</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B123" t="n">
+        <v>6051243</v>
+      </c>
+      <c r="C123" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Order 6051243 Swish +46705757460</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr"/>
+      <c r="F123" t="n">
+        <v>148.71</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B124" t="n">
+        <v>6051243</v>
+      </c>
+      <c r="C124" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Order 6051243 Swish +46705757460</t>
+        </is>
+      </c>
+      <c r="E124" t="n">
+        <v>1388</v>
+      </c>
+      <c r="F124" t="inlineStr"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B125" t="n">
+        <v>5051600</v>
+      </c>
+      <c r="C125" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Order 5051600 Swish +46793490885</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="n">
+        <v>928.5700000000001</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B126" t="n">
+        <v>5051600</v>
+      </c>
+      <c r="C126" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Order 5051600 Swish +46793490885</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="n">
+        <v>111.43</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B127" t="n">
+        <v>5051600</v>
+      </c>
+      <c r="C127" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Order 5051600 Swish +46793490885</t>
+        </is>
+      </c>
+      <c r="E127" t="n">
+        <v>1040</v>
+      </c>
+      <c r="F127" t="inlineStr"/>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B128" t="inlineStr"/>
+      <c r="C128" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E128" t="n">
+        <v>527.78</v>
+      </c>
+      <c r="F128" t="inlineStr"/>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B129" t="inlineStr"/>
+      <c r="C129" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E129" t="n">
+        <v>63.33</v>
+      </c>
+      <c r="F129" t="inlineStr"/>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>44232</v>
+      </c>
+      <c r="B130" t="inlineStr"/>
+      <c r="C130" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr"/>
+      <c r="F130" t="n">
+        <v>591.11</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1070903</v>
+      </c>
+      <c r="C131" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Order 1070903 Swish +46709224929</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="n">
+        <v>1008.93</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1070903</v>
+      </c>
+      <c r="C132" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Order 1070903 Swish +46709224929</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="n">
+        <v>121.07</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1070903</v>
+      </c>
+      <c r="C133" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Order 1070903 Swish +46709224929</t>
+        </is>
+      </c>
+      <c r="E133" t="n">
+        <v>1130</v>
+      </c>
+      <c r="F133" t="inlineStr"/>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1070927</v>
+      </c>
+      <c r="C134" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Order 1070927 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr"/>
+      <c r="F134" t="n">
+        <v>806.25</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1070927</v>
+      </c>
+      <c r="C135" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Order 1070927 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="n">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1070927</v>
+      </c>
+      <c r="C136" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Order 1070927 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E136" t="n">
+        <v>903</v>
+      </c>
+      <c r="F136" t="inlineStr"/>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B137" t="inlineStr"/>
+      <c r="C137" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E137" t="n">
+        <v>733.41</v>
+      </c>
+      <c r="F137" t="inlineStr"/>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B138" t="inlineStr"/>
+      <c r="C138" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E138" t="n">
+        <v>183.35</v>
+      </c>
+      <c r="F138" t="inlineStr"/>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>44234</v>
+      </c>
+      <c r="B139" t="inlineStr"/>
+      <c r="C139" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="n">
+        <v>916.76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 33 new rows for week ending 2021-02-14 (total 171 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3151,6 +3151,646 @@
         <v>916.76</v>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B140" t="n">
+        <v>4081100</v>
+      </c>
+      <c r="C140" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Order 4081100 Swish +46721731568</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr"/>
+      <c r="F140" t="n">
+        <v>493.75</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B141" t="n">
+        <v>4081100</v>
+      </c>
+      <c r="C141" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Order 4081100 Swish +46721731568</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr"/>
+      <c r="F141" t="n">
+        <v>59.25</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B142" t="n">
+        <v>4081100</v>
+      </c>
+      <c r="C142" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Order 4081100 Swish +46721731568</t>
+        </is>
+      </c>
+      <c r="E142" t="n">
+        <v>553</v>
+      </c>
+      <c r="F142" t="inlineStr"/>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>0081101</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Order 0081101 Swish +46704184802</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr"/>
+      <c r="F143" t="n">
+        <v>433.04</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>0081101</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Order 0081101Swish +46704184802</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr"/>
+      <c r="F144" t="n">
+        <v>51.96</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>44235</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>0081101</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Order 0081101Swish +46704184802</t>
+        </is>
+      </c>
+      <c r="E145" t="n">
+        <v>485</v>
+      </c>
+      <c r="F145" t="inlineStr"/>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B146" t="n">
+        <v>4092012</v>
+      </c>
+      <c r="C146" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Order 4092012 Swish +46703019983</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr"/>
+      <c r="F146" t="n">
+        <v>1116.07</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B147" t="n">
+        <v>4092012</v>
+      </c>
+      <c r="C147" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Order 4092012 Swish +46703019983</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr"/>
+      <c r="F147" t="n">
+        <v>133.93</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B148" t="n">
+        <v>4092012</v>
+      </c>
+      <c r="C148" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Order 4092012 Swish +46703019983</t>
+        </is>
+      </c>
+      <c r="E148" t="n">
+        <v>1250</v>
+      </c>
+      <c r="F148" t="inlineStr"/>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B149" t="n">
+        <v>4092240</v>
+      </c>
+      <c r="C149" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Order 4092240 Swish +46763160083</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr"/>
+      <c r="F149" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B150" t="n">
+        <v>4092240</v>
+      </c>
+      <c r="C150" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Order 4092240 Swish +46763160083</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr"/>
+      <c r="F150" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="n">
+        <v>44236</v>
+      </c>
+      <c r="B151" t="n">
+        <v>4092240</v>
+      </c>
+      <c r="C151" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Order 4092240 Swish +46763160083</t>
+        </is>
+      </c>
+      <c r="E151" t="n">
+        <v>474</v>
+      </c>
+      <c r="F151" t="inlineStr"/>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>44237</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1102020</v>
+      </c>
+      <c r="C152" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Order 1102020 Swish +46709703734</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr"/>
+      <c r="F152" t="n">
+        <v>493.75</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>44237</v>
+      </c>
+      <c r="B153" t="n">
+        <v>1102020</v>
+      </c>
+      <c r="C153" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Order 1102020 Swish +46709703734</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr"/>
+      <c r="F153" t="n">
+        <v>59.25</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>44237</v>
+      </c>
+      <c r="B154" t="n">
+        <v>1102020</v>
+      </c>
+      <c r="C154" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Order 1102020 Swish +46709703734</t>
+        </is>
+      </c>
+      <c r="E154" t="n">
+        <v>553</v>
+      </c>
+      <c r="F154" t="inlineStr"/>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B155" t="inlineStr"/>
+      <c r="C155" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>FACEBK HMUT22KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E155" t="n">
+        <v>415</v>
+      </c>
+      <c r="F155" t="inlineStr"/>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B156" t="inlineStr"/>
+      <c r="C156" t="inlineStr"/>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>FACEBK HMUT22KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E156" t="n">
+        <v>0</v>
+      </c>
+      <c r="F156" t="inlineStr"/>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B157" t="inlineStr"/>
+      <c r="C157" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>FACEBK HMUT22KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="n">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B158" t="inlineStr"/>
+      <c r="C158" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E158" t="n">
+        <v>845.01</v>
+      </c>
+      <c r="F158" t="inlineStr"/>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B159" t="inlineStr"/>
+      <c r="C159" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E159" t="n">
+        <v>101.4</v>
+      </c>
+      <c r="F159" t="inlineStr"/>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="n">
+        <v>44238</v>
+      </c>
+      <c r="B160" t="inlineStr"/>
+      <c r="C160" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr"/>
+      <c r="F160" t="n">
+        <v>946.41</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>44239</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>0122148</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Order 0122148 Swish +46732518928</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr"/>
+      <c r="F161" t="n">
+        <v>655.36</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>44239</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>0122148</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Order 0122148 Swish +46732518928</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr"/>
+      <c r="F162" t="n">
+        <v>78.64</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>44239</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>0122148</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Order 0122148 Swish +46732518928</t>
+        </is>
+      </c>
+      <c r="E163" t="n">
+        <v>734</v>
+      </c>
+      <c r="F163" t="inlineStr"/>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B164" t="inlineStr"/>
+      <c r="C164" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E164" t="n">
+        <v>645.16</v>
+      </c>
+      <c r="F164" t="inlineStr"/>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B165" t="inlineStr"/>
+      <c r="C165" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E165" t="n">
+        <v>161.29</v>
+      </c>
+      <c r="F165" t="inlineStr"/>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B166" t="inlineStr"/>
+      <c r="C166" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="n">
+        <v>806.45</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B167" t="inlineStr"/>
+      <c r="C167" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E167" t="n">
+        <v>272.32</v>
+      </c>
+      <c r="F167" t="inlineStr"/>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B168" t="inlineStr"/>
+      <c r="C168" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E168" t="n">
+        <v>32.68</v>
+      </c>
+      <c r="F168" t="inlineStr"/>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>44240</v>
+      </c>
+      <c r="B169" t="inlineStr"/>
+      <c r="C169" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr"/>
+      <c r="F169" t="n">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>44241</v>
+      </c>
+      <c r="B170" t="inlineStr"/>
+      <c r="C170" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E170" t="n">
+        <v>285.09</v>
+      </c>
+      <c r="F170" t="inlineStr"/>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>44241</v>
+      </c>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E171" t="n">
+        <v>34.21</v>
+      </c>
+      <c r="F171" t="inlineStr"/>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>44241</v>
+      </c>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr"/>
+      <c r="F172" t="n">
+        <v>319.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 18 new rows for week ending 2021-02-21 (total 189 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F172"/>
+  <dimension ref="A1:F190"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3791,6 +3791,338 @@
         <v>319.3</v>
       </c>
     </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>44242</v>
+      </c>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E173" t="n">
+        <v>156.88</v>
+      </c>
+      <c r="F173" t="inlineStr"/>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>44242</v>
+      </c>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E174" t="n">
+        <v>18.82</v>
+      </c>
+      <c r="F174" t="inlineStr"/>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>44242</v>
+      </c>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr"/>
+      <c r="F175" t="n">
+        <v>175.7</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B176" t="n">
+        <v>2181305</v>
+      </c>
+      <c r="C176" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Order 2181305 Swish +46734333950</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B177" t="n">
+        <v>2181305</v>
+      </c>
+      <c r="C177" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Order 2181305 Swish +46734333950</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr"/>
+      <c r="F177" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B178" t="n">
+        <v>2181305</v>
+      </c>
+      <c r="C178" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Order 2181305 Swish +46734333950</t>
+        </is>
+      </c>
+      <c r="E178" t="n">
+        <v>774</v>
+      </c>
+      <c r="F178" t="inlineStr"/>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B179" t="n">
+        <v>4181944</v>
+      </c>
+      <c r="C179" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Order 4181944 Swish +46763141239</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr"/>
+      <c r="F179" t="n">
+        <v>725.89</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B180" t="n">
+        <v>4181944</v>
+      </c>
+      <c r="C180" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Order 4181944 Swish +46763141239</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr"/>
+      <c r="F180" t="n">
+        <v>87.11</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>44245</v>
+      </c>
+      <c r="B181" t="n">
+        <v>4181944</v>
+      </c>
+      <c r="C181" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Order 4181944 Swish +46763141239</t>
+        </is>
+      </c>
+      <c r="E181" t="n">
+        <v>813</v>
+      </c>
+      <c r="F181" t="inlineStr"/>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>FACEBK J3NSNYWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E182" t="n">
+        <v>415</v>
+      </c>
+      <c r="F182" t="inlineStr"/>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>FACEBK J3NSNYWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E183" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" t="inlineStr"/>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B184" t="inlineStr"/>
+      <c r="C184" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>FACEBK YCYG9YSZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E184" t="n">
+        <v>3</v>
+      </c>
+      <c r="F184" t="inlineStr"/>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B185" t="inlineStr"/>
+      <c r="C185" t="inlineStr"/>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>FACEBK YCYG9YSZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E185" t="n">
+        <v>0</v>
+      </c>
+      <c r="F185" t="inlineStr"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B186" t="inlineStr"/>
+      <c r="C186" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>FACEBK YCYG9YSZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr"/>
+      <c r="F186" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B187" t="inlineStr"/>
+      <c r="C187" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>FACEBK J3NSNYWY62 K6885</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr"/>
+      <c r="F187" t="n">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B188" t="inlineStr"/>
+      <c r="C188" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E188" t="n">
+        <v>204.29</v>
+      </c>
+      <c r="F188" t="inlineStr"/>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B189" t="inlineStr"/>
+      <c r="C189" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E189" t="n">
+        <v>24.51</v>
+      </c>
+      <c r="F189" t="inlineStr"/>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="n">
+        <v>44247</v>
+      </c>
+      <c r="B190" t="inlineStr"/>
+      <c r="C190" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr"/>
+      <c r="F190" t="n">
+        <v>228.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 42 new rows for week ending 2021-02-28 (total 231 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F232"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4123,6 +4123,816 @@
         <v>228.8</v>
       </c>
     </row>
+    <row r="191">
+      <c r="A191" s="2" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>0221443</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Order 0221443 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr"/>
+      <c r="F191" t="n">
+        <v>502.68</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>0221443</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Order 0221443 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr"/>
+      <c r="F192" t="n">
+        <v>60.32</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="n">
+        <v>44249</v>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>0221443</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Order 0221443 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E193" t="n">
+        <v>563</v>
+      </c>
+      <c r="F193" t="inlineStr"/>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>0241219</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Order 0241219 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr"/>
+      <c r="F194" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>0241219</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Order 0241219 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="n">
+        <v>44251</v>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>0241219</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Order 0241219 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E196" t="n">
+        <v>774</v>
+      </c>
+      <c r="F196" t="inlineStr"/>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B197" t="n">
+        <v>6251432</v>
+      </c>
+      <c r="C197" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Order 6251432 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr"/>
+      <c r="F197" t="n">
+        <v>1085.71</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B198" t="n">
+        <v>6251432</v>
+      </c>
+      <c r="C198" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Order 6251432 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr"/>
+      <c r="F198" t="n">
+        <v>130.29</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="n">
+        <v>44252</v>
+      </c>
+      <c r="B199" t="n">
+        <v>6251432</v>
+      </c>
+      <c r="C199" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Order 6251432 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E199" t="n">
+        <v>1216</v>
+      </c>
+      <c r="F199" t="inlineStr"/>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B200" t="n">
+        <v>5271529</v>
+      </c>
+      <c r="C200" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Order 5271529 Swish +46705558420</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr"/>
+      <c r="F200" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B201" t="n">
+        <v>5271529</v>
+      </c>
+      <c r="C201" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Order 5271529 Swish +46705558420</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr"/>
+      <c r="F201" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B202" t="n">
+        <v>5271529</v>
+      </c>
+      <c r="C202" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Order 5271529 Swish +46705558420</t>
+        </is>
+      </c>
+      <c r="E202" t="n">
+        <v>690</v>
+      </c>
+      <c r="F202" t="inlineStr"/>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B203" t="n">
+        <v>9272123</v>
+      </c>
+      <c r="C203" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Order 9272123 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr"/>
+      <c r="F203" t="n">
+        <v>537.5</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B204" t="n">
+        <v>9272123</v>
+      </c>
+      <c r="C204" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Order 9272123 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr"/>
+      <c r="F204" t="n">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B205" t="n">
+        <v>9272123</v>
+      </c>
+      <c r="C205" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Order 9272123 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E205" t="n">
+        <v>602</v>
+      </c>
+      <c r="F205" t="inlineStr"/>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B206" t="inlineStr"/>
+      <c r="C206" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E206" t="n">
+        <v>2009.15</v>
+      </c>
+      <c r="F206" t="inlineStr"/>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B207" t="inlineStr"/>
+      <c r="C207" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E207" t="n">
+        <v>241.1</v>
+      </c>
+      <c r="F207" t="inlineStr"/>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B208" t="inlineStr"/>
+      <c r="C208" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr"/>
+      <c r="F208" t="n">
+        <v>2250.25</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B209" t="inlineStr"/>
+      <c r="C209" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E209" t="n">
+        <v>149.6</v>
+      </c>
+      <c r="F209" t="inlineStr"/>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B210" t="inlineStr"/>
+      <c r="C210" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E210" t="n">
+        <v>37.4</v>
+      </c>
+      <c r="F210" t="inlineStr"/>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="n">
+        <v>44253</v>
+      </c>
+      <c r="B211" t="inlineStr"/>
+      <c r="C211" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr"/>
+      <c r="F211" t="n">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B212" t="inlineStr"/>
+      <c r="C212" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E212" t="n">
+        <v>468.6</v>
+      </c>
+      <c r="F212" t="inlineStr"/>
+    </row>
+    <row r="213">
+      <c r="A213" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B213" t="inlineStr"/>
+      <c r="C213" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E213" t="n">
+        <v>56.23</v>
+      </c>
+      <c r="F213" t="inlineStr"/>
+    </row>
+    <row r="214">
+      <c r="A214" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B214" t="inlineStr"/>
+      <c r="C214" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr"/>
+      <c r="F214" t="n">
+        <v>524.83</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B215" t="inlineStr"/>
+      <c r="C215" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E215" t="n">
+        <v>785.47</v>
+      </c>
+      <c r="F215" t="inlineStr"/>
+    </row>
+    <row r="216">
+      <c r="A216" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B216" t="inlineStr"/>
+      <c r="C216" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E216" t="n">
+        <v>196.37</v>
+      </c>
+      <c r="F216" t="inlineStr"/>
+    </row>
+    <row r="217">
+      <c r="A217" s="2" t="n">
+        <v>44254</v>
+      </c>
+      <c r="B217" t="inlineStr"/>
+      <c r="C217" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr"/>
+      <c r="F217" t="n">
+        <v>981.84</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B218" t="n">
+        <v>3281219</v>
+      </c>
+      <c r="C218" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Order 3281219 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr"/>
+      <c r="F218" t="n">
+        <v>769.64</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B219" t="n">
+        <v>3281219</v>
+      </c>
+      <c r="C219" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Order 3281219 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr"/>
+      <c r="F219" t="n">
+        <v>92.36</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B220" t="n">
+        <v>3281219</v>
+      </c>
+      <c r="C220" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Order 3281219 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E220" t="n">
+        <v>862</v>
+      </c>
+      <c r="F220" t="inlineStr"/>
+    </row>
+    <row r="221">
+      <c r="A221" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B221" t="n">
+        <v>3282108</v>
+      </c>
+      <c r="C221" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Order 3282108 Swish +46707678891</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr"/>
+      <c r="F221" t="n">
+        <v>547.3200000000001</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B222" t="n">
+        <v>3282108</v>
+      </c>
+      <c r="C222" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Order 3282108 Swish +46707678891</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr"/>
+      <c r="F222" t="n">
+        <v>65.68000000000001</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B223" t="n">
+        <v>3282108</v>
+      </c>
+      <c r="C223" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Order 3282108 Swish +46707678891</t>
+        </is>
+      </c>
+      <c r="E223" t="n">
+        <v>613</v>
+      </c>
+      <c r="F223" t="inlineStr"/>
+    </row>
+    <row r="224">
+      <c r="A224" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B224" t="inlineStr"/>
+      <c r="C224" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E224" t="n">
+        <v>22.23</v>
+      </c>
+      <c r="F224" t="inlineStr"/>
+    </row>
+    <row r="225">
+      <c r="A225" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B225" t="inlineStr"/>
+      <c r="C225" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E225" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="F225" t="inlineStr"/>
+    </row>
+    <row r="226">
+      <c r="A226" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B226" t="inlineStr"/>
+      <c r="C226" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr"/>
+      <c r="F226" t="n">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B227" t="inlineStr"/>
+      <c r="C227" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E227" t="n">
+        <v>694.38</v>
+      </c>
+      <c r="F227" t="inlineStr"/>
+    </row>
+    <row r="228">
+      <c r="A228" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B228" t="inlineStr"/>
+      <c r="C228" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E228" t="n">
+        <v>83.33</v>
+      </c>
+      <c r="F228" t="inlineStr"/>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B229" t="inlineStr"/>
+      <c r="C229" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr"/>
+      <c r="F229" t="n">
+        <v>777.71</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B230" t="inlineStr"/>
+      <c r="C230" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E230" t="n">
+        <v>379.64</v>
+      </c>
+      <c r="F230" t="inlineStr"/>
+    </row>
+    <row r="231">
+      <c r="A231" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B231" t="inlineStr"/>
+      <c r="C231" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E231" t="n">
+        <v>45.56</v>
+      </c>
+      <c r="F231" t="inlineStr"/>
+    </row>
+    <row r="232">
+      <c r="A232" s="2" t="n">
+        <v>44255</v>
+      </c>
+      <c r="B232" t="inlineStr"/>
+      <c r="C232" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr"/>
+      <c r="F232" t="n">
+        <v>425.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 81 new rows for week ending 2021-03-07 (total 312 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F232"/>
+  <dimension ref="A1:F313"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4933,6 +4933,1716 @@
         <v>425.2</v>
       </c>
     </row>
+    <row r="233">
+      <c r="A233" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B233" t="n">
+        <v>8011921</v>
+      </c>
+      <c r="C233" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Order 8011921 Swish +46793490885</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr"/>
+      <c r="F233" t="n">
+        <v>1141.07</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B234" t="n">
+        <v>8011921</v>
+      </c>
+      <c r="C234" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Order 8011921 Swish +46793490885</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr"/>
+      <c r="F234" t="n">
+        <v>136.93</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B235" t="n">
+        <v>8011921</v>
+      </c>
+      <c r="C235" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Order 8011921 Swish +46793490885</t>
+        </is>
+      </c>
+      <c r="E235" t="n">
+        <v>1278</v>
+      </c>
+      <c r="F235" t="inlineStr"/>
+    </row>
+    <row r="236">
+      <c r="A236" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B236" t="n">
+        <v>1012229</v>
+      </c>
+      <c r="C236" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Order 1012229 Swish +46760633899</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr"/>
+      <c r="F236" t="n">
+        <v>836.61</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B237" t="n">
+        <v>1012229</v>
+      </c>
+      <c r="C237" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Order 1012229 Swish +46760633899</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr"/>
+      <c r="F237" t="n">
+        <v>100.39</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B238" t="n">
+        <v>1012229</v>
+      </c>
+      <c r="C238" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Order 1012229 Swish +46760633899</t>
+        </is>
+      </c>
+      <c r="E238" t="n">
+        <v>937</v>
+      </c>
+      <c r="F238" t="inlineStr"/>
+    </row>
+    <row r="239">
+      <c r="A239" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B239" t="inlineStr"/>
+      <c r="C239" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Multicooker reim</t>
+        </is>
+      </c>
+      <c r="E239" t="n">
+        <v>1278.4</v>
+      </c>
+      <c r="F239" t="inlineStr"/>
+    </row>
+    <row r="240">
+      <c r="A240" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B240" t="inlineStr"/>
+      <c r="C240" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Multicooker reim</t>
+        </is>
+      </c>
+      <c r="E240" t="n">
+        <v>319.6</v>
+      </c>
+      <c r="F240" t="inlineStr"/>
+    </row>
+    <row r="241">
+      <c r="A241" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B241" t="inlineStr"/>
+      <c r="C241" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Multicooker reim</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr"/>
+      <c r="F241" t="n">
+        <v>1598</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B242" t="inlineStr"/>
+      <c r="C242" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E242" t="n">
+        <v>266.96</v>
+      </c>
+      <c r="F242" t="inlineStr"/>
+    </row>
+    <row r="243">
+      <c r="A243" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B243" t="inlineStr"/>
+      <c r="C243" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E243" t="n">
+        <v>32.04</v>
+      </c>
+      <c r="F243" t="inlineStr"/>
+    </row>
+    <row r="244">
+      <c r="A244" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B244" t="inlineStr"/>
+      <c r="C244" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr"/>
+      <c r="F244" t="n">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>0021812</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Order 0021812 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr"/>
+      <c r="F245" t="n">
+        <v>547.3200000000001</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>0021812</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Order 0021812 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr"/>
+      <c r="F246" t="n">
+        <v>65.68000000000001</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>0021812</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Order 0021812 Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E247" t="n">
+        <v>613</v>
+      </c>
+      <c r="F247" t="inlineStr"/>
+    </row>
+    <row r="248">
+      <c r="A248" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>Reko1</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr"/>
+      <c r="F248" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>Reko1</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr"/>
+      <c r="F249" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>Reko1</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E250" t="n">
+        <v>258</v>
+      </c>
+      <c r="F250" t="inlineStr"/>
+    </row>
+    <row r="251">
+      <c r="A251" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>Reko2</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr"/>
+      <c r="F251" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>Reko2</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr"/>
+      <c r="F252" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Reko2</t>
+        </is>
+      </c>
+      <c r="C253" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E253" t="n">
+        <v>387</v>
+      </c>
+      <c r="F253" t="inlineStr"/>
+    </row>
+    <row r="254">
+      <c r="A254" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Reko3</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46702920861</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr"/>
+      <c r="F254" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Reko3</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46702920861</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr"/>
+      <c r="F255" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>Reko3</t>
+        </is>
+      </c>
+      <c r="C256" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46702920861</t>
+        </is>
+      </c>
+      <c r="E256" t="n">
+        <v>237</v>
+      </c>
+      <c r="F256" t="inlineStr"/>
+    </row>
+    <row r="257">
+      <c r="A257" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>Reko4</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46707697799</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr"/>
+      <c r="F257" t="n">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Reko4</t>
+        </is>
+      </c>
+      <c r="C258" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46707697799</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr"/>
+      <c r="F258" t="n">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Reko4</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46707697799</t>
+        </is>
+      </c>
+      <c r="E259" t="n">
+        <v>208</v>
+      </c>
+      <c r="F259" t="inlineStr"/>
+    </row>
+    <row r="260">
+      <c r="A260" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Reko5</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703721616</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr"/>
+      <c r="F260" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Reko5</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703721616</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr"/>
+      <c r="F261" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Reko5</t>
+        </is>
+      </c>
+      <c r="C262" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703721616</t>
+        </is>
+      </c>
+      <c r="E262" t="n">
+        <v>158</v>
+      </c>
+      <c r="F262" t="inlineStr"/>
+    </row>
+    <row r="263">
+      <c r="A263" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>Reko6</t>
+        </is>
+      </c>
+      <c r="C263" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46737600861</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr"/>
+      <c r="F263" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Reko6</t>
+        </is>
+      </c>
+      <c r="C264" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46737600861</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr"/>
+      <c r="F264" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Reko6</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46737600861</t>
+        </is>
+      </c>
+      <c r="E265" t="n">
+        <v>79</v>
+      </c>
+      <c r="F265" t="inlineStr"/>
+    </row>
+    <row r="266">
+      <c r="A266" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Reko7</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703344337</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr"/>
+      <c r="F266" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Reko7</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703344337</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr"/>
+      <c r="F267" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Reko7</t>
+        </is>
+      </c>
+      <c r="C268" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46703344337</t>
+        </is>
+      </c>
+      <c r="E268" t="n">
+        <v>258</v>
+      </c>
+      <c r="F268" t="inlineStr"/>
+    </row>
+    <row r="269">
+      <c r="A269" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Reko8</t>
+        </is>
+      </c>
+      <c r="C269" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46739321339</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr"/>
+      <c r="F269" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>Reko8</t>
+        </is>
+      </c>
+      <c r="C270" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D270" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46739321339</t>
+        </is>
+      </c>
+      <c r="E270" t="inlineStr"/>
+      <c r="F270" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="2" t="n">
+        <v>44256</v>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Reko8</t>
+        </is>
+      </c>
+      <c r="C271" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46739321339</t>
+        </is>
+      </c>
+      <c r="E271" t="n">
+        <v>79</v>
+      </c>
+      <c r="F271" t="inlineStr"/>
+    </row>
+    <row r="272">
+      <c r="A272" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Reko9</t>
+        </is>
+      </c>
+      <c r="C272" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D272" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46767782009</t>
+        </is>
+      </c>
+      <c r="E272" t="inlineStr"/>
+      <c r="F272" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>Reko9</t>
+        </is>
+      </c>
+      <c r="C273" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46767782009</t>
+        </is>
+      </c>
+      <c r="E273" t="inlineStr"/>
+      <c r="F273" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Reko9</t>
+        </is>
+      </c>
+      <c r="C274" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46767782009</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>237</v>
+      </c>
+      <c r="F274" t="inlineStr"/>
+    </row>
+    <row r="275">
+      <c r="A275" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Reko10</t>
+        </is>
+      </c>
+      <c r="C275" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E275" t="inlineStr"/>
+      <c r="F275" t="n">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Reko10</t>
+        </is>
+      </c>
+      <c r="C276" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E276" t="inlineStr"/>
+      <c r="F276" t="n">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Reko10</t>
+        </is>
+      </c>
+      <c r="C277" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>208</v>
+      </c>
+      <c r="F277" t="inlineStr"/>
+    </row>
+    <row r="278">
+      <c r="A278" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Reko11</t>
+        </is>
+      </c>
+      <c r="C278" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E278" t="inlineStr"/>
+      <c r="F278" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Reko11</t>
+        </is>
+      </c>
+      <c r="C279" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E279" t="inlineStr"/>
+      <c r="F279" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Reko11</t>
+        </is>
+      </c>
+      <c r="C280" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E280" t="n">
+        <v>258</v>
+      </c>
+      <c r="F280" t="inlineStr"/>
+    </row>
+    <row r="281">
+      <c r="A281" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Reko12</t>
+        </is>
+      </c>
+      <c r="C281" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E281" t="inlineStr"/>
+      <c r="F281" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Reko12</t>
+        </is>
+      </c>
+      <c r="C282" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E282" t="inlineStr"/>
+      <c r="F282" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Reko12</t>
+        </is>
+      </c>
+      <c r="C283" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D283" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E283" t="n">
+        <v>129</v>
+      </c>
+      <c r="F283" t="inlineStr"/>
+    </row>
+    <row r="284">
+      <c r="A284" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Reko13</t>
+        </is>
+      </c>
+      <c r="C284" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D284" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46723107438</t>
+        </is>
+      </c>
+      <c r="E284" t="inlineStr"/>
+      <c r="F284" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Reko13</t>
+        </is>
+      </c>
+      <c r="C285" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D285" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46723107438</t>
+        </is>
+      </c>
+      <c r="E285" t="inlineStr"/>
+      <c r="F285" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>Reko13</t>
+        </is>
+      </c>
+      <c r="C286" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D286" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46723107438</t>
+        </is>
+      </c>
+      <c r="E286" t="n">
+        <v>129</v>
+      </c>
+      <c r="F286" t="inlineStr"/>
+    </row>
+    <row r="287">
+      <c r="A287" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Reko14</t>
+        </is>
+      </c>
+      <c r="C287" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46722536136</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr"/>
+      <c r="F287" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>Reko14</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D288" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46722536136</t>
+        </is>
+      </c>
+      <c r="E288" t="inlineStr"/>
+      <c r="F288" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Reko14</t>
+        </is>
+      </c>
+      <c r="C289" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46722536136</t>
+        </is>
+      </c>
+      <c r="E289" t="n">
+        <v>129</v>
+      </c>
+      <c r="F289" t="inlineStr"/>
+    </row>
+    <row r="290">
+      <c r="A290" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B290" t="inlineStr">
+        <is>
+          <t>Reko15</t>
+        </is>
+      </c>
+      <c r="C290" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46708194592</t>
+        </is>
+      </c>
+      <c r="E290" t="inlineStr"/>
+      <c r="F290" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B291" t="inlineStr">
+        <is>
+          <t>Reko15</t>
+        </is>
+      </c>
+      <c r="C291" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46708194592</t>
+        </is>
+      </c>
+      <c r="E291" t="inlineStr"/>
+      <c r="F291" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>Reko15</t>
+        </is>
+      </c>
+      <c r="C292" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46708194592</t>
+        </is>
+      </c>
+      <c r="E292" t="n">
+        <v>474</v>
+      </c>
+      <c r="F292" t="inlineStr"/>
+    </row>
+    <row r="293">
+      <c r="A293" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Reko16</t>
+        </is>
+      </c>
+      <c r="C293" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46737600861 Return</t>
+        </is>
+      </c>
+      <c r="E293" t="n">
+        <v>70.54000000000001</v>
+      </c>
+      <c r="F293" t="inlineStr"/>
+    </row>
+    <row r="294">
+      <c r="A294" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Reko16</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46737600861 Return</t>
+        </is>
+      </c>
+      <c r="E294" t="n">
+        <v>8.460000000000001</v>
+      </c>
+      <c r="F294" t="inlineStr"/>
+    </row>
+    <row r="295">
+      <c r="A295" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Reko16</t>
+        </is>
+      </c>
+      <c r="C295" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D295" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46737600861 Return</t>
+        </is>
+      </c>
+      <c r="E295" t="inlineStr"/>
+      <c r="F295" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Reko17</t>
+        </is>
+      </c>
+      <c r="C296" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D296" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46760633899</t>
+        </is>
+      </c>
+      <c r="E296" t="inlineStr"/>
+      <c r="F296" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Reko17</t>
+        </is>
+      </c>
+      <c r="C297" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D297" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46760633899</t>
+        </is>
+      </c>
+      <c r="E297" t="inlineStr"/>
+      <c r="F297" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Reko17</t>
+        </is>
+      </c>
+      <c r="C298" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46760633899</t>
+        </is>
+      </c>
+      <c r="E298" t="n">
+        <v>258</v>
+      </c>
+      <c r="F298" t="inlineStr"/>
+    </row>
+    <row r="299">
+      <c r="A299" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Reko18</t>
+        </is>
+      </c>
+      <c r="C299" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46706033226</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr"/>
+      <c r="F299" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Reko18</t>
+        </is>
+      </c>
+      <c r="C300" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46706033226</t>
+        </is>
+      </c>
+      <c r="E300" t="inlineStr"/>
+      <c r="F300" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Reko18</t>
+        </is>
+      </c>
+      <c r="C301" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>Reko Sollentuna Swish +46706033226</t>
+        </is>
+      </c>
+      <c r="E301" t="n">
+        <v>258</v>
+      </c>
+      <c r="F301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>4031829</t>
+        </is>
+      </c>
+      <c r="C302" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>Order 4031829 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E302" t="inlineStr"/>
+      <c r="F302" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>4031829</t>
+        </is>
+      </c>
+      <c r="C303" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>Order 4031829 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E303" t="inlineStr"/>
+      <c r="F303" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>4031829</t>
+        </is>
+      </c>
+      <c r="C304" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>Order 4031829 Swish +46709526084</t>
+        </is>
+      </c>
+      <c r="E304" t="n">
+        <v>690</v>
+      </c>
+      <c r="F304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B305" t="inlineStr"/>
+      <c r="C305" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E305" t="n">
+        <v>393.97</v>
+      </c>
+      <c r="F305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B306" t="inlineStr"/>
+      <c r="C306" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E306" t="n">
+        <v>47.28</v>
+      </c>
+      <c r="F306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="2" t="n">
+        <v>44257</v>
+      </c>
+      <c r="B307" t="inlineStr"/>
+      <c r="C307" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>NGROCERIES AB K0135</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr"/>
+      <c r="F307" t="n">
+        <v>441.25</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="2" t="n">
+        <v>44262</v>
+      </c>
+      <c r="B308" t="inlineStr"/>
+      <c r="C308" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E308" t="n">
+        <v>1007.19</v>
+      </c>
+      <c r="F308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="2" t="n">
+        <v>44262</v>
+      </c>
+      <c r="B309" t="inlineStr"/>
+      <c r="C309" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E309" t="n">
+        <v>120.86</v>
+      </c>
+      <c r="F309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="2" t="n">
+        <v>44262</v>
+      </c>
+      <c r="B310" t="inlineStr"/>
+      <c r="C310" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>MATVARLDEN VEDD K0135</t>
+        </is>
+      </c>
+      <c r="E310" t="inlineStr"/>
+      <c r="F310" t="n">
+        <v>1128.05</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="2" t="n">
+        <v>44262</v>
+      </c>
+      <c r="B311" t="inlineStr"/>
+      <c r="C311" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E311" t="n">
+        <v>133.93</v>
+      </c>
+      <c r="F311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="2" t="n">
+        <v>44262</v>
+      </c>
+      <c r="B312" t="inlineStr"/>
+      <c r="C312" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E312" t="n">
+        <v>16.07</v>
+      </c>
+      <c r="F312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="2" t="n">
+        <v>44262</v>
+      </c>
+      <c r="B313" t="inlineStr"/>
+      <c r="C313" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E313" t="inlineStr"/>
+      <c r="F313" t="n">
+        <v>150</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 42 new rows for week ending 2021-03-14 (total 354 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F313"/>
+  <dimension ref="A1:F355"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6643,6 +6643,854 @@
         <v>150</v>
       </c>
     </row>
+    <row r="314">
+      <c r="A314" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>1081133</t>
+        </is>
+      </c>
+      <c r="C314" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>Order 1081133 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E314" t="inlineStr"/>
+      <c r="F314" t="n">
+        <v>396.43</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>1081133</t>
+        </is>
+      </c>
+      <c r="C315" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>Order 1081133 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E315" t="inlineStr"/>
+      <c r="F315" t="n">
+        <v>47.57</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>1081133</t>
+        </is>
+      </c>
+      <c r="C316" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>Order 1081133 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E316" t="n">
+        <v>444</v>
+      </c>
+      <c r="F316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Reko19</t>
+        </is>
+      </c>
+      <c r="C317" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E317" t="inlineStr"/>
+      <c r="F317" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Reko19</t>
+        </is>
+      </c>
+      <c r="C318" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E318" t="inlineStr"/>
+      <c r="F318" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Reko19</t>
+        </is>
+      </c>
+      <c r="C319" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E319" t="n">
+        <v>316</v>
+      </c>
+      <c r="F319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Reko20</t>
+        </is>
+      </c>
+      <c r="C320" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704972332</t>
+        </is>
+      </c>
+      <c r="E320" t="inlineStr"/>
+      <c r="F320" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Reko20</t>
+        </is>
+      </c>
+      <c r="C321" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704972332</t>
+        </is>
+      </c>
+      <c r="E321" t="inlineStr"/>
+      <c r="F321" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="2" t="n">
+        <v>44263</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Reko20</t>
+        </is>
+      </c>
+      <c r="C322" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704972332</t>
+        </is>
+      </c>
+      <c r="E322" t="n">
+        <v>158</v>
+      </c>
+      <c r="F322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="2" t="n">
+        <v>44264</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Reko21</t>
+        </is>
+      </c>
+      <c r="C323" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E323" t="inlineStr"/>
+      <c r="F323" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="2" t="n">
+        <v>44264</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Reko21</t>
+        </is>
+      </c>
+      <c r="C324" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E324" t="inlineStr"/>
+      <c r="F324" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="2" t="n">
+        <v>44264</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Reko21</t>
+        </is>
+      </c>
+      <c r="C325" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E325" t="n">
+        <v>316</v>
+      </c>
+      <c r="F325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="2" t="n">
+        <v>44264</v>
+      </c>
+      <c r="B326" t="inlineStr"/>
+      <c r="C326" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>FACEBK 7SAS3ZEZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E326" t="n">
+        <v>410</v>
+      </c>
+      <c r="F326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="2" t="n">
+        <v>44264</v>
+      </c>
+      <c r="B327" t="inlineStr"/>
+      <c r="C327" t="inlineStr"/>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>FACEBK 7SAS3ZEZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E327" t="n">
+        <v>0</v>
+      </c>
+      <c r="F327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="2" t="n">
+        <v>44264</v>
+      </c>
+      <c r="B328" t="inlineStr"/>
+      <c r="C328" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>FACEBK 7SAS3ZEZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E328" t="inlineStr"/>
+      <c r="F328" t="n">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Reko22</t>
+        </is>
+      </c>
+      <c r="C329" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708688090</t>
+        </is>
+      </c>
+      <c r="E329" t="inlineStr"/>
+      <c r="F329" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Reko22</t>
+        </is>
+      </c>
+      <c r="C330" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D330" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708688090</t>
+        </is>
+      </c>
+      <c r="E330" t="inlineStr"/>
+      <c r="F330" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Reko22</t>
+        </is>
+      </c>
+      <c r="C331" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D331" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708688090</t>
+        </is>
+      </c>
+      <c r="E331" t="n">
+        <v>258</v>
+      </c>
+      <c r="F331" t="inlineStr"/>
+    </row>
+    <row r="332">
+      <c r="A332" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>3102253</t>
+        </is>
+      </c>
+      <c r="C332" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D332" t="inlineStr">
+        <is>
+          <t>Order 3102253 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E332" t="inlineStr"/>
+      <c r="F332" t="n">
+        <v>431.25</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>3102253</t>
+        </is>
+      </c>
+      <c r="C333" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D333" t="inlineStr">
+        <is>
+          <t>Order 3102253 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E333" t="inlineStr"/>
+      <c r="F333" t="n">
+        <v>51.75</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="2" t="n">
+        <v>44265</v>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>3102253</t>
+        </is>
+      </c>
+      <c r="C334" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D334" t="inlineStr">
+        <is>
+          <t>Order 3102253 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E334" t="n">
+        <v>483</v>
+      </c>
+      <c r="F334" t="inlineStr"/>
+    </row>
+    <row r="335">
+      <c r="A335" s="2" t="n">
+        <v>44266</v>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>8111258</t>
+        </is>
+      </c>
+      <c r="C335" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D335" t="inlineStr">
+        <is>
+          <t>Order 8111258 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E335" t="inlineStr"/>
+      <c r="F335" t="n">
+        <v>1201.79</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="2" t="n">
+        <v>44266</v>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>8111258</t>
+        </is>
+      </c>
+      <c r="C336" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D336" t="inlineStr">
+        <is>
+          <t>Order 8111258 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E336" t="inlineStr"/>
+      <c r="F336" t="n">
+        <v>144.21</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="2" t="n">
+        <v>44266</v>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>8111258</t>
+        </is>
+      </c>
+      <c r="C337" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D337" t="inlineStr">
+        <is>
+          <t>Order 8111258 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E337" t="n">
+        <v>1346</v>
+      </c>
+      <c r="F337" t="inlineStr"/>
+    </row>
+    <row r="338">
+      <c r="A338" s="2" t="n">
+        <v>44267</v>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Reko23</t>
+        </is>
+      </c>
+      <c r="C338" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D338" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702129177</t>
+        </is>
+      </c>
+      <c r="E338" t="inlineStr"/>
+      <c r="F338" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="2" t="n">
+        <v>44267</v>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Reko23</t>
+        </is>
+      </c>
+      <c r="C339" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D339" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702129177</t>
+        </is>
+      </c>
+      <c r="E339" t="inlineStr"/>
+      <c r="F339" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="2" t="n">
+        <v>44267</v>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Reko23</t>
+        </is>
+      </c>
+      <c r="C340" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D340" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702129177</t>
+        </is>
+      </c>
+      <c r="E340" t="n">
+        <v>387</v>
+      </c>
+      <c r="F340" t="inlineStr"/>
+    </row>
+    <row r="341">
+      <c r="A341" s="2" t="n">
+        <v>44267</v>
+      </c>
+      <c r="B341" t="inlineStr"/>
+      <c r="C341" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D341" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E341" t="n">
+        <v>437.67</v>
+      </c>
+      <c r="F341" t="inlineStr"/>
+    </row>
+    <row r="342">
+      <c r="A342" s="2" t="n">
+        <v>44267</v>
+      </c>
+      <c r="B342" t="inlineStr"/>
+      <c r="C342" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D342" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E342" t="n">
+        <v>52.52</v>
+      </c>
+      <c r="F342" t="inlineStr"/>
+    </row>
+    <row r="343">
+      <c r="A343" s="2" t="n">
+        <v>44267</v>
+      </c>
+      <c r="B343" t="inlineStr"/>
+      <c r="C343" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D343" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E343" t="inlineStr"/>
+      <c r="F343" t="n">
+        <v>490.19</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="2" t="n">
+        <v>44268</v>
+      </c>
+      <c r="B344" t="inlineStr"/>
+      <c r="C344" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D344" t="inlineStr">
+        <is>
+          <t>KAHLS THE &amp; KAFFEHANDE K6885</t>
+        </is>
+      </c>
+      <c r="E344" t="n">
+        <v>269.64</v>
+      </c>
+      <c r="F344" t="inlineStr"/>
+    </row>
+    <row r="345">
+      <c r="A345" s="2" t="n">
+        <v>44268</v>
+      </c>
+      <c r="B345" t="inlineStr"/>
+      <c r="C345" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D345" t="inlineStr">
+        <is>
+          <t>KAHLS THE &amp; KAFFEHANDE K6885</t>
+        </is>
+      </c>
+      <c r="E345" t="n">
+        <v>32.36</v>
+      </c>
+      <c r="F345" t="inlineStr"/>
+    </row>
+    <row r="346">
+      <c r="A346" s="2" t="n">
+        <v>44268</v>
+      </c>
+      <c r="B346" t="inlineStr"/>
+      <c r="C346" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D346" t="inlineStr">
+        <is>
+          <t>KAHLS THE &amp; KAFFEHANDE K6885</t>
+        </is>
+      </c>
+      <c r="E346" t="inlineStr"/>
+      <c r="F346" t="n">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B347" t="inlineStr"/>
+      <c r="C347" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D347" t="inlineStr">
+        <is>
+          <t>Dec-MarKitchen</t>
+        </is>
+      </c>
+      <c r="E347" t="n">
+        <v>15066</v>
+      </c>
+      <c r="F347" t="inlineStr"/>
+    </row>
+    <row r="348">
+      <c r="A348" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B348" t="inlineStr"/>
+      <c r="C348" t="inlineStr"/>
+      <c r="D348" t="inlineStr">
+        <is>
+          <t>Dec-MarKitchen</t>
+        </is>
+      </c>
+      <c r="E348" t="n">
+        <v>0</v>
+      </c>
+      <c r="F348" t="inlineStr"/>
+    </row>
+    <row r="349">
+      <c r="A349" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B349" t="inlineStr"/>
+      <c r="C349" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D349" t="inlineStr">
+        <is>
+          <t>Dec-MarKitchen</t>
+        </is>
+      </c>
+      <c r="E349" t="inlineStr"/>
+      <c r="F349" t="n">
+        <v>15066</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B350" t="inlineStr"/>
+      <c r="C350" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D350" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E350" t="n">
+        <v>668.77</v>
+      </c>
+      <c r="F350" t="inlineStr"/>
+    </row>
+    <row r="351">
+      <c r="A351" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B351" t="inlineStr"/>
+      <c r="C351" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E351" t="n">
+        <v>167.19</v>
+      </c>
+      <c r="F351" t="inlineStr"/>
+    </row>
+    <row r="352">
+      <c r="A352" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B352" t="inlineStr"/>
+      <c r="C352" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr"/>
+      <c r="F352" t="n">
+        <v>835.96</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B353" t="inlineStr"/>
+      <c r="C353" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>DECATHLON K0135</t>
+        </is>
+      </c>
+      <c r="E353" t="n">
+        <v>319.2</v>
+      </c>
+      <c r="F353" t="inlineStr"/>
+    </row>
+    <row r="354">
+      <c r="A354" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B354" t="inlineStr"/>
+      <c r="C354" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>DECATHLON K0135</t>
+        </is>
+      </c>
+      <c r="E354" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="F354" t="inlineStr"/>
+    </row>
+    <row r="355">
+      <c r="A355" s="2" t="n">
+        <v>44269</v>
+      </c>
+      <c r="B355" t="inlineStr"/>
+      <c r="C355" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D355" t="inlineStr">
+        <is>
+          <t>DECATHLON K0135</t>
+        </is>
+      </c>
+      <c r="E355" t="inlineStr"/>
+      <c r="F355" t="n">
+        <v>399</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 123 new rows for week ending 2021-03-21 (total 477 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F355"/>
+  <dimension ref="A1:F478"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7491,6 +7491,2652 @@
         <v>399</v>
       </c>
     </row>
+    <row r="356">
+      <c r="A356" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Reko24</t>
+        </is>
+      </c>
+      <c r="C356" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D356" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730266946</t>
+        </is>
+      </c>
+      <c r="E356" t="inlineStr"/>
+      <c r="F356" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Reko24</t>
+        </is>
+      </c>
+      <c r="C357" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D357" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730266946</t>
+        </is>
+      </c>
+      <c r="E357" t="inlineStr"/>
+      <c r="F357" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Reko24</t>
+        </is>
+      </c>
+      <c r="C358" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D358" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730266946</t>
+        </is>
+      </c>
+      <c r="E358" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F358" t="inlineStr"/>
+    </row>
+    <row r="359">
+      <c r="A359" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Reko25</t>
+        </is>
+      </c>
+      <c r="C359" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D359" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703363169</t>
+        </is>
+      </c>
+      <c r="E359" t="inlineStr"/>
+      <c r="F359" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Reko25</t>
+        </is>
+      </c>
+      <c r="C360" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703363169</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr"/>
+      <c r="F360" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Reko25</t>
+        </is>
+      </c>
+      <c r="C361" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D361" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703363169</t>
+        </is>
+      </c>
+      <c r="E361" t="n">
+        <v>158</v>
+      </c>
+      <c r="F361" t="inlineStr"/>
+    </row>
+    <row r="362">
+      <c r="A362" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Reko26</t>
+        </is>
+      </c>
+      <c r="C362" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D362" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E362" t="inlineStr"/>
+      <c r="F362" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Reko26</t>
+        </is>
+      </c>
+      <c r="C363" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D363" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E363" t="inlineStr"/>
+      <c r="F363" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Reko26</t>
+        </is>
+      </c>
+      <c r="C364" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D364" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E364" t="n">
+        <v>258</v>
+      </c>
+      <c r="F364" t="inlineStr"/>
+    </row>
+    <row r="365">
+      <c r="A365" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Reko27</t>
+        </is>
+      </c>
+      <c r="C365" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D365" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730493900</t>
+        </is>
+      </c>
+      <c r="E365" t="inlineStr"/>
+      <c r="F365" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Reko27</t>
+        </is>
+      </c>
+      <c r="C366" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D366" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730493900</t>
+        </is>
+      </c>
+      <c r="E366" t="inlineStr"/>
+      <c r="F366" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Reko27</t>
+        </is>
+      </c>
+      <c r="C367" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D367" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730493900</t>
+        </is>
+      </c>
+      <c r="E367" t="n">
+        <v>316</v>
+      </c>
+      <c r="F367" t="inlineStr"/>
+    </row>
+    <row r="368">
+      <c r="A368" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Reko28</t>
+        </is>
+      </c>
+      <c r="C368" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D368" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E368" t="inlineStr"/>
+      <c r="F368" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Reko28</t>
+        </is>
+      </c>
+      <c r="C369" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D369" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E369" t="inlineStr"/>
+      <c r="F369" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Reko28</t>
+        </is>
+      </c>
+      <c r="C370" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D370" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E370" t="n">
+        <v>516</v>
+      </c>
+      <c r="F370" t="inlineStr"/>
+    </row>
+    <row r="371">
+      <c r="A371" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Reko29</t>
+        </is>
+      </c>
+      <c r="C371" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D371" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725227200</t>
+        </is>
+      </c>
+      <c r="E371" t="inlineStr"/>
+      <c r="F371" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Reko29</t>
+        </is>
+      </c>
+      <c r="C372" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D372" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725227200</t>
+        </is>
+      </c>
+      <c r="E372" t="inlineStr"/>
+      <c r="F372" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Reko29</t>
+        </is>
+      </c>
+      <c r="C373" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D373" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725227200</t>
+        </is>
+      </c>
+      <c r="E373" t="n">
+        <v>316</v>
+      </c>
+      <c r="F373" t="inlineStr"/>
+    </row>
+    <row r="374">
+      <c r="A374" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Reko30</t>
+        </is>
+      </c>
+      <c r="C374" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D374" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704657942</t>
+        </is>
+      </c>
+      <c r="E374" t="inlineStr"/>
+      <c r="F374" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Reko30</t>
+        </is>
+      </c>
+      <c r="C375" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D375" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704657942</t>
+        </is>
+      </c>
+      <c r="E375" t="inlineStr"/>
+      <c r="F375" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Reko30</t>
+        </is>
+      </c>
+      <c r="C376" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D376" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704657942</t>
+        </is>
+      </c>
+      <c r="E376" t="n">
+        <v>316</v>
+      </c>
+      <c r="F376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Reko31</t>
+        </is>
+      </c>
+      <c r="C377" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D377" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702087212</t>
+        </is>
+      </c>
+      <c r="E377" t="inlineStr"/>
+      <c r="F377" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>Reko31</t>
+        </is>
+      </c>
+      <c r="C378" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D378" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702087212</t>
+        </is>
+      </c>
+      <c r="E378" t="inlineStr"/>
+      <c r="F378" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Reko31</t>
+        </is>
+      </c>
+      <c r="C379" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D379" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702087212</t>
+        </is>
+      </c>
+      <c r="E379" t="n">
+        <v>237</v>
+      </c>
+      <c r="F379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>Reko32</t>
+        </is>
+      </c>
+      <c r="C380" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D380" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736506798</t>
+        </is>
+      </c>
+      <c r="E380" t="inlineStr"/>
+      <c r="F380" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Reko32</t>
+        </is>
+      </c>
+      <c r="C381" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D381" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736506798</t>
+        </is>
+      </c>
+      <c r="E381" t="inlineStr"/>
+      <c r="F381" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Reko32</t>
+        </is>
+      </c>
+      <c r="C382" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D382" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736506798</t>
+        </is>
+      </c>
+      <c r="E382" t="n">
+        <v>387</v>
+      </c>
+      <c r="F382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Reko33</t>
+        </is>
+      </c>
+      <c r="C383" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D383" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736374629</t>
+        </is>
+      </c>
+      <c r="E383" t="inlineStr"/>
+      <c r="F383" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Reko33</t>
+        </is>
+      </c>
+      <c r="C384" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D384" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736374629</t>
+        </is>
+      </c>
+      <c r="E384" t="inlineStr"/>
+      <c r="F384" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Reko33</t>
+        </is>
+      </c>
+      <c r="C385" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D385" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736374629</t>
+        </is>
+      </c>
+      <c r="E385" t="n">
+        <v>516</v>
+      </c>
+      <c r="F385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Reko34</t>
+        </is>
+      </c>
+      <c r="C386" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D386" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727070411</t>
+        </is>
+      </c>
+      <c r="E386" t="inlineStr"/>
+      <c r="F386" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Reko34</t>
+        </is>
+      </c>
+      <c r="C387" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D387" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727070411</t>
+        </is>
+      </c>
+      <c r="E387" t="inlineStr"/>
+      <c r="F387" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Reko34</t>
+        </is>
+      </c>
+      <c r="C388" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D388" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727070411</t>
+        </is>
+      </c>
+      <c r="E388" t="n">
+        <v>387</v>
+      </c>
+      <c r="F388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Reko35</t>
+        </is>
+      </c>
+      <c r="C389" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D389" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707512338</t>
+        </is>
+      </c>
+      <c r="E389" t="inlineStr"/>
+      <c r="F389" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Reko35</t>
+        </is>
+      </c>
+      <c r="C390" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D390" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707512338</t>
+        </is>
+      </c>
+      <c r="E390" t="inlineStr"/>
+      <c r="F390" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Reko35</t>
+        </is>
+      </c>
+      <c r="C391" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D391" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707512338</t>
+        </is>
+      </c>
+      <c r="E391" t="n">
+        <v>258</v>
+      </c>
+      <c r="F391" t="inlineStr"/>
+    </row>
+    <row r="392">
+      <c r="A392" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Reko36</t>
+        </is>
+      </c>
+      <c r="C392" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D392" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709820782</t>
+        </is>
+      </c>
+      <c r="E392" t="inlineStr"/>
+      <c r="F392" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Reko36</t>
+        </is>
+      </c>
+      <c r="C393" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D393" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709820782</t>
+        </is>
+      </c>
+      <c r="E393" t="inlineStr"/>
+      <c r="F393" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Reko36</t>
+        </is>
+      </c>
+      <c r="C394" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D394" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709820782</t>
+        </is>
+      </c>
+      <c r="E394" t="n">
+        <v>129</v>
+      </c>
+      <c r="F394" t="inlineStr"/>
+    </row>
+    <row r="395">
+      <c r="A395" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Reko37</t>
+        </is>
+      </c>
+      <c r="C395" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D395" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703148926</t>
+        </is>
+      </c>
+      <c r="E395" t="inlineStr"/>
+      <c r="F395" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Reko37</t>
+        </is>
+      </c>
+      <c r="C396" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D396" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703148926</t>
+        </is>
+      </c>
+      <c r="E396" t="inlineStr"/>
+      <c r="F396" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Reko37</t>
+        </is>
+      </c>
+      <c r="C397" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D397" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703148926</t>
+        </is>
+      </c>
+      <c r="E397" t="n">
+        <v>158</v>
+      </c>
+      <c r="F397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Reko38</t>
+        </is>
+      </c>
+      <c r="C398" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D398" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706383888</t>
+        </is>
+      </c>
+      <c r="E398" t="inlineStr"/>
+      <c r="F398" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Reko38</t>
+        </is>
+      </c>
+      <c r="C399" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D399" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706383888</t>
+        </is>
+      </c>
+      <c r="E399" t="inlineStr"/>
+      <c r="F399" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Reko38</t>
+        </is>
+      </c>
+      <c r="C400" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D400" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706383888</t>
+        </is>
+      </c>
+      <c r="E400" t="n">
+        <v>395</v>
+      </c>
+      <c r="F400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Reko39</t>
+        </is>
+      </c>
+      <c r="C401" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D401" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737611828</t>
+        </is>
+      </c>
+      <c r="E401" t="inlineStr"/>
+      <c r="F401" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Reko39</t>
+        </is>
+      </c>
+      <c r="C402" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D402" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737611828</t>
+        </is>
+      </c>
+      <c r="E402" t="inlineStr"/>
+      <c r="F402" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Reko39</t>
+        </is>
+      </c>
+      <c r="C403" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D403" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737611828</t>
+        </is>
+      </c>
+      <c r="E403" t="n">
+        <v>387</v>
+      </c>
+      <c r="F403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Reko40</t>
+        </is>
+      </c>
+      <c r="C404" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D404" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703685831</t>
+        </is>
+      </c>
+      <c r="E404" t="inlineStr"/>
+      <c r="F404" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Reko40</t>
+        </is>
+      </c>
+      <c r="C405" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D405" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703685831</t>
+        </is>
+      </c>
+      <c r="E405" t="inlineStr"/>
+      <c r="F405" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Reko40</t>
+        </is>
+      </c>
+      <c r="C406" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D406" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703685831</t>
+        </is>
+      </c>
+      <c r="E406" t="n">
+        <v>258</v>
+      </c>
+      <c r="F406" t="inlineStr"/>
+    </row>
+    <row r="407">
+      <c r="A407" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Reko41</t>
+        </is>
+      </c>
+      <c r="C407" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D407" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734663122</t>
+        </is>
+      </c>
+      <c r="E407" t="inlineStr"/>
+      <c r="F407" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Reko41</t>
+        </is>
+      </c>
+      <c r="C408" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D408" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734663122</t>
+        </is>
+      </c>
+      <c r="E408" t="inlineStr"/>
+      <c r="F408" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Reko41</t>
+        </is>
+      </c>
+      <c r="C409" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D409" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734663122</t>
+        </is>
+      </c>
+      <c r="E409" t="n">
+        <v>129</v>
+      </c>
+      <c r="F409" t="inlineStr"/>
+    </row>
+    <row r="410">
+      <c r="A410" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Reko42</t>
+        </is>
+      </c>
+      <c r="C410" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D410" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E410" t="inlineStr"/>
+      <c r="F410" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Reko42</t>
+        </is>
+      </c>
+      <c r="C411" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D411" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E411" t="inlineStr"/>
+      <c r="F411" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Reko42</t>
+        </is>
+      </c>
+      <c r="C412" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D412" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E412" t="n">
+        <v>258</v>
+      </c>
+      <c r="F412" t="inlineStr"/>
+    </row>
+    <row r="413">
+      <c r="A413" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Reko43</t>
+        </is>
+      </c>
+      <c r="C413" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D413" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706439842</t>
+        </is>
+      </c>
+      <c r="E413" t="inlineStr"/>
+      <c r="F413" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Reko43</t>
+        </is>
+      </c>
+      <c r="C414" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D414" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706439842</t>
+        </is>
+      </c>
+      <c r="E414" t="inlineStr"/>
+      <c r="F414" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Reko43</t>
+        </is>
+      </c>
+      <c r="C415" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D415" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706439842</t>
+        </is>
+      </c>
+      <c r="E415" t="n">
+        <v>690</v>
+      </c>
+      <c r="F415" t="inlineStr"/>
+    </row>
+    <row r="416">
+      <c r="A416" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Reko44</t>
+        </is>
+      </c>
+      <c r="C416" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D416" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723616343</t>
+        </is>
+      </c>
+      <c r="E416" t="inlineStr"/>
+      <c r="F416" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>Reko44</t>
+        </is>
+      </c>
+      <c r="C417" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D417" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723616343</t>
+        </is>
+      </c>
+      <c r="E417" t="inlineStr"/>
+      <c r="F417" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Reko44</t>
+        </is>
+      </c>
+      <c r="C418" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D418" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723616343</t>
+        </is>
+      </c>
+      <c r="E418" t="n">
+        <v>395</v>
+      </c>
+      <c r="F418" t="inlineStr"/>
+    </row>
+    <row r="419">
+      <c r="A419" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Reko45</t>
+        </is>
+      </c>
+      <c r="C419" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D419" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768268221</t>
+        </is>
+      </c>
+      <c r="E419" t="inlineStr"/>
+      <c r="F419" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Reko45</t>
+        </is>
+      </c>
+      <c r="C420" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D420" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768268221</t>
+        </is>
+      </c>
+      <c r="E420" t="inlineStr"/>
+      <c r="F420" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Reko45</t>
+        </is>
+      </c>
+      <c r="C421" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D421" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768268221</t>
+        </is>
+      </c>
+      <c r="E421" t="n">
+        <v>79</v>
+      </c>
+      <c r="F421" t="inlineStr"/>
+    </row>
+    <row r="422">
+      <c r="A422" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B422" t="inlineStr"/>
+      <c r="C422" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D422" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E422" t="n">
+        <v>877.88</v>
+      </c>
+      <c r="F422" t="inlineStr"/>
+    </row>
+    <row r="423">
+      <c r="A423" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B423" t="inlineStr"/>
+      <c r="C423" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D423" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E423" t="n">
+        <v>105.35</v>
+      </c>
+      <c r="F423" t="inlineStr"/>
+    </row>
+    <row r="424">
+      <c r="A424" s="2" t="n">
+        <v>44270</v>
+      </c>
+      <c r="B424" t="inlineStr"/>
+      <c r="C424" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D424" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E424" t="inlineStr"/>
+      <c r="F424" t="n">
+        <v>983.23</v>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Reko46</t>
+        </is>
+      </c>
+      <c r="C425" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D425" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720444719</t>
+        </is>
+      </c>
+      <c r="E425" t="inlineStr"/>
+      <c r="F425" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Reko46</t>
+        </is>
+      </c>
+      <c r="C426" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D426" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720444719</t>
+        </is>
+      </c>
+      <c r="E426" t="inlineStr"/>
+      <c r="F426" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Reko46</t>
+        </is>
+      </c>
+      <c r="C427" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D427" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720444719</t>
+        </is>
+      </c>
+      <c r="E427" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F427" t="inlineStr"/>
+    </row>
+    <row r="428">
+      <c r="A428" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Reko47</t>
+        </is>
+      </c>
+      <c r="C428" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D428" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767161778</t>
+        </is>
+      </c>
+      <c r="E428" t="inlineStr"/>
+      <c r="F428" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Reko47</t>
+        </is>
+      </c>
+      <c r="C429" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D429" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767161778</t>
+        </is>
+      </c>
+      <c r="E429" t="inlineStr"/>
+      <c r="F429" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Reko47</t>
+        </is>
+      </c>
+      <c r="C430" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D430" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767161778</t>
+        </is>
+      </c>
+      <c r="E430" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F430" t="inlineStr"/>
+    </row>
+    <row r="431">
+      <c r="A431" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Reko48</t>
+        </is>
+      </c>
+      <c r="C431" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D431" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739701408</t>
+        </is>
+      </c>
+      <c r="E431" t="inlineStr"/>
+      <c r="F431" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Reko48</t>
+        </is>
+      </c>
+      <c r="C432" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D432" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739701408</t>
+        </is>
+      </c>
+      <c r="E432" t="inlineStr"/>
+      <c r="F432" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Reko48</t>
+        </is>
+      </c>
+      <c r="C433" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D433" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739701408</t>
+        </is>
+      </c>
+      <c r="E433" t="n">
+        <v>316</v>
+      </c>
+      <c r="F433" t="inlineStr"/>
+    </row>
+    <row r="434">
+      <c r="A434" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Reko49</t>
+        </is>
+      </c>
+      <c r="C434" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D434" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E434" t="inlineStr"/>
+      <c r="F434" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Reko49</t>
+        </is>
+      </c>
+      <c r="C435" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D435" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E435" t="inlineStr"/>
+      <c r="F435" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Reko49</t>
+        </is>
+      </c>
+      <c r="C436" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D436" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E436" t="n">
+        <v>158</v>
+      </c>
+      <c r="F436" t="inlineStr"/>
+    </row>
+    <row r="437">
+      <c r="A437" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Reko50</t>
+        </is>
+      </c>
+      <c r="C437" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D437" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707923308</t>
+        </is>
+      </c>
+      <c r="E437" t="inlineStr"/>
+      <c r="F437" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>Reko50</t>
+        </is>
+      </c>
+      <c r="C438" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D438" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707923308</t>
+        </is>
+      </c>
+      <c r="E438" t="inlineStr"/>
+      <c r="F438" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Reko50</t>
+        </is>
+      </c>
+      <c r="C439" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D439" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707923308</t>
+        </is>
+      </c>
+      <c r="E439" t="n">
+        <v>690</v>
+      </c>
+      <c r="F439" t="inlineStr"/>
+    </row>
+    <row r="440">
+      <c r="A440" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Reko51</t>
+        </is>
+      </c>
+      <c r="C440" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D440" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735214288</t>
+        </is>
+      </c>
+      <c r="E440" t="inlineStr"/>
+      <c r="F440" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Reko51</t>
+        </is>
+      </c>
+      <c r="C441" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D441" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735214288</t>
+        </is>
+      </c>
+      <c r="E441" t="inlineStr"/>
+      <c r="F441" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Reko51</t>
+        </is>
+      </c>
+      <c r="C442" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D442" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735214288</t>
+        </is>
+      </c>
+      <c r="E442" t="n">
+        <v>258</v>
+      </c>
+      <c r="F442" t="inlineStr"/>
+    </row>
+    <row r="443">
+      <c r="A443" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Reko52</t>
+        </is>
+      </c>
+      <c r="C443" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D443" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709838537</t>
+        </is>
+      </c>
+      <c r="E443" t="inlineStr"/>
+      <c r="F443" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>Reko52</t>
+        </is>
+      </c>
+      <c r="C444" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D444" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709838537</t>
+        </is>
+      </c>
+      <c r="E444" t="inlineStr"/>
+      <c r="F444" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>Reko52</t>
+        </is>
+      </c>
+      <c r="C445" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D445" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709838537</t>
+        </is>
+      </c>
+      <c r="E445" t="n">
+        <v>158</v>
+      </c>
+      <c r="F445" t="inlineStr"/>
+    </row>
+    <row r="446">
+      <c r="A446" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Reko53</t>
+        </is>
+      </c>
+      <c r="C446" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D446" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725248271</t>
+        </is>
+      </c>
+      <c r="E446" t="inlineStr"/>
+      <c r="F446" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Reko53</t>
+        </is>
+      </c>
+      <c r="C447" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D447" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725248271</t>
+        </is>
+      </c>
+      <c r="E447" t="inlineStr"/>
+      <c r="F447" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Reko53</t>
+        </is>
+      </c>
+      <c r="C448" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D448" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725248271</t>
+        </is>
+      </c>
+      <c r="E448" t="n">
+        <v>258</v>
+      </c>
+      <c r="F448" t="inlineStr"/>
+    </row>
+    <row r="449">
+      <c r="A449" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>Reko54</t>
+        </is>
+      </c>
+      <c r="C449" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D449" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736564703</t>
+        </is>
+      </c>
+      <c r="E449" t="inlineStr"/>
+      <c r="F449" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Reko54</t>
+        </is>
+      </c>
+      <c r="C450" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D450" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736564703</t>
+        </is>
+      </c>
+      <c r="E450" t="inlineStr"/>
+      <c r="F450" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>Reko54</t>
+        </is>
+      </c>
+      <c r="C451" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D451" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736564703</t>
+        </is>
+      </c>
+      <c r="E451" t="n">
+        <v>258</v>
+      </c>
+      <c r="F451" t="inlineStr"/>
+    </row>
+    <row r="452">
+      <c r="A452" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Reko55</t>
+        </is>
+      </c>
+      <c r="C452" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D452" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733442725</t>
+        </is>
+      </c>
+      <c r="E452" t="inlineStr"/>
+      <c r="F452" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Reko55</t>
+        </is>
+      </c>
+      <c r="C453" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D453" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733442725</t>
+        </is>
+      </c>
+      <c r="E453" t="inlineStr"/>
+      <c r="F453" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Reko55</t>
+        </is>
+      </c>
+      <c r="C454" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D454" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733442725</t>
+        </is>
+      </c>
+      <c r="E454" t="n">
+        <v>387</v>
+      </c>
+      <c r="F454" t="inlineStr"/>
+    </row>
+    <row r="455">
+      <c r="A455" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Reko56</t>
+        </is>
+      </c>
+      <c r="C455" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D455" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706645955</t>
+        </is>
+      </c>
+      <c r="E455" t="inlineStr"/>
+      <c r="F455" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Reko56</t>
+        </is>
+      </c>
+      <c r="C456" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D456" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706645955</t>
+        </is>
+      </c>
+      <c r="E456" t="inlineStr"/>
+      <c r="F456" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Reko56</t>
+        </is>
+      </c>
+      <c r="C457" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D457" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706645955</t>
+        </is>
+      </c>
+      <c r="E457" t="n">
+        <v>387</v>
+      </c>
+      <c r="F457" t="inlineStr"/>
+    </row>
+    <row r="458">
+      <c r="A458" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B458" t="inlineStr"/>
+      <c r="C458" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D458" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E458" t="n">
+        <v>285.12</v>
+      </c>
+      <c r="F458" t="inlineStr"/>
+    </row>
+    <row r="459">
+      <c r="A459" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B459" t="inlineStr"/>
+      <c r="C459" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D459" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E459" t="n">
+        <v>34.21</v>
+      </c>
+      <c r="F459" t="inlineStr"/>
+    </row>
+    <row r="460">
+      <c r="A460" s="2" t="n">
+        <v>44271</v>
+      </c>
+      <c r="B460" t="inlineStr"/>
+      <c r="C460" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D460" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E460" t="inlineStr"/>
+      <c r="F460" t="n">
+        <v>319.33</v>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" s="2" t="n">
+        <v>44274</v>
+      </c>
+      <c r="B461" t="inlineStr"/>
+      <c r="C461" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D461" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E461" t="n">
+        <v>719.2</v>
+      </c>
+      <c r="F461" t="inlineStr"/>
+    </row>
+    <row r="462">
+      <c r="A462" s="2" t="n">
+        <v>44274</v>
+      </c>
+      <c r="B462" t="inlineStr"/>
+      <c r="C462" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D462" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E462" t="n">
+        <v>86.3</v>
+      </c>
+      <c r="F462" t="inlineStr"/>
+    </row>
+    <row r="463">
+      <c r="A463" s="2" t="n">
+        <v>44274</v>
+      </c>
+      <c r="B463" t="inlineStr"/>
+      <c r="C463" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D463" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E463" t="inlineStr"/>
+      <c r="F463" t="n">
+        <v>805.5</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" s="2" t="n">
+        <v>44274</v>
+      </c>
+      <c r="B464" t="inlineStr"/>
+      <c r="C464" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D464" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E464" t="n">
+        <v>424.7</v>
+      </c>
+      <c r="F464" t="inlineStr"/>
+    </row>
+    <row r="465">
+      <c r="A465" s="2" t="n">
+        <v>44274</v>
+      </c>
+      <c r="B465" t="inlineStr"/>
+      <c r="C465" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D465" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E465" t="n">
+        <v>50.96</v>
+      </c>
+      <c r="F465" t="inlineStr"/>
+    </row>
+    <row r="466">
+      <c r="A466" s="2" t="n">
+        <v>44274</v>
+      </c>
+      <c r="B466" t="inlineStr"/>
+      <c r="C466" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D466" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E466" t="inlineStr"/>
+      <c r="F466" t="n">
+        <v>475.66</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>Reko57</t>
+        </is>
+      </c>
+      <c r="C467" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D467" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704926349</t>
+        </is>
+      </c>
+      <c r="E467" t="inlineStr"/>
+      <c r="F467" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Reko57</t>
+        </is>
+      </c>
+      <c r="C468" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D468" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704926349</t>
+        </is>
+      </c>
+      <c r="E468" t="inlineStr"/>
+      <c r="F468" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Reko57</t>
+        </is>
+      </c>
+      <c r="C469" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D469" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704926349</t>
+        </is>
+      </c>
+      <c r="E469" t="n">
+        <v>387</v>
+      </c>
+      <c r="F469" t="inlineStr"/>
+    </row>
+    <row r="470">
+      <c r="A470" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Reko58</t>
+        </is>
+      </c>
+      <c r="C470" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D470" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706645955 Return</t>
+        </is>
+      </c>
+      <c r="E470" t="n">
+        <v>345.54</v>
+      </c>
+      <c r="F470" t="inlineStr"/>
+    </row>
+    <row r="471">
+      <c r="A471" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Reko58</t>
+        </is>
+      </c>
+      <c r="C471" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D471" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706645955 Return</t>
+        </is>
+      </c>
+      <c r="E471" t="n">
+        <v>41.46</v>
+      </c>
+      <c r="F471" t="inlineStr"/>
+    </row>
+    <row r="472">
+      <c r="A472" s="2" t="n">
+        <v>44272</v>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Reko58</t>
+        </is>
+      </c>
+      <c r="C472" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D472" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706645955 Return</t>
+        </is>
+      </c>
+      <c r="E472" t="inlineStr"/>
+      <c r="F472" t="n">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" s="2" t="n">
+        <v>44275</v>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>4201221</t>
+        </is>
+      </c>
+      <c r="C473" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D473" t="inlineStr">
+        <is>
+          <t>Order 4201221 Swish +46768548534</t>
+        </is>
+      </c>
+      <c r="E473" t="inlineStr"/>
+      <c r="F473" t="n">
+        <v>433.04</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" s="2" t="n">
+        <v>44275</v>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>4201221</t>
+        </is>
+      </c>
+      <c r="C474" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D474" t="inlineStr">
+        <is>
+          <t>Order 4201221 Swish +46768548534</t>
+        </is>
+      </c>
+      <c r="E474" t="inlineStr"/>
+      <c r="F474" t="n">
+        <v>51.96</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" s="2" t="n">
+        <v>44275</v>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>4201221</t>
+        </is>
+      </c>
+      <c r="C475" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D475" t="inlineStr">
+        <is>
+          <t>Order 4201221 Swish +46768548534</t>
+        </is>
+      </c>
+      <c r="E475" t="n">
+        <v>485</v>
+      </c>
+      <c r="F475" t="inlineStr"/>
+    </row>
+    <row r="476">
+      <c r="A476" s="2" t="n">
+        <v>44275</v>
+      </c>
+      <c r="B476" t="inlineStr"/>
+      <c r="C476" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D476" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E476" t="n">
+        <v>796.74</v>
+      </c>
+      <c r="F476" t="inlineStr"/>
+    </row>
+    <row r="477">
+      <c r="A477" s="2" t="n">
+        <v>44275</v>
+      </c>
+      <c r="B477" t="inlineStr"/>
+      <c r="C477" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D477" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E477" t="n">
+        <v>199.19</v>
+      </c>
+      <c r="F477" t="inlineStr"/>
+    </row>
+    <row r="478">
+      <c r="A478" s="2" t="n">
+        <v>44275</v>
+      </c>
+      <c r="B478" t="inlineStr"/>
+      <c r="C478" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D478" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E478" t="inlineStr"/>
+      <c r="F478" t="n">
+        <v>995.9299999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 27 new rows for week ending 2021-03-28 (total 504 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F478"/>
+  <dimension ref="A1:F505"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10137,6 +10137,526 @@
         <v>995.9299999999999</v>
       </c>
     </row>
+    <row r="479">
+      <c r="A479" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B479" t="inlineStr"/>
+      <c r="C479" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D479" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E479" t="n">
+        <v>60</v>
+      </c>
+      <c r="F479" t="inlineStr"/>
+    </row>
+    <row r="480">
+      <c r="A480" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B480" t="inlineStr"/>
+      <c r="C480" t="inlineStr"/>
+      <c r="D480" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E480" t="n">
+        <v>0</v>
+      </c>
+      <c r="F480" t="inlineStr"/>
+    </row>
+    <row r="481">
+      <c r="A481" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B481" t="inlineStr"/>
+      <c r="C481" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D481" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E481" t="inlineStr"/>
+      <c r="F481" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B482" t="inlineStr"/>
+      <c r="C482" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D482" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E482" t="n">
+        <v>355.36</v>
+      </c>
+      <c r="F482" t="inlineStr"/>
+    </row>
+    <row r="483">
+      <c r="A483" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B483" t="inlineStr"/>
+      <c r="C483" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D483" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E483" t="n">
+        <v>42.64</v>
+      </c>
+      <c r="F483" t="inlineStr"/>
+    </row>
+    <row r="484">
+      <c r="A484" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B484" t="inlineStr"/>
+      <c r="C484" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D484" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E484" t="inlineStr"/>
+      <c r="F484" t="n">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B485" t="inlineStr"/>
+      <c r="C485" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D485" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E485" t="n">
+        <v>278</v>
+      </c>
+      <c r="F485" t="inlineStr"/>
+    </row>
+    <row r="486">
+      <c r="A486" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B486" t="inlineStr"/>
+      <c r="C486" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D486" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E486" t="n">
+        <v>33.36</v>
+      </c>
+      <c r="F486" t="inlineStr"/>
+    </row>
+    <row r="487">
+      <c r="A487" s="2" t="n">
+        <v>44277</v>
+      </c>
+      <c r="B487" t="inlineStr"/>
+      <c r="C487" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D487" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E487" t="inlineStr"/>
+      <c r="F487" t="n">
+        <v>311.36</v>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>Reko59</t>
+        </is>
+      </c>
+      <c r="C488" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D488" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725248271</t>
+        </is>
+      </c>
+      <c r="E488" t="inlineStr"/>
+      <c r="F488" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Reko59</t>
+        </is>
+      </c>
+      <c r="C489" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D489" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725248271</t>
+        </is>
+      </c>
+      <c r="E489" t="inlineStr"/>
+      <c r="F489" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Reko59</t>
+        </is>
+      </c>
+      <c r="C490" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D490" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725248271</t>
+        </is>
+      </c>
+      <c r="E490" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F490" t="inlineStr"/>
+    </row>
+    <row r="491">
+      <c r="A491" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B491" t="inlineStr"/>
+      <c r="C491" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D491" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E491" t="n">
+        <v>657.54</v>
+      </c>
+      <c r="F491" t="inlineStr"/>
+    </row>
+    <row r="492">
+      <c r="A492" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B492" t="inlineStr"/>
+      <c r="C492" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D492" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E492" t="n">
+        <v>78.90000000000001</v>
+      </c>
+      <c r="F492" t="inlineStr"/>
+    </row>
+    <row r="493">
+      <c r="A493" s="2" t="n">
+        <v>44279</v>
+      </c>
+      <c r="B493" t="inlineStr"/>
+      <c r="C493" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D493" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E493" t="inlineStr"/>
+      <c r="F493" t="n">
+        <v>736.4400000000001</v>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Reko60</t>
+        </is>
+      </c>
+      <c r="C494" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D494" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700376635</t>
+        </is>
+      </c>
+      <c r="E494" t="inlineStr"/>
+      <c r="F494" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Reko60</t>
+        </is>
+      </c>
+      <c r="C495" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D495" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700376635</t>
+        </is>
+      </c>
+      <c r="E495" t="inlineStr"/>
+      <c r="F495" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>Reko60</t>
+        </is>
+      </c>
+      <c r="C496" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D496" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700376635</t>
+        </is>
+      </c>
+      <c r="E496" t="n">
+        <v>387</v>
+      </c>
+      <c r="F496" t="inlineStr"/>
+    </row>
+    <row r="497">
+      <c r="A497" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>8251020</t>
+        </is>
+      </c>
+      <c r="C497" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D497" t="inlineStr">
+        <is>
+          <t>Order 8251020 Swish +46707678891</t>
+        </is>
+      </c>
+      <c r="E497" t="inlineStr"/>
+      <c r="F497" t="n">
+        <v>588.39</v>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>8251020</t>
+        </is>
+      </c>
+      <c r="C498" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D498" t="inlineStr">
+        <is>
+          <t>Order 8251020 Swish +46707678891</t>
+        </is>
+      </c>
+      <c r="E498" t="inlineStr"/>
+      <c r="F498" t="n">
+        <v>70.61</v>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>8251020</t>
+        </is>
+      </c>
+      <c r="C499" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D499" t="inlineStr">
+        <is>
+          <t>Order 8251020 Swish +46707678891</t>
+        </is>
+      </c>
+      <c r="E499" t="n">
+        <v>659</v>
+      </c>
+      <c r="F499" t="inlineStr"/>
+    </row>
+    <row r="500">
+      <c r="A500" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B500" t="inlineStr"/>
+      <c r="C500" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D500" t="inlineStr">
+        <is>
+          <t>VISTAPRINT K0135</t>
+        </is>
+      </c>
+      <c r="E500" t="n">
+        <v>844</v>
+      </c>
+      <c r="F500" t="inlineStr"/>
+    </row>
+    <row r="501">
+      <c r="A501" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B501" t="inlineStr"/>
+      <c r="C501" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D501" t="inlineStr">
+        <is>
+          <t>VISTAPRINT K0135</t>
+        </is>
+      </c>
+      <c r="E501" t="n">
+        <v>211</v>
+      </c>
+      <c r="F501" t="inlineStr"/>
+    </row>
+    <row r="502">
+      <c r="A502" s="2" t="n">
+        <v>44280</v>
+      </c>
+      <c r="B502" t="inlineStr"/>
+      <c r="C502" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D502" t="inlineStr">
+        <is>
+          <t>VISTAPRINT K0135</t>
+        </is>
+      </c>
+      <c r="E502" t="inlineStr"/>
+      <c r="F502" t="n">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" s="2" t="n">
+        <v>44282</v>
+      </c>
+      <c r="B503" t="inlineStr"/>
+      <c r="C503" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D503" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E503" t="n">
+        <v>1333.05</v>
+      </c>
+      <c r="F503" t="inlineStr"/>
+    </row>
+    <row r="504">
+      <c r="A504" s="2" t="n">
+        <v>44282</v>
+      </c>
+      <c r="B504" t="inlineStr"/>
+      <c r="C504" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D504" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E504" t="n">
+        <v>159.97</v>
+      </c>
+      <c r="F504" t="inlineStr"/>
+    </row>
+    <row r="505">
+      <c r="A505" s="2" t="n">
+        <v>44282</v>
+      </c>
+      <c r="B505" t="inlineStr"/>
+      <c r="C505" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D505" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E505" t="inlineStr"/>
+      <c r="F505" t="n">
+        <v>1493.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 54 new rows for week ending 2021-04-04 (total 558 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F505"/>
+  <dimension ref="A1:F559"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10657,6 +10657,1158 @@
         <v>1493.02</v>
       </c>
     </row>
+    <row r="506">
+      <c r="A506" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Reko61</t>
+        </is>
+      </c>
+      <c r="C506" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D506" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E506" t="inlineStr"/>
+      <c r="F506" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Reko61</t>
+        </is>
+      </c>
+      <c r="C507" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D507" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E507" t="inlineStr"/>
+      <c r="F507" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Reko61</t>
+        </is>
+      </c>
+      <c r="C508" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D508" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E508" t="n">
+        <v>516</v>
+      </c>
+      <c r="F508" t="inlineStr"/>
+    </row>
+    <row r="509">
+      <c r="A509" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Reko62</t>
+        </is>
+      </c>
+      <c r="C509" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E509" t="inlineStr"/>
+      <c r="F509" t="n">
+        <v>371.43</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Reko62</t>
+        </is>
+      </c>
+      <c r="C510" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E510" t="inlineStr"/>
+      <c r="F510" t="n">
+        <v>44.57</v>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Reko62</t>
+        </is>
+      </c>
+      <c r="C511" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D511" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E511" t="n">
+        <v>416</v>
+      </c>
+      <c r="F511" t="inlineStr"/>
+    </row>
+    <row r="512">
+      <c r="A512" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Reko63</t>
+        </is>
+      </c>
+      <c r="C512" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D512" t="inlineStr">
+        <is>
+          <t>Reko Swish +46721459019</t>
+        </is>
+      </c>
+      <c r="E512" t="inlineStr"/>
+      <c r="F512" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Reko63</t>
+        </is>
+      </c>
+      <c r="C513" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D513" t="inlineStr">
+        <is>
+          <t>Reko Swish +46721459019</t>
+        </is>
+      </c>
+      <c r="E513" t="inlineStr"/>
+      <c r="F513" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Reko63</t>
+        </is>
+      </c>
+      <c r="C514" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D514" t="inlineStr">
+        <is>
+          <t>Reko Swish +46721459019</t>
+        </is>
+      </c>
+      <c r="E514" t="n">
+        <v>774</v>
+      </c>
+      <c r="F514" t="inlineStr"/>
+    </row>
+    <row r="515">
+      <c r="A515" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Reko64</t>
+        </is>
+      </c>
+      <c r="C515" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D515" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737032257</t>
+        </is>
+      </c>
+      <c r="E515" t="inlineStr"/>
+      <c r="F515" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Reko64</t>
+        </is>
+      </c>
+      <c r="C516" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D516" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737032257</t>
+        </is>
+      </c>
+      <c r="E516" t="inlineStr"/>
+      <c r="F516" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Reko64</t>
+        </is>
+      </c>
+      <c r="C517" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D517" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737032257</t>
+        </is>
+      </c>
+      <c r="E517" t="n">
+        <v>258</v>
+      </c>
+      <c r="F517" t="inlineStr"/>
+    </row>
+    <row r="518">
+      <c r="A518" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Reko65</t>
+        </is>
+      </c>
+      <c r="C518" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D518" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E518" t="inlineStr"/>
+      <c r="F518" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Reko65</t>
+        </is>
+      </c>
+      <c r="C519" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D519" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E519" t="inlineStr"/>
+      <c r="F519" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Reko65</t>
+        </is>
+      </c>
+      <c r="C520" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D520" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E520" t="n">
+        <v>690</v>
+      </c>
+      <c r="F520" t="inlineStr"/>
+    </row>
+    <row r="521">
+      <c r="A521" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Reko66</t>
+        </is>
+      </c>
+      <c r="C521" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D521" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E521" t="inlineStr"/>
+      <c r="F521" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Reko66</t>
+        </is>
+      </c>
+      <c r="C522" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D522" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E522" t="inlineStr"/>
+      <c r="F522" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Reko66</t>
+        </is>
+      </c>
+      <c r="C523" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D523" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E523" t="n">
+        <v>258</v>
+      </c>
+      <c r="F523" t="inlineStr"/>
+    </row>
+    <row r="524">
+      <c r="A524" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Reko67</t>
+        </is>
+      </c>
+      <c r="C524" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D524" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737600861</t>
+        </is>
+      </c>
+      <c r="E524" t="inlineStr"/>
+      <c r="F524" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Reko67</t>
+        </is>
+      </c>
+      <c r="C525" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D525" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737600861</t>
+        </is>
+      </c>
+      <c r="E525" t="inlineStr"/>
+      <c r="F525" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Reko67</t>
+        </is>
+      </c>
+      <c r="C526" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D526" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737600861</t>
+        </is>
+      </c>
+      <c r="E526" t="n">
+        <v>258</v>
+      </c>
+      <c r="F526" t="inlineStr"/>
+    </row>
+    <row r="527">
+      <c r="A527" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B527" t="inlineStr"/>
+      <c r="C527" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D527" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E527" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="F527" t="inlineStr"/>
+    </row>
+    <row r="528">
+      <c r="A528" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B528" t="inlineStr"/>
+      <c r="C528" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D528" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E528" t="n">
+        <v>10.19</v>
+      </c>
+      <c r="F528" t="inlineStr"/>
+    </row>
+    <row r="529">
+      <c r="A529" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B529" t="inlineStr"/>
+      <c r="C529" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D529" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E529" t="inlineStr"/>
+      <c r="F529" t="n">
+        <v>95.09</v>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B530" t="inlineStr"/>
+      <c r="C530" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D530" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E530" t="n">
+        <v>328.1</v>
+      </c>
+      <c r="F530" t="inlineStr"/>
+    </row>
+    <row r="531">
+      <c r="A531" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B531" t="inlineStr"/>
+      <c r="C531" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D531" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E531" t="n">
+        <v>39.37</v>
+      </c>
+      <c r="F531" t="inlineStr"/>
+    </row>
+    <row r="532">
+      <c r="A532" s="2" t="n">
+        <v>44284</v>
+      </c>
+      <c r="B532" t="inlineStr"/>
+      <c r="C532" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D532" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E532" t="inlineStr"/>
+      <c r="F532" t="n">
+        <v>367.47</v>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Reko68</t>
+        </is>
+      </c>
+      <c r="C533" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D533" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703384055</t>
+        </is>
+      </c>
+      <c r="E533" t="inlineStr"/>
+      <c r="F533" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Reko68</t>
+        </is>
+      </c>
+      <c r="C534" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D534" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703384055</t>
+        </is>
+      </c>
+      <c r="E534" t="inlineStr"/>
+      <c r="F534" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Reko68</t>
+        </is>
+      </c>
+      <c r="C535" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D535" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703384055</t>
+        </is>
+      </c>
+      <c r="E535" t="n">
+        <v>258</v>
+      </c>
+      <c r="F535" t="inlineStr"/>
+    </row>
+    <row r="536">
+      <c r="A536" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Reko69</t>
+        </is>
+      </c>
+      <c r="C536" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D536" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708649109</t>
+        </is>
+      </c>
+      <c r="E536" t="inlineStr"/>
+      <c r="F536" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Reko69</t>
+        </is>
+      </c>
+      <c r="C537" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D537" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708649109</t>
+        </is>
+      </c>
+      <c r="E537" t="inlineStr"/>
+      <c r="F537" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Reko69</t>
+        </is>
+      </c>
+      <c r="C538" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D538" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708649109</t>
+        </is>
+      </c>
+      <c r="E538" t="n">
+        <v>690</v>
+      </c>
+      <c r="F538" t="inlineStr"/>
+    </row>
+    <row r="539">
+      <c r="A539" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Reko70</t>
+        </is>
+      </c>
+      <c r="C539" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D539" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704545110</t>
+        </is>
+      </c>
+      <c r="E539" t="inlineStr"/>
+      <c r="F539" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Reko70</t>
+        </is>
+      </c>
+      <c r="C540" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D540" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704545110</t>
+        </is>
+      </c>
+      <c r="E540" t="inlineStr"/>
+      <c r="F540" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Reko70</t>
+        </is>
+      </c>
+      <c r="C541" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D541" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704545110</t>
+        </is>
+      </c>
+      <c r="E541" t="n">
+        <v>516</v>
+      </c>
+      <c r="F541" t="inlineStr"/>
+    </row>
+    <row r="542">
+      <c r="A542" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Reko71</t>
+        </is>
+      </c>
+      <c r="C542" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D542" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723047499</t>
+        </is>
+      </c>
+      <c r="E542" t="inlineStr"/>
+      <c r="F542" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Reko71</t>
+        </is>
+      </c>
+      <c r="C543" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D543" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723047499</t>
+        </is>
+      </c>
+      <c r="E543" t="inlineStr"/>
+      <c r="F543" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Reko71</t>
+        </is>
+      </c>
+      <c r="C544" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D544" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723047499</t>
+        </is>
+      </c>
+      <c r="E544" t="n">
+        <v>474</v>
+      </c>
+      <c r="F544" t="inlineStr"/>
+    </row>
+    <row r="545">
+      <c r="A545" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Reko72</t>
+        </is>
+      </c>
+      <c r="C545" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D545" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703242407</t>
+        </is>
+      </c>
+      <c r="E545" t="inlineStr"/>
+      <c r="F545" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Reko72</t>
+        </is>
+      </c>
+      <c r="C546" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D546" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703242407</t>
+        </is>
+      </c>
+      <c r="E546" t="inlineStr"/>
+      <c r="F546" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Reko72</t>
+        </is>
+      </c>
+      <c r="C547" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D547" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703242407</t>
+        </is>
+      </c>
+      <c r="E547" t="n">
+        <v>690</v>
+      </c>
+      <c r="F547" t="inlineStr"/>
+    </row>
+    <row r="548">
+      <c r="A548" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Reko73</t>
+        </is>
+      </c>
+      <c r="C548" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D548" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707964655</t>
+        </is>
+      </c>
+      <c r="E548" t="inlineStr"/>
+      <c r="F548" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Reko73</t>
+        </is>
+      </c>
+      <c r="C549" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D549" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707964655</t>
+        </is>
+      </c>
+      <c r="E549" t="inlineStr"/>
+      <c r="F549" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" s="2" t="n">
+        <v>44285</v>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Reko73</t>
+        </is>
+      </c>
+      <c r="C550" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D550" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707964655</t>
+        </is>
+      </c>
+      <c r="E550" t="n">
+        <v>237</v>
+      </c>
+      <c r="F550" t="inlineStr"/>
+    </row>
+    <row r="551">
+      <c r="A551" s="2" t="n">
+        <v>44286</v>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>Reko74</t>
+        </is>
+      </c>
+      <c r="C551" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D551" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704608939</t>
+        </is>
+      </c>
+      <c r="E551" t="inlineStr"/>
+      <c r="F551" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" s="2" t="n">
+        <v>44286</v>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Reko74</t>
+        </is>
+      </c>
+      <c r="C552" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D552" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704608939</t>
+        </is>
+      </c>
+      <c r="E552" t="inlineStr"/>
+      <c r="F552" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" s="2" t="n">
+        <v>44286</v>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Reko74</t>
+        </is>
+      </c>
+      <c r="C553" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D553" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704608939</t>
+        </is>
+      </c>
+      <c r="E553" t="n">
+        <v>258</v>
+      </c>
+      <c r="F553" t="inlineStr"/>
+    </row>
+    <row r="554">
+      <c r="A554" s="2" t="n">
+        <v>44287</v>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>1012353</t>
+        </is>
+      </c>
+      <c r="C554" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D554" t="inlineStr">
+        <is>
+          <t>Order 1012353 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E554" t="inlineStr"/>
+      <c r="F554" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" s="2" t="n">
+        <v>44287</v>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>1012353</t>
+        </is>
+      </c>
+      <c r="C555" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D555" t="inlineStr">
+        <is>
+          <t>Order 1012353 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E555" t="inlineStr"/>
+      <c r="F555" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" s="2" t="n">
+        <v>44287</v>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>1012353</t>
+        </is>
+      </c>
+      <c r="C556" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D556" t="inlineStr">
+        <is>
+          <t>Order 1012353 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E556" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F556" t="inlineStr"/>
+    </row>
+    <row r="557">
+      <c r="A557" s="2" t="n">
+        <v>44290</v>
+      </c>
+      <c r="B557" t="inlineStr"/>
+      <c r="C557" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D557" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E557" t="n">
+        <v>172.32</v>
+      </c>
+      <c r="F557" t="inlineStr"/>
+    </row>
+    <row r="558">
+      <c r="A558" s="2" t="n">
+        <v>44290</v>
+      </c>
+      <c r="B558" t="inlineStr"/>
+      <c r="C558" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D558" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E558" t="n">
+        <v>20.68</v>
+      </c>
+      <c r="F558" t="inlineStr"/>
+    </row>
+    <row r="559">
+      <c r="A559" s="2" t="n">
+        <v>44290</v>
+      </c>
+      <c r="B559" t="inlineStr"/>
+      <c r="C559" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D559" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E559" t="inlineStr"/>
+      <c r="F559" t="n">
+        <v>193</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 45 new rows for week ending 2021-04-11 (total 603 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F559"/>
+  <dimension ref="A1:F604"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11809,6 +11809,946 @@
         <v>193</v>
       </c>
     </row>
+    <row r="560">
+      <c r="A560" s="2" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>1051155</t>
+        </is>
+      </c>
+      <c r="C560" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D560" t="inlineStr">
+        <is>
+          <t>Order 1051155 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E560" t="inlineStr"/>
+      <c r="F560" t="n">
+        <v>330.36</v>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" s="2" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>1051155</t>
+        </is>
+      </c>
+      <c r="C561" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D561" t="inlineStr">
+        <is>
+          <t>Order 1051155 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E561" t="inlineStr"/>
+      <c r="F561" t="n">
+        <v>39.64</v>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" s="2" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>1051155</t>
+        </is>
+      </c>
+      <c r="C562" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D562" t="inlineStr">
+        <is>
+          <t>Order 1051155 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E562" t="n">
+        <v>370</v>
+      </c>
+      <c r="F562" t="inlineStr"/>
+    </row>
+    <row r="563">
+      <c r="A563" s="2" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B563" t="inlineStr"/>
+      <c r="C563" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D563" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E563" t="n">
+        <v>663.73</v>
+      </c>
+      <c r="F563" t="inlineStr"/>
+    </row>
+    <row r="564">
+      <c r="A564" s="2" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B564" t="inlineStr"/>
+      <c r="C564" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D564" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E564" t="n">
+        <v>165.93</v>
+      </c>
+      <c r="F564" t="inlineStr"/>
+    </row>
+    <row r="565">
+      <c r="A565" s="2" t="n">
+        <v>44291</v>
+      </c>
+      <c r="B565" t="inlineStr"/>
+      <c r="C565" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D565" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K6885</t>
+        </is>
+      </c>
+      <c r="E565" t="inlineStr"/>
+      <c r="F565" t="n">
+        <v>829.66</v>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Reko75</t>
+        </is>
+      </c>
+      <c r="C566" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D566" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733035539</t>
+        </is>
+      </c>
+      <c r="E566" t="inlineStr"/>
+      <c r="F566" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Reko75</t>
+        </is>
+      </c>
+      <c r="C567" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D567" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733035539</t>
+        </is>
+      </c>
+      <c r="E567" t="inlineStr"/>
+      <c r="F567" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Reko75</t>
+        </is>
+      </c>
+      <c r="C568" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D568" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733035539</t>
+        </is>
+      </c>
+      <c r="E568" t="n">
+        <v>516</v>
+      </c>
+      <c r="F568" t="inlineStr"/>
+    </row>
+    <row r="569">
+      <c r="A569" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Reko76</t>
+        </is>
+      </c>
+      <c r="C569" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D569" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731835553</t>
+        </is>
+      </c>
+      <c r="E569" t="inlineStr"/>
+      <c r="F569" t="n">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Reko76</t>
+        </is>
+      </c>
+      <c r="C570" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D570" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731835553</t>
+        </is>
+      </c>
+      <c r="E570" t="inlineStr"/>
+      <c r="F570" t="n">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Reko76</t>
+        </is>
+      </c>
+      <c r="C571" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D571" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731835553</t>
+        </is>
+      </c>
+      <c r="E571" t="n">
+        <v>208</v>
+      </c>
+      <c r="F571" t="inlineStr"/>
+    </row>
+    <row r="572">
+      <c r="A572" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>9061234</t>
+        </is>
+      </c>
+      <c r="C572" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D572" t="inlineStr">
+        <is>
+          <t>Order 9061234 Swish +46705293845</t>
+        </is>
+      </c>
+      <c r="E572" t="inlineStr"/>
+      <c r="F572" t="n">
+        <v>610.71</v>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>9061234</t>
+        </is>
+      </c>
+      <c r="C573" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D573" t="inlineStr">
+        <is>
+          <t>Order 9061234 Swish +46705293845</t>
+        </is>
+      </c>
+      <c r="E573" t="inlineStr"/>
+      <c r="F573" t="n">
+        <v>73.29000000000001</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>9061234</t>
+        </is>
+      </c>
+      <c r="C574" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>Order 9061234 Swish +46705293845</t>
+        </is>
+      </c>
+      <c r="E574" t="n">
+        <v>684</v>
+      </c>
+      <c r="F574" t="inlineStr"/>
+    </row>
+    <row r="575">
+      <c r="A575" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Reko77</t>
+        </is>
+      </c>
+      <c r="C575" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709622907</t>
+        </is>
+      </c>
+      <c r="E575" t="inlineStr"/>
+      <c r="F575" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Reko77</t>
+        </is>
+      </c>
+      <c r="C576" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709622907</t>
+        </is>
+      </c>
+      <c r="E576" t="inlineStr"/>
+      <c r="F576" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="2" t="n">
+        <v>44292</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Reko77</t>
+        </is>
+      </c>
+      <c r="C577" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709622907</t>
+        </is>
+      </c>
+      <c r="E577" t="n">
+        <v>316</v>
+      </c>
+      <c r="F577" t="inlineStr"/>
+    </row>
+    <row r="578">
+      <c r="A578" s="2" t="n">
+        <v>44293</v>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Reko78</t>
+        </is>
+      </c>
+      <c r="C578" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E578" t="inlineStr"/>
+      <c r="F578" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="2" t="n">
+        <v>44293</v>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Reko78</t>
+        </is>
+      </c>
+      <c r="C579" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E579" t="inlineStr"/>
+      <c r="F579" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="2" t="n">
+        <v>44293</v>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Reko78</t>
+        </is>
+      </c>
+      <c r="C580" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E580" t="n">
+        <v>158</v>
+      </c>
+      <c r="F580" t="inlineStr"/>
+    </row>
+    <row r="581">
+      <c r="A581" s="2" t="n">
+        <v>44293</v>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>5072119</t>
+        </is>
+      </c>
+      <c r="C581" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>Order 5072119 Swish +46730402047</t>
+        </is>
+      </c>
+      <c r="E581" t="inlineStr"/>
+      <c r="F581" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="2" t="n">
+        <v>44293</v>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>5072119</t>
+        </is>
+      </c>
+      <c r="C582" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>Order 5072119 Swish +46730402047</t>
+        </is>
+      </c>
+      <c r="E582" t="inlineStr"/>
+      <c r="F582" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="2" t="n">
+        <v>44293</v>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>5072119</t>
+        </is>
+      </c>
+      <c r="C583" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>Order 5072119 Swish +46730402047</t>
+        </is>
+      </c>
+      <c r="E583" t="n">
+        <v>395</v>
+      </c>
+      <c r="F583" t="inlineStr"/>
+    </row>
+    <row r="584">
+      <c r="A584" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>3081627</t>
+        </is>
+      </c>
+      <c r="C584" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>Order 3081627 Swish +46768551925</t>
+        </is>
+      </c>
+      <c r="E584" t="inlineStr"/>
+      <c r="F584" t="n">
+        <v>956.25</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>3081627</t>
+        </is>
+      </c>
+      <c r="C585" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>Order 3081627 Swish +46768551925</t>
+        </is>
+      </c>
+      <c r="E585" t="inlineStr"/>
+      <c r="F585" t="n">
+        <v>114.75</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>3081627</t>
+        </is>
+      </c>
+      <c r="C586" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>Order 3081627 Swish +46768551925</t>
+        </is>
+      </c>
+      <c r="E586" t="n">
+        <v>1071</v>
+      </c>
+      <c r="F586" t="inlineStr"/>
+    </row>
+    <row r="587">
+      <c r="A587" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>7082223</t>
+        </is>
+      </c>
+      <c r="C587" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>Order 7082223 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E587" t="inlineStr"/>
+      <c r="F587" t="n">
+        <v>806.25</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>7082223</t>
+        </is>
+      </c>
+      <c r="C588" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>Order 7082223 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E588" t="inlineStr"/>
+      <c r="F588" t="n">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>7082223</t>
+        </is>
+      </c>
+      <c r="C589" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>Order 7082223 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E589" t="n">
+        <v>903</v>
+      </c>
+      <c r="F589" t="inlineStr"/>
+    </row>
+    <row r="590">
+      <c r="A590" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B590" t="inlineStr"/>
+      <c r="C590" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>FACEBK FZDBG3KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E590" t="n">
+        <v>430</v>
+      </c>
+      <c r="F590" t="inlineStr"/>
+    </row>
+    <row r="591">
+      <c r="A591" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B591" t="inlineStr"/>
+      <c r="C591" t="inlineStr"/>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>FACEBK FZDBG3KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E591" t="n">
+        <v>0</v>
+      </c>
+      <c r="F591" t="inlineStr"/>
+    </row>
+    <row r="592">
+      <c r="A592" s="2" t="n">
+        <v>44294</v>
+      </c>
+      <c r="B592" t="inlineStr"/>
+      <c r="C592" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>FACEBK FZDBG3KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E592" t="inlineStr"/>
+      <c r="F592" t="n">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" s="2" t="n">
+        <v>44295</v>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Reko79</t>
+        </is>
+      </c>
+      <c r="C593" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D593" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703344337</t>
+        </is>
+      </c>
+      <c r="E593" t="inlineStr"/>
+      <c r="F593" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" s="2" t="n">
+        <v>44295</v>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Reko79</t>
+        </is>
+      </c>
+      <c r="C594" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D594" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703344337</t>
+        </is>
+      </c>
+      <c r="E594" t="inlineStr"/>
+      <c r="F594" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" s="2" t="n">
+        <v>44295</v>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Reko79</t>
+        </is>
+      </c>
+      <c r="C595" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D595" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703344337</t>
+        </is>
+      </c>
+      <c r="E595" t="n">
+        <v>387</v>
+      </c>
+      <c r="F595" t="inlineStr"/>
+    </row>
+    <row r="596">
+      <c r="A596" s="2" t="n">
+        <v>44295</v>
+      </c>
+      <c r="B596" t="inlineStr"/>
+      <c r="C596" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D596" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E596" t="n">
+        <v>1929.28</v>
+      </c>
+      <c r="F596" t="inlineStr"/>
+    </row>
+    <row r="597">
+      <c r="A597" s="2" t="n">
+        <v>44295</v>
+      </c>
+      <c r="B597" t="inlineStr"/>
+      <c r="C597" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D597" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E597" t="n">
+        <v>231.51</v>
+      </c>
+      <c r="F597" t="inlineStr"/>
+    </row>
+    <row r="598">
+      <c r="A598" s="2" t="n">
+        <v>44295</v>
+      </c>
+      <c r="B598" t="inlineStr"/>
+      <c r="C598" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D598" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E598" t="inlineStr"/>
+      <c r="F598" t="n">
+        <v>2160.79</v>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" s="2" t="n">
+        <v>44296</v>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>6101315</t>
+        </is>
+      </c>
+      <c r="C599" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D599" t="inlineStr">
+        <is>
+          <t>Order 6101315 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E599" t="inlineStr"/>
+      <c r="F599" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" s="2" t="n">
+        <v>44296</v>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>6101315</t>
+        </is>
+      </c>
+      <c r="C600" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D600" t="inlineStr">
+        <is>
+          <t>Order 6101315 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E600" t="inlineStr"/>
+      <c r="F600" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" s="2" t="n">
+        <v>44296</v>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>6101315</t>
+        </is>
+      </c>
+      <c r="C601" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D601" t="inlineStr">
+        <is>
+          <t>Order 6101315 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E601" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F601" t="inlineStr"/>
+    </row>
+    <row r="602">
+      <c r="A602" s="2" t="n">
+        <v>44297</v>
+      </c>
+      <c r="B602" t="inlineStr"/>
+      <c r="C602" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D602" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E602" t="n">
+        <v>176.79</v>
+      </c>
+      <c r="F602" t="inlineStr"/>
+    </row>
+    <row r="603">
+      <c r="A603" s="2" t="n">
+        <v>44297</v>
+      </c>
+      <c r="B603" t="inlineStr"/>
+      <c r="C603" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D603" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E603" t="n">
+        <v>21.21</v>
+      </c>
+      <c r="F603" t="inlineStr"/>
+    </row>
+    <row r="604">
+      <c r="A604" s="2" t="n">
+        <v>44297</v>
+      </c>
+      <c r="B604" t="inlineStr"/>
+      <c r="C604" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D604" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E604" t="inlineStr"/>
+      <c r="F604" t="n">
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 45 new rows for week ending 2021-04-18 (total 648 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F604"/>
+  <dimension ref="A1:F649"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12749,6 +12749,972 @@
         <v>198</v>
       </c>
     </row>
+    <row r="605">
+      <c r="A605" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Reko80</t>
+        </is>
+      </c>
+      <c r="C605" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D605" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723047499</t>
+        </is>
+      </c>
+      <c r="E605" t="inlineStr"/>
+      <c r="F605" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Reko80</t>
+        </is>
+      </c>
+      <c r="C606" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723047499</t>
+        </is>
+      </c>
+      <c r="E606" t="inlineStr"/>
+      <c r="F606" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Reko80</t>
+        </is>
+      </c>
+      <c r="C607" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723047499</t>
+        </is>
+      </c>
+      <c r="E607" t="n">
+        <v>474</v>
+      </c>
+      <c r="F607" t="inlineStr"/>
+    </row>
+    <row r="608">
+      <c r="A608" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Reko81</t>
+        </is>
+      </c>
+      <c r="C608" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734058272</t>
+        </is>
+      </c>
+      <c r="E608" t="inlineStr"/>
+      <c r="F608" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Reko81</t>
+        </is>
+      </c>
+      <c r="C609" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734058272</t>
+        </is>
+      </c>
+      <c r="E609" t="inlineStr"/>
+      <c r="F609" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Reko81</t>
+        </is>
+      </c>
+      <c r="C610" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734058272</t>
+        </is>
+      </c>
+      <c r="E610" t="n">
+        <v>158</v>
+      </c>
+      <c r="F610" t="inlineStr"/>
+    </row>
+    <row r="611">
+      <c r="A611" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Reko82</t>
+        </is>
+      </c>
+      <c r="C611" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D611" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E611" t="inlineStr"/>
+      <c r="F611" t="n">
+        <v>512.5</v>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Reko82</t>
+        </is>
+      </c>
+      <c r="C612" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D612" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E612" t="inlineStr"/>
+      <c r="F612" t="n">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Reko82</t>
+        </is>
+      </c>
+      <c r="C613" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D613" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E613" t="n">
+        <v>574</v>
+      </c>
+      <c r="F613" t="inlineStr"/>
+    </row>
+    <row r="614">
+      <c r="A614" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>Reko83</t>
+        </is>
+      </c>
+      <c r="C614" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D614" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733706356</t>
+        </is>
+      </c>
+      <c r="E614" t="inlineStr"/>
+      <c r="F614" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Reko83</t>
+        </is>
+      </c>
+      <c r="C615" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D615" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733706356</t>
+        </is>
+      </c>
+      <c r="E615" t="inlineStr"/>
+      <c r="F615" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Reko83</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D616" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733706356</t>
+        </is>
+      </c>
+      <c r="E616" t="inlineStr"/>
+      <c r="F616" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>Reko84</t>
+        </is>
+      </c>
+      <c r="C617" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D617" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733706356</t>
+        </is>
+      </c>
+      <c r="E617" t="inlineStr"/>
+      <c r="F617" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Reko84</t>
+        </is>
+      </c>
+      <c r="C618" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D618" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733706356</t>
+        </is>
+      </c>
+      <c r="E618" t="n">
+        <v>158</v>
+      </c>
+      <c r="F618" t="inlineStr"/>
+    </row>
+    <row r="619">
+      <c r="A619" s="2" t="n">
+        <v>44298</v>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Reko84</t>
+        </is>
+      </c>
+      <c r="C619" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D619" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733706356</t>
+        </is>
+      </c>
+      <c r="E619" t="n">
+        <v>158</v>
+      </c>
+      <c r="F619" t="inlineStr"/>
+    </row>
+    <row r="620">
+      <c r="A620" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Reko85</t>
+        </is>
+      </c>
+      <c r="C620" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D620" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720444719</t>
+        </is>
+      </c>
+      <c r="E620" t="inlineStr"/>
+      <c r="F620" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Reko85</t>
+        </is>
+      </c>
+      <c r="C621" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D621" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720444719</t>
+        </is>
+      </c>
+      <c r="E621" t="inlineStr"/>
+      <c r="F621" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Reko85</t>
+        </is>
+      </c>
+      <c r="C622" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D622" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720444719</t>
+        </is>
+      </c>
+      <c r="E622" t="n">
+        <v>158</v>
+      </c>
+      <c r="F622" t="inlineStr"/>
+    </row>
+    <row r="623">
+      <c r="A623" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Reko86</t>
+        </is>
+      </c>
+      <c r="C623" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D623" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E623" t="inlineStr"/>
+      <c r="F623" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Reko86</t>
+        </is>
+      </c>
+      <c r="C624" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D624" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E624" t="inlineStr"/>
+      <c r="F624" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Reko86</t>
+        </is>
+      </c>
+      <c r="C625" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E625" t="n">
+        <v>690</v>
+      </c>
+      <c r="F625" t="inlineStr"/>
+    </row>
+    <row r="626">
+      <c r="A626" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Reko87</t>
+        </is>
+      </c>
+      <c r="C626" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E626" t="inlineStr"/>
+      <c r="F626" t="n">
+        <v>398.21</v>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Reko87</t>
+        </is>
+      </c>
+      <c r="C627" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E627" t="inlineStr"/>
+      <c r="F627" t="n">
+        <v>47.79</v>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Reko87</t>
+        </is>
+      </c>
+      <c r="C628" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E628" t="n">
+        <v>446</v>
+      </c>
+      <c r="F628" t="inlineStr"/>
+    </row>
+    <row r="629">
+      <c r="A629" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Reko88</t>
+        </is>
+      </c>
+      <c r="C629" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705716511</t>
+        </is>
+      </c>
+      <c r="E629" t="inlineStr"/>
+      <c r="F629" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Reko88</t>
+        </is>
+      </c>
+      <c r="C630" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705716511</t>
+        </is>
+      </c>
+      <c r="E630" t="inlineStr"/>
+      <c r="F630" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Reko88</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705716511</t>
+        </is>
+      </c>
+      <c r="E631" t="n">
+        <v>316</v>
+      </c>
+      <c r="F631" t="inlineStr"/>
+    </row>
+    <row r="632">
+      <c r="A632" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Reko89</t>
+        </is>
+      </c>
+      <c r="C632" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D632" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705725419</t>
+        </is>
+      </c>
+      <c r="E632" t="inlineStr"/>
+      <c r="F632" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Reko89</t>
+        </is>
+      </c>
+      <c r="C633" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D633" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705725419</t>
+        </is>
+      </c>
+      <c r="E633" t="inlineStr"/>
+      <c r="F633" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" s="2" t="n">
+        <v>44299</v>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Reko89</t>
+        </is>
+      </c>
+      <c r="C634" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D634" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705725419</t>
+        </is>
+      </c>
+      <c r="E634" t="n">
+        <v>258</v>
+      </c>
+      <c r="F634" t="inlineStr"/>
+    </row>
+    <row r="635">
+      <c r="A635" s="2" t="n">
+        <v>44300</v>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Reko90</t>
+        </is>
+      </c>
+      <c r="C635" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D635" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703384055</t>
+        </is>
+      </c>
+      <c r="E635" t="inlineStr"/>
+      <c r="F635" t="n">
+        <v>610.71</v>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" s="2" t="n">
+        <v>44300</v>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Reko90</t>
+        </is>
+      </c>
+      <c r="C636" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D636" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703384055</t>
+        </is>
+      </c>
+      <c r="E636" t="inlineStr"/>
+      <c r="F636" t="n">
+        <v>73.29000000000001</v>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" s="2" t="n">
+        <v>44300</v>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Reko90</t>
+        </is>
+      </c>
+      <c r="C637" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D637" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703384055</t>
+        </is>
+      </c>
+      <c r="E637" t="n">
+        <v>684</v>
+      </c>
+      <c r="F637" t="inlineStr"/>
+    </row>
+    <row r="638">
+      <c r="A638" s="2" t="n">
+        <v>44301</v>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Reko91</t>
+        </is>
+      </c>
+      <c r="C638" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D638" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706649892</t>
+        </is>
+      </c>
+      <c r="E638" t="inlineStr"/>
+      <c r="F638" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" s="2" t="n">
+        <v>44301</v>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>Reko91</t>
+        </is>
+      </c>
+      <c r="C639" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D639" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706649892</t>
+        </is>
+      </c>
+      <c r="E639" t="inlineStr"/>
+      <c r="F639" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" s="2" t="n">
+        <v>44301</v>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Reko91</t>
+        </is>
+      </c>
+      <c r="C640" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D640" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706649892</t>
+        </is>
+      </c>
+      <c r="E640" t="n">
+        <v>474</v>
+      </c>
+      <c r="F640" t="inlineStr"/>
+    </row>
+    <row r="641">
+      <c r="A641" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Reko92</t>
+        </is>
+      </c>
+      <c r="C641" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D641" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E641" t="inlineStr"/>
+      <c r="F641" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Reko92</t>
+        </is>
+      </c>
+      <c r="C642" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D642" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E642" t="inlineStr"/>
+      <c r="F642" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Reko92</t>
+        </is>
+      </c>
+      <c r="C643" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D643" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739582203</t>
+        </is>
+      </c>
+      <c r="E643" t="n">
+        <v>645</v>
+      </c>
+      <c r="F643" t="inlineStr"/>
+    </row>
+    <row r="644">
+      <c r="A644" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B644" t="inlineStr"/>
+      <c r="C644" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D644" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E644" t="n">
+        <v>3104</v>
+      </c>
+      <c r="F644" t="inlineStr"/>
+    </row>
+    <row r="645">
+      <c r="A645" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B645" t="inlineStr"/>
+      <c r="C645" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D645" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E645" t="n">
+        <v>776</v>
+      </c>
+      <c r="F645" t="inlineStr"/>
+    </row>
+    <row r="646">
+      <c r="A646" s="2" t="n">
+        <v>44302</v>
+      </c>
+      <c r="B646" t="inlineStr"/>
+      <c r="C646" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D646" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E646" t="inlineStr"/>
+      <c r="F646" t="n">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" s="2" t="n">
+        <v>44303</v>
+      </c>
+      <c r="B647" t="inlineStr"/>
+      <c r="C647" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D647" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E647" t="n">
+        <v>14845.6</v>
+      </c>
+      <c r="F647" t="inlineStr"/>
+    </row>
+    <row r="648">
+      <c r="A648" s="2" t="n">
+        <v>44303</v>
+      </c>
+      <c r="B648" t="inlineStr"/>
+      <c r="C648" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D648" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E648" t="n">
+        <v>3711.4</v>
+      </c>
+      <c r="F648" t="inlineStr"/>
+    </row>
+    <row r="649">
+      <c r="A649" s="2" t="n">
+        <v>44303</v>
+      </c>
+      <c r="B649" t="inlineStr"/>
+      <c r="C649" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D649" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E649" t="inlineStr"/>
+      <c r="F649" t="n">
+        <v>18557</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 24 new rows for week ending 2021-04-25 (total 672 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F649"/>
+  <dimension ref="A1:F673"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13715,6 +13715,496 @@
         <v>18557</v>
       </c>
     </row>
+    <row r="650">
+      <c r="A650" s="2" t="n">
+        <v>44305</v>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Reko93</t>
+        </is>
+      </c>
+      <c r="C650" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D650" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708261018</t>
+        </is>
+      </c>
+      <c r="E650" t="inlineStr"/>
+      <c r="F650" t="n">
+        <v>610.71</v>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" s="2" t="n">
+        <v>44305</v>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Reko93</t>
+        </is>
+      </c>
+      <c r="C651" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D651" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708261018</t>
+        </is>
+      </c>
+      <c r="E651" t="inlineStr"/>
+      <c r="F651" t="n">
+        <v>73.29000000000001</v>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" s="2" t="n">
+        <v>44305</v>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Reko93</t>
+        </is>
+      </c>
+      <c r="C652" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D652" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708261018</t>
+        </is>
+      </c>
+      <c r="E652" t="n">
+        <v>684</v>
+      </c>
+      <c r="F652" t="inlineStr"/>
+    </row>
+    <row r="653">
+      <c r="A653" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B653" t="inlineStr"/>
+      <c r="C653" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D653" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E653" t="n">
+        <v>123</v>
+      </c>
+      <c r="F653" t="inlineStr"/>
+    </row>
+    <row r="654">
+      <c r="A654" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B654" t="inlineStr"/>
+      <c r="C654" t="inlineStr"/>
+      <c r="D654" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E654" t="n">
+        <v>0</v>
+      </c>
+      <c r="F654" t="inlineStr"/>
+    </row>
+    <row r="655">
+      <c r="A655" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B655" t="inlineStr"/>
+      <c r="C655" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D655" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E655" t="inlineStr"/>
+      <c r="F655" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>8201150</t>
+        </is>
+      </c>
+      <c r="C656" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D656" t="inlineStr">
+        <is>
+          <t>Order 8201150 Swish +46764282407</t>
+        </is>
+      </c>
+      <c r="E656" t="inlineStr"/>
+      <c r="F656" t="n">
+        <v>935.71</v>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>8201150</t>
+        </is>
+      </c>
+      <c r="C657" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D657" t="inlineStr">
+        <is>
+          <t>Order 8201150 Swish +46764282407</t>
+        </is>
+      </c>
+      <c r="E657" t="inlineStr"/>
+      <c r="F657" t="n">
+        <v>112.29</v>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>8201150</t>
+        </is>
+      </c>
+      <c r="C658" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D658" t="inlineStr">
+        <is>
+          <t>Order 8201150 Swish +46764282407</t>
+        </is>
+      </c>
+      <c r="E658" t="n">
+        <v>1048</v>
+      </c>
+      <c r="F658" t="inlineStr"/>
+    </row>
+    <row r="659">
+      <c r="A659" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B659" t="inlineStr"/>
+      <c r="C659" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D659" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E659" t="n">
+        <v>4988</v>
+      </c>
+      <c r="F659" t="inlineStr"/>
+    </row>
+    <row r="660">
+      <c r="A660" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B660" t="inlineStr"/>
+      <c r="C660" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D660" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E660" t="n">
+        <v>1247</v>
+      </c>
+      <c r="F660" t="inlineStr"/>
+    </row>
+    <row r="661">
+      <c r="A661" s="2" t="n">
+        <v>44306</v>
+      </c>
+      <c r="B661" t="inlineStr"/>
+      <c r="C661" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D661" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E661" t="inlineStr"/>
+      <c r="F661" t="n">
+        <v>6235</v>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" s="2" t="n">
+        <v>44308</v>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Reko94</t>
+        </is>
+      </c>
+      <c r="C662" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D662" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E662" t="inlineStr"/>
+      <c r="F662" t="n">
+        <v>739.29</v>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" s="2" t="n">
+        <v>44308</v>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Reko94</t>
+        </is>
+      </c>
+      <c r="C663" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D663" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E663" t="inlineStr"/>
+      <c r="F663" t="n">
+        <v>88.70999999999999</v>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" s="2" t="n">
+        <v>44308</v>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Reko94</t>
+        </is>
+      </c>
+      <c r="C664" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D664" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E664" t="n">
+        <v>828</v>
+      </c>
+      <c r="F664" t="inlineStr"/>
+    </row>
+    <row r="665">
+      <c r="A665" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Reko95</t>
+        </is>
+      </c>
+      <c r="C665" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D665" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E665" t="inlineStr"/>
+      <c r="F665" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Reko95</t>
+        </is>
+      </c>
+      <c r="C666" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D666" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E666" t="inlineStr"/>
+      <c r="F666" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Reko95</t>
+        </is>
+      </c>
+      <c r="C667" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D667" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E667" t="n">
+        <v>129</v>
+      </c>
+      <c r="F667" t="inlineStr"/>
+    </row>
+    <row r="668">
+      <c r="A668" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B668" t="inlineStr"/>
+      <c r="C668" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D668" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E668" t="n">
+        <v>795.1</v>
+      </c>
+      <c r="F668" t="inlineStr"/>
+    </row>
+    <row r="669">
+      <c r="A669" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B669" t="inlineStr"/>
+      <c r="C669" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D669" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E669" t="n">
+        <v>198.78</v>
+      </c>
+      <c r="F669" t="inlineStr"/>
+    </row>
+    <row r="670">
+      <c r="A670" s="2" t="n">
+        <v>44309</v>
+      </c>
+      <c r="B670" t="inlineStr"/>
+      <c r="C670" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D670" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E670" t="inlineStr"/>
+      <c r="F670" t="n">
+        <v>993.88</v>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" s="2" t="n">
+        <v>44311</v>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>7251015</t>
+        </is>
+      </c>
+      <c r="C671" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D671" t="inlineStr">
+        <is>
+          <t>Order 7251015 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E671" t="inlineStr"/>
+      <c r="F671" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" s="2" t="n">
+        <v>44311</v>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>7251015</t>
+        </is>
+      </c>
+      <c r="C672" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D672" t="inlineStr">
+        <is>
+          <t>Order 7251015 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E672" t="inlineStr"/>
+      <c r="F672" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" s="2" t="n">
+        <v>44311</v>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>7251015</t>
+        </is>
+      </c>
+      <c r="C673" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D673" t="inlineStr">
+        <is>
+          <t>Order 7251015 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E673" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F673" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 147 new rows for week ending 2021-05-02 (total 819 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F673"/>
+  <dimension ref="A1:F820"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14205,6 +14205,3144 @@
       </c>
       <c r="F673" t="inlineStr"/>
     </row>
+    <row r="674">
+      <c r="A674" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Reko96</t>
+        </is>
+      </c>
+      <c r="C674" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D674" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722459871</t>
+        </is>
+      </c>
+      <c r="E674" t="inlineStr"/>
+      <c r="F674" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Reko96</t>
+        </is>
+      </c>
+      <c r="C675" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D675" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722459871</t>
+        </is>
+      </c>
+      <c r="E675" t="inlineStr"/>
+      <c r="F675" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Reko96</t>
+        </is>
+      </c>
+      <c r="C676" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D676" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722459871</t>
+        </is>
+      </c>
+      <c r="E676" t="n">
+        <v>258</v>
+      </c>
+      <c r="F676" t="inlineStr"/>
+    </row>
+    <row r="677">
+      <c r="A677" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Reko97</t>
+        </is>
+      </c>
+      <c r="C677" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D677" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E677" t="inlineStr"/>
+      <c r="F677" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Reko97</t>
+        </is>
+      </c>
+      <c r="C678" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D678" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E678" t="inlineStr"/>
+      <c r="F678" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Reko97</t>
+        </is>
+      </c>
+      <c r="C679" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D679" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E679" t="n">
+        <v>129</v>
+      </c>
+      <c r="F679" t="inlineStr"/>
+    </row>
+    <row r="680">
+      <c r="A680" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Reko98</t>
+        </is>
+      </c>
+      <c r="C680" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D680" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705408280</t>
+        </is>
+      </c>
+      <c r="E680" t="inlineStr"/>
+      <c r="F680" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Reko98</t>
+        </is>
+      </c>
+      <c r="C681" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D681" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705408280</t>
+        </is>
+      </c>
+      <c r="E681" t="inlineStr"/>
+      <c r="F681" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Reko98</t>
+        </is>
+      </c>
+      <c r="C682" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D682" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705408280</t>
+        </is>
+      </c>
+      <c r="E682" t="n">
+        <v>258</v>
+      </c>
+      <c r="F682" t="inlineStr"/>
+    </row>
+    <row r="683">
+      <c r="A683" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Reko99</t>
+        </is>
+      </c>
+      <c r="C683" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D683" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703189513</t>
+        </is>
+      </c>
+      <c r="E683" t="inlineStr"/>
+      <c r="F683" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Reko99</t>
+        </is>
+      </c>
+      <c r="C684" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D684" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703189513</t>
+        </is>
+      </c>
+      <c r="E684" t="inlineStr"/>
+      <c r="F684" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Reko99</t>
+        </is>
+      </c>
+      <c r="C685" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D685" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703189513</t>
+        </is>
+      </c>
+      <c r="E685" t="n">
+        <v>258</v>
+      </c>
+      <c r="F685" t="inlineStr"/>
+    </row>
+    <row r="686">
+      <c r="A686" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Reko100</t>
+        </is>
+      </c>
+      <c r="C686" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D686" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735730525</t>
+        </is>
+      </c>
+      <c r="E686" t="inlineStr"/>
+      <c r="F686" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Reko100</t>
+        </is>
+      </c>
+      <c r="C687" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D687" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735730525</t>
+        </is>
+      </c>
+      <c r="E687" t="inlineStr"/>
+      <c r="F687" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Reko100</t>
+        </is>
+      </c>
+      <c r="C688" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D688" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735730525</t>
+        </is>
+      </c>
+      <c r="E688" t="n">
+        <v>258</v>
+      </c>
+      <c r="F688" t="inlineStr"/>
+    </row>
+    <row r="689">
+      <c r="A689" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Reko101</t>
+        </is>
+      </c>
+      <c r="C689" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D689" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E689" t="inlineStr"/>
+      <c r="F689" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Reko101</t>
+        </is>
+      </c>
+      <c r="C690" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D690" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E690" t="inlineStr"/>
+      <c r="F690" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Reko101</t>
+        </is>
+      </c>
+      <c r="C691" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D691" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E691" t="n">
+        <v>258</v>
+      </c>
+      <c r="F691" t="inlineStr"/>
+    </row>
+    <row r="692">
+      <c r="A692" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Reko102</t>
+        </is>
+      </c>
+      <c r="C692" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D692" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735955012</t>
+        </is>
+      </c>
+      <c r="E692" t="inlineStr"/>
+      <c r="F692" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Reko102</t>
+        </is>
+      </c>
+      <c r="C693" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D693" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735955012</t>
+        </is>
+      </c>
+      <c r="E693" t="inlineStr"/>
+      <c r="F693" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Reko102</t>
+        </is>
+      </c>
+      <c r="C694" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D694" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735955012</t>
+        </is>
+      </c>
+      <c r="E694" t="n">
+        <v>258</v>
+      </c>
+      <c r="F694" t="inlineStr"/>
+    </row>
+    <row r="695">
+      <c r="A695" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Reko103</t>
+        </is>
+      </c>
+      <c r="C695" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D695" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E695" t="inlineStr"/>
+      <c r="F695" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Reko103</t>
+        </is>
+      </c>
+      <c r="C696" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D696" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E696" t="inlineStr"/>
+      <c r="F696" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Reko103</t>
+        </is>
+      </c>
+      <c r="C697" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D697" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E697" t="n">
+        <v>395</v>
+      </c>
+      <c r="F697" t="inlineStr"/>
+    </row>
+    <row r="698">
+      <c r="A698" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Reko104</t>
+        </is>
+      </c>
+      <c r="C698" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D698" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775555</t>
+        </is>
+      </c>
+      <c r="E698" t="inlineStr"/>
+      <c r="F698" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Reko104</t>
+        </is>
+      </c>
+      <c r="C699" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D699" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775555</t>
+        </is>
+      </c>
+      <c r="E699" t="inlineStr"/>
+      <c r="F699" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Reko104</t>
+        </is>
+      </c>
+      <c r="C700" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D700" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775555</t>
+        </is>
+      </c>
+      <c r="E700" t="n">
+        <v>129</v>
+      </c>
+      <c r="F700" t="inlineStr"/>
+    </row>
+    <row r="701">
+      <c r="A701" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Reko105</t>
+        </is>
+      </c>
+      <c r="C701" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D701" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708168648</t>
+        </is>
+      </c>
+      <c r="E701" t="inlineStr"/>
+      <c r="F701" t="n">
+        <v>664.29</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Reko105</t>
+        </is>
+      </c>
+      <c r="C702" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D702" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708168648</t>
+        </is>
+      </c>
+      <c r="E702" t="inlineStr"/>
+      <c r="F702" t="n">
+        <v>79.70999999999999</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Reko105</t>
+        </is>
+      </c>
+      <c r="C703" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D703" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708168648</t>
+        </is>
+      </c>
+      <c r="E703" t="n">
+        <v>744</v>
+      </c>
+      <c r="F703" t="inlineStr"/>
+    </row>
+    <row r="704">
+      <c r="A704" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Reko106</t>
+        </is>
+      </c>
+      <c r="C704" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D704" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E704" t="inlineStr"/>
+      <c r="F704" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Reko106</t>
+        </is>
+      </c>
+      <c r="C705" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D705" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E705" t="inlineStr"/>
+      <c r="F705" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Reko106</t>
+        </is>
+      </c>
+      <c r="C706" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D706" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E706" t="n">
+        <v>258</v>
+      </c>
+      <c r="F706" t="inlineStr"/>
+    </row>
+    <row r="707">
+      <c r="A707" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Reko107</t>
+        </is>
+      </c>
+      <c r="C707" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D707" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705697204</t>
+        </is>
+      </c>
+      <c r="E707" t="inlineStr"/>
+      <c r="F707" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Reko107</t>
+        </is>
+      </c>
+      <c r="C708" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D708" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705697204</t>
+        </is>
+      </c>
+      <c r="E708" t="inlineStr"/>
+      <c r="F708" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>Reko107</t>
+        </is>
+      </c>
+      <c r="C709" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D709" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705697204</t>
+        </is>
+      </c>
+      <c r="E709" t="n">
+        <v>258</v>
+      </c>
+      <c r="F709" t="inlineStr"/>
+    </row>
+    <row r="710">
+      <c r="A710" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Reko108</t>
+        </is>
+      </c>
+      <c r="C710" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D710" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703536455</t>
+        </is>
+      </c>
+      <c r="E710" t="inlineStr"/>
+      <c r="F710" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Reko108</t>
+        </is>
+      </c>
+      <c r="C711" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D711" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703536455</t>
+        </is>
+      </c>
+      <c r="E711" t="inlineStr"/>
+      <c r="F711" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Reko108</t>
+        </is>
+      </c>
+      <c r="C712" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D712" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703536455</t>
+        </is>
+      </c>
+      <c r="E712" t="n">
+        <v>258</v>
+      </c>
+      <c r="F712" t="inlineStr"/>
+    </row>
+    <row r="713">
+      <c r="A713" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Reko109</t>
+        </is>
+      </c>
+      <c r="C713" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D713" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E713" t="inlineStr"/>
+      <c r="F713" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Reko109</t>
+        </is>
+      </c>
+      <c r="C714" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D714" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E714" t="inlineStr"/>
+      <c r="F714" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Reko109</t>
+        </is>
+      </c>
+      <c r="C715" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D715" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E715" t="n">
+        <v>395</v>
+      </c>
+      <c r="F715" t="inlineStr"/>
+    </row>
+    <row r="716">
+      <c r="A716" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Reko110</t>
+        </is>
+      </c>
+      <c r="C716" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D716" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733492183</t>
+        </is>
+      </c>
+      <c r="E716" t="inlineStr"/>
+      <c r="F716" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>Reko110</t>
+        </is>
+      </c>
+      <c r="C717" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D717" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733492183</t>
+        </is>
+      </c>
+      <c r="E717" t="inlineStr"/>
+      <c r="F717" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Reko110</t>
+        </is>
+      </c>
+      <c r="C718" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D718" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733492183</t>
+        </is>
+      </c>
+      <c r="E718" t="n">
+        <v>516</v>
+      </c>
+      <c r="F718" t="inlineStr"/>
+    </row>
+    <row r="719">
+      <c r="A719" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Reko111</t>
+        </is>
+      </c>
+      <c r="C719" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D719" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707563434</t>
+        </is>
+      </c>
+      <c r="E719" t="inlineStr"/>
+      <c r="F719" t="n">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>Reko111</t>
+        </is>
+      </c>
+      <c r="C720" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D720" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707563434</t>
+        </is>
+      </c>
+      <c r="E720" t="inlineStr"/>
+      <c r="F720" t="n">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Reko111</t>
+        </is>
+      </c>
+      <c r="C721" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D721" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707563434</t>
+        </is>
+      </c>
+      <c r="E721" t="n">
+        <v>208</v>
+      </c>
+      <c r="F721" t="inlineStr"/>
+    </row>
+    <row r="722">
+      <c r="A722" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B722" t="inlineStr"/>
+      <c r="C722" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D722" t="inlineStr">
+        <is>
+          <t>FRESH STOCKHOLM HÄSSEL K0135</t>
+        </is>
+      </c>
+      <c r="E722" t="n">
+        <v>88.70999999999999</v>
+      </c>
+      <c r="F722" t="inlineStr"/>
+    </row>
+    <row r="723">
+      <c r="A723" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B723" t="inlineStr"/>
+      <c r="C723" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D723" t="inlineStr">
+        <is>
+          <t>FRESH STOCKHOLM HÄSSEL K0135</t>
+        </is>
+      </c>
+      <c r="E723" t="n">
+        <v>10.65</v>
+      </c>
+      <c r="F723" t="inlineStr"/>
+    </row>
+    <row r="724">
+      <c r="A724" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B724" t="inlineStr"/>
+      <c r="C724" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D724" t="inlineStr">
+        <is>
+          <t>FRESH STOCKHOLM HÄSSEL K0135</t>
+        </is>
+      </c>
+      <c r="E724" t="inlineStr"/>
+      <c r="F724" t="n">
+        <v>99.36</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B725" t="inlineStr"/>
+      <c r="C725" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D725" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E725" t="n">
+        <v>1255.9</v>
+      </c>
+      <c r="F725" t="inlineStr"/>
+    </row>
+    <row r="726">
+      <c r="A726" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B726" t="inlineStr"/>
+      <c r="C726" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D726" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E726" t="n">
+        <v>150.71</v>
+      </c>
+      <c r="F726" t="inlineStr"/>
+    </row>
+    <row r="727">
+      <c r="A727" s="2" t="n">
+        <v>44312</v>
+      </c>
+      <c r="B727" t="inlineStr"/>
+      <c r="C727" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D727" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E727" t="inlineStr"/>
+      <c r="F727" t="n">
+        <v>1406.61</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Reko112</t>
+        </is>
+      </c>
+      <c r="C728" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D728" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E728" t="inlineStr"/>
+      <c r="F728" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Reko112</t>
+        </is>
+      </c>
+      <c r="C729" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D729" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E729" t="inlineStr"/>
+      <c r="F729" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Reko112</t>
+        </is>
+      </c>
+      <c r="C730" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D730" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E730" t="n">
+        <v>237</v>
+      </c>
+      <c r="F730" t="inlineStr"/>
+    </row>
+    <row r="731">
+      <c r="A731" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Reko113</t>
+        </is>
+      </c>
+      <c r="C731" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D731" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704773309</t>
+        </is>
+      </c>
+      <c r="E731" t="inlineStr"/>
+      <c r="F731" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Reko113</t>
+        </is>
+      </c>
+      <c r="C732" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D732" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704773309</t>
+        </is>
+      </c>
+      <c r="E732" t="inlineStr"/>
+      <c r="F732" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Reko113</t>
+        </is>
+      </c>
+      <c r="C733" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D733" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704773309</t>
+        </is>
+      </c>
+      <c r="E733" t="n">
+        <v>158</v>
+      </c>
+      <c r="F733" t="inlineStr"/>
+    </row>
+    <row r="734">
+      <c r="A734" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Reko114</t>
+        </is>
+      </c>
+      <c r="C734" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D734" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733341080</t>
+        </is>
+      </c>
+      <c r="E734" t="inlineStr"/>
+      <c r="F734" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Reko114</t>
+        </is>
+      </c>
+      <c r="C735" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D735" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733341080</t>
+        </is>
+      </c>
+      <c r="E735" t="inlineStr"/>
+      <c r="F735" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Reko114</t>
+        </is>
+      </c>
+      <c r="C736" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D736" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733341080</t>
+        </is>
+      </c>
+      <c r="E736" t="n">
+        <v>258</v>
+      </c>
+      <c r="F736" t="inlineStr"/>
+    </row>
+    <row r="737">
+      <c r="A737" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Reko115</t>
+        </is>
+      </c>
+      <c r="C737" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D737" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E737" t="inlineStr"/>
+      <c r="F737" t="n">
+        <v>371.43</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Reko115</t>
+        </is>
+      </c>
+      <c r="C738" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D738" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E738" t="inlineStr"/>
+      <c r="F738" t="n">
+        <v>44.57</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Reko115</t>
+        </is>
+      </c>
+      <c r="C739" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D739" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E739" t="n">
+        <v>416</v>
+      </c>
+      <c r="F739" t="inlineStr"/>
+    </row>
+    <row r="740">
+      <c r="A740" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Reko116</t>
+        </is>
+      </c>
+      <c r="C740" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D740" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730265465</t>
+        </is>
+      </c>
+      <c r="E740" t="inlineStr"/>
+      <c r="F740" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Reko116</t>
+        </is>
+      </c>
+      <c r="C741" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D741" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730265465</t>
+        </is>
+      </c>
+      <c r="E741" t="inlineStr"/>
+      <c r="F741" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>Reko116</t>
+        </is>
+      </c>
+      <c r="C742" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D742" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730265465</t>
+        </is>
+      </c>
+      <c r="E742" t="n">
+        <v>237</v>
+      </c>
+      <c r="F742" t="inlineStr"/>
+    </row>
+    <row r="743">
+      <c r="A743" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>Reko117</t>
+        </is>
+      </c>
+      <c r="C743" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D743" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708632117</t>
+        </is>
+      </c>
+      <c r="E743" t="inlineStr"/>
+      <c r="F743" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Reko117</t>
+        </is>
+      </c>
+      <c r="C744" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D744" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708632117</t>
+        </is>
+      </c>
+      <c r="E744" t="inlineStr"/>
+      <c r="F744" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Reko117</t>
+        </is>
+      </c>
+      <c r="C745" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D745" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708632117</t>
+        </is>
+      </c>
+      <c r="E745" t="n">
+        <v>129</v>
+      </c>
+      <c r="F745" t="inlineStr"/>
+    </row>
+    <row r="746">
+      <c r="A746" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Reko118</t>
+        </is>
+      </c>
+      <c r="C746" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D746" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736506798</t>
+        </is>
+      </c>
+      <c r="E746" t="inlineStr"/>
+      <c r="F746" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Reko118</t>
+        </is>
+      </c>
+      <c r="C747" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D747" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736506798</t>
+        </is>
+      </c>
+      <c r="E747" t="inlineStr"/>
+      <c r="F747" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Reko118</t>
+        </is>
+      </c>
+      <c r="C748" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D748" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736506798</t>
+        </is>
+      </c>
+      <c r="E748" t="n">
+        <v>387</v>
+      </c>
+      <c r="F748" t="inlineStr"/>
+    </row>
+    <row r="749">
+      <c r="A749" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Reko119</t>
+        </is>
+      </c>
+      <c r="C749" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D749" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E749" t="inlineStr"/>
+      <c r="F749" t="n">
+        <v>397.32</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Reko119</t>
+        </is>
+      </c>
+      <c r="C750" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D750" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E750" t="inlineStr"/>
+      <c r="F750" t="n">
+        <v>47.68</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Reko119</t>
+        </is>
+      </c>
+      <c r="C751" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D751" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E751" t="n">
+        <v>445</v>
+      </c>
+      <c r="F751" t="inlineStr"/>
+    </row>
+    <row r="752">
+      <c r="A752" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Reko120</t>
+        </is>
+      </c>
+      <c r="C752" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D752" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727470500</t>
+        </is>
+      </c>
+      <c r="E752" t="inlineStr"/>
+      <c r="F752" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Reko120</t>
+        </is>
+      </c>
+      <c r="C753" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D753" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727470500</t>
+        </is>
+      </c>
+      <c r="E753" t="inlineStr"/>
+      <c r="F753" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Reko120</t>
+        </is>
+      </c>
+      <c r="C754" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D754" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727470500</t>
+        </is>
+      </c>
+      <c r="E754" t="n">
+        <v>158</v>
+      </c>
+      <c r="F754" t="inlineStr"/>
+    </row>
+    <row r="755">
+      <c r="A755" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Reko121</t>
+        </is>
+      </c>
+      <c r="C755" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D755" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708164414</t>
+        </is>
+      </c>
+      <c r="E755" t="inlineStr"/>
+      <c r="F755" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>Reko121</t>
+        </is>
+      </c>
+      <c r="C756" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D756" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708164414</t>
+        </is>
+      </c>
+      <c r="E756" t="inlineStr"/>
+      <c r="F756" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Reko121</t>
+        </is>
+      </c>
+      <c r="C757" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D757" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708164414</t>
+        </is>
+      </c>
+      <c r="E757" t="n">
+        <v>129</v>
+      </c>
+      <c r="F757" t="inlineStr"/>
+    </row>
+    <row r="758">
+      <c r="A758" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Reko122</t>
+        </is>
+      </c>
+      <c r="C758" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D758" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730728731</t>
+        </is>
+      </c>
+      <c r="E758" t="inlineStr"/>
+      <c r="F758" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Reko122</t>
+        </is>
+      </c>
+      <c r="C759" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D759" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730728731</t>
+        </is>
+      </c>
+      <c r="E759" t="inlineStr"/>
+      <c r="F759" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" s="2" t="n">
+        <v>44313</v>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>Reko122</t>
+        </is>
+      </c>
+      <c r="C760" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D760" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730728731</t>
+        </is>
+      </c>
+      <c r="E760" t="n">
+        <v>258</v>
+      </c>
+      <c r="F760" t="inlineStr"/>
+    </row>
+    <row r="761">
+      <c r="A761" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Reko123</t>
+        </is>
+      </c>
+      <c r="C761" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D761" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708163936</t>
+        </is>
+      </c>
+      <c r="E761" t="inlineStr"/>
+      <c r="F761" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Reko123</t>
+        </is>
+      </c>
+      <c r="C762" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D762" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708163936</t>
+        </is>
+      </c>
+      <c r="E762" t="inlineStr"/>
+      <c r="F762" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Reko123</t>
+        </is>
+      </c>
+      <c r="C763" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D763" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708163936</t>
+        </is>
+      </c>
+      <c r="E763" t="n">
+        <v>258</v>
+      </c>
+      <c r="F763" t="inlineStr"/>
+    </row>
+    <row r="764">
+      <c r="A764" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Reko124</t>
+        </is>
+      </c>
+      <c r="C764" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D764" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709466079</t>
+        </is>
+      </c>
+      <c r="E764" t="inlineStr"/>
+      <c r="F764" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Reko124</t>
+        </is>
+      </c>
+      <c r="C765" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D765" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709466079</t>
+        </is>
+      </c>
+      <c r="E765" t="inlineStr"/>
+      <c r="F765" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Reko124</t>
+        </is>
+      </c>
+      <c r="C766" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D766" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709466079</t>
+        </is>
+      </c>
+      <c r="E766" t="n">
+        <v>258</v>
+      </c>
+      <c r="F766" t="inlineStr"/>
+    </row>
+    <row r="767">
+      <c r="A767" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Reko125</t>
+        </is>
+      </c>
+      <c r="C767" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D767" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768172729</t>
+        </is>
+      </c>
+      <c r="E767" t="inlineStr"/>
+      <c r="F767" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Reko125</t>
+        </is>
+      </c>
+      <c r="C768" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D768" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768172729</t>
+        </is>
+      </c>
+      <c r="E768" t="inlineStr"/>
+      <c r="F768" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Reko125</t>
+        </is>
+      </c>
+      <c r="C769" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D769" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768172729</t>
+        </is>
+      </c>
+      <c r="E769" t="n">
+        <v>258</v>
+      </c>
+      <c r="F769" t="inlineStr"/>
+    </row>
+    <row r="770">
+      <c r="A770" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>0282036</t>
+        </is>
+      </c>
+      <c r="C770" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D770" t="inlineStr">
+        <is>
+          <t>Order 0282036 Swish +46725969231</t>
+        </is>
+      </c>
+      <c r="E770" t="inlineStr"/>
+      <c r="F770" t="n">
+        <v>1168.75</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>0282036</t>
+        </is>
+      </c>
+      <c r="C771" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D771" t="inlineStr">
+        <is>
+          <t>Order 0282036 Swish +46725969231</t>
+        </is>
+      </c>
+      <c r="E771" t="inlineStr"/>
+      <c r="F771" t="n">
+        <v>140.25</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>0282036</t>
+        </is>
+      </c>
+      <c r="C772" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D772" t="inlineStr">
+        <is>
+          <t>Order 0282036 Swish +46725969231</t>
+        </is>
+      </c>
+      <c r="E772" t="n">
+        <v>1309</v>
+      </c>
+      <c r="F772" t="inlineStr"/>
+    </row>
+    <row r="773">
+      <c r="A773" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Reko126</t>
+        </is>
+      </c>
+      <c r="C773" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D773" t="inlineStr">
+        <is>
+          <t>Reko Swish +46728774058</t>
+        </is>
+      </c>
+      <c r="E773" t="inlineStr"/>
+      <c r="F773" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Reko126</t>
+        </is>
+      </c>
+      <c r="C774" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D774" t="inlineStr">
+        <is>
+          <t>Reko Swish +46728774058</t>
+        </is>
+      </c>
+      <c r="E774" t="inlineStr"/>
+      <c r="F774" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>Reko126</t>
+        </is>
+      </c>
+      <c r="C775" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D775" t="inlineStr">
+        <is>
+          <t>Reko Swish +46728774058</t>
+        </is>
+      </c>
+      <c r="E775" t="n">
+        <v>316</v>
+      </c>
+      <c r="F775" t="inlineStr"/>
+    </row>
+    <row r="776">
+      <c r="A776" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Reko127</t>
+        </is>
+      </c>
+      <c r="C776" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D776" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E776" t="inlineStr"/>
+      <c r="F776" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Reko127</t>
+        </is>
+      </c>
+      <c r="C777" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D777" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E777" t="inlineStr"/>
+      <c r="F777" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Reko127</t>
+        </is>
+      </c>
+      <c r="C778" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D778" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E778" t="n">
+        <v>387</v>
+      </c>
+      <c r="F778" t="inlineStr"/>
+    </row>
+    <row r="779">
+      <c r="A779" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B779" t="inlineStr"/>
+      <c r="C779" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D779" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E779" t="n">
+        <v>2255.82</v>
+      </c>
+      <c r="F779" t="inlineStr"/>
+    </row>
+    <row r="780">
+      <c r="A780" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B780" t="inlineStr"/>
+      <c r="C780" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D780" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E780" t="n">
+        <v>270.7</v>
+      </c>
+      <c r="F780" t="inlineStr"/>
+    </row>
+    <row r="781">
+      <c r="A781" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B781" t="inlineStr"/>
+      <c r="C781" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D781" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E781" t="inlineStr"/>
+      <c r="F781" t="n">
+        <v>2526.52</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B782" t="inlineStr"/>
+      <c r="C782" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D782" t="inlineStr">
+        <is>
+          <t>WWW.BAUHAUS.SE K0135</t>
+        </is>
+      </c>
+      <c r="E782" t="n">
+        <v>1036</v>
+      </c>
+      <c r="F782" t="inlineStr"/>
+    </row>
+    <row r="783">
+      <c r="A783" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B783" t="inlineStr"/>
+      <c r="C783" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D783" t="inlineStr">
+        <is>
+          <t>WWW.BAUHAUS.SE K0135</t>
+        </is>
+      </c>
+      <c r="E783" t="n">
+        <v>259</v>
+      </c>
+      <c r="F783" t="inlineStr"/>
+    </row>
+    <row r="784">
+      <c r="A784" s="2" t="n">
+        <v>44314</v>
+      </c>
+      <c r="B784" t="inlineStr"/>
+      <c r="C784" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D784" t="inlineStr">
+        <is>
+          <t>WWW.BAUHAUS.SE K0135</t>
+        </is>
+      </c>
+      <c r="E784" t="inlineStr"/>
+      <c r="F784" t="n">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Reko128</t>
+        </is>
+      </c>
+      <c r="C785" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D785" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706314152</t>
+        </is>
+      </c>
+      <c r="E785" t="inlineStr"/>
+      <c r="F785" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Reko128</t>
+        </is>
+      </c>
+      <c r="C786" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D786" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706314152</t>
+        </is>
+      </c>
+      <c r="E786" t="inlineStr"/>
+      <c r="F786" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Reko128</t>
+        </is>
+      </c>
+      <c r="C787" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D787" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706314152</t>
+        </is>
+      </c>
+      <c r="E787" t="n">
+        <v>79</v>
+      </c>
+      <c r="F787" t="inlineStr"/>
+    </row>
+    <row r="788">
+      <c r="A788" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Reko129</t>
+        </is>
+      </c>
+      <c r="C788" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D788" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736241792</t>
+        </is>
+      </c>
+      <c r="E788" t="inlineStr"/>
+      <c r="F788" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Reko129</t>
+        </is>
+      </c>
+      <c r="C789" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D789" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736241792</t>
+        </is>
+      </c>
+      <c r="E789" t="inlineStr"/>
+      <c r="F789" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Reko129</t>
+        </is>
+      </c>
+      <c r="C790" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D790" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736241792</t>
+        </is>
+      </c>
+      <c r="E790" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F790" t="inlineStr"/>
+    </row>
+    <row r="791">
+      <c r="A791" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Reko130</t>
+        </is>
+      </c>
+      <c r="C791" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D791" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760438</t>
+        </is>
+      </c>
+      <c r="E791" t="inlineStr"/>
+      <c r="F791" t="n">
+        <v>794.64</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Reko130</t>
+        </is>
+      </c>
+      <c r="C792" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D792" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760438</t>
+        </is>
+      </c>
+      <c r="E792" t="inlineStr"/>
+      <c r="F792" t="n">
+        <v>95.36</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Reko130</t>
+        </is>
+      </c>
+      <c r="C793" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D793" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760438</t>
+        </is>
+      </c>
+      <c r="E793" t="n">
+        <v>890</v>
+      </c>
+      <c r="F793" t="inlineStr"/>
+    </row>
+    <row r="794">
+      <c r="A794" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Reko131</t>
+        </is>
+      </c>
+      <c r="C794" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D794" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702513252</t>
+        </is>
+      </c>
+      <c r="E794" t="inlineStr"/>
+      <c r="F794" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Reko131</t>
+        </is>
+      </c>
+      <c r="C795" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D795" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702513252</t>
+        </is>
+      </c>
+      <c r="E795" t="inlineStr"/>
+      <c r="F795" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Reko131</t>
+        </is>
+      </c>
+      <c r="C796" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D796" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702513252</t>
+        </is>
+      </c>
+      <c r="E796" t="n">
+        <v>258</v>
+      </c>
+      <c r="F796" t="inlineStr"/>
+    </row>
+    <row r="797">
+      <c r="A797" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Reko132</t>
+        </is>
+      </c>
+      <c r="C797" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D797" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705098093</t>
+        </is>
+      </c>
+      <c r="E797" t="inlineStr"/>
+      <c r="F797" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Reko132</t>
+        </is>
+      </c>
+      <c r="C798" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D798" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705098093</t>
+        </is>
+      </c>
+      <c r="E798" t="inlineStr"/>
+      <c r="F798" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>Reko132</t>
+        </is>
+      </c>
+      <c r="C799" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D799" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705098093</t>
+        </is>
+      </c>
+      <c r="E799" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F799" t="inlineStr"/>
+    </row>
+    <row r="800">
+      <c r="A800" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Reko133</t>
+        </is>
+      </c>
+      <c r="C800" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D800" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739837997</t>
+        </is>
+      </c>
+      <c r="E800" t="inlineStr"/>
+      <c r="F800" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Reko133</t>
+        </is>
+      </c>
+      <c r="C801" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D801" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739837997</t>
+        </is>
+      </c>
+      <c r="E801" t="inlineStr"/>
+      <c r="F801" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Reko133</t>
+        </is>
+      </c>
+      <c r="C802" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D802" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739837997</t>
+        </is>
+      </c>
+      <c r="E802" t="n">
+        <v>516</v>
+      </c>
+      <c r="F802" t="inlineStr"/>
+    </row>
+    <row r="803">
+      <c r="A803" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>Reko134</t>
+        </is>
+      </c>
+      <c r="C803" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D803" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706658317</t>
+        </is>
+      </c>
+      <c r="E803" t="inlineStr"/>
+      <c r="F803" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Reko134</t>
+        </is>
+      </c>
+      <c r="C804" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D804" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706658317</t>
+        </is>
+      </c>
+      <c r="E804" t="inlineStr"/>
+      <c r="F804" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" s="2" t="n">
+        <v>44315</v>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Reko134</t>
+        </is>
+      </c>
+      <c r="C805" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D805" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706658317</t>
+        </is>
+      </c>
+      <c r="E805" t="n">
+        <v>237</v>
+      </c>
+      <c r="F805" t="inlineStr"/>
+    </row>
+    <row r="806">
+      <c r="A806" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B806" t="inlineStr"/>
+      <c r="C806" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D806" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E806" t="n">
+        <v>319.2</v>
+      </c>
+      <c r="F806" t="inlineStr"/>
+    </row>
+    <row r="807">
+      <c r="A807" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B807" t="inlineStr"/>
+      <c r="C807" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D807" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E807" t="n">
+        <v>79.8</v>
+      </c>
+      <c r="F807" t="inlineStr"/>
+    </row>
+    <row r="808">
+      <c r="A808" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B808" t="inlineStr"/>
+      <c r="C808" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D808" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E808" t="inlineStr"/>
+      <c r="F808" t="n">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B809" t="inlineStr"/>
+      <c r="C809" t="n">
+        <v>5460</v>
+      </c>
+      <c r="D809" t="inlineStr">
+        <is>
+          <t>HORNBACH SUNDBYBERG K0135</t>
+        </is>
+      </c>
+      <c r="E809" t="n">
+        <v>1171.58</v>
+      </c>
+      <c r="F809" t="inlineStr"/>
+    </row>
+    <row r="810">
+      <c r="A810" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B810" t="inlineStr"/>
+      <c r="C810" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D810" t="inlineStr">
+        <is>
+          <t>HORNBACH SUNDBYBERG K0135</t>
+        </is>
+      </c>
+      <c r="E810" t="n">
+        <v>292.9</v>
+      </c>
+      <c r="F810" t="inlineStr"/>
+    </row>
+    <row r="811">
+      <c r="A811" s="2" t="n">
+        <v>44316</v>
+      </c>
+      <c r="B811" t="inlineStr"/>
+      <c r="C811" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D811" t="inlineStr">
+        <is>
+          <t>HORNBACH SUNDBYBERG K0135</t>
+        </is>
+      </c>
+      <c r="E811" t="inlineStr"/>
+      <c r="F811" t="n">
+        <v>1464.48</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>0011329</t>
+        </is>
+      </c>
+      <c r="C812" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D812" t="inlineStr">
+        <is>
+          <t>Order 0011329 Swish +46730947199</t>
+        </is>
+      </c>
+      <c r="E812" t="inlineStr"/>
+      <c r="F812" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>0011329</t>
+        </is>
+      </c>
+      <c r="C813" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D813" t="inlineStr">
+        <is>
+          <t>Order 0011329 Swish +46730947199</t>
+        </is>
+      </c>
+      <c r="E813" t="inlineStr"/>
+      <c r="F813" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>0011329</t>
+        </is>
+      </c>
+      <c r="C814" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D814" t="inlineStr">
+        <is>
+          <t>Order 0011329 Swish +46730947199</t>
+        </is>
+      </c>
+      <c r="E814" t="n">
+        <v>395</v>
+      </c>
+      <c r="F814" t="inlineStr"/>
+    </row>
+    <row r="815">
+      <c r="A815" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B815" t="inlineStr"/>
+      <c r="C815" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D815" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E815" t="n">
+        <v>555.48</v>
+      </c>
+      <c r="F815" t="inlineStr"/>
+    </row>
+    <row r="816">
+      <c r="A816" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B816" t="inlineStr"/>
+      <c r="C816" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D816" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E816" t="n">
+        <v>66.66</v>
+      </c>
+      <c r="F816" t="inlineStr"/>
+    </row>
+    <row r="817">
+      <c r="A817" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="B817" t="inlineStr"/>
+      <c r="C817" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D817" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E817" t="inlineStr"/>
+      <c r="F817" t="n">
+        <v>622.14</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" s="2" t="n">
+        <v>44318</v>
+      </c>
+      <c r="B818" t="inlineStr"/>
+      <c r="C818" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D818" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E818" t="n">
+        <v>187.5</v>
+      </c>
+      <c r="F818" t="inlineStr"/>
+    </row>
+    <row r="819">
+      <c r="A819" s="2" t="n">
+        <v>44318</v>
+      </c>
+      <c r="B819" t="inlineStr"/>
+      <c r="C819" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D819" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E819" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="F819" t="inlineStr"/>
+    </row>
+    <row r="820">
+      <c r="A820" s="2" t="n">
+        <v>44318</v>
+      </c>
+      <c r="B820" t="inlineStr"/>
+      <c r="C820" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D820" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E820" t="inlineStr"/>
+      <c r="F820" t="n">
+        <v>210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 18 new rows for week ending 2021-05-09 (total 837 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F820"/>
+  <dimension ref="A1:F838"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17343,6 +17343,352 @@
         <v>210</v>
       </c>
     </row>
+    <row r="821">
+      <c r="A821" s="2" t="n">
+        <v>44320</v>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>5040739</t>
+        </is>
+      </c>
+      <c r="C821" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D821" t="inlineStr">
+        <is>
+          <t>Order 5040739 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E821" t="inlineStr"/>
+      <c r="F821" t="n">
+        <v>973.21</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" s="2" t="n">
+        <v>44320</v>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>5040739</t>
+        </is>
+      </c>
+      <c r="C822" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D822" t="inlineStr">
+        <is>
+          <t>Order 5040739 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E822" t="inlineStr"/>
+      <c r="F822" t="n">
+        <v>116.79</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" s="2" t="n">
+        <v>44320</v>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>5040739</t>
+        </is>
+      </c>
+      <c r="C823" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D823" t="inlineStr">
+        <is>
+          <t>Order 5040739 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E823" t="n">
+        <v>1090</v>
+      </c>
+      <c r="F823" t="inlineStr"/>
+    </row>
+    <row r="824">
+      <c r="A824" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B824" t="inlineStr"/>
+      <c r="C824" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D824" t="inlineStr">
+        <is>
+          <t>TINGSTAD PAPPER</t>
+        </is>
+      </c>
+      <c r="E824" t="n">
+        <v>3102.4</v>
+      </c>
+      <c r="F824" t="inlineStr"/>
+    </row>
+    <row r="825">
+      <c r="A825" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B825" t="inlineStr"/>
+      <c r="C825" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D825" t="inlineStr">
+        <is>
+          <t>TINGSTAD PAPPER</t>
+        </is>
+      </c>
+      <c r="E825" t="n">
+        <v>775.6</v>
+      </c>
+      <c r="F825" t="inlineStr"/>
+    </row>
+    <row r="826">
+      <c r="A826" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B826" t="inlineStr"/>
+      <c r="C826" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D826" t="inlineStr">
+        <is>
+          <t>TINGSTAD PAPPER</t>
+        </is>
+      </c>
+      <c r="E826" t="inlineStr"/>
+      <c r="F826" t="n">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B827" t="inlineStr"/>
+      <c r="C827" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D827" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E827" t="n">
+        <v>213.39</v>
+      </c>
+      <c r="F827" t="inlineStr"/>
+    </row>
+    <row r="828">
+      <c r="A828" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B828" t="inlineStr"/>
+      <c r="C828" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D828" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E828" t="n">
+        <v>25.61</v>
+      </c>
+      <c r="F828" t="inlineStr"/>
+    </row>
+    <row r="829">
+      <c r="A829" s="2" t="n">
+        <v>44321</v>
+      </c>
+      <c r="B829" t="inlineStr"/>
+      <c r="C829" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D829" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E829" t="inlineStr"/>
+      <c r="F829" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>5061308</t>
+        </is>
+      </c>
+      <c r="C830" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D830" t="inlineStr">
+        <is>
+          <t>Order 5061308 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E830" t="inlineStr"/>
+      <c r="F830" t="n">
+        <v>806.25</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>5061308</t>
+        </is>
+      </c>
+      <c r="C831" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D831" t="inlineStr">
+        <is>
+          <t>Order 5061308 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E831" t="inlineStr"/>
+      <c r="F831" t="n">
+        <v>96.75</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>5061308</t>
+        </is>
+      </c>
+      <c r="C832" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D832" t="inlineStr">
+        <is>
+          <t>Order 5061308 Swish +46723656673</t>
+        </is>
+      </c>
+      <c r="E832" t="n">
+        <v>903</v>
+      </c>
+      <c r="F832" t="inlineStr"/>
+    </row>
+    <row r="833">
+      <c r="A833" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B833" t="inlineStr"/>
+      <c r="C833" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D833" t="inlineStr">
+        <is>
+          <t>April hyra</t>
+        </is>
+      </c>
+      <c r="E833" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F833" t="inlineStr"/>
+    </row>
+    <row r="834">
+      <c r="A834" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B834" t="inlineStr"/>
+      <c r="C834" t="inlineStr"/>
+      <c r="D834" t="inlineStr">
+        <is>
+          <t>April hyra</t>
+        </is>
+      </c>
+      <c r="E834" t="n">
+        <v>0</v>
+      </c>
+      <c r="F834" t="inlineStr"/>
+    </row>
+    <row r="835">
+      <c r="A835" s="2" t="n">
+        <v>44322</v>
+      </c>
+      <c r="B835" t="inlineStr"/>
+      <c r="C835" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D835" t="inlineStr">
+        <is>
+          <t>April hyra</t>
+        </is>
+      </c>
+      <c r="E835" t="inlineStr"/>
+      <c r="F835" t="n">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" s="2" t="n">
+        <v>44325</v>
+      </c>
+      <c r="B836" t="inlineStr"/>
+      <c r="C836" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D836" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E836" t="n">
+        <v>844.58</v>
+      </c>
+      <c r="F836" t="inlineStr"/>
+    </row>
+    <row r="837">
+      <c r="A837" s="2" t="n">
+        <v>44325</v>
+      </c>
+      <c r="B837" t="inlineStr"/>
+      <c r="C837" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D837" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E837" t="n">
+        <v>211.14</v>
+      </c>
+      <c r="F837" t="inlineStr"/>
+    </row>
+    <row r="838">
+      <c r="A838" s="2" t="n">
+        <v>44325</v>
+      </c>
+      <c r="B838" t="inlineStr"/>
+      <c r="C838" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D838" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E838" t="inlineStr"/>
+      <c r="F838" t="n">
+        <v>1055.72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 15 new rows for week ending 2021-05-16 (total 852 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F838"/>
+  <dimension ref="A1:F853"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17689,6 +17689,336 @@
         <v>1055.72</v>
       </c>
     </row>
+    <row r="839">
+      <c r="A839" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>0110925</t>
+        </is>
+      </c>
+      <c r="C839" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D839" t="inlineStr">
+        <is>
+          <t>Order 0110925 Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E839" t="inlineStr"/>
+      <c r="F839" t="n">
+        <v>610.71</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>0110925</t>
+        </is>
+      </c>
+      <c r="C840" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D840" t="inlineStr">
+        <is>
+          <t>Order 0110925 Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E840" t="inlineStr"/>
+      <c r="F840" t="n">
+        <v>73.29000000000001</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>0110925</t>
+        </is>
+      </c>
+      <c r="C841" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D841" t="inlineStr">
+        <is>
+          <t>Order 0110925 Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E841" t="n">
+        <v>684</v>
+      </c>
+      <c r="F841" t="inlineStr"/>
+    </row>
+    <row r="842">
+      <c r="A842" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>3111510</t>
+        </is>
+      </c>
+      <c r="C842" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D842" t="inlineStr">
+        <is>
+          <t>Order 3111510 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E842" t="inlineStr"/>
+      <c r="F842" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>3111510</t>
+        </is>
+      </c>
+      <c r="C843" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D843" t="inlineStr">
+        <is>
+          <t>Order 3111510 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E843" t="inlineStr"/>
+      <c r="F843" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" s="2" t="n">
+        <v>44327</v>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>3111510</t>
+        </is>
+      </c>
+      <c r="C844" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D844" t="inlineStr">
+        <is>
+          <t>Order 3111510 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E844" t="n">
+        <v>690</v>
+      </c>
+      <c r="F844" t="inlineStr"/>
+    </row>
+    <row r="845">
+      <c r="A845" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>5141236</t>
+        </is>
+      </c>
+      <c r="C845" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D845" t="inlineStr">
+        <is>
+          <t>Order 5141236 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E845" t="inlineStr"/>
+      <c r="F845" t="n">
+        <v>486.61</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>5141236</t>
+        </is>
+      </c>
+      <c r="C846" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D846" t="inlineStr">
+        <is>
+          <t>Order 5141236 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E846" t="inlineStr"/>
+      <c r="F846" t="n">
+        <v>58.39</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>5141236</t>
+        </is>
+      </c>
+      <c r="C847" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D847" t="inlineStr">
+        <is>
+          <t>Order 5141236 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E847" t="n">
+        <v>545</v>
+      </c>
+      <c r="F847" t="inlineStr"/>
+    </row>
+    <row r="848">
+      <c r="A848" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>1142223</t>
+        </is>
+      </c>
+      <c r="C848" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D848" t="inlineStr">
+        <is>
+          <t>Order 1142223 Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E848" t="inlineStr"/>
+      <c r="F848" t="n">
+        <v>994.64</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>1142223</t>
+        </is>
+      </c>
+      <c r="C849" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D849" t="inlineStr">
+        <is>
+          <t>Order 1142223 Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E849" t="inlineStr"/>
+      <c r="F849" t="n">
+        <v>119.36</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>1142223</t>
+        </is>
+      </c>
+      <c r="C850" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D850" t="inlineStr">
+        <is>
+          <t>Order 1142223 Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E850" t="n">
+        <v>1114</v>
+      </c>
+      <c r="F850" t="inlineStr"/>
+    </row>
+    <row r="851">
+      <c r="A851" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Reko135</t>
+        </is>
+      </c>
+      <c r="C851" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D851" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727028531</t>
+        </is>
+      </c>
+      <c r="E851" t="inlineStr"/>
+      <c r="F851" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Reko135</t>
+        </is>
+      </c>
+      <c r="C852" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D852" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727028531</t>
+        </is>
+      </c>
+      <c r="E852" t="inlineStr"/>
+      <c r="F852" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="2" t="n">
+        <v>44330</v>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Reko135</t>
+        </is>
+      </c>
+      <c r="C853" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D853" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727028531</t>
+        </is>
+      </c>
+      <c r="E853" t="n">
+        <v>258</v>
+      </c>
+      <c r="F853" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 111 new rows for week ending 2021-05-23 (total 963 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F853"/>
+  <dimension ref="A1:F964"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18019,6 +18019,2252 @@
       </c>
       <c r="F853" t="inlineStr"/>
     </row>
+    <row r="854">
+      <c r="A854" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Reko136</t>
+        </is>
+      </c>
+      <c r="C854" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D854" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E854" t="inlineStr"/>
+      <c r="F854" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Reko136</t>
+        </is>
+      </c>
+      <c r="C855" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D855" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E855" t="inlineStr"/>
+      <c r="F855" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Reko136</t>
+        </is>
+      </c>
+      <c r="C856" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D856" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E856" t="n">
+        <v>387</v>
+      </c>
+      <c r="F856" t="inlineStr"/>
+    </row>
+    <row r="857">
+      <c r="A857" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>Reko137</t>
+        </is>
+      </c>
+      <c r="C857" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D857" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708285106</t>
+        </is>
+      </c>
+      <c r="E857" t="inlineStr"/>
+      <c r="F857" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Reko137</t>
+        </is>
+      </c>
+      <c r="C858" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D858" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708285106</t>
+        </is>
+      </c>
+      <c r="E858" t="inlineStr"/>
+      <c r="F858" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Reko137</t>
+        </is>
+      </c>
+      <c r="C859" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D859" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708285106</t>
+        </is>
+      </c>
+      <c r="E859" t="n">
+        <v>158</v>
+      </c>
+      <c r="F859" t="inlineStr"/>
+    </row>
+    <row r="860">
+      <c r="A860" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Reko138</t>
+        </is>
+      </c>
+      <c r="C860" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D860" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708915662</t>
+        </is>
+      </c>
+      <c r="E860" t="inlineStr"/>
+      <c r="F860" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Reko138</t>
+        </is>
+      </c>
+      <c r="C861" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D861" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708915662</t>
+        </is>
+      </c>
+      <c r="E861" t="inlineStr"/>
+      <c r="F861" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Reko138</t>
+        </is>
+      </c>
+      <c r="C862" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D862" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708915662</t>
+        </is>
+      </c>
+      <c r="E862" t="n">
+        <v>258</v>
+      </c>
+      <c r="F862" t="inlineStr"/>
+    </row>
+    <row r="863">
+      <c r="A863" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Reko139</t>
+        </is>
+      </c>
+      <c r="C863" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D863" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448</t>
+        </is>
+      </c>
+      <c r="E863" t="inlineStr"/>
+      <c r="F863" t="n">
+        <v>256.25</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Reko139</t>
+        </is>
+      </c>
+      <c r="C864" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D864" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448</t>
+        </is>
+      </c>
+      <c r="E864" t="inlineStr"/>
+      <c r="F864" t="n">
+        <v>30.75</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Reko139</t>
+        </is>
+      </c>
+      <c r="C865" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D865" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448</t>
+        </is>
+      </c>
+      <c r="E865" t="n">
+        <v>287</v>
+      </c>
+      <c r="F865" t="inlineStr"/>
+    </row>
+    <row r="866">
+      <c r="A866" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Reko140</t>
+        </is>
+      </c>
+      <c r="C866" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D866" t="inlineStr">
+        <is>
+          <t>Reko Swish +447930169686</t>
+        </is>
+      </c>
+      <c r="E866" t="inlineStr"/>
+      <c r="F866" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Reko140</t>
+        </is>
+      </c>
+      <c r="C867" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D867" t="inlineStr">
+        <is>
+          <t>Reko Swish +447930169686</t>
+        </is>
+      </c>
+      <c r="E867" t="inlineStr"/>
+      <c r="F867" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Reko140</t>
+        </is>
+      </c>
+      <c r="C868" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D868" t="inlineStr">
+        <is>
+          <t>Reko Swish +447930169686</t>
+        </is>
+      </c>
+      <c r="E868" t="n">
+        <v>387</v>
+      </c>
+      <c r="F868" t="inlineStr"/>
+    </row>
+    <row r="869">
+      <c r="A869" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B869" t="inlineStr"/>
+      <c r="C869" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D869" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E869" t="n">
+        <v>1083.26</v>
+      </c>
+      <c r="F869" t="inlineStr"/>
+    </row>
+    <row r="870">
+      <c r="A870" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B870" t="inlineStr"/>
+      <c r="C870" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D870" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E870" t="n">
+        <v>129.99</v>
+      </c>
+      <c r="F870" t="inlineStr"/>
+    </row>
+    <row r="871">
+      <c r="A871" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B871" t="inlineStr"/>
+      <c r="C871" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D871" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E871" t="inlineStr"/>
+      <c r="F871" t="n">
+        <v>1213.25</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B872" t="inlineStr"/>
+      <c r="C872" t="n">
+        <v>5410</v>
+      </c>
+      <c r="D872" t="inlineStr">
+        <is>
+          <t>BILTEMA SWEDEN VEDDEST K0135</t>
+        </is>
+      </c>
+      <c r="E872" t="n">
+        <v>247.6</v>
+      </c>
+      <c r="F872" t="inlineStr"/>
+    </row>
+    <row r="873">
+      <c r="A873" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B873" t="inlineStr"/>
+      <c r="C873" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D873" t="inlineStr">
+        <is>
+          <t>BILTEMA SWEDEN VEDDEST K0135</t>
+        </is>
+      </c>
+      <c r="E873" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="F873" t="inlineStr"/>
+    </row>
+    <row r="874">
+      <c r="A874" s="2" t="n">
+        <v>44333</v>
+      </c>
+      <c r="B874" t="inlineStr"/>
+      <c r="C874" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D874" t="inlineStr">
+        <is>
+          <t>BILTEMA SWEDEN VEDDEST K0135</t>
+        </is>
+      </c>
+      <c r="E874" t="inlineStr"/>
+      <c r="F874" t="n">
+        <v>309.5</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Reko141</t>
+        </is>
+      </c>
+      <c r="C875" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D875" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702179776</t>
+        </is>
+      </c>
+      <c r="E875" t="inlineStr"/>
+      <c r="F875" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>Reko141</t>
+        </is>
+      </c>
+      <c r="C876" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D876" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702179776</t>
+        </is>
+      </c>
+      <c r="E876" t="inlineStr"/>
+      <c r="F876" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Reko141</t>
+        </is>
+      </c>
+      <c r="C877" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D877" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702179776</t>
+        </is>
+      </c>
+      <c r="E877" t="n">
+        <v>258</v>
+      </c>
+      <c r="F877" t="inlineStr"/>
+    </row>
+    <row r="878">
+      <c r="A878" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Reko142</t>
+        </is>
+      </c>
+      <c r="C878" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D878" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733035539</t>
+        </is>
+      </c>
+      <c r="E878" t="inlineStr"/>
+      <c r="F878" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Reko142</t>
+        </is>
+      </c>
+      <c r="C879" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D879" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733035539</t>
+        </is>
+      </c>
+      <c r="E879" t="inlineStr"/>
+      <c r="F879" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Reko142</t>
+        </is>
+      </c>
+      <c r="C880" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D880" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733035539</t>
+        </is>
+      </c>
+      <c r="E880" t="n">
+        <v>258</v>
+      </c>
+      <c r="F880" t="inlineStr"/>
+    </row>
+    <row r="881">
+      <c r="A881" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Reko143</t>
+        </is>
+      </c>
+      <c r="C881" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D881" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702112838</t>
+        </is>
+      </c>
+      <c r="E881" t="inlineStr"/>
+      <c r="F881" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Reko143</t>
+        </is>
+      </c>
+      <c r="C882" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D882" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702112838</t>
+        </is>
+      </c>
+      <c r="E882" t="inlineStr"/>
+      <c r="F882" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Reko143</t>
+        </is>
+      </c>
+      <c r="C883" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D883" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702112838</t>
+        </is>
+      </c>
+      <c r="E883" t="n">
+        <v>158</v>
+      </c>
+      <c r="F883" t="inlineStr"/>
+    </row>
+    <row r="884">
+      <c r="A884" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Reko144</t>
+        </is>
+      </c>
+      <c r="C884" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D884" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702779264</t>
+        </is>
+      </c>
+      <c r="E884" t="inlineStr"/>
+      <c r="F884" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Reko144</t>
+        </is>
+      </c>
+      <c r="C885" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D885" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702779264</t>
+        </is>
+      </c>
+      <c r="E885" t="inlineStr"/>
+      <c r="F885" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Reko144</t>
+        </is>
+      </c>
+      <c r="C886" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D886" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702779264</t>
+        </is>
+      </c>
+      <c r="E886" t="n">
+        <v>316</v>
+      </c>
+      <c r="F886" t="inlineStr"/>
+    </row>
+    <row r="887">
+      <c r="A887" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B887" t="inlineStr"/>
+      <c r="C887" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D887" t="inlineStr">
+        <is>
+          <t>KISTA GROSSEN K0135</t>
+        </is>
+      </c>
+      <c r="E887" t="n">
+        <v>363.93</v>
+      </c>
+      <c r="F887" t="inlineStr"/>
+    </row>
+    <row r="888">
+      <c r="A888" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B888" t="inlineStr"/>
+      <c r="C888" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D888" t="inlineStr">
+        <is>
+          <t>KISTA GROSSEN K0135</t>
+        </is>
+      </c>
+      <c r="E888" t="n">
+        <v>43.67</v>
+      </c>
+      <c r="F888" t="inlineStr"/>
+    </row>
+    <row r="889">
+      <c r="A889" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B889" t="inlineStr"/>
+      <c r="C889" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D889" t="inlineStr">
+        <is>
+          <t>KISTA GROSSEN K0135</t>
+        </is>
+      </c>
+      <c r="E889" t="inlineStr"/>
+      <c r="F889" t="n">
+        <v>407.6</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B890" t="inlineStr"/>
+      <c r="C890" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D890" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E890" t="n">
+        <v>684.55</v>
+      </c>
+      <c r="F890" t="inlineStr"/>
+    </row>
+    <row r="891">
+      <c r="A891" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B891" t="inlineStr"/>
+      <c r="C891" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D891" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E891" t="n">
+        <v>82.15000000000001</v>
+      </c>
+      <c r="F891" t="inlineStr"/>
+    </row>
+    <row r="892">
+      <c r="A892" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B892" t="inlineStr"/>
+      <c r="C892" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D892" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E892" t="inlineStr"/>
+      <c r="F892" t="n">
+        <v>766.7</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B893" t="inlineStr"/>
+      <c r="C893" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D893" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E893" t="n">
+        <v>650</v>
+      </c>
+      <c r="F893" t="inlineStr"/>
+    </row>
+    <row r="894">
+      <c r="A894" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B894" t="inlineStr"/>
+      <c r="C894" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D894" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E894" t="n">
+        <v>78</v>
+      </c>
+      <c r="F894" t="inlineStr"/>
+    </row>
+    <row r="895">
+      <c r="A895" s="2" t="n">
+        <v>44334</v>
+      </c>
+      <c r="B895" t="inlineStr"/>
+      <c r="C895" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D895" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E895" t="inlineStr"/>
+      <c r="F895" t="n">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Reko145</t>
+        </is>
+      </c>
+      <c r="C896" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D896" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705144392</t>
+        </is>
+      </c>
+      <c r="E896" t="inlineStr"/>
+      <c r="F896" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Reko145</t>
+        </is>
+      </c>
+      <c r="C897" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D897" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705144392</t>
+        </is>
+      </c>
+      <c r="E897" t="inlineStr"/>
+      <c r="F897" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Reko145</t>
+        </is>
+      </c>
+      <c r="C898" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D898" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705144392</t>
+        </is>
+      </c>
+      <c r="E898" t="n">
+        <v>237</v>
+      </c>
+      <c r="F898" t="inlineStr"/>
+    </row>
+    <row r="899">
+      <c r="A899" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>3191235</t>
+        </is>
+      </c>
+      <c r="C899" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D899" t="inlineStr">
+        <is>
+          <t>Order 3191235 Swish +46707943004</t>
+        </is>
+      </c>
+      <c r="E899" t="inlineStr"/>
+      <c r="F899" t="n">
+        <v>247.32</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>3191235</t>
+        </is>
+      </c>
+      <c r="C900" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D900" t="inlineStr">
+        <is>
+          <t>Order 3191235 Swish +46707943004</t>
+        </is>
+      </c>
+      <c r="E900" t="inlineStr"/>
+      <c r="F900" t="n">
+        <v>29.68</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>3191235</t>
+        </is>
+      </c>
+      <c r="C901" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D901" t="inlineStr">
+        <is>
+          <t>Order 3191235 Swish +46707943004</t>
+        </is>
+      </c>
+      <c r="E901" t="n">
+        <v>277</v>
+      </c>
+      <c r="F901" t="inlineStr"/>
+    </row>
+    <row r="902">
+      <c r="A902" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>1191653</t>
+        </is>
+      </c>
+      <c r="C902" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D902" t="inlineStr">
+        <is>
+          <t>Order 1191653 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E902" t="inlineStr"/>
+      <c r="F902" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>1191653</t>
+        </is>
+      </c>
+      <c r="C903" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D903" t="inlineStr">
+        <is>
+          <t>Order 1191653 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E903" t="inlineStr"/>
+      <c r="F903" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>1191653</t>
+        </is>
+      </c>
+      <c r="C904" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D904" t="inlineStr">
+        <is>
+          <t>Order 1191653 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E904" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F904" t="inlineStr"/>
+    </row>
+    <row r="905">
+      <c r="A905" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>7191941</t>
+        </is>
+      </c>
+      <c r="C905" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D905" t="inlineStr">
+        <is>
+          <t>Order 7191941 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E905" t="inlineStr"/>
+      <c r="F905" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>7191941</t>
+        </is>
+      </c>
+      <c r="C906" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D906" t="inlineStr">
+        <is>
+          <t>Order 7191941 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E906" t="inlineStr"/>
+      <c r="F906" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>7191941</t>
+        </is>
+      </c>
+      <c r="C907" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D907" t="inlineStr">
+        <is>
+          <t>Order 7191941 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E907" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F907" t="inlineStr"/>
+    </row>
+    <row r="908">
+      <c r="A908" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>0192135</t>
+        </is>
+      </c>
+      <c r="C908" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D908" t="inlineStr">
+        <is>
+          <t>Order 0192135 Swish +46703084774</t>
+        </is>
+      </c>
+      <c r="E908" t="inlineStr"/>
+      <c r="F908" t="n">
+        <v>557.14</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>0192135</t>
+        </is>
+      </c>
+      <c r="C909" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D909" t="inlineStr">
+        <is>
+          <t>Order 0192135 Swish +46703084774</t>
+        </is>
+      </c>
+      <c r="E909" t="inlineStr"/>
+      <c r="F909" t="n">
+        <v>66.86</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>0192135</t>
+        </is>
+      </c>
+      <c r="C910" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D910" t="inlineStr">
+        <is>
+          <t>Order 0192135 Swish +46703084774</t>
+        </is>
+      </c>
+      <c r="E910" t="n">
+        <v>624</v>
+      </c>
+      <c r="F910" t="inlineStr"/>
+    </row>
+    <row r="911">
+      <c r="A911" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B911" t="inlineStr"/>
+      <c r="C911" t="n">
+        <v>5410</v>
+      </c>
+      <c r="D911" t="inlineStr">
+        <is>
+          <t>AMAZONMKTPLC*MK9180YA4 K0135</t>
+        </is>
+      </c>
+      <c r="E911" t="n">
+        <v>202.32</v>
+      </c>
+      <c r="F911" t="inlineStr"/>
+    </row>
+    <row r="912">
+      <c r="A912" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B912" t="inlineStr"/>
+      <c r="C912" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D912" t="inlineStr">
+        <is>
+          <t>AMAZONMKTPLC*MK9180YA4 K0135</t>
+        </is>
+      </c>
+      <c r="E912" t="n">
+        <v>50.58</v>
+      </c>
+      <c r="F912" t="inlineStr"/>
+    </row>
+    <row r="913">
+      <c r="A913" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B913" t="inlineStr"/>
+      <c r="C913" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D913" t="inlineStr">
+        <is>
+          <t>AMAZONMKTPLC*MK9180YA4 K0135</t>
+        </is>
+      </c>
+      <c r="E913" t="inlineStr"/>
+      <c r="F913" t="n">
+        <v>252.9</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B914" t="inlineStr"/>
+      <c r="C914" t="n">
+        <v>6540</v>
+      </c>
+      <c r="D914" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E914" t="n">
+        <v>588</v>
+      </c>
+      <c r="F914" t="inlineStr"/>
+    </row>
+    <row r="915">
+      <c r="A915" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B915" t="inlineStr"/>
+      <c r="C915" t="n">
+        <v>6540</v>
+      </c>
+      <c r="D915" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E915" t="n">
+        <v>139</v>
+      </c>
+      <c r="F915" t="inlineStr"/>
+    </row>
+    <row r="916">
+      <c r="A916" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B916" t="inlineStr"/>
+      <c r="C916" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D916" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E916" t="n">
+        <v>147</v>
+      </c>
+      <c r="F916" t="inlineStr"/>
+    </row>
+    <row r="917">
+      <c r="A917" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B917" t="inlineStr"/>
+      <c r="C917" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D917" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E917" t="n">
+        <v>34.75</v>
+      </c>
+      <c r="F917" t="inlineStr"/>
+    </row>
+    <row r="918">
+      <c r="A918" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B918" t="inlineStr"/>
+      <c r="C918" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D918" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E918" t="inlineStr"/>
+      <c r="F918" t="n">
+        <v>173.75</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="2" t="n">
+        <v>44335</v>
+      </c>
+      <c r="B919" t="inlineStr"/>
+      <c r="C919" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D919" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E919" t="inlineStr"/>
+      <c r="F919" t="n">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Reko146</t>
+        </is>
+      </c>
+      <c r="C920" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D920" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738941039</t>
+        </is>
+      </c>
+      <c r="E920" t="inlineStr"/>
+      <c r="F920" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Reko146</t>
+        </is>
+      </c>
+      <c r="C921" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D921" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738941039</t>
+        </is>
+      </c>
+      <c r="E921" t="inlineStr"/>
+      <c r="F921" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Reko146</t>
+        </is>
+      </c>
+      <c r="C922" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D922" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738941039</t>
+        </is>
+      </c>
+      <c r="E922" t="n">
+        <v>258</v>
+      </c>
+      <c r="F922" t="inlineStr"/>
+    </row>
+    <row r="923">
+      <c r="A923" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B923" t="inlineStr"/>
+      <c r="C923" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D923" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E923" t="n">
+        <v>100.5</v>
+      </c>
+      <c r="F923" t="inlineStr"/>
+    </row>
+    <row r="924">
+      <c r="A924" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B924" t="inlineStr"/>
+      <c r="C924" t="inlineStr"/>
+      <c r="D924" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E924" t="n">
+        <v>0</v>
+      </c>
+      <c r="F924" t="inlineStr"/>
+    </row>
+    <row r="925">
+      <c r="A925" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B925" t="inlineStr"/>
+      <c r="C925" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D925" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E925" t="inlineStr"/>
+      <c r="F925" t="n">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Reko147</t>
+        </is>
+      </c>
+      <c r="C926" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D926" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E926" t="inlineStr"/>
+      <c r="F926" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Reko147</t>
+        </is>
+      </c>
+      <c r="C927" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D927" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E927" t="inlineStr"/>
+      <c r="F927" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Reko147</t>
+        </is>
+      </c>
+      <c r="C928" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D928" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E928" t="n">
+        <v>316</v>
+      </c>
+      <c r="F928" t="inlineStr"/>
+    </row>
+    <row r="929">
+      <c r="A929" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B929" t="inlineStr"/>
+      <c r="C929" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D929" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E929" t="n">
+        <v>645.7</v>
+      </c>
+      <c r="F929" t="inlineStr"/>
+    </row>
+    <row r="930">
+      <c r="A930" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B930" t="inlineStr"/>
+      <c r="C930" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D930" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E930" t="n">
+        <v>77.48</v>
+      </c>
+      <c r="F930" t="inlineStr"/>
+    </row>
+    <row r="931">
+      <c r="A931" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B931" t="inlineStr"/>
+      <c r="C931" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D931" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E931" t="inlineStr"/>
+      <c r="F931" t="n">
+        <v>723.1799999999999</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B932" t="inlineStr"/>
+      <c r="C932" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D932" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K6885</t>
+        </is>
+      </c>
+      <c r="E932" t="n">
+        <v>475.73</v>
+      </c>
+      <c r="F932" t="inlineStr"/>
+    </row>
+    <row r="933">
+      <c r="A933" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B933" t="inlineStr"/>
+      <c r="C933" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D933" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K6885</t>
+        </is>
+      </c>
+      <c r="E933" t="n">
+        <v>57.09</v>
+      </c>
+      <c r="F933" t="inlineStr"/>
+    </row>
+    <row r="934">
+      <c r="A934" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B934" t="inlineStr"/>
+      <c r="C934" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D934" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K6885</t>
+        </is>
+      </c>
+      <c r="E934" t="inlineStr"/>
+      <c r="F934" t="n">
+        <v>532.8200000000001</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B935" t="inlineStr"/>
+      <c r="C935" t="n">
+        <v>5410</v>
+      </c>
+      <c r="D935" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E935" t="n">
+        <v>422.4</v>
+      </c>
+      <c r="F935" t="inlineStr"/>
+    </row>
+    <row r="936">
+      <c r="A936" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B936" t="inlineStr"/>
+      <c r="C936" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D936" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E936" t="n">
+        <v>105.6</v>
+      </c>
+      <c r="F936" t="inlineStr"/>
+    </row>
+    <row r="937">
+      <c r="A937" s="2" t="n">
+        <v>44336</v>
+      </c>
+      <c r="B937" t="inlineStr"/>
+      <c r="C937" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D937" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E937" t="inlineStr"/>
+      <c r="F937" t="n">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Reko148</t>
+        </is>
+      </c>
+      <c r="C938" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D938" t="inlineStr">
+        <is>
+          <t>Reko Swish +46765675543</t>
+        </is>
+      </c>
+      <c r="E938" t="inlineStr"/>
+      <c r="F938" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Reko148</t>
+        </is>
+      </c>
+      <c r="C939" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D939" t="inlineStr">
+        <is>
+          <t>Reko Swish +46765675543</t>
+        </is>
+      </c>
+      <c r="E939" t="inlineStr"/>
+      <c r="F939" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Reko148</t>
+        </is>
+      </c>
+      <c r="C940" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D940" t="inlineStr">
+        <is>
+          <t>Reko Swish +46765675543</t>
+        </is>
+      </c>
+      <c r="E940" t="n">
+        <v>516</v>
+      </c>
+      <c r="F940" t="inlineStr"/>
+    </row>
+    <row r="941">
+      <c r="A941" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Reko149</t>
+        </is>
+      </c>
+      <c r="C941" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D941" t="inlineStr">
+        <is>
+          <t>Reko Swish +46763230055</t>
+        </is>
+      </c>
+      <c r="E941" t="inlineStr"/>
+      <c r="F941" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Reko149</t>
+        </is>
+      </c>
+      <c r="C942" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D942" t="inlineStr">
+        <is>
+          <t>Reko Swish +46763230055</t>
+        </is>
+      </c>
+      <c r="E942" t="inlineStr"/>
+      <c r="F942" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Reko149</t>
+        </is>
+      </c>
+      <c r="C943" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D943" t="inlineStr">
+        <is>
+          <t>Reko Swish +46763230055</t>
+        </is>
+      </c>
+      <c r="E943" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F943" t="inlineStr"/>
+    </row>
+    <row r="944">
+      <c r="A944" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B944" t="inlineStr"/>
+      <c r="C944" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D944" t="inlineStr">
+        <is>
+          <t>May hyra</t>
+        </is>
+      </c>
+      <c r="E944" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F944" t="inlineStr"/>
+    </row>
+    <row r="945">
+      <c r="A945" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B945" t="inlineStr"/>
+      <c r="C945" t="inlineStr"/>
+      <c r="D945" t="inlineStr">
+        <is>
+          <t>May hyra</t>
+        </is>
+      </c>
+      <c r="E945" t="n">
+        <v>0</v>
+      </c>
+      <c r="F945" t="inlineStr"/>
+    </row>
+    <row r="946">
+      <c r="A946" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B946" t="inlineStr"/>
+      <c r="C946" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D946" t="inlineStr">
+        <is>
+          <t>May hyra</t>
+        </is>
+      </c>
+      <c r="E946" t="inlineStr"/>
+      <c r="F946" t="n">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Reko150</t>
+        </is>
+      </c>
+      <c r="C947" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D947" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735221954</t>
+        </is>
+      </c>
+      <c r="E947" t="inlineStr"/>
+      <c r="F947" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Reko150</t>
+        </is>
+      </c>
+      <c r="C948" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D948" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735221954</t>
+        </is>
+      </c>
+      <c r="E948" t="inlineStr"/>
+      <c r="F948" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Reko150</t>
+        </is>
+      </c>
+      <c r="C949" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D949" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735221954</t>
+        </is>
+      </c>
+      <c r="E949" t="n">
+        <v>258</v>
+      </c>
+      <c r="F949" t="inlineStr"/>
+    </row>
+    <row r="950">
+      <c r="A950" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Reko151</t>
+        </is>
+      </c>
+      <c r="C950" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D950" t="inlineStr">
+        <is>
+          <t>Reko Swish +46728774058</t>
+        </is>
+      </c>
+      <c r="E950" t="inlineStr"/>
+      <c r="F950" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Reko151</t>
+        </is>
+      </c>
+      <c r="C951" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D951" t="inlineStr">
+        <is>
+          <t>Reko Swish +46728774058</t>
+        </is>
+      </c>
+      <c r="E951" t="inlineStr"/>
+      <c r="F951" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Reko151</t>
+        </is>
+      </c>
+      <c r="C952" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D952" t="inlineStr">
+        <is>
+          <t>Reko Swish +46728774058</t>
+        </is>
+      </c>
+      <c r="E952" t="n">
+        <v>316</v>
+      </c>
+      <c r="F952" t="inlineStr"/>
+    </row>
+    <row r="953">
+      <c r="A953" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B953" t="inlineStr"/>
+      <c r="C953" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D953" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E953" t="n">
+        <v>262.5</v>
+      </c>
+      <c r="F953" t="inlineStr"/>
+    </row>
+    <row r="954">
+      <c r="A954" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B954" t="inlineStr"/>
+      <c r="C954" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D954" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E954" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="F954" t="inlineStr"/>
+    </row>
+    <row r="955">
+      <c r="A955" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B955" t="inlineStr"/>
+      <c r="C955" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D955" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E955" t="inlineStr"/>
+      <c r="F955" t="n">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B956" t="inlineStr"/>
+      <c r="C956" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D956" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E956" t="n">
+        <v>151.35</v>
+      </c>
+      <c r="F956" t="inlineStr"/>
+    </row>
+    <row r="957">
+      <c r="A957" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B957" t="inlineStr"/>
+      <c r="C957" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D957" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E957" t="n">
+        <v>18.16</v>
+      </c>
+      <c r="F957" t="inlineStr"/>
+    </row>
+    <row r="958">
+      <c r="A958" s="2" t="n">
+        <v>44337</v>
+      </c>
+      <c r="B958" t="inlineStr"/>
+      <c r="C958" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D958" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E958" t="inlineStr"/>
+      <c r="F958" t="n">
+        <v>169.51</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>4222034</t>
+        </is>
+      </c>
+      <c r="C959" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D959" t="inlineStr">
+        <is>
+          <t>Order 4222034 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E959" t="inlineStr"/>
+      <c r="F959" t="n">
+        <v>1097.32</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>4222034</t>
+        </is>
+      </c>
+      <c r="C960" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D960" t="inlineStr">
+        <is>
+          <t>Order 4222034 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E960" t="inlineStr"/>
+      <c r="F960" t="n">
+        <v>131.68</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="2" t="n">
+        <v>44338</v>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>4222034</t>
+        </is>
+      </c>
+      <c r="C961" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D961" t="inlineStr">
+        <is>
+          <t>Order 4222034 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E961" t="n">
+        <v>1229</v>
+      </c>
+      <c r="F961" t="inlineStr"/>
+    </row>
+    <row r="962">
+      <c r="A962" s="2" t="n">
+        <v>44339</v>
+      </c>
+      <c r="B962" t="inlineStr"/>
+      <c r="C962" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D962" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E962" t="n">
+        <v>785.3</v>
+      </c>
+      <c r="F962" t="inlineStr"/>
+    </row>
+    <row r="963">
+      <c r="A963" s="2" t="n">
+        <v>44339</v>
+      </c>
+      <c r="B963" t="inlineStr"/>
+      <c r="C963" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D963" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E963" t="n">
+        <v>196.33</v>
+      </c>
+      <c r="F963" t="inlineStr"/>
+    </row>
+    <row r="964">
+      <c r="A964" s="2" t="n">
+        <v>44339</v>
+      </c>
+      <c r="B964" t="inlineStr"/>
+      <c r="C964" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D964" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E964" t="inlineStr"/>
+      <c r="F964" t="n">
+        <v>981.63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 138 new rows for week ending 2021-05-30 (total 1101 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F964"/>
+  <dimension ref="A1:F1102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20265,6 +20265,2982 @@
         <v>981.63</v>
       </c>
     </row>
+    <row r="965">
+      <c r="A965" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>Reko152</t>
+        </is>
+      </c>
+      <c r="C965" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D965" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705544642</t>
+        </is>
+      </c>
+      <c r="E965" t="inlineStr"/>
+      <c r="F965" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Reko152</t>
+        </is>
+      </c>
+      <c r="C966" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D966" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705544642</t>
+        </is>
+      </c>
+      <c r="E966" t="inlineStr"/>
+      <c r="F966" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Reko152</t>
+        </is>
+      </c>
+      <c r="C967" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D967" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705544642</t>
+        </is>
+      </c>
+      <c r="E967" t="n">
+        <v>129</v>
+      </c>
+      <c r="F967" t="inlineStr"/>
+    </row>
+    <row r="968">
+      <c r="A968" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Reko153</t>
+        </is>
+      </c>
+      <c r="C968" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D968" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739131200</t>
+        </is>
+      </c>
+      <c r="E968" t="inlineStr"/>
+      <c r="F968" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Reko153</t>
+        </is>
+      </c>
+      <c r="C969" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D969" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739131200</t>
+        </is>
+      </c>
+      <c r="E969" t="inlineStr"/>
+      <c r="F969" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Reko153</t>
+        </is>
+      </c>
+      <c r="C970" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D970" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739131200</t>
+        </is>
+      </c>
+      <c r="E970" t="n">
+        <v>516</v>
+      </c>
+      <c r="F970" t="inlineStr"/>
+    </row>
+    <row r="971">
+      <c r="A971" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Reko154</t>
+        </is>
+      </c>
+      <c r="C971" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D971" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704546524</t>
+        </is>
+      </c>
+      <c r="E971" t="inlineStr"/>
+      <c r="F971" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Reko154</t>
+        </is>
+      </c>
+      <c r="C972" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D972" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704546524</t>
+        </is>
+      </c>
+      <c r="E972" t="inlineStr"/>
+      <c r="F972" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Reko154</t>
+        </is>
+      </c>
+      <c r="C973" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D973" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704546524</t>
+        </is>
+      </c>
+      <c r="E973" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F973" t="inlineStr"/>
+    </row>
+    <row r="974">
+      <c r="A974" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Reko155</t>
+        </is>
+      </c>
+      <c r="C974" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D974" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761192525</t>
+        </is>
+      </c>
+      <c r="E974" t="inlineStr"/>
+      <c r="F974" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Reko155</t>
+        </is>
+      </c>
+      <c r="C975" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D975" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761192525</t>
+        </is>
+      </c>
+      <c r="E975" t="inlineStr"/>
+      <c r="F975" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Reko155</t>
+        </is>
+      </c>
+      <c r="C976" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D976" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761192525</t>
+        </is>
+      </c>
+      <c r="E976" t="n">
+        <v>258</v>
+      </c>
+      <c r="F976" t="inlineStr"/>
+    </row>
+    <row r="977">
+      <c r="A977" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Reko156</t>
+        </is>
+      </c>
+      <c r="C977" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D977" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700391434</t>
+        </is>
+      </c>
+      <c r="E977" t="inlineStr"/>
+      <c r="F977" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Reko156</t>
+        </is>
+      </c>
+      <c r="C978" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D978" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700391434</t>
+        </is>
+      </c>
+      <c r="E978" t="inlineStr"/>
+      <c r="F978" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Reko156</t>
+        </is>
+      </c>
+      <c r="C979" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D979" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700391434</t>
+        </is>
+      </c>
+      <c r="E979" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F979" t="inlineStr"/>
+    </row>
+    <row r="980">
+      <c r="A980" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Reko157</t>
+        </is>
+      </c>
+      <c r="C980" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D980" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739955670</t>
+        </is>
+      </c>
+      <c r="E980" t="inlineStr"/>
+      <c r="F980" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Reko157</t>
+        </is>
+      </c>
+      <c r="C981" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D981" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739955670</t>
+        </is>
+      </c>
+      <c r="E981" t="inlineStr"/>
+      <c r="F981" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Reko157</t>
+        </is>
+      </c>
+      <c r="C982" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D982" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739955670</t>
+        </is>
+      </c>
+      <c r="E982" t="n">
+        <v>645</v>
+      </c>
+      <c r="F982" t="inlineStr"/>
+    </row>
+    <row r="983">
+      <c r="A983" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Reko158</t>
+        </is>
+      </c>
+      <c r="C983" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D983" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703251291</t>
+        </is>
+      </c>
+      <c r="E983" t="inlineStr"/>
+      <c r="F983" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Reko158</t>
+        </is>
+      </c>
+      <c r="C984" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D984" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703251291</t>
+        </is>
+      </c>
+      <c r="E984" t="inlineStr"/>
+      <c r="F984" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Reko158</t>
+        </is>
+      </c>
+      <c r="C985" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D985" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703251291</t>
+        </is>
+      </c>
+      <c r="E985" t="n">
+        <v>258</v>
+      </c>
+      <c r="F985" t="inlineStr"/>
+    </row>
+    <row r="986">
+      <c r="A986" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Reko159</t>
+        </is>
+      </c>
+      <c r="C986" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D986" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707364050</t>
+        </is>
+      </c>
+      <c r="E986" t="inlineStr"/>
+      <c r="F986" t="n">
+        <v>300.89</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Reko159</t>
+        </is>
+      </c>
+      <c r="C987" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D987" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707364050</t>
+        </is>
+      </c>
+      <c r="E987" t="inlineStr"/>
+      <c r="F987" t="n">
+        <v>36.11</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Reko159</t>
+        </is>
+      </c>
+      <c r="C988" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D988" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707364050</t>
+        </is>
+      </c>
+      <c r="E988" t="n">
+        <v>337</v>
+      </c>
+      <c r="F988" t="inlineStr"/>
+    </row>
+    <row r="989">
+      <c r="A989" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Reko160</t>
+        </is>
+      </c>
+      <c r="C989" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D989" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768311010</t>
+        </is>
+      </c>
+      <c r="E989" t="inlineStr"/>
+      <c r="F989" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Reko160</t>
+        </is>
+      </c>
+      <c r="C990" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D990" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768311010</t>
+        </is>
+      </c>
+      <c r="E990" t="inlineStr"/>
+      <c r="F990" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Reko160</t>
+        </is>
+      </c>
+      <c r="C991" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D991" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768311010</t>
+        </is>
+      </c>
+      <c r="E991" t="n">
+        <v>258</v>
+      </c>
+      <c r="F991" t="inlineStr"/>
+    </row>
+    <row r="992">
+      <c r="A992" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Reko161</t>
+        </is>
+      </c>
+      <c r="C992" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D992" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E992" t="inlineStr"/>
+      <c r="F992" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Reko161</t>
+        </is>
+      </c>
+      <c r="C993" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D993" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E993" t="inlineStr"/>
+      <c r="F993" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Reko161</t>
+        </is>
+      </c>
+      <c r="C994" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D994" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E994" t="n">
+        <v>258</v>
+      </c>
+      <c r="F994" t="inlineStr"/>
+    </row>
+    <row r="995">
+      <c r="A995" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Reko162</t>
+        </is>
+      </c>
+      <c r="C995" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D995" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E995" t="inlineStr"/>
+      <c r="F995" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Reko162</t>
+        </is>
+      </c>
+      <c r="C996" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D996" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E996" t="inlineStr"/>
+      <c r="F996" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Reko162</t>
+        </is>
+      </c>
+      <c r="C997" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D997" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E997" t="n">
+        <v>316</v>
+      </c>
+      <c r="F997" t="inlineStr"/>
+    </row>
+    <row r="998">
+      <c r="A998" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Reko163</t>
+        </is>
+      </c>
+      <c r="C998" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D998" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720506071</t>
+        </is>
+      </c>
+      <c r="E998" t="inlineStr"/>
+      <c r="F998" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Reko163</t>
+        </is>
+      </c>
+      <c r="C999" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D999" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720506071</t>
+        </is>
+      </c>
+      <c r="E999" t="inlineStr"/>
+      <c r="F999" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Reko163</t>
+        </is>
+      </c>
+      <c r="C1000" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1000" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720506071</t>
+        </is>
+      </c>
+      <c r="E1000" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1000" t="inlineStr"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Reko164</t>
+        </is>
+      </c>
+      <c r="C1001" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1001" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1001" t="inlineStr"/>
+      <c r="F1001" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Reko164</t>
+        </is>
+      </c>
+      <c r="C1002" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1002" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1002" t="inlineStr"/>
+      <c r="F1002" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Reko164</t>
+        </is>
+      </c>
+      <c r="C1003" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1003" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1003" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1003" t="inlineStr"/>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Reko165</t>
+        </is>
+      </c>
+      <c r="C1004" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1004" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E1004" t="inlineStr"/>
+      <c r="F1004" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Reko165</t>
+        </is>
+      </c>
+      <c r="C1005" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1005" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E1005" t="inlineStr"/>
+      <c r="F1005" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Reko165</t>
+        </is>
+      </c>
+      <c r="C1006" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1006" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E1006" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1006" t="inlineStr"/>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Reko166</t>
+        </is>
+      </c>
+      <c r="C1007" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1007" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E1007" t="inlineStr"/>
+      <c r="F1007" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Reko166</t>
+        </is>
+      </c>
+      <c r="C1008" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1008" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E1008" t="inlineStr"/>
+      <c r="F1008" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Reko166</t>
+        </is>
+      </c>
+      <c r="C1009" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1009" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705629304</t>
+        </is>
+      </c>
+      <c r="E1009" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1009" t="inlineStr"/>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Reko167</t>
+        </is>
+      </c>
+      <c r="C1010" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1010" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722332390</t>
+        </is>
+      </c>
+      <c r="E1010" t="inlineStr"/>
+      <c r="F1010" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Reko167</t>
+        </is>
+      </c>
+      <c r="C1011" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1011" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722332390</t>
+        </is>
+      </c>
+      <c r="E1011" t="inlineStr"/>
+      <c r="F1011" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Reko167</t>
+        </is>
+      </c>
+      <c r="C1012" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1012" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722332390</t>
+        </is>
+      </c>
+      <c r="E1012" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1012" t="inlineStr"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Reko168</t>
+        </is>
+      </c>
+      <c r="C1013" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1013" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E1013" t="inlineStr"/>
+      <c r="F1013" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Reko168</t>
+        </is>
+      </c>
+      <c r="C1014" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1014" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E1014" t="inlineStr"/>
+      <c r="F1014" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Reko168</t>
+        </is>
+      </c>
+      <c r="C1015" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1015" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702331968</t>
+        </is>
+      </c>
+      <c r="E1015" t="n">
+        <v>690</v>
+      </c>
+      <c r="F1015" t="inlineStr"/>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Reko169</t>
+        </is>
+      </c>
+      <c r="C1016" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1016" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720106501</t>
+        </is>
+      </c>
+      <c r="E1016" t="inlineStr"/>
+      <c r="F1016" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Reko169</t>
+        </is>
+      </c>
+      <c r="C1017" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1017" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720106501</t>
+        </is>
+      </c>
+      <c r="E1017" t="inlineStr"/>
+      <c r="F1017" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Reko169</t>
+        </is>
+      </c>
+      <c r="C1018" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1018" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720106501</t>
+        </is>
+      </c>
+      <c r="E1018" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1018" t="inlineStr"/>
+    </row>
+    <row r="1019">
+      <c r="A1019" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Reko170</t>
+        </is>
+      </c>
+      <c r="C1019" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1019" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761956046</t>
+        </is>
+      </c>
+      <c r="E1019" t="inlineStr"/>
+      <c r="F1019" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Reko170</t>
+        </is>
+      </c>
+      <c r="C1020" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1020" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761956046</t>
+        </is>
+      </c>
+      <c r="E1020" t="inlineStr"/>
+      <c r="F1020" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>Reko170</t>
+        </is>
+      </c>
+      <c r="C1021" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1021" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761956046</t>
+        </is>
+      </c>
+      <c r="E1021" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1021" t="inlineStr"/>
+    </row>
+    <row r="1022">
+      <c r="A1022" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Reko171</t>
+        </is>
+      </c>
+      <c r="C1022" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1022" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E1022" t="inlineStr"/>
+      <c r="F1022" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Reko171</t>
+        </is>
+      </c>
+      <c r="C1023" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1023" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E1023" t="inlineStr"/>
+      <c r="F1023" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Reko171</t>
+        </is>
+      </c>
+      <c r="C1024" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1024" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E1024" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1024" t="inlineStr"/>
+    </row>
+    <row r="1025">
+      <c r="A1025" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Reko172</t>
+        </is>
+      </c>
+      <c r="C1025" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1025" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703626756</t>
+        </is>
+      </c>
+      <c r="E1025" t="inlineStr"/>
+      <c r="F1025" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Reko172</t>
+        </is>
+      </c>
+      <c r="C1026" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1026" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703626756</t>
+        </is>
+      </c>
+      <c r="E1026" t="inlineStr"/>
+      <c r="F1026" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Reko172</t>
+        </is>
+      </c>
+      <c r="C1027" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1027" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703626756</t>
+        </is>
+      </c>
+      <c r="E1027" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1027" t="inlineStr"/>
+    </row>
+    <row r="1028">
+      <c r="A1028" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1028" t="inlineStr"/>
+      <c r="C1028" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1028" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1028" t="n">
+        <v>2559.67</v>
+      </c>
+      <c r="F1028" t="inlineStr"/>
+    </row>
+    <row r="1029">
+      <c r="A1029" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1029" t="inlineStr"/>
+      <c r="C1029" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1029" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1029" t="n">
+        <v>307.16</v>
+      </c>
+      <c r="F1029" t="inlineStr"/>
+    </row>
+    <row r="1030">
+      <c r="A1030" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1030" t="inlineStr"/>
+      <c r="C1030" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1030" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1030" t="inlineStr"/>
+      <c r="F1030" t="n">
+        <v>2866.83</v>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1031" t="inlineStr"/>
+      <c r="C1031" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1031" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1031" t="n">
+        <v>1280.25</v>
+      </c>
+      <c r="F1031" t="inlineStr"/>
+    </row>
+    <row r="1032">
+      <c r="A1032" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1032" t="inlineStr"/>
+      <c r="C1032" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1032" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1032" t="n">
+        <v>153.63</v>
+      </c>
+      <c r="F1032" t="inlineStr"/>
+    </row>
+    <row r="1033">
+      <c r="A1033" s="2" t="n">
+        <v>44340</v>
+      </c>
+      <c r="B1033" t="inlineStr"/>
+      <c r="C1033" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1033" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1033" t="inlineStr"/>
+      <c r="F1033" t="n">
+        <v>1433.88</v>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Reko173</t>
+        </is>
+      </c>
+      <c r="C1034" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1034" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705544642 Return</t>
+        </is>
+      </c>
+      <c r="E1034" t="n">
+        <v>115.18</v>
+      </c>
+      <c r="F1034" t="inlineStr"/>
+    </row>
+    <row r="1035">
+      <c r="A1035" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Reko173</t>
+        </is>
+      </c>
+      <c r="C1035" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1035" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705544642 Return</t>
+        </is>
+      </c>
+      <c r="E1035" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="F1035" t="inlineStr"/>
+    </row>
+    <row r="1036">
+      <c r="A1036" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Reko173</t>
+        </is>
+      </c>
+      <c r="C1036" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1036" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705544642 Return</t>
+        </is>
+      </c>
+      <c r="E1036" t="inlineStr"/>
+      <c r="F1036" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Reko174</t>
+        </is>
+      </c>
+      <c r="C1037" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1037" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720506071 Return</t>
+        </is>
+      </c>
+      <c r="E1037" t="n">
+        <v>115.18</v>
+      </c>
+      <c r="F1037" t="inlineStr"/>
+    </row>
+    <row r="1038">
+      <c r="A1038" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Reko174</t>
+        </is>
+      </c>
+      <c r="C1038" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1038" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720506071 Return</t>
+        </is>
+      </c>
+      <c r="E1038" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="F1038" t="inlineStr"/>
+    </row>
+    <row r="1039">
+      <c r="A1039" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Reko174</t>
+        </is>
+      </c>
+      <c r="C1039" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1039" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720506071 Return</t>
+        </is>
+      </c>
+      <c r="E1039" t="inlineStr"/>
+      <c r="F1039" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Reko175</t>
+        </is>
+      </c>
+      <c r="C1040" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1040" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709820782</t>
+        </is>
+      </c>
+      <c r="E1040" t="inlineStr"/>
+      <c r="F1040" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Reko175</t>
+        </is>
+      </c>
+      <c r="C1041" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1041" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709820782</t>
+        </is>
+      </c>
+      <c r="E1041" t="inlineStr"/>
+      <c r="F1041" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Reko175</t>
+        </is>
+      </c>
+      <c r="C1042" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1042" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709820782</t>
+        </is>
+      </c>
+      <c r="E1042" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1042" t="inlineStr"/>
+    </row>
+    <row r="1043">
+      <c r="A1043" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Reko176</t>
+        </is>
+      </c>
+      <c r="C1043" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1043" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736241792</t>
+        </is>
+      </c>
+      <c r="E1043" t="inlineStr"/>
+      <c r="F1043" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Reko176</t>
+        </is>
+      </c>
+      <c r="C1044" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1044" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736241792</t>
+        </is>
+      </c>
+      <c r="E1044" t="inlineStr"/>
+      <c r="F1044" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Reko176</t>
+        </is>
+      </c>
+      <c r="C1045" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1045" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736241792</t>
+        </is>
+      </c>
+      <c r="E1045" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1045" t="inlineStr"/>
+    </row>
+    <row r="1046">
+      <c r="A1046" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Reko177</t>
+        </is>
+      </c>
+      <c r="C1046" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1046" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727070411</t>
+        </is>
+      </c>
+      <c r="E1046" t="inlineStr"/>
+      <c r="F1046" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Reko177</t>
+        </is>
+      </c>
+      <c r="C1047" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1047" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727070411</t>
+        </is>
+      </c>
+      <c r="E1047" t="inlineStr"/>
+      <c r="F1047" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Reko177</t>
+        </is>
+      </c>
+      <c r="C1048" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1048" t="inlineStr">
+        <is>
+          <t>Reko Swish +46727070411</t>
+        </is>
+      </c>
+      <c r="E1048" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1048" t="inlineStr"/>
+    </row>
+    <row r="1049">
+      <c r="A1049" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Reko178</t>
+        </is>
+      </c>
+      <c r="C1049" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1049" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1049" t="inlineStr"/>
+      <c r="F1049" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Reko178</t>
+        </is>
+      </c>
+      <c r="C1050" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1050" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1050" t="inlineStr"/>
+      <c r="F1050" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Reko178</t>
+        </is>
+      </c>
+      <c r="C1051" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1051" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1051" t="n">
+        <v>395</v>
+      </c>
+      <c r="F1051" t="inlineStr"/>
+    </row>
+    <row r="1052">
+      <c r="A1052" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1052" t="inlineStr"/>
+      <c r="C1052" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1052" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1052" t="n">
+        <v>311.7</v>
+      </c>
+      <c r="F1052" t="inlineStr"/>
+    </row>
+    <row r="1053">
+      <c r="A1053" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1053" t="inlineStr"/>
+      <c r="C1053" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1053" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1053" t="n">
+        <v>37.4</v>
+      </c>
+      <c r="F1053" t="inlineStr"/>
+    </row>
+    <row r="1054">
+      <c r="A1054" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1054" t="inlineStr"/>
+      <c r="C1054" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1054" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1054" t="inlineStr"/>
+      <c r="F1054" t="n">
+        <v>349.1</v>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1055" t="inlineStr"/>
+      <c r="C1055" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D1055" t="inlineStr">
+        <is>
+          <t>NETS*link.getgifted. K0135</t>
+        </is>
+      </c>
+      <c r="E1055" t="n">
+        <v>1520</v>
+      </c>
+      <c r="F1055" t="inlineStr"/>
+    </row>
+    <row r="1056">
+      <c r="A1056" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1056" t="inlineStr"/>
+      <c r="C1056" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1056" t="inlineStr">
+        <is>
+          <t>NETS*link.getgifted. K0135</t>
+        </is>
+      </c>
+      <c r="E1056" t="n">
+        <v>380</v>
+      </c>
+      <c r="F1056" t="inlineStr"/>
+    </row>
+    <row r="1057">
+      <c r="A1057" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1057" t="inlineStr"/>
+      <c r="C1057" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1057" t="inlineStr">
+        <is>
+          <t>NETS*link.getgifted. K0135</t>
+        </is>
+      </c>
+      <c r="E1057" t="inlineStr"/>
+      <c r="F1057" t="n">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1058" t="inlineStr"/>
+      <c r="C1058" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D1058" t="inlineStr">
+        <is>
+          <t>Klarna *webhallen com K0135</t>
+        </is>
+      </c>
+      <c r="E1058" t="n">
+        <v>799.2</v>
+      </c>
+      <c r="F1058" t="inlineStr"/>
+    </row>
+    <row r="1059">
+      <c r="A1059" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1059" t="inlineStr"/>
+      <c r="C1059" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1059" t="inlineStr">
+        <is>
+          <t>Klarna *webhallen com K0135</t>
+        </is>
+      </c>
+      <c r="E1059" t="n">
+        <v>199.8</v>
+      </c>
+      <c r="F1059" t="inlineStr"/>
+    </row>
+    <row r="1060">
+      <c r="A1060" s="2" t="n">
+        <v>44341</v>
+      </c>
+      <c r="B1060" t="inlineStr"/>
+      <c r="C1060" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1060" t="inlineStr">
+        <is>
+          <t>Klarna *webhallen com K0135</t>
+        </is>
+      </c>
+      <c r="E1060" t="inlineStr"/>
+      <c r="F1060" t="n">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Reko179</t>
+        </is>
+      </c>
+      <c r="C1061" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1061" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760819</t>
+        </is>
+      </c>
+      <c r="E1061" t="inlineStr"/>
+      <c r="F1061" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Reko179</t>
+        </is>
+      </c>
+      <c r="C1062" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1062" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760819</t>
+        </is>
+      </c>
+      <c r="E1062" t="inlineStr"/>
+      <c r="F1062" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>Reko179</t>
+        </is>
+      </c>
+      <c r="C1063" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1063" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760819</t>
+        </is>
+      </c>
+      <c r="E1063" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1063" t="inlineStr"/>
+    </row>
+    <row r="1064">
+      <c r="A1064" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Reko180</t>
+        </is>
+      </c>
+      <c r="C1064" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1064" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E1064" t="inlineStr"/>
+      <c r="F1064" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Reko180</t>
+        </is>
+      </c>
+      <c r="C1065" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1065" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E1065" t="inlineStr"/>
+      <c r="F1065" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Reko180</t>
+        </is>
+      </c>
+      <c r="C1066" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1066" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E1066" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1066" t="inlineStr"/>
+    </row>
+    <row r="1067">
+      <c r="A1067" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Reko181</t>
+        </is>
+      </c>
+      <c r="C1067" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1067" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040</t>
+        </is>
+      </c>
+      <c r="E1067" t="inlineStr"/>
+      <c r="F1067" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Reko181</t>
+        </is>
+      </c>
+      <c r="C1068" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1068" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040</t>
+        </is>
+      </c>
+      <c r="E1068" t="inlineStr"/>
+      <c r="F1068" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" s="2" t="n">
+        <v>44342</v>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Reko181</t>
+        </is>
+      </c>
+      <c r="C1069" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1069" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040</t>
+        </is>
+      </c>
+      <c r="E1069" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1069" t="inlineStr"/>
+    </row>
+    <row r="1070">
+      <c r="A1070" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Reko182</t>
+        </is>
+      </c>
+      <c r="C1070" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1070" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775394</t>
+        </is>
+      </c>
+      <c r="E1070" t="inlineStr"/>
+      <c r="F1070" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Reko182</t>
+        </is>
+      </c>
+      <c r="C1071" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1071" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775394</t>
+        </is>
+      </c>
+      <c r="E1071" t="inlineStr"/>
+      <c r="F1071" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Reko182</t>
+        </is>
+      </c>
+      <c r="C1072" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1072" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775394</t>
+        </is>
+      </c>
+      <c r="E1072" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1072" t="inlineStr"/>
+    </row>
+    <row r="1073">
+      <c r="A1073" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Reko183</t>
+        </is>
+      </c>
+      <c r="C1073" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1073" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760819 Return</t>
+        </is>
+      </c>
+      <c r="E1073" t="n">
+        <v>230.36</v>
+      </c>
+      <c r="F1073" t="inlineStr"/>
+    </row>
+    <row r="1074">
+      <c r="A1074" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Reko183</t>
+        </is>
+      </c>
+      <c r="C1074" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1074" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760819 Return</t>
+        </is>
+      </c>
+      <c r="E1074" t="n">
+        <v>27.64</v>
+      </c>
+      <c r="F1074" t="inlineStr"/>
+    </row>
+    <row r="1075">
+      <c r="A1075" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Reko183</t>
+        </is>
+      </c>
+      <c r="C1075" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1075" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760819 Return</t>
+        </is>
+      </c>
+      <c r="E1075" t="inlineStr"/>
+      <c r="F1075" t="n">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Reko184</t>
+        </is>
+      </c>
+      <c r="C1076" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1076" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775394 Return</t>
+        </is>
+      </c>
+      <c r="E1076" t="n">
+        <v>141.07</v>
+      </c>
+      <c r="F1076" t="inlineStr"/>
+    </row>
+    <row r="1077">
+      <c r="A1077" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Reko184</t>
+        </is>
+      </c>
+      <c r="C1077" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1077" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775394 Return</t>
+        </is>
+      </c>
+      <c r="E1077" t="n">
+        <v>16.93</v>
+      </c>
+      <c r="F1077" t="inlineStr"/>
+    </row>
+    <row r="1078">
+      <c r="A1078" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Reko184</t>
+        </is>
+      </c>
+      <c r="C1078" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1078" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707775394 Return</t>
+        </is>
+      </c>
+      <c r="E1078" t="inlineStr"/>
+      <c r="F1078" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Reko185</t>
+        </is>
+      </c>
+      <c r="C1079" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1079" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040 Return</t>
+        </is>
+      </c>
+      <c r="E1079" t="n">
+        <v>70.54000000000001</v>
+      </c>
+      <c r="F1079" t="inlineStr"/>
+    </row>
+    <row r="1080">
+      <c r="A1080" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Reko185</t>
+        </is>
+      </c>
+      <c r="C1080" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1080" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040 Return</t>
+        </is>
+      </c>
+      <c r="E1080" t="n">
+        <v>8.460000000000001</v>
+      </c>
+      <c r="F1080" t="inlineStr"/>
+    </row>
+    <row r="1081">
+      <c r="A1081" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>Reko185</t>
+        </is>
+      </c>
+      <c r="C1081" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1081" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040 Return</t>
+        </is>
+      </c>
+      <c r="E1081" t="inlineStr"/>
+      <c r="F1081" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Reko186</t>
+        </is>
+      </c>
+      <c r="C1082" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1082" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704034490</t>
+        </is>
+      </c>
+      <c r="E1082" t="inlineStr"/>
+      <c r="F1082" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Reko186</t>
+        </is>
+      </c>
+      <c r="C1083" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1083" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704034490</t>
+        </is>
+      </c>
+      <c r="E1083" t="inlineStr"/>
+      <c r="F1083" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Reko186</t>
+        </is>
+      </c>
+      <c r="C1084" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1084" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704034490</t>
+        </is>
+      </c>
+      <c r="E1084" t="n">
+        <v>316</v>
+      </c>
+      <c r="F1084" t="inlineStr"/>
+    </row>
+    <row r="1085">
+      <c r="A1085" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Reko187</t>
+        </is>
+      </c>
+      <c r="C1085" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1085" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738042919</t>
+        </is>
+      </c>
+      <c r="E1085" t="inlineStr"/>
+      <c r="F1085" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Reko187</t>
+        </is>
+      </c>
+      <c r="C1086" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1086" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738042919</t>
+        </is>
+      </c>
+      <c r="E1086" t="inlineStr"/>
+      <c r="F1086" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Reko187</t>
+        </is>
+      </c>
+      <c r="C1087" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1087" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738042919</t>
+        </is>
+      </c>
+      <c r="E1087" t="inlineStr"/>
+      <c r="F1087" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>Reko188</t>
+        </is>
+      </c>
+      <c r="C1088" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1088" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738042919</t>
+        </is>
+      </c>
+      <c r="E1088" t="inlineStr"/>
+      <c r="F1088" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Reko188</t>
+        </is>
+      </c>
+      <c r="C1089" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1089" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738042919</t>
+        </is>
+      </c>
+      <c r="E1089" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1089" t="inlineStr"/>
+    </row>
+    <row r="1090">
+      <c r="A1090" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Reko188</t>
+        </is>
+      </c>
+      <c r="C1090" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1090" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738042919</t>
+        </is>
+      </c>
+      <c r="E1090" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1090" t="inlineStr"/>
+    </row>
+    <row r="1091">
+      <c r="A1091" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Reko189</t>
+        </is>
+      </c>
+      <c r="C1091" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1091" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767081933</t>
+        </is>
+      </c>
+      <c r="E1091" t="inlineStr"/>
+      <c r="F1091" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Reko189</t>
+        </is>
+      </c>
+      <c r="C1092" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1092" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767081933</t>
+        </is>
+      </c>
+      <c r="E1092" t="inlineStr"/>
+      <c r="F1092" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Reko189</t>
+        </is>
+      </c>
+      <c r="C1093" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1093" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767081933</t>
+        </is>
+      </c>
+      <c r="E1093" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1093" t="inlineStr"/>
+    </row>
+    <row r="1094">
+      <c r="A1094" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Reko190</t>
+        </is>
+      </c>
+      <c r="C1094" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1094" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737078797</t>
+        </is>
+      </c>
+      <c r="E1094" t="inlineStr"/>
+      <c r="F1094" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Reko190</t>
+        </is>
+      </c>
+      <c r="C1095" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1095" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737078797</t>
+        </is>
+      </c>
+      <c r="E1095" t="inlineStr"/>
+      <c r="F1095" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Reko190</t>
+        </is>
+      </c>
+      <c r="C1096" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1096" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737078797</t>
+        </is>
+      </c>
+      <c r="E1096" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1096" t="inlineStr"/>
+    </row>
+    <row r="1097">
+      <c r="A1097" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Reko191</t>
+        </is>
+      </c>
+      <c r="C1097" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1097" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768415467</t>
+        </is>
+      </c>
+      <c r="E1097" t="inlineStr"/>
+      <c r="F1097" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Reko191</t>
+        </is>
+      </c>
+      <c r="C1098" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1098" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768415467</t>
+        </is>
+      </c>
+      <c r="E1098" t="inlineStr"/>
+      <c r="F1098" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Reko191</t>
+        </is>
+      </c>
+      <c r="C1099" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1099" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768415467</t>
+        </is>
+      </c>
+      <c r="E1099" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1099" t="inlineStr"/>
+    </row>
+    <row r="1100">
+      <c r="A1100" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Reko192</t>
+        </is>
+      </c>
+      <c r="C1100" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1100" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708244846</t>
+        </is>
+      </c>
+      <c r="E1100" t="inlineStr"/>
+      <c r="F1100" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Reko192</t>
+        </is>
+      </c>
+      <c r="C1101" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1101" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708244846</t>
+        </is>
+      </c>
+      <c r="E1101" t="inlineStr"/>
+      <c r="F1101" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" s="2" t="n">
+        <v>44343</v>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Reko192</t>
+        </is>
+      </c>
+      <c r="C1102" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1102" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708244846</t>
+        </is>
+      </c>
+      <c r="E1102" t="n">
+        <v>395</v>
+      </c>
+      <c r="F1102" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 54 new rows for week ending 2021-06-06 (total 1155 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1102"/>
+  <dimension ref="A1:F1156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23241,6 +23241,1144 @@
       </c>
       <c r="F1102" t="inlineStr"/>
     </row>
+    <row r="1103">
+      <c r="A1103" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Reko193</t>
+        </is>
+      </c>
+      <c r="C1103" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1103" t="inlineStr">
+        <is>
+          <t>Reko Swish +447930169686</t>
+        </is>
+      </c>
+      <c r="E1103" t="inlineStr"/>
+      <c r="F1103" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Reko193</t>
+        </is>
+      </c>
+      <c r="C1104" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1104" t="inlineStr">
+        <is>
+          <t>Reko Swish +447930169686</t>
+        </is>
+      </c>
+      <c r="E1104" t="inlineStr"/>
+      <c r="F1104" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Reko193</t>
+        </is>
+      </c>
+      <c r="C1105" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1105" t="inlineStr">
+        <is>
+          <t>Reko Swish +447930169686</t>
+        </is>
+      </c>
+      <c r="E1105" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1105" t="inlineStr"/>
+    </row>
+    <row r="1106">
+      <c r="A1106" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>Reko194</t>
+        </is>
+      </c>
+      <c r="C1106" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1106" t="inlineStr">
+        <is>
+          <t>Reko Swish +46732447361</t>
+        </is>
+      </c>
+      <c r="E1106" t="inlineStr"/>
+      <c r="F1106" t="n">
+        <v>495.54</v>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Reko194</t>
+        </is>
+      </c>
+      <c r="C1107" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1107" t="inlineStr">
+        <is>
+          <t>Reko Swish +46732447361</t>
+        </is>
+      </c>
+      <c r="E1107" t="inlineStr"/>
+      <c r="F1107" t="n">
+        <v>59.46</v>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Reko194</t>
+        </is>
+      </c>
+      <c r="C1108" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1108" t="inlineStr">
+        <is>
+          <t>Reko Swish +46732447361</t>
+        </is>
+      </c>
+      <c r="E1108" t="n">
+        <v>555</v>
+      </c>
+      <c r="F1108" t="inlineStr"/>
+    </row>
+    <row r="1109">
+      <c r="A1109" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Reko195</t>
+        </is>
+      </c>
+      <c r="C1109" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1109" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702179776</t>
+        </is>
+      </c>
+      <c r="E1109" t="inlineStr"/>
+      <c r="F1109" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Reko195</t>
+        </is>
+      </c>
+      <c r="C1110" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1110" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702179776</t>
+        </is>
+      </c>
+      <c r="E1110" t="inlineStr"/>
+      <c r="F1110" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Reko195</t>
+        </is>
+      </c>
+      <c r="C1111" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1111" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702179776</t>
+        </is>
+      </c>
+      <c r="E1111" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1111" t="inlineStr"/>
+    </row>
+    <row r="1112">
+      <c r="A1112" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Reko196</t>
+        </is>
+      </c>
+      <c r="C1112" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1112" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707473778</t>
+        </is>
+      </c>
+      <c r="E1112" t="inlineStr"/>
+      <c r="F1112" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Reko196</t>
+        </is>
+      </c>
+      <c r="C1113" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1113" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707473778</t>
+        </is>
+      </c>
+      <c r="E1113" t="inlineStr"/>
+      <c r="F1113" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" s="2" t="n">
+        <v>44347</v>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Reko196</t>
+        </is>
+      </c>
+      <c r="C1114" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1114" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707473778</t>
+        </is>
+      </c>
+      <c r="E1114" t="n">
+        <v>474</v>
+      </c>
+      <c r="F1114" t="inlineStr"/>
+    </row>
+    <row r="1115">
+      <c r="A1115" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Reko197</t>
+        </is>
+      </c>
+      <c r="C1115" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1115" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731587473</t>
+        </is>
+      </c>
+      <c r="E1115" t="inlineStr"/>
+      <c r="F1115" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Reko197</t>
+        </is>
+      </c>
+      <c r="C1116" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1116" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731587473</t>
+        </is>
+      </c>
+      <c r="E1116" t="inlineStr"/>
+      <c r="F1116" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Reko197</t>
+        </is>
+      </c>
+      <c r="C1117" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1117" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731587473</t>
+        </is>
+      </c>
+      <c r="E1117" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1117" t="inlineStr"/>
+    </row>
+    <row r="1118">
+      <c r="A1118" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Reko198</t>
+        </is>
+      </c>
+      <c r="C1118" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1118" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1118" t="inlineStr"/>
+      <c r="F1118" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Reko198</t>
+        </is>
+      </c>
+      <c r="C1119" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1119" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1119" t="inlineStr"/>
+      <c r="F1119" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Reko198</t>
+        </is>
+      </c>
+      <c r="C1120" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1120" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1120" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1120" t="inlineStr"/>
+    </row>
+    <row r="1121">
+      <c r="A1121" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Reko199</t>
+        </is>
+      </c>
+      <c r="C1121" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1121" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739881331</t>
+        </is>
+      </c>
+      <c r="E1121" t="inlineStr"/>
+      <c r="F1121" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Reko199</t>
+        </is>
+      </c>
+      <c r="C1122" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1122" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739881331</t>
+        </is>
+      </c>
+      <c r="E1122" t="inlineStr"/>
+      <c r="F1122" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" s="2" t="n">
+        <v>44348</v>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Reko199</t>
+        </is>
+      </c>
+      <c r="C1123" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1123" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739881331</t>
+        </is>
+      </c>
+      <c r="E1123" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1123" t="inlineStr"/>
+    </row>
+    <row r="1124">
+      <c r="A1124" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Reko200</t>
+        </is>
+      </c>
+      <c r="C1124" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1124" t="inlineStr">
+        <is>
+          <t>Reko Swish +46769256976</t>
+        </is>
+      </c>
+      <c r="E1124" t="inlineStr"/>
+      <c r="F1124" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Reko200</t>
+        </is>
+      </c>
+      <c r="C1125" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1125" t="inlineStr">
+        <is>
+          <t>Reko Swish +46769256976</t>
+        </is>
+      </c>
+      <c r="E1125" t="inlineStr"/>
+      <c r="F1125" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Reko200</t>
+        </is>
+      </c>
+      <c r="C1126" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1126" t="inlineStr">
+        <is>
+          <t>Reko Swish +46769256976</t>
+        </is>
+      </c>
+      <c r="E1126" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1126" t="inlineStr"/>
+    </row>
+    <row r="1127">
+      <c r="A1127" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Reko201</t>
+        </is>
+      </c>
+      <c r="C1127" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1127" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731587473 return</t>
+        </is>
+      </c>
+      <c r="E1127" t="n">
+        <v>115.18</v>
+      </c>
+      <c r="F1127" t="inlineStr"/>
+    </row>
+    <row r="1128">
+      <c r="A1128" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Reko201</t>
+        </is>
+      </c>
+      <c r="C1128" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1128" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731587473 return</t>
+        </is>
+      </c>
+      <c r="E1128" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="F1128" t="inlineStr"/>
+    </row>
+    <row r="1129">
+      <c r="A1129" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Reko201</t>
+        </is>
+      </c>
+      <c r="C1129" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1129" t="inlineStr">
+        <is>
+          <t>Reko Swish +46731587473 return</t>
+        </is>
+      </c>
+      <c r="E1129" t="inlineStr"/>
+      <c r="F1129" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Reko202</t>
+        </is>
+      </c>
+      <c r="C1130" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1130" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735426728</t>
+        </is>
+      </c>
+      <c r="E1130" t="inlineStr"/>
+      <c r="F1130" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Reko202</t>
+        </is>
+      </c>
+      <c r="C1131" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1131" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735426728</t>
+        </is>
+      </c>
+      <c r="E1131" t="inlineStr"/>
+      <c r="F1131" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Reko202</t>
+        </is>
+      </c>
+      <c r="C1132" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1132" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735426728</t>
+        </is>
+      </c>
+      <c r="E1132" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1132" t="inlineStr"/>
+    </row>
+    <row r="1133">
+      <c r="A1133" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1133" t="inlineStr"/>
+      <c r="C1133" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1133" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1133" t="n">
+        <v>757.17</v>
+      </c>
+      <c r="F1133" t="inlineStr"/>
+    </row>
+    <row r="1134">
+      <c r="A1134" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1134" t="inlineStr"/>
+      <c r="C1134" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1134" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1134" t="n">
+        <v>189.29</v>
+      </c>
+      <c r="F1134" t="inlineStr"/>
+    </row>
+    <row r="1135">
+      <c r="A1135" s="2" t="n">
+        <v>44349</v>
+      </c>
+      <c r="B1135" t="inlineStr"/>
+      <c r="C1135" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1135" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1135" t="inlineStr"/>
+      <c r="F1135" t="n">
+        <v>946.46</v>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>3030924</t>
+        </is>
+      </c>
+      <c r="C1136" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1136" t="inlineStr">
+        <is>
+          <t>Order 3030924 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1136" t="inlineStr"/>
+      <c r="F1136" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>3030924</t>
+        </is>
+      </c>
+      <c r="C1137" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1137" t="inlineStr">
+        <is>
+          <t>Order 3030924 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1137" t="inlineStr"/>
+      <c r="F1137" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>3030924</t>
+        </is>
+      </c>
+      <c r="C1138" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1138" t="inlineStr">
+        <is>
+          <t>Order 3030924 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1138" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1138" t="inlineStr"/>
+    </row>
+    <row r="1139">
+      <c r="A1139" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Reko203</t>
+        </is>
+      </c>
+      <c r="C1139" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1139" t="inlineStr">
+        <is>
+          <t>Reko Swish +46701825067</t>
+        </is>
+      </c>
+      <c r="E1139" t="inlineStr"/>
+      <c r="F1139" t="n">
+        <v>642.86</v>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Reko203</t>
+        </is>
+      </c>
+      <c r="C1140" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1140" t="inlineStr">
+        <is>
+          <t>Reko Swish +46701825067</t>
+        </is>
+      </c>
+      <c r="E1140" t="inlineStr"/>
+      <c r="F1140" t="n">
+        <v>8.039999999999999</v>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Reko203</t>
+        </is>
+      </c>
+      <c r="C1141" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1141" t="inlineStr">
+        <is>
+          <t>Reko Swish +46701825067</t>
+        </is>
+      </c>
+      <c r="E1141" t="inlineStr"/>
+      <c r="F1141" t="n">
+        <v>77.14</v>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Reko204</t>
+        </is>
+      </c>
+      <c r="C1142" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1142" t="inlineStr">
+        <is>
+          <t>Reko Swish +46701825067</t>
+        </is>
+      </c>
+      <c r="E1142" t="inlineStr"/>
+      <c r="F1142" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Reko204</t>
+        </is>
+      </c>
+      <c r="C1143" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1143" t="inlineStr">
+        <is>
+          <t>Reko Swish +46701825067</t>
+        </is>
+      </c>
+      <c r="E1143" t="n">
+        <v>720</v>
+      </c>
+      <c r="F1143" t="inlineStr"/>
+    </row>
+    <row r="1144">
+      <c r="A1144" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Reko204</t>
+        </is>
+      </c>
+      <c r="C1144" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1144" t="inlineStr">
+        <is>
+          <t>Reko Swish +46701825067</t>
+        </is>
+      </c>
+      <c r="E1144" t="n">
+        <v>9</v>
+      </c>
+      <c r="F1144" t="inlineStr"/>
+    </row>
+    <row r="1145">
+      <c r="A1145" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Reko205</t>
+        </is>
+      </c>
+      <c r="C1145" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1145" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706395839</t>
+        </is>
+      </c>
+      <c r="E1145" t="inlineStr"/>
+      <c r="F1145" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Reko205</t>
+        </is>
+      </c>
+      <c r="C1146" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1146" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706395839</t>
+        </is>
+      </c>
+      <c r="E1146" t="inlineStr"/>
+      <c r="F1146" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Reko205</t>
+        </is>
+      </c>
+      <c r="C1147" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1147" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706395839</t>
+        </is>
+      </c>
+      <c r="E1147" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1147" t="inlineStr"/>
+    </row>
+    <row r="1148">
+      <c r="A1148" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1148" t="inlineStr"/>
+      <c r="C1148" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1148" t="inlineStr">
+        <is>
+          <t>FACEBK 62FYW4KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E1148" t="n">
+        <v>415</v>
+      </c>
+      <c r="F1148" t="inlineStr"/>
+    </row>
+    <row r="1149">
+      <c r="A1149" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1149" t="inlineStr"/>
+      <c r="C1149" t="inlineStr"/>
+      <c r="D1149" t="inlineStr">
+        <is>
+          <t>FACEBK 62FYW4KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E1149" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1149" t="inlineStr"/>
+    </row>
+    <row r="1150">
+      <c r="A1150" s="2" t="n">
+        <v>44350</v>
+      </c>
+      <c r="B1150" t="inlineStr"/>
+      <c r="C1150" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1150" t="inlineStr">
+        <is>
+          <t>FACEBK 62FYW4KZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E1150" t="inlineStr"/>
+      <c r="F1150" t="n">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" s="2" t="n">
+        <v>44351</v>
+      </c>
+      <c r="B1151" t="inlineStr"/>
+      <c r="C1151" t="n">
+        <v>6540</v>
+      </c>
+      <c r="D1151" t="inlineStr">
+        <is>
+          <t>TELIA K0135</t>
+        </is>
+      </c>
+      <c r="E1151" t="n">
+        <v>79.2</v>
+      </c>
+      <c r="F1151" t="inlineStr"/>
+    </row>
+    <row r="1152">
+      <c r="A1152" s="2" t="n">
+        <v>44351</v>
+      </c>
+      <c r="B1152" t="inlineStr"/>
+      <c r="C1152" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1152" t="inlineStr">
+        <is>
+          <t>TELIA K0135</t>
+        </is>
+      </c>
+      <c r="E1152" t="n">
+        <v>19.8</v>
+      </c>
+      <c r="F1152" t="inlineStr"/>
+    </row>
+    <row r="1153">
+      <c r="A1153" s="2" t="n">
+        <v>44351</v>
+      </c>
+      <c r="B1153" t="inlineStr"/>
+      <c r="C1153" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1153" t="inlineStr">
+        <is>
+          <t>TELIA K0135</t>
+        </is>
+      </c>
+      <c r="E1153" t="inlineStr"/>
+      <c r="F1153" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" s="2" t="n">
+        <v>44352</v>
+      </c>
+      <c r="B1154" t="inlineStr"/>
+      <c r="C1154" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D1154" t="inlineStr">
+        <is>
+          <t>CDON SE K0135</t>
+        </is>
+      </c>
+      <c r="E1154" t="n">
+        <v>10463.2</v>
+      </c>
+      <c r="F1154" t="inlineStr"/>
+    </row>
+    <row r="1155">
+      <c r="A1155" s="2" t="n">
+        <v>44352</v>
+      </c>
+      <c r="B1155" t="inlineStr"/>
+      <c r="C1155" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1155" t="inlineStr">
+        <is>
+          <t>CDON SE K0135</t>
+        </is>
+      </c>
+      <c r="E1155" t="n">
+        <v>2615.8</v>
+      </c>
+      <c r="F1155" t="inlineStr"/>
+    </row>
+    <row r="1156">
+      <c r="A1156" s="2" t="n">
+        <v>44352</v>
+      </c>
+      <c r="B1156" t="inlineStr"/>
+      <c r="C1156" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1156" t="inlineStr">
+        <is>
+          <t>CDON SE K0135</t>
+        </is>
+      </c>
+      <c r="E1156" t="inlineStr"/>
+      <c r="F1156" t="n">
+        <v>13079</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 66 new rows for week ending 2021-06-13 (total 1221 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1156"/>
+  <dimension ref="A1:F1222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24379,6 +24379,1410 @@
         <v>13079</v>
       </c>
     </row>
+    <row r="1157">
+      <c r="A1157" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Reko206</t>
+        </is>
+      </c>
+      <c r="C1157" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1157" t="inlineStr">
+        <is>
+          <t>Reko Swish +46764256008</t>
+        </is>
+      </c>
+      <c r="E1157" t="inlineStr"/>
+      <c r="F1157" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Reko206</t>
+        </is>
+      </c>
+      <c r="C1158" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1158" t="inlineStr">
+        <is>
+          <t>Reko Swish +46764256008</t>
+        </is>
+      </c>
+      <c r="E1158" t="inlineStr"/>
+      <c r="F1158" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Reko206</t>
+        </is>
+      </c>
+      <c r="C1159" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1159" t="inlineStr">
+        <is>
+          <t>Reko Swish +46764256008</t>
+        </is>
+      </c>
+      <c r="E1159" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1159" t="inlineStr"/>
+    </row>
+    <row r="1160">
+      <c r="A1160" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Reko207</t>
+        </is>
+      </c>
+      <c r="C1160" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1160" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1160" t="inlineStr"/>
+      <c r="F1160" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Reko207</t>
+        </is>
+      </c>
+      <c r="C1161" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1161" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1161" t="inlineStr"/>
+      <c r="F1161" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Reko207</t>
+        </is>
+      </c>
+      <c r="C1162" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1162" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1162" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1162" t="inlineStr"/>
+    </row>
+    <row r="1163">
+      <c r="A1163" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Reko208</t>
+        </is>
+      </c>
+      <c r="C1163" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1163" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1163" t="inlineStr"/>
+      <c r="F1163" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Reko208</t>
+        </is>
+      </c>
+      <c r="C1164" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1164" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1164" t="inlineStr"/>
+      <c r="F1164" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Reko208</t>
+        </is>
+      </c>
+      <c r="C1165" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1165" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1165" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1165" t="inlineStr"/>
+    </row>
+    <row r="1166">
+      <c r="A1166" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>Reko209</t>
+        </is>
+      </c>
+      <c r="C1166" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1166" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708363000</t>
+        </is>
+      </c>
+      <c r="E1166" t="inlineStr"/>
+      <c r="F1166" t="n">
+        <v>300.89</v>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Reko209</t>
+        </is>
+      </c>
+      <c r="C1167" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1167" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708363000</t>
+        </is>
+      </c>
+      <c r="E1167" t="inlineStr"/>
+      <c r="F1167" t="n">
+        <v>36.11</v>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Reko209</t>
+        </is>
+      </c>
+      <c r="C1168" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1168" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708363000</t>
+        </is>
+      </c>
+      <c r="E1168" t="n">
+        <v>337</v>
+      </c>
+      <c r="F1168" t="inlineStr"/>
+    </row>
+    <row r="1169">
+      <c r="A1169" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>Reko210</t>
+        </is>
+      </c>
+      <c r="C1169" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1169" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1169" t="inlineStr"/>
+      <c r="F1169" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Reko210</t>
+        </is>
+      </c>
+      <c r="C1170" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1170" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1170" t="inlineStr"/>
+      <c r="F1170" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Reko210</t>
+        </is>
+      </c>
+      <c r="C1171" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1171" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1171" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1171" t="inlineStr"/>
+    </row>
+    <row r="1172">
+      <c r="A1172" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Reko211</t>
+        </is>
+      </c>
+      <c r="C1172" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1172" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704212362</t>
+        </is>
+      </c>
+      <c r="E1172" t="inlineStr"/>
+      <c r="F1172" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Reko211</t>
+        </is>
+      </c>
+      <c r="C1173" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1173" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704212362</t>
+        </is>
+      </c>
+      <c r="E1173" t="inlineStr"/>
+      <c r="F1173" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Reko211</t>
+        </is>
+      </c>
+      <c r="C1174" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1174" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704212362</t>
+        </is>
+      </c>
+      <c r="E1174" t="n">
+        <v>316</v>
+      </c>
+      <c r="F1174" t="inlineStr"/>
+    </row>
+    <row r="1175">
+      <c r="A1175" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Reko212</t>
+        </is>
+      </c>
+      <c r="C1175" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1175" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1175" t="inlineStr"/>
+      <c r="F1175" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Reko212</t>
+        </is>
+      </c>
+      <c r="C1176" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1176" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1176" t="inlineStr"/>
+      <c r="F1176" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>Reko212</t>
+        </is>
+      </c>
+      <c r="C1177" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1177" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1177" t="n">
+        <v>645</v>
+      </c>
+      <c r="F1177" t="inlineStr"/>
+    </row>
+    <row r="1178">
+      <c r="A1178" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Reko213</t>
+        </is>
+      </c>
+      <c r="C1178" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1178" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702129177</t>
+        </is>
+      </c>
+      <c r="E1178" t="inlineStr"/>
+      <c r="F1178" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Reko213</t>
+        </is>
+      </c>
+      <c r="C1179" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702129177</t>
+        </is>
+      </c>
+      <c r="E1179" t="inlineStr"/>
+      <c r="F1179" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Reko213</t>
+        </is>
+      </c>
+      <c r="C1180" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1180" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702129177</t>
+        </is>
+      </c>
+      <c r="E1180" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1180" t="inlineStr"/>
+    </row>
+    <row r="1181">
+      <c r="A1181" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>Reko214</t>
+        </is>
+      </c>
+      <c r="C1181" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1181" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1181" t="inlineStr"/>
+      <c r="F1181" t="n">
+        <v>371.43</v>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Reko214</t>
+        </is>
+      </c>
+      <c r="C1182" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1182" t="inlineStr"/>
+      <c r="F1182" t="n">
+        <v>44.57</v>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Reko214</t>
+        </is>
+      </c>
+      <c r="C1183" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1183" t="n">
+        <v>416</v>
+      </c>
+      <c r="F1183" t="inlineStr"/>
+    </row>
+    <row r="1184">
+      <c r="A1184" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Reko215</t>
+        </is>
+      </c>
+      <c r="C1184" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739658007</t>
+        </is>
+      </c>
+      <c r="E1184" t="inlineStr"/>
+      <c r="F1184" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>Reko215</t>
+        </is>
+      </c>
+      <c r="C1185" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739658007</t>
+        </is>
+      </c>
+      <c r="E1185" t="inlineStr"/>
+      <c r="F1185" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Reko215</t>
+        </is>
+      </c>
+      <c r="C1186" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739658007</t>
+        </is>
+      </c>
+      <c r="E1186" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1186" t="inlineStr"/>
+    </row>
+    <row r="1187">
+      <c r="A1187" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Reko216</t>
+        </is>
+      </c>
+      <c r="C1187" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>Reko Swish +46764256008 Return</t>
+        </is>
+      </c>
+      <c r="E1187" t="n">
+        <v>115.18</v>
+      </c>
+      <c r="F1187" t="inlineStr"/>
+    </row>
+    <row r="1188">
+      <c r="A1188" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Reko216</t>
+        </is>
+      </c>
+      <c r="C1188" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>Reko Swish +46764256008 Return</t>
+        </is>
+      </c>
+      <c r="E1188" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="F1188" t="inlineStr"/>
+    </row>
+    <row r="1189">
+      <c r="A1189" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Reko216</t>
+        </is>
+      </c>
+      <c r="C1189" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>Reko Swish +46764256008 Return</t>
+        </is>
+      </c>
+      <c r="E1189" t="inlineStr"/>
+      <c r="F1189" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Reko217</t>
+        </is>
+      </c>
+      <c r="C1190" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E1190" t="inlineStr"/>
+      <c r="F1190" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Reko217</t>
+        </is>
+      </c>
+      <c r="C1191" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1191" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E1191" t="inlineStr"/>
+      <c r="F1191" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Reko217</t>
+        </is>
+      </c>
+      <c r="C1192" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1192" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E1192" t="n">
+        <v>395</v>
+      </c>
+      <c r="F1192" t="inlineStr"/>
+    </row>
+    <row r="1193">
+      <c r="A1193" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Reko218</t>
+        </is>
+      </c>
+      <c r="C1193" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1193" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707364050</t>
+        </is>
+      </c>
+      <c r="E1193" t="inlineStr"/>
+      <c r="F1193" t="n">
+        <v>300.89</v>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Reko218</t>
+        </is>
+      </c>
+      <c r="C1194" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1194" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707364050</t>
+        </is>
+      </c>
+      <c r="E1194" t="inlineStr"/>
+      <c r="F1194" t="n">
+        <v>36.11</v>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Reko218</t>
+        </is>
+      </c>
+      <c r="C1195" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1195" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707364050</t>
+        </is>
+      </c>
+      <c r="E1195" t="n">
+        <v>337</v>
+      </c>
+      <c r="F1195" t="inlineStr"/>
+    </row>
+    <row r="1196">
+      <c r="A1196" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1196" t="inlineStr"/>
+      <c r="C1196" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1196" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1196" t="n">
+        <v>980.66</v>
+      </c>
+      <c r="F1196" t="inlineStr"/>
+    </row>
+    <row r="1197">
+      <c r="A1197" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1197" t="inlineStr"/>
+      <c r="C1197" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1197" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1197" t="n">
+        <v>117.68</v>
+      </c>
+      <c r="F1197" t="inlineStr"/>
+    </row>
+    <row r="1198">
+      <c r="A1198" s="2" t="n">
+        <v>44354</v>
+      </c>
+      <c r="B1198" t="inlineStr"/>
+      <c r="C1198" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1198" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1198" t="inlineStr"/>
+      <c r="F1198" t="n">
+        <v>1098.34</v>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Reko219</t>
+        </is>
+      </c>
+      <c r="C1199" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708511401</t>
+        </is>
+      </c>
+      <c r="E1199" t="inlineStr"/>
+      <c r="F1199" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Reko219</t>
+        </is>
+      </c>
+      <c r="C1200" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708511401</t>
+        </is>
+      </c>
+      <c r="E1200" t="inlineStr"/>
+      <c r="F1200" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Reko219</t>
+        </is>
+      </c>
+      <c r="C1201" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1201" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708511401</t>
+        </is>
+      </c>
+      <c r="E1201" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1201" t="inlineStr"/>
+    </row>
+    <row r="1202">
+      <c r="A1202" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Reko220</t>
+        </is>
+      </c>
+      <c r="C1202" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1202" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708827848</t>
+        </is>
+      </c>
+      <c r="E1202" t="inlineStr"/>
+      <c r="F1202" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Reko220</t>
+        </is>
+      </c>
+      <c r="C1203" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1203" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708827848</t>
+        </is>
+      </c>
+      <c r="E1203" t="inlineStr"/>
+      <c r="F1203" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Reko220</t>
+        </is>
+      </c>
+      <c r="C1204" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1204" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708827848</t>
+        </is>
+      </c>
+      <c r="E1204" t="n">
+        <v>316</v>
+      </c>
+      <c r="F1204" t="inlineStr"/>
+    </row>
+    <row r="1205">
+      <c r="A1205" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Reko221</t>
+        </is>
+      </c>
+      <c r="C1205" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1205" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708217045</t>
+        </is>
+      </c>
+      <c r="E1205" t="inlineStr"/>
+      <c r="F1205" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Reko221</t>
+        </is>
+      </c>
+      <c r="C1206" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1206" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708217045</t>
+        </is>
+      </c>
+      <c r="E1206" t="inlineStr"/>
+      <c r="F1206" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" s="2" t="n">
+        <v>44355</v>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Reko221</t>
+        </is>
+      </c>
+      <c r="C1207" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1207" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708217045</t>
+        </is>
+      </c>
+      <c r="E1207" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1207" t="inlineStr"/>
+    </row>
+    <row r="1208">
+      <c r="A1208" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Reko222</t>
+        </is>
+      </c>
+      <c r="C1208" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1208" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E1208" t="inlineStr"/>
+      <c r="F1208" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Reko222</t>
+        </is>
+      </c>
+      <c r="C1209" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E1209" t="inlineStr"/>
+      <c r="F1209" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Reko222</t>
+        </is>
+      </c>
+      <c r="C1210" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1210" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730929992</t>
+        </is>
+      </c>
+      <c r="E1210" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1210" t="inlineStr"/>
+    </row>
+    <row r="1211">
+      <c r="A1211" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Reko223</t>
+        </is>
+      </c>
+      <c r="C1211" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1211" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E1211" t="inlineStr"/>
+      <c r="F1211" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Reko223</t>
+        </is>
+      </c>
+      <c r="C1212" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1212" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E1212" t="inlineStr"/>
+      <c r="F1212" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Reko223</t>
+        </is>
+      </c>
+      <c r="C1213" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1213" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707157329</t>
+        </is>
+      </c>
+      <c r="E1213" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1213" t="inlineStr"/>
+    </row>
+    <row r="1214">
+      <c r="A1214" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1214" t="inlineStr"/>
+      <c r="C1214" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1214" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1214" t="n">
+        <v>511.2</v>
+      </c>
+      <c r="F1214" t="inlineStr"/>
+    </row>
+    <row r="1215">
+      <c r="A1215" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1215" t="inlineStr"/>
+      <c r="C1215" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1215" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1215" t="n">
+        <v>61.34</v>
+      </c>
+      <c r="F1215" t="inlineStr"/>
+    </row>
+    <row r="1216">
+      <c r="A1216" s="2" t="n">
+        <v>44356</v>
+      </c>
+      <c r="B1216" t="inlineStr"/>
+      <c r="C1216" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1216" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1216" t="inlineStr"/>
+      <c r="F1216" t="n">
+        <v>572.54</v>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" s="2" t="n">
+        <v>44358</v>
+      </c>
+      <c r="B1217" t="inlineStr"/>
+      <c r="C1217" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1217" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1217" t="n">
+        <v>889</v>
+      </c>
+      <c r="F1217" t="inlineStr"/>
+    </row>
+    <row r="1218">
+      <c r="A1218" s="2" t="n">
+        <v>44358</v>
+      </c>
+      <c r="B1218" t="inlineStr"/>
+      <c r="C1218" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1218" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1218" t="n">
+        <v>106.68</v>
+      </c>
+      <c r="F1218" t="inlineStr"/>
+    </row>
+    <row r="1219">
+      <c r="A1219" s="2" t="n">
+        <v>44358</v>
+      </c>
+      <c r="B1219" t="inlineStr"/>
+      <c r="C1219" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1219" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1219" t="inlineStr"/>
+      <c r="F1219" t="n">
+        <v>995.6799999999999</v>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" s="2" t="n">
+        <v>44360</v>
+      </c>
+      <c r="B1220" t="inlineStr"/>
+      <c r="C1220" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1220" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1220" t="n">
+        <v>832.64</v>
+      </c>
+      <c r="F1220" t="inlineStr"/>
+    </row>
+    <row r="1221">
+      <c r="A1221" s="2" t="n">
+        <v>44360</v>
+      </c>
+      <c r="B1221" t="inlineStr"/>
+      <c r="C1221" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1221" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1221" t="n">
+        <v>99.92</v>
+      </c>
+      <c r="F1221" t="inlineStr"/>
+    </row>
+    <row r="1222">
+      <c r="A1222" s="2" t="n">
+        <v>44360</v>
+      </c>
+      <c r="B1222" t="inlineStr"/>
+      <c r="C1222" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1222" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1222" t="inlineStr"/>
+      <c r="F1222" t="n">
+        <v>932.5599999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 45 new rows for week ending 2021-06-20 (total 1266 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1222"/>
+  <dimension ref="A1:F1267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25783,6 +25783,948 @@
         <v>932.5599999999999</v>
       </c>
     </row>
+    <row r="1223">
+      <c r="A1223" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Reko224</t>
+        </is>
+      </c>
+      <c r="C1223" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1223" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448</t>
+        </is>
+      </c>
+      <c r="E1223" t="inlineStr"/>
+      <c r="F1223" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>Reko224</t>
+        </is>
+      </c>
+      <c r="C1224" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1224" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448</t>
+        </is>
+      </c>
+      <c r="E1224" t="inlineStr"/>
+      <c r="F1224" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Reko224</t>
+        </is>
+      </c>
+      <c r="C1225" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1225" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448</t>
+        </is>
+      </c>
+      <c r="E1225" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1225" t="inlineStr"/>
+    </row>
+    <row r="1226">
+      <c r="A1226" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>Reko225</t>
+        </is>
+      </c>
+      <c r="C1226" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1226" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739806822</t>
+        </is>
+      </c>
+      <c r="E1226" t="inlineStr"/>
+      <c r="F1226" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Reko225</t>
+        </is>
+      </c>
+      <c r="C1227" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1227" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739806822</t>
+        </is>
+      </c>
+      <c r="E1227" t="inlineStr"/>
+      <c r="F1227" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Reko225</t>
+        </is>
+      </c>
+      <c r="C1228" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1228" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739806822</t>
+        </is>
+      </c>
+      <c r="E1228" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1228" t="inlineStr"/>
+    </row>
+    <row r="1229">
+      <c r="A1229" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Reko226</t>
+        </is>
+      </c>
+      <c r="C1229" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1229" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709334300</t>
+        </is>
+      </c>
+      <c r="E1229" t="inlineStr"/>
+      <c r="F1229" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Reko226</t>
+        </is>
+      </c>
+      <c r="C1230" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1230" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709334300</t>
+        </is>
+      </c>
+      <c r="E1230" t="inlineStr"/>
+      <c r="F1230" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Reko226</t>
+        </is>
+      </c>
+      <c r="C1231" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1231" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709334300</t>
+        </is>
+      </c>
+      <c r="E1231" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1231" t="inlineStr"/>
+    </row>
+    <row r="1232">
+      <c r="A1232" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Reko227</t>
+        </is>
+      </c>
+      <c r="C1232" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1232" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E1232" t="inlineStr"/>
+      <c r="F1232" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Reko227</t>
+        </is>
+      </c>
+      <c r="C1233" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1233" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E1233" t="inlineStr"/>
+      <c r="F1233" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" s="2" t="n">
+        <v>44361</v>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Reko227</t>
+        </is>
+      </c>
+      <c r="C1234" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1234" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E1234" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1234" t="inlineStr"/>
+    </row>
+    <row r="1235">
+      <c r="A1235" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>3151843</t>
+        </is>
+      </c>
+      <c r="C1235" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1235" t="inlineStr">
+        <is>
+          <t>Order 3151843 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1235" t="inlineStr"/>
+      <c r="F1235" t="n">
+        <v>1912.5</v>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>3151843</t>
+        </is>
+      </c>
+      <c r="C1236" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1236" t="inlineStr">
+        <is>
+          <t>Order 3151843 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1236" t="inlineStr"/>
+      <c r="F1236" t="n">
+        <v>229.5</v>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>3151843</t>
+        </is>
+      </c>
+      <c r="C1237" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1237" t="inlineStr">
+        <is>
+          <t>Order 3151843 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1237" t="n">
+        <v>2142</v>
+      </c>
+      <c r="F1237" t="inlineStr"/>
+    </row>
+    <row r="1238">
+      <c r="A1238" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Reko228</t>
+        </is>
+      </c>
+      <c r="C1238" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1238" t="inlineStr">
+        <is>
+          <t>Reko Swish +46762568457</t>
+        </is>
+      </c>
+      <c r="E1238" t="inlineStr"/>
+      <c r="F1238" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Reko228</t>
+        </is>
+      </c>
+      <c r="C1239" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1239" t="inlineStr">
+        <is>
+          <t>Reko Swish +46762568457</t>
+        </is>
+      </c>
+      <c r="E1239" t="inlineStr"/>
+      <c r="F1239" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>Reko228</t>
+        </is>
+      </c>
+      <c r="C1240" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1240" t="inlineStr">
+        <is>
+          <t>Reko Swish +46762568457</t>
+        </is>
+      </c>
+      <c r="E1240" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1240" t="inlineStr"/>
+    </row>
+    <row r="1241">
+      <c r="A1241" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1241" t="inlineStr"/>
+      <c r="C1241" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1241" t="inlineStr">
+        <is>
+          <t>TINGSTAD PAPPER</t>
+        </is>
+      </c>
+      <c r="E1241" t="n">
+        <v>4156.8</v>
+      </c>
+      <c r="F1241" t="inlineStr"/>
+    </row>
+    <row r="1242">
+      <c r="A1242" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1242" t="inlineStr"/>
+      <c r="C1242" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1242" t="inlineStr">
+        <is>
+          <t>TINGSTAD PAPPER</t>
+        </is>
+      </c>
+      <c r="E1242" t="n">
+        <v>1039.2</v>
+      </c>
+      <c r="F1242" t="inlineStr"/>
+    </row>
+    <row r="1243">
+      <c r="A1243" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1243" t="inlineStr"/>
+      <c r="C1243" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1243" t="inlineStr">
+        <is>
+          <t>TINGSTAD PAPPER</t>
+        </is>
+      </c>
+      <c r="E1243" t="inlineStr"/>
+      <c r="F1243" t="n">
+        <v>5196</v>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1244" t="inlineStr"/>
+      <c r="C1244" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1244" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1244" t="n">
+        <v>317.2</v>
+      </c>
+      <c r="F1244" t="inlineStr"/>
+    </row>
+    <row r="1245">
+      <c r="A1245" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1245" t="inlineStr"/>
+      <c r="C1245" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1245" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1245" t="n">
+        <v>38.06</v>
+      </c>
+      <c r="F1245" t="inlineStr"/>
+    </row>
+    <row r="1246">
+      <c r="A1246" s="2" t="n">
+        <v>44362</v>
+      </c>
+      <c r="B1246" t="inlineStr"/>
+      <c r="C1246" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1246" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1246" t="inlineStr"/>
+      <c r="F1246" t="n">
+        <v>355.26</v>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Reko229</t>
+        </is>
+      </c>
+      <c r="C1247" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1247" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448 Return</t>
+        </is>
+      </c>
+      <c r="E1247" t="n">
+        <v>44.64</v>
+      </c>
+      <c r="F1247" t="inlineStr"/>
+    </row>
+    <row r="1248">
+      <c r="A1248" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Reko229</t>
+        </is>
+      </c>
+      <c r="C1248" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1248" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448 Return</t>
+        </is>
+      </c>
+      <c r="E1248" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="F1248" t="inlineStr"/>
+    </row>
+    <row r="1249">
+      <c r="A1249" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Reko229</t>
+        </is>
+      </c>
+      <c r="C1249" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1249" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704564448 Return</t>
+        </is>
+      </c>
+      <c r="E1249" t="inlineStr"/>
+      <c r="F1249" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Reko230</t>
+        </is>
+      </c>
+      <c r="C1250" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1250" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1250" t="inlineStr"/>
+      <c r="F1250" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>Reko230</t>
+        </is>
+      </c>
+      <c r="C1251" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1251" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1251" t="inlineStr"/>
+      <c r="F1251" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" s="2" t="n">
+        <v>44363</v>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>Reko230</t>
+        </is>
+      </c>
+      <c r="C1252" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1252" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1252" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1252" t="inlineStr"/>
+    </row>
+    <row r="1253">
+      <c r="A1253" s="2" t="n">
+        <v>44364</v>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>0172055</t>
+        </is>
+      </c>
+      <c r="C1253" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1253" t="inlineStr">
+        <is>
+          <t>Order 0172055 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1253" t="inlineStr"/>
+      <c r="F1253" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" s="2" t="n">
+        <v>44364</v>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>0172055</t>
+        </is>
+      </c>
+      <c r="C1254" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1254" t="inlineStr">
+        <is>
+          <t>Order 0172055 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1254" t="inlineStr"/>
+      <c r="F1254" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" s="2" t="n">
+        <v>44364</v>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>0172055</t>
+        </is>
+      </c>
+      <c r="C1255" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1255" t="inlineStr">
+        <is>
+          <t>Order 0172055 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1255" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1255" t="inlineStr"/>
+    </row>
+    <row r="1256">
+      <c r="A1256" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Reko231</t>
+        </is>
+      </c>
+      <c r="C1256" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1256" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706183071</t>
+        </is>
+      </c>
+      <c r="E1256" t="inlineStr"/>
+      <c r="F1256" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Reko231</t>
+        </is>
+      </c>
+      <c r="C1257" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1257" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706183071</t>
+        </is>
+      </c>
+      <c r="E1257" t="inlineStr"/>
+      <c r="F1257" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Reko231</t>
+        </is>
+      </c>
+      <c r="C1258" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706183071</t>
+        </is>
+      </c>
+      <c r="E1258" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1258" t="inlineStr"/>
+    </row>
+    <row r="1259">
+      <c r="A1259" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Reko232</t>
+        </is>
+      </c>
+      <c r="C1259" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722208030</t>
+        </is>
+      </c>
+      <c r="E1259" t="inlineStr"/>
+      <c r="F1259" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Reko232</t>
+        </is>
+      </c>
+      <c r="C1260" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1260" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722208030</t>
+        </is>
+      </c>
+      <c r="E1260" t="inlineStr"/>
+      <c r="F1260" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Reko232</t>
+        </is>
+      </c>
+      <c r="C1261" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1261" t="inlineStr">
+        <is>
+          <t>Reko Swish +46722208030</t>
+        </is>
+      </c>
+      <c r="E1261" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1261" t="inlineStr"/>
+    </row>
+    <row r="1262">
+      <c r="A1262" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1262" t="inlineStr"/>
+      <c r="C1262" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1262" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1262" t="n">
+        <v>841.16</v>
+      </c>
+      <c r="F1262" t="inlineStr"/>
+    </row>
+    <row r="1263">
+      <c r="A1263" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1263" t="inlineStr"/>
+      <c r="C1263" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1263" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1263" t="n">
+        <v>210.29</v>
+      </c>
+      <c r="F1263" t="inlineStr"/>
+    </row>
+    <row r="1264">
+      <c r="A1264" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1264" t="inlineStr"/>
+      <c r="C1264" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1264" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1264" t="inlineStr"/>
+      <c r="F1264" t="n">
+        <v>1051.45</v>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1265" t="inlineStr"/>
+      <c r="C1265" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1265" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1265" t="n">
+        <v>529.4</v>
+      </c>
+      <c r="F1265" t="inlineStr"/>
+    </row>
+    <row r="1266">
+      <c r="A1266" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1266" t="inlineStr"/>
+      <c r="C1266" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1266" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1266" t="n">
+        <v>63.53</v>
+      </c>
+      <c r="F1266" t="inlineStr"/>
+    </row>
+    <row r="1267">
+      <c r="A1267" s="2" t="n">
+        <v>44365</v>
+      </c>
+      <c r="B1267" t="inlineStr"/>
+      <c r="C1267" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1267" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1267" t="inlineStr"/>
+      <c r="F1267" t="n">
+        <v>592.9299999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 63 new rows for week ending 2021-06-27 (total 1329 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1267"/>
+  <dimension ref="A1:F1330"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26725,6 +26725,1352 @@
         <v>592.9299999999999</v>
       </c>
     </row>
+    <row r="1268">
+      <c r="A1268" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1268" t="inlineStr"/>
+      <c r="C1268" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D1268" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1268" t="n">
+        <v>97.5</v>
+      </c>
+      <c r="F1268" t="inlineStr"/>
+    </row>
+    <row r="1269">
+      <c r="A1269" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1269" t="inlineStr"/>
+      <c r="C1269" t="inlineStr"/>
+      <c r="D1269" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1269" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1269" t="inlineStr"/>
+    </row>
+    <row r="1270">
+      <c r="A1270" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1270" t="inlineStr"/>
+      <c r="C1270" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1270" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1270" t="inlineStr"/>
+      <c r="F1270" t="n">
+        <v>97.5</v>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Reko233</t>
+        </is>
+      </c>
+      <c r="C1271" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1271" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1271" t="inlineStr"/>
+      <c r="F1271" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Reko233</t>
+        </is>
+      </c>
+      <c r="C1272" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1272" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1272" t="inlineStr"/>
+      <c r="F1272" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Reko233</t>
+        </is>
+      </c>
+      <c r="C1273" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1273" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1273" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1273" t="inlineStr"/>
+    </row>
+    <row r="1274">
+      <c r="A1274" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Reko234</t>
+        </is>
+      </c>
+      <c r="C1274" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709696209</t>
+        </is>
+      </c>
+      <c r="E1274" t="inlineStr"/>
+      <c r="F1274" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Reko234</t>
+        </is>
+      </c>
+      <c r="C1275" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1275" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709696209</t>
+        </is>
+      </c>
+      <c r="E1275" t="inlineStr"/>
+      <c r="F1275" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Reko234</t>
+        </is>
+      </c>
+      <c r="C1276" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1276" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709696209</t>
+        </is>
+      </c>
+      <c r="E1276" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1276" t="inlineStr"/>
+    </row>
+    <row r="1277">
+      <c r="A1277" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Reko235</t>
+        </is>
+      </c>
+      <c r="C1277" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1277" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737812422</t>
+        </is>
+      </c>
+      <c r="E1277" t="inlineStr"/>
+      <c r="F1277" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Reko235</t>
+        </is>
+      </c>
+      <c r="C1278" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1278" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737812422</t>
+        </is>
+      </c>
+      <c r="E1278" t="inlineStr"/>
+      <c r="F1278" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Reko235</t>
+        </is>
+      </c>
+      <c r="C1279" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737812422</t>
+        </is>
+      </c>
+      <c r="E1279" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1279" t="inlineStr"/>
+    </row>
+    <row r="1280">
+      <c r="A1280" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Reko236</t>
+        </is>
+      </c>
+      <c r="C1280" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1280" t="inlineStr"/>
+      <c r="F1280" t="n">
+        <v>742.86</v>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Reko236</t>
+        </is>
+      </c>
+      <c r="C1281" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1281" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1281" t="inlineStr"/>
+      <c r="F1281" t="n">
+        <v>89.14</v>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Reko236</t>
+        </is>
+      </c>
+      <c r="C1282" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1282" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1282" t="n">
+        <v>832</v>
+      </c>
+      <c r="F1282" t="inlineStr"/>
+    </row>
+    <row r="1283">
+      <c r="A1283" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Reko237</t>
+        </is>
+      </c>
+      <c r="C1283" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1283" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704105733</t>
+        </is>
+      </c>
+      <c r="E1283" t="inlineStr"/>
+      <c r="F1283" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Reko237</t>
+        </is>
+      </c>
+      <c r="C1284" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1284" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704105733</t>
+        </is>
+      </c>
+      <c r="E1284" t="inlineStr"/>
+      <c r="F1284" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" s="2" t="n">
+        <v>44368</v>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Reko237</t>
+        </is>
+      </c>
+      <c r="C1285" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1285" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704105733</t>
+        </is>
+      </c>
+      <c r="E1285" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1285" t="inlineStr"/>
+    </row>
+    <row r="1286">
+      <c r="A1286" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>Reko238</t>
+        </is>
+      </c>
+      <c r="C1286" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1286" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767137127</t>
+        </is>
+      </c>
+      <c r="E1286" t="inlineStr"/>
+      <c r="F1286" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Reko238</t>
+        </is>
+      </c>
+      <c r="C1287" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1287" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767137127</t>
+        </is>
+      </c>
+      <c r="E1287" t="inlineStr"/>
+      <c r="F1287" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Reko238</t>
+        </is>
+      </c>
+      <c r="C1288" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1288" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767137127</t>
+        </is>
+      </c>
+      <c r="E1288" t="n">
+        <v>774</v>
+      </c>
+      <c r="F1288" t="inlineStr"/>
+    </row>
+    <row r="1289">
+      <c r="A1289" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Reko239</t>
+        </is>
+      </c>
+      <c r="C1289" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1289" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702174945</t>
+        </is>
+      </c>
+      <c r="E1289" t="inlineStr"/>
+      <c r="F1289" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Reko239</t>
+        </is>
+      </c>
+      <c r="C1290" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1290" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702174945</t>
+        </is>
+      </c>
+      <c r="E1290" t="inlineStr"/>
+      <c r="F1290" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Reko239</t>
+        </is>
+      </c>
+      <c r="C1291" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1291" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702174945</t>
+        </is>
+      </c>
+      <c r="E1291" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1291" t="inlineStr"/>
+    </row>
+    <row r="1292">
+      <c r="A1292" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Reko240</t>
+        </is>
+      </c>
+      <c r="C1292" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1292" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1292" t="inlineStr"/>
+      <c r="F1292" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Reko240</t>
+        </is>
+      </c>
+      <c r="C1293" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1293" t="inlineStr"/>
+      <c r="F1293" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Reko240</t>
+        </is>
+      </c>
+      <c r="C1294" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1294" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1294" t="inlineStr"/>
+    </row>
+    <row r="1295">
+      <c r="A1295" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Reko241</t>
+        </is>
+      </c>
+      <c r="C1295" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1295" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702453366</t>
+        </is>
+      </c>
+      <c r="E1295" t="inlineStr"/>
+      <c r="F1295" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Reko241</t>
+        </is>
+      </c>
+      <c r="C1296" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1296" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702453366</t>
+        </is>
+      </c>
+      <c r="E1296" t="inlineStr"/>
+      <c r="F1296" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Reko241</t>
+        </is>
+      </c>
+      <c r="C1297" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1297" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702453366</t>
+        </is>
+      </c>
+      <c r="E1297" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1297" t="inlineStr"/>
+    </row>
+    <row r="1298">
+      <c r="A1298" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Reko242</t>
+        </is>
+      </c>
+      <c r="C1298" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1298" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761170330</t>
+        </is>
+      </c>
+      <c r="E1298" t="inlineStr"/>
+      <c r="F1298" t="n">
+        <v>34.82</v>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Reko242</t>
+        </is>
+      </c>
+      <c r="C1299" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1299" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761170330</t>
+        </is>
+      </c>
+      <c r="E1299" t="inlineStr"/>
+      <c r="F1299" t="n">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Reko242</t>
+        </is>
+      </c>
+      <c r="C1300" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1300" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761170330</t>
+        </is>
+      </c>
+      <c r="E1300" t="n">
+        <v>39</v>
+      </c>
+      <c r="F1300" t="inlineStr"/>
+    </row>
+    <row r="1301">
+      <c r="A1301" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Reko243</t>
+        </is>
+      </c>
+      <c r="C1301" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1301" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E1301" t="inlineStr"/>
+      <c r="F1301" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Reko243</t>
+        </is>
+      </c>
+      <c r="C1302" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1302" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E1302" t="inlineStr"/>
+      <c r="F1302" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Reko243</t>
+        </is>
+      </c>
+      <c r="C1303" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1303" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761910051</t>
+        </is>
+      </c>
+      <c r="E1303" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1303" t="inlineStr"/>
+    </row>
+    <row r="1304">
+      <c r="A1304" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Reko244</t>
+        </is>
+      </c>
+      <c r="C1304" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768674881</t>
+        </is>
+      </c>
+      <c r="E1304" t="inlineStr"/>
+      <c r="F1304" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Reko244</t>
+        </is>
+      </c>
+      <c r="C1305" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768674881</t>
+        </is>
+      </c>
+      <c r="E1305" t="inlineStr"/>
+      <c r="F1305" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Reko244</t>
+        </is>
+      </c>
+      <c r="C1306" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768674881</t>
+        </is>
+      </c>
+      <c r="E1306" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1306" t="inlineStr"/>
+    </row>
+    <row r="1307">
+      <c r="A1307" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Reko245</t>
+        </is>
+      </c>
+      <c r="C1307" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734029350</t>
+        </is>
+      </c>
+      <c r="E1307" t="inlineStr"/>
+      <c r="F1307" t="n">
+        <v>25.89</v>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Reko245</t>
+        </is>
+      </c>
+      <c r="C1308" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734029350</t>
+        </is>
+      </c>
+      <c r="E1308" t="inlineStr"/>
+      <c r="F1308" t="n">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Reko245</t>
+        </is>
+      </c>
+      <c r="C1309" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>Reko Swish +46734029350</t>
+        </is>
+      </c>
+      <c r="E1309" t="n">
+        <v>29</v>
+      </c>
+      <c r="F1309" t="inlineStr"/>
+    </row>
+    <row r="1310">
+      <c r="A1310" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Reko246</t>
+        </is>
+      </c>
+      <c r="C1310" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705832242</t>
+        </is>
+      </c>
+      <c r="E1310" t="inlineStr"/>
+      <c r="F1310" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Reko246</t>
+        </is>
+      </c>
+      <c r="C1311" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705832242</t>
+        </is>
+      </c>
+      <c r="E1311" t="inlineStr"/>
+      <c r="F1311" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Reko246</t>
+        </is>
+      </c>
+      <c r="C1312" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1312" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705832242</t>
+        </is>
+      </c>
+      <c r="E1312" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1312" t="inlineStr"/>
+    </row>
+    <row r="1313">
+      <c r="A1313" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Reko247</t>
+        </is>
+      </c>
+      <c r="C1313" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1313" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736699903</t>
+        </is>
+      </c>
+      <c r="E1313" t="inlineStr"/>
+      <c r="F1313" t="n">
+        <v>397.32</v>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Reko247</t>
+        </is>
+      </c>
+      <c r="C1314" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1314" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736699903</t>
+        </is>
+      </c>
+      <c r="E1314" t="inlineStr"/>
+      <c r="F1314" t="n">
+        <v>47.68</v>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Reko247</t>
+        </is>
+      </c>
+      <c r="C1315" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1315" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736699903</t>
+        </is>
+      </c>
+      <c r="E1315" t="n">
+        <v>445</v>
+      </c>
+      <c r="F1315" t="inlineStr"/>
+    </row>
+    <row r="1316">
+      <c r="A1316" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Reko248</t>
+        </is>
+      </c>
+      <c r="C1316" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1316" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737080200</t>
+        </is>
+      </c>
+      <c r="E1316" t="inlineStr"/>
+      <c r="F1316" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Reko248</t>
+        </is>
+      </c>
+      <c r="C1317" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1317" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737080200</t>
+        </is>
+      </c>
+      <c r="E1317" t="inlineStr"/>
+      <c r="F1317" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Reko248</t>
+        </is>
+      </c>
+      <c r="C1318" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1318" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737080200</t>
+        </is>
+      </c>
+      <c r="E1318" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1318" t="inlineStr"/>
+    </row>
+    <row r="1319">
+      <c r="A1319" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Reko249</t>
+        </is>
+      </c>
+      <c r="C1319" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1319" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768674881 Return</t>
+        </is>
+      </c>
+      <c r="E1319" t="n">
+        <v>8.93</v>
+      </c>
+      <c r="F1319" t="inlineStr"/>
+    </row>
+    <row r="1320">
+      <c r="A1320" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Reko249</t>
+        </is>
+      </c>
+      <c r="C1320" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1320" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768674881 Return</t>
+        </is>
+      </c>
+      <c r="E1320" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="F1320" t="inlineStr"/>
+    </row>
+    <row r="1321">
+      <c r="A1321" s="2" t="n">
+        <v>44369</v>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Reko249</t>
+        </is>
+      </c>
+      <c r="C1321" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1321" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768674881 Return</t>
+        </is>
+      </c>
+      <c r="E1321" t="inlineStr"/>
+      <c r="F1321" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" s="2" t="n">
+        <v>44370</v>
+      </c>
+      <c r="B1322" t="inlineStr"/>
+      <c r="C1322" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D1322" t="inlineStr">
+        <is>
+          <t>Jun hyra</t>
+        </is>
+      </c>
+      <c r="E1322" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F1322" t="inlineStr"/>
+    </row>
+    <row r="1323">
+      <c r="A1323" s="2" t="n">
+        <v>44370</v>
+      </c>
+      <c r="B1323" t="inlineStr"/>
+      <c r="C1323" t="inlineStr"/>
+      <c r="D1323" t="inlineStr">
+        <is>
+          <t>Jun hyra</t>
+        </is>
+      </c>
+      <c r="E1323" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1323" t="inlineStr"/>
+    </row>
+    <row r="1324">
+      <c r="A1324" s="2" t="n">
+        <v>44370</v>
+      </c>
+      <c r="B1324" t="inlineStr"/>
+      <c r="C1324" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1324" t="inlineStr">
+        <is>
+          <t>Jun hyra</t>
+        </is>
+      </c>
+      <c r="E1324" t="inlineStr"/>
+      <c r="F1324" t="n">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B1325" t="inlineStr"/>
+      <c r="C1325" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1325" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1325" t="n">
+        <v>334.82</v>
+      </c>
+      <c r="F1325" t="inlineStr"/>
+    </row>
+    <row r="1326">
+      <c r="A1326" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B1326" t="inlineStr"/>
+      <c r="C1326" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1326" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1326" t="n">
+        <v>40.18</v>
+      </c>
+      <c r="F1326" t="inlineStr"/>
+    </row>
+    <row r="1327">
+      <c r="A1327" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B1327" t="inlineStr"/>
+      <c r="C1327" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1327" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1327" t="inlineStr"/>
+      <c r="F1327" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>2261137</t>
+        </is>
+      </c>
+      <c r="C1328" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1328" t="inlineStr">
+        <is>
+          <t>Order 2261137 Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1328" t="inlineStr"/>
+      <c r="F1328" t="n">
+        <v>530.36</v>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>2261137</t>
+        </is>
+      </c>
+      <c r="C1329" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1329" t="inlineStr">
+        <is>
+          <t>Order 2261137 Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1329" t="inlineStr"/>
+      <c r="F1329" t="n">
+        <v>63.64</v>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" s="2" t="n">
+        <v>44373</v>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>2261137</t>
+        </is>
+      </c>
+      <c r="C1330" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1330" t="inlineStr">
+        <is>
+          <t>Order 2261137 Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1330" t="n">
+        <v>594</v>
+      </c>
+      <c r="F1330" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 9 new rows for week ending 2021-07-04 (total 1338 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1330"/>
+  <dimension ref="A1:F1339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28071,6 +28071,204 @@
       </c>
       <c r="F1330" t="inlineStr"/>
     </row>
+    <row r="1331">
+      <c r="A1331" s="2" t="n">
+        <v>44375</v>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Reko250</t>
+        </is>
+      </c>
+      <c r="C1331" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1331" t="inlineStr">
+        <is>
+          <t>Reko Swish +46760844133</t>
+        </is>
+      </c>
+      <c r="E1331" t="inlineStr"/>
+      <c r="F1331" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" s="2" t="n">
+        <v>44375</v>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Reko250</t>
+        </is>
+      </c>
+      <c r="C1332" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1332" t="inlineStr">
+        <is>
+          <t>Reko Swish +46760844133</t>
+        </is>
+      </c>
+      <c r="E1332" t="inlineStr"/>
+      <c r="F1332" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" s="2" t="n">
+        <v>44375</v>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Reko250</t>
+        </is>
+      </c>
+      <c r="C1333" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1333" t="inlineStr">
+        <is>
+          <t>Reko Swish +46760844133</t>
+        </is>
+      </c>
+      <c r="E1333" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1333" t="inlineStr"/>
+    </row>
+    <row r="1334">
+      <c r="A1334" s="2" t="n">
+        <v>44376</v>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Reko251</t>
+        </is>
+      </c>
+      <c r="C1334" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1334" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730623695</t>
+        </is>
+      </c>
+      <c r="E1334" t="inlineStr"/>
+      <c r="F1334" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" s="2" t="n">
+        <v>44376</v>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Reko251</t>
+        </is>
+      </c>
+      <c r="C1335" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1335" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730623695</t>
+        </is>
+      </c>
+      <c r="E1335" t="inlineStr"/>
+      <c r="F1335" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" s="2" t="n">
+        <v>44376</v>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Reko251</t>
+        </is>
+      </c>
+      <c r="C1336" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1336" t="inlineStr">
+        <is>
+          <t>Reko Swish +46730623695</t>
+        </is>
+      </c>
+      <c r="E1336" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1336" t="inlineStr"/>
+    </row>
+    <row r="1337">
+      <c r="A1337" s="2" t="n">
+        <v>44377</v>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Reko252</t>
+        </is>
+      </c>
+      <c r="C1337" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1337" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761246137</t>
+        </is>
+      </c>
+      <c r="E1337" t="inlineStr"/>
+      <c r="F1337" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" s="2" t="n">
+        <v>44377</v>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Reko252</t>
+        </is>
+      </c>
+      <c r="C1338" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1338" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761246137</t>
+        </is>
+      </c>
+      <c r="E1338" t="inlineStr"/>
+      <c r="F1338" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" s="2" t="n">
+        <v>44377</v>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Reko252</t>
+        </is>
+      </c>
+      <c r="C1339" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1339" t="inlineStr">
+        <is>
+          <t>Reko Swish +46761246137</t>
+        </is>
+      </c>
+      <c r="E1339" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1339" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 18 new rows for week ending 2021-07-11 (total 1356 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1339"/>
+  <dimension ref="A1:F1357"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28269,6 +28269,388 @@
       </c>
       <c r="F1339" t="inlineStr"/>
     </row>
+    <row r="1340">
+      <c r="A1340" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>Reko253</t>
+        </is>
+      </c>
+      <c r="C1340" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1340" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733496329</t>
+        </is>
+      </c>
+      <c r="E1340" t="inlineStr"/>
+      <c r="F1340" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Reko253</t>
+        </is>
+      </c>
+      <c r="C1341" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1341" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733496329</t>
+        </is>
+      </c>
+      <c r="E1341" t="inlineStr"/>
+      <c r="F1341" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Reko253</t>
+        </is>
+      </c>
+      <c r="C1342" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1342" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733496329</t>
+        </is>
+      </c>
+      <c r="E1342" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1342" t="inlineStr"/>
+    </row>
+    <row r="1343">
+      <c r="A1343" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Reko254</t>
+        </is>
+      </c>
+      <c r="C1343" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1343" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1343" t="inlineStr"/>
+      <c r="F1343" t="n">
+        <v>282.14</v>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Reko254</t>
+        </is>
+      </c>
+      <c r="C1344" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1344" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1344" t="inlineStr"/>
+      <c r="F1344" t="n">
+        <v>33.86</v>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" s="2" t="n">
+        <v>44384</v>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Reko254</t>
+        </is>
+      </c>
+      <c r="C1345" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1345" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702597315</t>
+        </is>
+      </c>
+      <c r="E1345" t="n">
+        <v>316</v>
+      </c>
+      <c r="F1345" t="inlineStr"/>
+    </row>
+    <row r="1346">
+      <c r="A1346" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Reko255</t>
+        </is>
+      </c>
+      <c r="C1346" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1346" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040</t>
+        </is>
+      </c>
+      <c r="E1346" t="inlineStr"/>
+      <c r="F1346" t="n">
+        <v>211.61</v>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Reko255</t>
+        </is>
+      </c>
+      <c r="C1347" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1347" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040</t>
+        </is>
+      </c>
+      <c r="E1347" t="inlineStr"/>
+      <c r="F1347" t="n">
+        <v>25.39</v>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Reko255</t>
+        </is>
+      </c>
+      <c r="C1348" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1348" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707255040</t>
+        </is>
+      </c>
+      <c r="E1348" t="n">
+        <v>237</v>
+      </c>
+      <c r="F1348" t="inlineStr"/>
+    </row>
+    <row r="1349">
+      <c r="A1349" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>Reko256</t>
+        </is>
+      </c>
+      <c r="C1349" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1349" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723030040</t>
+        </is>
+      </c>
+      <c r="E1349" t="inlineStr"/>
+      <c r="F1349" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Reko256</t>
+        </is>
+      </c>
+      <c r="C1350" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1350" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723030040</t>
+        </is>
+      </c>
+      <c r="E1350" t="inlineStr"/>
+      <c r="F1350" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Reko256</t>
+        </is>
+      </c>
+      <c r="C1351" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1351" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723030040</t>
+        </is>
+      </c>
+      <c r="E1351" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1351" t="inlineStr"/>
+    </row>
+    <row r="1352">
+      <c r="A1352" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>5081937</t>
+        </is>
+      </c>
+      <c r="C1352" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1352" t="inlineStr">
+        <is>
+          <t>Order 5081937 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1352" t="inlineStr"/>
+      <c r="F1352" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>5081937</t>
+        </is>
+      </c>
+      <c r="C1353" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1353" t="inlineStr">
+        <is>
+          <t>Order 5081937 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1353" t="inlineStr"/>
+      <c r="F1353" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" s="2" t="n">
+        <v>44385</v>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>5081937</t>
+        </is>
+      </c>
+      <c r="C1354" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1354" t="inlineStr">
+        <is>
+          <t>Order 5081937 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1354" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1354" t="inlineStr"/>
+    </row>
+    <row r="1355">
+      <c r="A1355" s="2" t="n">
+        <v>44388</v>
+      </c>
+      <c r="B1355" t="inlineStr"/>
+      <c r="C1355" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D1355" t="inlineStr">
+        <is>
+          <t>July hyra</t>
+        </is>
+      </c>
+      <c r="E1355" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F1355" t="inlineStr"/>
+    </row>
+    <row r="1356">
+      <c r="A1356" s="2" t="n">
+        <v>44388</v>
+      </c>
+      <c r="B1356" t="inlineStr"/>
+      <c r="C1356" t="inlineStr"/>
+      <c r="D1356" t="inlineStr">
+        <is>
+          <t>July hyra</t>
+        </is>
+      </c>
+      <c r="E1356" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1356" t="inlineStr"/>
+    </row>
+    <row r="1357">
+      <c r="A1357" s="2" t="n">
+        <v>44388</v>
+      </c>
+      <c r="B1357" t="inlineStr"/>
+      <c r="C1357" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1357" t="inlineStr">
+        <is>
+          <t>July hyra</t>
+        </is>
+      </c>
+      <c r="E1357" t="inlineStr"/>
+      <c r="F1357" t="n">
+        <v>4166</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 12 new rows for week ending 2021-07-18 (total 1368 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1357"/>
+  <dimension ref="A1:F1369"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28651,6 +28651,246 @@
         <v>4166</v>
       </c>
     </row>
+    <row r="1358">
+      <c r="A1358" s="2" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>9121145</t>
+        </is>
+      </c>
+      <c r="C1358" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1358" t="inlineStr">
+        <is>
+          <t>Order 9121145 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E1358" t="inlineStr"/>
+      <c r="F1358" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" s="2" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>9121145</t>
+        </is>
+      </c>
+      <c r="C1359" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1359" t="inlineStr">
+        <is>
+          <t>Order 9121145 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E1359" t="inlineStr"/>
+      <c r="F1359" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" s="2" t="n">
+        <v>44389</v>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>9121145</t>
+        </is>
+      </c>
+      <c r="C1360" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1360" t="inlineStr">
+        <is>
+          <t>Order 9121145 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E1360" t="n">
+        <v>690</v>
+      </c>
+      <c r="F1360" t="inlineStr"/>
+    </row>
+    <row r="1361">
+      <c r="A1361" s="2" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B1361" t="inlineStr"/>
+      <c r="C1361" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1361" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1361" t="n">
+        <v>838.78</v>
+      </c>
+      <c r="F1361" t="inlineStr"/>
+    </row>
+    <row r="1362">
+      <c r="A1362" s="2" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B1362" t="inlineStr"/>
+      <c r="C1362" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1362" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1362" t="n">
+        <v>209.7</v>
+      </c>
+      <c r="F1362" t="inlineStr"/>
+    </row>
+    <row r="1363">
+      <c r="A1363" s="2" t="n">
+        <v>44390</v>
+      </c>
+      <c r="B1363" t="inlineStr"/>
+      <c r="C1363" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1363" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1363" t="inlineStr"/>
+      <c r="F1363" t="n">
+        <v>1048.48</v>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" s="2" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>9161836</t>
+        </is>
+      </c>
+      <c r="C1364" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1364" t="inlineStr">
+        <is>
+          <t>Order 9161836 Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1364" t="inlineStr"/>
+      <c r="F1364" t="n">
+        <v>210.71</v>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" s="2" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>9161836</t>
+        </is>
+      </c>
+      <c r="C1365" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1365" t="inlineStr">
+        <is>
+          <t>Order 9161836 Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1365" t="inlineStr"/>
+      <c r="F1365" t="n">
+        <v>25.29</v>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" s="2" t="n">
+        <v>44393</v>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>9161836</t>
+        </is>
+      </c>
+      <c r="C1366" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1366" t="inlineStr">
+        <is>
+          <t>Order 9161836 Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1366" t="n">
+        <v>236</v>
+      </c>
+      <c r="F1366" t="inlineStr"/>
+    </row>
+    <row r="1367">
+      <c r="A1367" s="2" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B1367" t="inlineStr"/>
+      <c r="C1367" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1367" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1367" t="n">
+        <v>648.26</v>
+      </c>
+      <c r="F1367" t="inlineStr"/>
+    </row>
+    <row r="1368">
+      <c r="A1368" s="2" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B1368" t="inlineStr"/>
+      <c r="C1368" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1368" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1368" t="n">
+        <v>162.06</v>
+      </c>
+      <c r="F1368" t="inlineStr"/>
+    </row>
+    <row r="1369">
+      <c r="A1369" s="2" t="n">
+        <v>44395</v>
+      </c>
+      <c r="B1369" t="inlineStr"/>
+      <c r="C1369" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1369" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1369" t="inlineStr"/>
+      <c r="F1369" t="n">
+        <v>810.3200000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2021-07-25 (total 1371 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1369"/>
+  <dimension ref="A1:F1372"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28891,6 +28891,58 @@
         <v>810.3200000000001</v>
       </c>
     </row>
+    <row r="1370">
+      <c r="A1370" s="2" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B1370" t="inlineStr"/>
+      <c r="C1370" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D1370" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1370" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="F1370" t="inlineStr"/>
+    </row>
+    <row r="1371">
+      <c r="A1371" s="2" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B1371" t="inlineStr"/>
+      <c r="C1371" t="inlineStr"/>
+      <c r="D1371" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1371" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1371" t="inlineStr"/>
+    </row>
+    <row r="1372">
+      <c r="A1372" s="2" t="n">
+        <v>44397</v>
+      </c>
+      <c r="B1372" t="inlineStr"/>
+      <c r="C1372" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1372" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1372" t="inlineStr"/>
+      <c r="F1372" t="n">
+        <v>82.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2021-08-08 (total 1377 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1372"/>
+  <dimension ref="A1:F1378"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -28943,6 +28943,124 @@
         <v>82.5</v>
       </c>
     </row>
+    <row r="1373">
+      <c r="A1373" s="2" t="n">
+        <v>44414</v>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>1062053</t>
+        </is>
+      </c>
+      <c r="C1373" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1373" t="inlineStr">
+        <is>
+          <t>Order 1062053 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1373" t="inlineStr"/>
+      <c r="F1373" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" s="2" t="n">
+        <v>44414</v>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>1062053</t>
+        </is>
+      </c>
+      <c r="C1374" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1374" t="inlineStr">
+        <is>
+          <t>Order 1062053 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1374" t="inlineStr"/>
+      <c r="F1374" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" s="2" t="n">
+        <v>44414</v>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>1062053</t>
+        </is>
+      </c>
+      <c r="C1375" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1375" t="inlineStr">
+        <is>
+          <t>Order 1062053 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1375" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1375" t="inlineStr"/>
+    </row>
+    <row r="1376">
+      <c r="A1376" s="2" t="n">
+        <v>44416</v>
+      </c>
+      <c r="B1376" t="inlineStr"/>
+      <c r="C1376" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1376" t="inlineStr">
+        <is>
+          <t>FACEBK N96RQ4XZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E1376" t="n">
+        <v>79.03</v>
+      </c>
+      <c r="F1376" t="inlineStr"/>
+    </row>
+    <row r="1377">
+      <c r="A1377" s="2" t="n">
+        <v>44416</v>
+      </c>
+      <c r="B1377" t="inlineStr"/>
+      <c r="C1377" t="inlineStr"/>
+      <c r="D1377" t="inlineStr">
+        <is>
+          <t>FACEBK N96RQ4XZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E1377" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1377" t="inlineStr"/>
+    </row>
+    <row r="1378">
+      <c r="A1378" s="2" t="n">
+        <v>44416</v>
+      </c>
+      <c r="B1378" t="inlineStr"/>
+      <c r="C1378" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1378" t="inlineStr">
+        <is>
+          <t>FACEBK N96RQ4XZ62 K6885</t>
+        </is>
+      </c>
+      <c r="E1378" t="inlineStr"/>
+      <c r="F1378" t="n">
+        <v>79.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2021-08-15 (total 1380 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1378"/>
+  <dimension ref="A1:F1381"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29061,6 +29061,72 @@
         <v>79.03</v>
       </c>
     </row>
+    <row r="1379">
+      <c r="A1379" s="2" t="n">
+        <v>44423</v>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>4151821</t>
+        </is>
+      </c>
+      <c r="C1379" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1379" t="inlineStr">
+        <is>
+          <t>Order 4151821 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1379" t="inlineStr"/>
+      <c r="F1379" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" s="2" t="n">
+        <v>44423</v>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>4151821</t>
+        </is>
+      </c>
+      <c r="C1380" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1380" t="inlineStr">
+        <is>
+          <t>Order 4151821 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1380" t="inlineStr"/>
+      <c r="F1380" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" s="2" t="n">
+        <v>44423</v>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>4151821</t>
+        </is>
+      </c>
+      <c r="C1381" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1381" t="inlineStr">
+        <is>
+          <t>Order 4151821 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1381" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1381" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 18 new rows for week ending 2021-08-22 (total 1398 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1381"/>
+  <dimension ref="A1:F1399"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29127,6 +29127,364 @@
       </c>
       <c r="F1381" t="inlineStr"/>
     </row>
+    <row r="1382">
+      <c r="A1382" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>1161309</t>
+        </is>
+      </c>
+      <c r="C1382" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1382" t="inlineStr">
+        <is>
+          <t>Order 1161309 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1382" t="inlineStr"/>
+      <c r="F1382" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>1161309</t>
+        </is>
+      </c>
+      <c r="C1383" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1383" t="inlineStr">
+        <is>
+          <t>Order 1161309 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1383" t="inlineStr"/>
+      <c r="F1383" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>1161309</t>
+        </is>
+      </c>
+      <c r="C1384" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1384" t="inlineStr">
+        <is>
+          <t>Order 1161309 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1384" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1384" t="inlineStr"/>
+    </row>
+    <row r="1385">
+      <c r="A1385" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>5161753</t>
+        </is>
+      </c>
+      <c r="C1385" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1385" t="inlineStr">
+        <is>
+          <t>Order 5161753 Swish +46725255185</t>
+        </is>
+      </c>
+      <c r="E1385" t="inlineStr"/>
+      <c r="F1385" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t>5161753</t>
+        </is>
+      </c>
+      <c r="C1386" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1386" t="inlineStr">
+        <is>
+          <t>Order 5161753 Swish +46725255185</t>
+        </is>
+      </c>
+      <c r="E1386" t="inlineStr"/>
+      <c r="F1386" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" s="2" t="n">
+        <v>44424</v>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>5161753</t>
+        </is>
+      </c>
+      <c r="C1387" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1387" t="inlineStr">
+        <is>
+          <t>Order 5161753 Swish +46725255185</t>
+        </is>
+      </c>
+      <c r="E1387" t="n">
+        <v>645</v>
+      </c>
+      <c r="F1387" t="inlineStr"/>
+    </row>
+    <row r="1388">
+      <c r="A1388" s="2" t="n">
+        <v>44425</v>
+      </c>
+      <c r="B1388" t="inlineStr"/>
+      <c r="C1388" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D1388" t="inlineStr">
+        <is>
+          <t>Hyra Augusti</t>
+        </is>
+      </c>
+      <c r="E1388" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F1388" t="inlineStr"/>
+    </row>
+    <row r="1389">
+      <c r="A1389" s="2" t="n">
+        <v>44425</v>
+      </c>
+      <c r="B1389" t="inlineStr"/>
+      <c r="C1389" t="inlineStr"/>
+      <c r="D1389" t="inlineStr">
+        <is>
+          <t>Hyra Augusti</t>
+        </is>
+      </c>
+      <c r="E1389" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1389" t="inlineStr"/>
+    </row>
+    <row r="1390">
+      <c r="A1390" s="2" t="n">
+        <v>44425</v>
+      </c>
+      <c r="B1390" t="inlineStr"/>
+      <c r="C1390" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1390" t="inlineStr">
+        <is>
+          <t>Hyra Augusti</t>
+        </is>
+      </c>
+      <c r="E1390" t="inlineStr"/>
+      <c r="F1390" t="n">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B1391" t="inlineStr"/>
+      <c r="C1391" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1391" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1391" t="n">
+        <v>324.83</v>
+      </c>
+      <c r="F1391" t="inlineStr"/>
+    </row>
+    <row r="1392">
+      <c r="A1392" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B1392" t="inlineStr"/>
+      <c r="C1392" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1392" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1392" t="n">
+        <v>38.98</v>
+      </c>
+      <c r="F1392" t="inlineStr"/>
+    </row>
+    <row r="1393">
+      <c r="A1393" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B1393" t="inlineStr"/>
+      <c r="C1393" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1393" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1393" t="inlineStr"/>
+      <c r="F1393" t="n">
+        <v>363.81</v>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B1394" t="inlineStr"/>
+      <c r="C1394" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1394" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1394" t="n">
+        <v>184.82</v>
+      </c>
+      <c r="F1394" t="inlineStr"/>
+    </row>
+    <row r="1395">
+      <c r="A1395" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B1395" t="inlineStr"/>
+      <c r="C1395" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1395" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1395" t="n">
+        <v>22.18</v>
+      </c>
+      <c r="F1395" t="inlineStr"/>
+    </row>
+    <row r="1396">
+      <c r="A1396" s="2" t="n">
+        <v>44427</v>
+      </c>
+      <c r="B1396" t="inlineStr"/>
+      <c r="C1396" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1396" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1396" t="inlineStr"/>
+      <c r="F1396" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" s="2" t="n">
+        <v>44429</v>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>9211417</t>
+        </is>
+      </c>
+      <c r="C1397" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1397" t="inlineStr">
+        <is>
+          <t>Order 9211417 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1397" t="inlineStr"/>
+      <c r="F1397" t="n">
+        <v>655.36</v>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" s="2" t="n">
+        <v>44429</v>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>9211417</t>
+        </is>
+      </c>
+      <c r="C1398" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1398" t="inlineStr">
+        <is>
+          <t>Order 9211417 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1398" t="inlineStr"/>
+      <c r="F1398" t="n">
+        <v>78.64</v>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" s="2" t="n">
+        <v>44429</v>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>9211417</t>
+        </is>
+      </c>
+      <c r="C1399" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1399" t="inlineStr">
+        <is>
+          <t>Order 9211417 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1399" t="n">
+        <v>734</v>
+      </c>
+      <c r="F1399" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 9 new rows for week ending 2021-08-29 (total 1407 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1399"/>
+  <dimension ref="A1:F1408"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29485,6 +29485,204 @@
       </c>
       <c r="F1399" t="inlineStr"/>
     </row>
+    <row r="1400">
+      <c r="A1400" s="2" t="n">
+        <v>44431</v>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>8231933</t>
+        </is>
+      </c>
+      <c r="C1400" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1400" t="inlineStr">
+        <is>
+          <t>Order 8231933 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E1400" t="inlineStr"/>
+      <c r="F1400" t="n">
+        <v>441.96</v>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" s="2" t="n">
+        <v>44431</v>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>8231933</t>
+        </is>
+      </c>
+      <c r="C1401" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1401" t="inlineStr">
+        <is>
+          <t>Order 8231933 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E1401" t="inlineStr"/>
+      <c r="F1401" t="n">
+        <v>53.04</v>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" s="2" t="n">
+        <v>44431</v>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>8231933</t>
+        </is>
+      </c>
+      <c r="C1402" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1402" t="inlineStr">
+        <is>
+          <t>Order 8231933 Swish +46734869113</t>
+        </is>
+      </c>
+      <c r="E1402" t="n">
+        <v>495</v>
+      </c>
+      <c r="F1402" t="inlineStr"/>
+    </row>
+    <row r="1403">
+      <c r="A1403" s="2" t="n">
+        <v>44434</v>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>8261449</t>
+        </is>
+      </c>
+      <c r="C1403" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1403" t="inlineStr">
+        <is>
+          <t>Order 8261449 Swish +46725255185</t>
+        </is>
+      </c>
+      <c r="E1403" t="inlineStr"/>
+      <c r="F1403" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" s="2" t="n">
+        <v>44434</v>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>8261449</t>
+        </is>
+      </c>
+      <c r="C1404" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1404" t="inlineStr">
+        <is>
+          <t>Order 8261449 Swish +46725255185</t>
+        </is>
+      </c>
+      <c r="E1404" t="inlineStr"/>
+      <c r="F1404" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" s="2" t="n">
+        <v>44434</v>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>8261449</t>
+        </is>
+      </c>
+      <c r="C1405" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1405" t="inlineStr">
+        <is>
+          <t>Order 8261449 Swish +46725255185</t>
+        </is>
+      </c>
+      <c r="E1405" t="n">
+        <v>774</v>
+      </c>
+      <c r="F1405" t="inlineStr"/>
+    </row>
+    <row r="1406">
+      <c r="A1406" s="2" t="n">
+        <v>44436</v>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>1282250</t>
+        </is>
+      </c>
+      <c r="C1406" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1406" t="inlineStr">
+        <is>
+          <t>Order 1282250 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1406" t="inlineStr"/>
+      <c r="F1406" t="n">
+        <v>770.54</v>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" s="2" t="n">
+        <v>44436</v>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>1282250</t>
+        </is>
+      </c>
+      <c r="C1407" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1407" t="inlineStr">
+        <is>
+          <t>Order 1282250 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1407" t="inlineStr"/>
+      <c r="F1407" t="n">
+        <v>92.45999999999999</v>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" s="2" t="n">
+        <v>44436</v>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>1282250</t>
+        </is>
+      </c>
+      <c r="C1408" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1408" t="inlineStr">
+        <is>
+          <t>Order 1282250 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1408" t="n">
+        <v>863</v>
+      </c>
+      <c r="F1408" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 9 new rows for week ending 2021-09-05 (total 1416 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1408"/>
+  <dimension ref="A1:F1417"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29683,6 +29683,180 @@
       </c>
       <c r="F1408" t="inlineStr"/>
     </row>
+    <row r="1409">
+      <c r="A1409" s="2" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>3011951</t>
+        </is>
+      </c>
+      <c r="C1409" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1409" t="inlineStr">
+        <is>
+          <t>Order 3011951 Swish +46703019983</t>
+        </is>
+      </c>
+      <c r="E1409" t="inlineStr"/>
+      <c r="F1409" t="n">
+        <v>1141.96</v>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" s="2" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>3011951</t>
+        </is>
+      </c>
+      <c r="C1410" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1410" t="inlineStr">
+        <is>
+          <t>Order 3011951 Swish +46703019983</t>
+        </is>
+      </c>
+      <c r="E1410" t="inlineStr"/>
+      <c r="F1410" t="n">
+        <v>137.04</v>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" s="2" t="n">
+        <v>44440</v>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>3011951</t>
+        </is>
+      </c>
+      <c r="C1411" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1411" t="inlineStr">
+        <is>
+          <t>Order 3011951 Swish +46703019983</t>
+        </is>
+      </c>
+      <c r="E1411" t="n">
+        <v>1279</v>
+      </c>
+      <c r="F1411" t="inlineStr"/>
+    </row>
+    <row r="1412">
+      <c r="A1412" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B1412" t="inlineStr"/>
+      <c r="C1412" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1412" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1412" t="n">
+        <v>122.66</v>
+      </c>
+      <c r="F1412" t="inlineStr"/>
+    </row>
+    <row r="1413">
+      <c r="A1413" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B1413" t="inlineStr"/>
+      <c r="C1413" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1413" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1413" t="n">
+        <v>14.72</v>
+      </c>
+      <c r="F1413" t="inlineStr"/>
+    </row>
+    <row r="1414">
+      <c r="A1414" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B1414" t="inlineStr"/>
+      <c r="C1414" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1414" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1414" t="inlineStr"/>
+      <c r="F1414" t="n">
+        <v>137.38</v>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B1415" t="inlineStr"/>
+      <c r="C1415" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1415" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1415" t="n">
+        <v>524</v>
+      </c>
+      <c r="F1415" t="inlineStr"/>
+    </row>
+    <row r="1416">
+      <c r="A1416" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B1416" t="inlineStr"/>
+      <c r="C1416" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1416" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1416" t="n">
+        <v>62.88</v>
+      </c>
+      <c r="F1416" t="inlineStr"/>
+    </row>
+    <row r="1417">
+      <c r="A1417" s="2" t="n">
+        <v>44441</v>
+      </c>
+      <c r="B1417" t="inlineStr"/>
+      <c r="C1417" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1417" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1417" t="inlineStr"/>
+      <c r="F1417" t="n">
+        <v>586.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 27 new rows for week ending 2021-09-12 (total 1443 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1417"/>
+  <dimension ref="A1:F1444"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -29857,6 +29857,550 @@
         <v>586.88</v>
       </c>
     </row>
+    <row r="1418">
+      <c r="A1418" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>9061618</t>
+        </is>
+      </c>
+      <c r="C1418" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1418" t="inlineStr">
+        <is>
+          <t>Order 9061618 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1418" t="inlineStr"/>
+      <c r="F1418" t="n">
+        <v>883.9299999999999</v>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>9061618</t>
+        </is>
+      </c>
+      <c r="C1419" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1419" t="inlineStr">
+        <is>
+          <t>Order 9061618 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1419" t="inlineStr"/>
+      <c r="F1419" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>9061618</t>
+        </is>
+      </c>
+      <c r="C1420" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1420" t="inlineStr">
+        <is>
+          <t>Order 9061618 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1420" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1420" t="inlineStr"/>
+    </row>
+    <row r="1421">
+      <c r="A1421" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>7061821</t>
+        </is>
+      </c>
+      <c r="C1421" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1421" t="inlineStr">
+        <is>
+          <t>Order 7061821 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1421" t="inlineStr"/>
+      <c r="F1421" t="n">
+        <v>1132.14</v>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>7061821</t>
+        </is>
+      </c>
+      <c r="C1422" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1422" t="inlineStr">
+        <is>
+          <t>Order 7061821 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1422" t="inlineStr"/>
+      <c r="F1422" t="n">
+        <v>135.86</v>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>7061821</t>
+        </is>
+      </c>
+      <c r="C1423" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1423" t="inlineStr">
+        <is>
+          <t>Order 7061821 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1423" t="n">
+        <v>1268</v>
+      </c>
+      <c r="F1423" t="inlineStr"/>
+    </row>
+    <row r="1424">
+      <c r="A1424" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>3092057</t>
+        </is>
+      </c>
+      <c r="C1424" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1424" t="inlineStr">
+        <is>
+          <t>Order 3092057 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1424" t="inlineStr"/>
+      <c r="F1424" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>3092057</t>
+        </is>
+      </c>
+      <c r="C1425" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1425" t="inlineStr">
+        <is>
+          <t>Order 3092057 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1425" t="inlineStr"/>
+      <c r="F1425" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t>3092057</t>
+        </is>
+      </c>
+      <c r="C1426" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1426" t="inlineStr">
+        <is>
+          <t>Order 3092057 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1426" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1426" t="inlineStr"/>
+    </row>
+    <row r="1427">
+      <c r="A1427" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>5101004</t>
+        </is>
+      </c>
+      <c r="C1427" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1427" t="inlineStr">
+        <is>
+          <t>Order 5101004 Swish +46704483544</t>
+        </is>
+      </c>
+      <c r="E1427" t="inlineStr"/>
+      <c r="F1427" t="n">
+        <v>1176.79</v>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>5101004</t>
+        </is>
+      </c>
+      <c r="C1428" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1428" t="inlineStr">
+        <is>
+          <t>Order 5101004 Swish +46704483544</t>
+        </is>
+      </c>
+      <c r="E1428" t="inlineStr"/>
+      <c r="F1428" t="n">
+        <v>141.21</v>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" s="2" t="n">
+        <v>44448</v>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>5101004</t>
+        </is>
+      </c>
+      <c r="C1429" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1429" t="inlineStr">
+        <is>
+          <t>Order 5101004 Swish +46704483544</t>
+        </is>
+      </c>
+      <c r="E1429" t="n">
+        <v>1318</v>
+      </c>
+      <c r="F1429" t="inlineStr"/>
+    </row>
+    <row r="1430">
+      <c r="A1430" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B1430" t="inlineStr"/>
+      <c r="C1430" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1430" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1430" t="n">
+        <v>546.4299999999999</v>
+      </c>
+      <c r="F1430" t="inlineStr"/>
+    </row>
+    <row r="1431">
+      <c r="A1431" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B1431" t="inlineStr"/>
+      <c r="C1431" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1431" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1431" t="n">
+        <v>65.56999999999999</v>
+      </c>
+      <c r="F1431" t="inlineStr"/>
+    </row>
+    <row r="1432">
+      <c r="A1432" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B1432" t="inlineStr"/>
+      <c r="C1432" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1432" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1432" t="inlineStr"/>
+      <c r="F1432" t="n">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B1433" t="inlineStr"/>
+      <c r="C1433" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1433" t="inlineStr">
+        <is>
+          <t>FACEBK 48MLK53Z62 K6885</t>
+        </is>
+      </c>
+      <c r="E1433" t="n">
+        <v>200</v>
+      </c>
+      <c r="F1433" t="inlineStr"/>
+    </row>
+    <row r="1434">
+      <c r="A1434" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B1434" t="inlineStr"/>
+      <c r="C1434" t="inlineStr"/>
+      <c r="D1434" t="inlineStr">
+        <is>
+          <t>FACEBK 48MLK53Z62 K6885</t>
+        </is>
+      </c>
+      <c r="E1434" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1434" t="inlineStr"/>
+    </row>
+    <row r="1435">
+      <c r="A1435" s="2" t="n">
+        <v>44450</v>
+      </c>
+      <c r="B1435" t="inlineStr"/>
+      <c r="C1435" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1435" t="inlineStr">
+        <is>
+          <t>FACEBK 48MLK53Z62 K6885</t>
+        </is>
+      </c>
+      <c r="E1435" t="inlineStr"/>
+      <c r="F1435" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>6121637</t>
+        </is>
+      </c>
+      <c r="C1436" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1436" t="inlineStr">
+        <is>
+          <t>Order 6121637 Swish +46735689616</t>
+        </is>
+      </c>
+      <c r="E1436" t="inlineStr"/>
+      <c r="F1436" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>6121637</t>
+        </is>
+      </c>
+      <c r="C1437" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1437" t="inlineStr">
+        <is>
+          <t>Order 6121637 Swish +46735689616</t>
+        </is>
+      </c>
+      <c r="E1437" t="inlineStr"/>
+      <c r="F1437" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>6121637</t>
+        </is>
+      </c>
+      <c r="C1438" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1438" t="inlineStr">
+        <is>
+          <t>Order 6121637 Swish +46735689616</t>
+        </is>
+      </c>
+      <c r="E1438" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1438" t="inlineStr"/>
+    </row>
+    <row r="1439">
+      <c r="A1439" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1439" t="inlineStr"/>
+      <c r="C1439" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1439" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1439" t="n">
+        <v>1516.12</v>
+      </c>
+      <c r="F1439" t="inlineStr"/>
+    </row>
+    <row r="1440">
+      <c r="A1440" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1440" t="inlineStr"/>
+      <c r="C1440" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1440" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1440" t="n">
+        <v>181.93</v>
+      </c>
+      <c r="F1440" t="inlineStr"/>
+    </row>
+    <row r="1441">
+      <c r="A1441" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1441" t="inlineStr"/>
+      <c r="C1441" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1441" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1441" t="inlineStr"/>
+      <c r="F1441" t="n">
+        <v>1698.05</v>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1442" t="inlineStr"/>
+      <c r="C1442" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1442" t="inlineStr">
+        <is>
+          <t>SRI LANKA LIVS K0135</t>
+        </is>
+      </c>
+      <c r="E1442" t="n">
+        <v>705.1799999999999</v>
+      </c>
+      <c r="F1442" t="inlineStr"/>
+    </row>
+    <row r="1443">
+      <c r="A1443" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1443" t="inlineStr"/>
+      <c r="C1443" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1443" t="inlineStr">
+        <is>
+          <t>SRI LANKA LIVS K0135</t>
+        </is>
+      </c>
+      <c r="E1443" t="n">
+        <v>84.62</v>
+      </c>
+      <c r="F1443" t="inlineStr"/>
+    </row>
+    <row r="1444">
+      <c r="A1444" s="2" t="n">
+        <v>44451</v>
+      </c>
+      <c r="B1444" t="inlineStr"/>
+      <c r="C1444" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1444" t="inlineStr">
+        <is>
+          <t>SRI LANKA LIVS K0135</t>
+        </is>
+      </c>
+      <c r="E1444" t="inlineStr"/>
+      <c r="F1444" t="n">
+        <v>789.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 72 new rows for week ending 2021-09-19 (total 1515 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1444"/>
+  <dimension ref="A1:F1516"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -30401,6 +30401,1490 @@
         <v>789.8</v>
       </c>
     </row>
+    <row r="1445">
+      <c r="A1445" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1445" t="inlineStr">
+        <is>
+          <t>Reko257</t>
+        </is>
+      </c>
+      <c r="C1445" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1445" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702920861</t>
+        </is>
+      </c>
+      <c r="E1445" t="inlineStr"/>
+      <c r="F1445" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1446" t="inlineStr">
+        <is>
+          <t>Reko257</t>
+        </is>
+      </c>
+      <c r="C1446" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1446" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702920861</t>
+        </is>
+      </c>
+      <c r="E1446" t="inlineStr"/>
+      <c r="F1446" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1447" t="inlineStr">
+        <is>
+          <t>Reko257</t>
+        </is>
+      </c>
+      <c r="C1447" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1447" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702920861</t>
+        </is>
+      </c>
+      <c r="E1447" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1447" t="inlineStr"/>
+    </row>
+    <row r="1448">
+      <c r="A1448" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1448" t="inlineStr">
+        <is>
+          <t>Reko258</t>
+        </is>
+      </c>
+      <c r="C1448" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1448" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1448" t="inlineStr"/>
+      <c r="F1448" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1449" t="inlineStr">
+        <is>
+          <t>Reko258</t>
+        </is>
+      </c>
+      <c r="C1449" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1449" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1449" t="inlineStr"/>
+      <c r="F1449" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>Reko258</t>
+        </is>
+      </c>
+      <c r="C1450" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1450" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1450" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1450" t="inlineStr"/>
+    </row>
+    <row r="1451">
+      <c r="A1451" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>Reko259</t>
+        </is>
+      </c>
+      <c r="C1451" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1451" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720106501</t>
+        </is>
+      </c>
+      <c r="E1451" t="inlineStr"/>
+      <c r="F1451" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>Reko259</t>
+        </is>
+      </c>
+      <c r="C1452" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1452" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720106501</t>
+        </is>
+      </c>
+      <c r="E1452" t="inlineStr"/>
+      <c r="F1452" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>Reko259</t>
+        </is>
+      </c>
+      <c r="C1453" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1453" t="inlineStr">
+        <is>
+          <t>Reko Swish +46720106501</t>
+        </is>
+      </c>
+      <c r="E1453" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1453" t="inlineStr"/>
+    </row>
+    <row r="1454">
+      <c r="A1454" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>Reko260</t>
+        </is>
+      </c>
+      <c r="C1454" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1454" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703299060</t>
+        </is>
+      </c>
+      <c r="E1454" t="inlineStr"/>
+      <c r="F1454" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>Reko260</t>
+        </is>
+      </c>
+      <c r="C1455" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1455" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703299060</t>
+        </is>
+      </c>
+      <c r="E1455" t="inlineStr"/>
+      <c r="F1455" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>Reko260</t>
+        </is>
+      </c>
+      <c r="C1456" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1456" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703299060</t>
+        </is>
+      </c>
+      <c r="E1456" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1456" t="inlineStr"/>
+    </row>
+    <row r="1457">
+      <c r="A1457" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>Reko261</t>
+        </is>
+      </c>
+      <c r="C1457" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1457" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E1457" t="inlineStr"/>
+      <c r="F1457" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>Reko261</t>
+        </is>
+      </c>
+      <c r="C1458" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1458" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E1458" t="inlineStr"/>
+      <c r="F1458" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>Reko261</t>
+        </is>
+      </c>
+      <c r="C1459" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1459" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739012974</t>
+        </is>
+      </c>
+      <c r="E1459" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1459" t="inlineStr"/>
+    </row>
+    <row r="1460">
+      <c r="A1460" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>Reko262</t>
+        </is>
+      </c>
+      <c r="C1460" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1460" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708217045</t>
+        </is>
+      </c>
+      <c r="E1460" t="inlineStr"/>
+      <c r="F1460" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>Reko262</t>
+        </is>
+      </c>
+      <c r="C1461" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1461" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708217045</t>
+        </is>
+      </c>
+      <c r="E1461" t="inlineStr"/>
+      <c r="F1461" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>Reko262</t>
+        </is>
+      </c>
+      <c r="C1462" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1462" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708217045</t>
+        </is>
+      </c>
+      <c r="E1462" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1462" t="inlineStr"/>
+    </row>
+    <row r="1463">
+      <c r="A1463" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>Reko263</t>
+        </is>
+      </c>
+      <c r="C1463" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1463" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1463" t="inlineStr"/>
+      <c r="F1463" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>Reko263</t>
+        </is>
+      </c>
+      <c r="C1464" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1464" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1464" t="inlineStr"/>
+      <c r="F1464" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>Reko263</t>
+        </is>
+      </c>
+      <c r="C1465" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1465" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767736486</t>
+        </is>
+      </c>
+      <c r="E1465" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1465" t="inlineStr"/>
+    </row>
+    <row r="1466">
+      <c r="A1466" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1466" t="inlineStr"/>
+      <c r="C1466" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1466" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E1466" t="n">
+        <v>76.43000000000001</v>
+      </c>
+      <c r="F1466" t="inlineStr"/>
+    </row>
+    <row r="1467">
+      <c r="A1467" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1467" t="inlineStr"/>
+      <c r="C1467" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1467" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E1467" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="F1467" t="inlineStr"/>
+    </row>
+    <row r="1468">
+      <c r="A1468" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1468" t="inlineStr"/>
+      <c r="C1468" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1468" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E1468" t="inlineStr"/>
+      <c r="F1468" t="n">
+        <v>85.59999999999999</v>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1469" t="inlineStr"/>
+      <c r="C1469" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1469" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1469" t="n">
+        <v>492.5</v>
+      </c>
+      <c r="F1469" t="inlineStr"/>
+    </row>
+    <row r="1470">
+      <c r="A1470" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1470" t="inlineStr"/>
+      <c r="C1470" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1470" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1470" t="n">
+        <v>59.1</v>
+      </c>
+      <c r="F1470" t="inlineStr"/>
+    </row>
+    <row r="1471">
+      <c r="A1471" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1471" t="inlineStr"/>
+      <c r="C1471" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1471" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1471" t="inlineStr"/>
+      <c r="F1471" t="n">
+        <v>551.6</v>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1472" t="inlineStr"/>
+      <c r="C1472" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1472" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1472" t="n">
+        <v>722.6799999999999</v>
+      </c>
+      <c r="F1472" t="inlineStr"/>
+    </row>
+    <row r="1473">
+      <c r="A1473" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1473" t="inlineStr"/>
+      <c r="C1473" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1473" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1473" t="n">
+        <v>86.72</v>
+      </c>
+      <c r="F1473" t="inlineStr"/>
+    </row>
+    <row r="1474">
+      <c r="A1474" s="2" t="n">
+        <v>44452</v>
+      </c>
+      <c r="B1474" t="inlineStr"/>
+      <c r="C1474" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1474" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1474" t="inlineStr"/>
+      <c r="F1474" t="n">
+        <v>809.4</v>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1475" t="inlineStr">
+        <is>
+          <t>Reko264</t>
+        </is>
+      </c>
+      <c r="C1475" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1475" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709959656</t>
+        </is>
+      </c>
+      <c r="E1475" t="inlineStr"/>
+      <c r="F1475" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1476" t="inlineStr">
+        <is>
+          <t>Reko264</t>
+        </is>
+      </c>
+      <c r="C1476" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1476" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709959656</t>
+        </is>
+      </c>
+      <c r="E1476" t="inlineStr"/>
+      <c r="F1476" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1477" t="inlineStr">
+        <is>
+          <t>Reko264</t>
+        </is>
+      </c>
+      <c r="C1477" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1477" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709959656</t>
+        </is>
+      </c>
+      <c r="E1477" t="n">
+        <v>774</v>
+      </c>
+      <c r="F1477" t="inlineStr"/>
+    </row>
+    <row r="1478">
+      <c r="A1478" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1478" t="inlineStr">
+        <is>
+          <t>Reko265</t>
+        </is>
+      </c>
+      <c r="C1478" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1478" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709959656 Return</t>
+        </is>
+      </c>
+      <c r="E1478" t="n">
+        <v>691.0700000000001</v>
+      </c>
+      <c r="F1478" t="inlineStr"/>
+    </row>
+    <row r="1479">
+      <c r="A1479" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1479" t="inlineStr">
+        <is>
+          <t>Reko265</t>
+        </is>
+      </c>
+      <c r="C1479" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1479" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709959656 Return</t>
+        </is>
+      </c>
+      <c r="E1479" t="n">
+        <v>82.93000000000001</v>
+      </c>
+      <c r="F1479" t="inlineStr"/>
+    </row>
+    <row r="1480">
+      <c r="A1480" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1480" t="inlineStr">
+        <is>
+          <t>Reko265</t>
+        </is>
+      </c>
+      <c r="C1480" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1480" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709959656 Return</t>
+        </is>
+      </c>
+      <c r="E1480" t="inlineStr"/>
+      <c r="F1480" t="n">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1481" t="inlineStr">
+        <is>
+          <t>Reko266</t>
+        </is>
+      </c>
+      <c r="C1481" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1481" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739966118</t>
+        </is>
+      </c>
+      <c r="E1481" t="inlineStr"/>
+      <c r="F1481" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1482" t="inlineStr">
+        <is>
+          <t>Reko266</t>
+        </is>
+      </c>
+      <c r="C1482" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1482" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739966118</t>
+        </is>
+      </c>
+      <c r="E1482" t="inlineStr"/>
+      <c r="F1482" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1483" t="inlineStr">
+        <is>
+          <t>Reko266</t>
+        </is>
+      </c>
+      <c r="C1483" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1483" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739966118</t>
+        </is>
+      </c>
+      <c r="E1483" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1483" t="inlineStr"/>
+    </row>
+    <row r="1484">
+      <c r="A1484" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1484" t="inlineStr">
+        <is>
+          <t>Reko267</t>
+        </is>
+      </c>
+      <c r="C1484" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1484" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702701127</t>
+        </is>
+      </c>
+      <c r="E1484" t="inlineStr"/>
+      <c r="F1484" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1485" t="inlineStr">
+        <is>
+          <t>Reko267</t>
+        </is>
+      </c>
+      <c r="C1485" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1485" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702701127</t>
+        </is>
+      </c>
+      <c r="E1485" t="inlineStr"/>
+      <c r="F1485" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1486" t="inlineStr">
+        <is>
+          <t>Reko267</t>
+        </is>
+      </c>
+      <c r="C1486" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1486" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702701127</t>
+        </is>
+      </c>
+      <c r="E1486" t="n">
+        <v>774</v>
+      </c>
+      <c r="F1486" t="inlineStr"/>
+    </row>
+    <row r="1487">
+      <c r="A1487" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1487" t="inlineStr"/>
+      <c r="C1487" t="n">
+        <v>6990</v>
+      </c>
+      <c r="D1487" t="inlineStr">
+        <is>
+          <t>BOLAGSVERKET (INTERNET K0135</t>
+        </is>
+      </c>
+      <c r="E1487" t="n">
+        <v>700</v>
+      </c>
+      <c r="F1487" t="inlineStr"/>
+    </row>
+    <row r="1488">
+      <c r="A1488" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1488" t="inlineStr"/>
+      <c r="C1488" t="inlineStr"/>
+      <c r="D1488" t="inlineStr">
+        <is>
+          <t>BOLAGSVERKET (INTERNET K0135</t>
+        </is>
+      </c>
+      <c r="E1488" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1488" t="inlineStr"/>
+    </row>
+    <row r="1489">
+      <c r="A1489" s="2" t="n">
+        <v>44453</v>
+      </c>
+      <c r="B1489" t="inlineStr"/>
+      <c r="C1489" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1489" t="inlineStr">
+        <is>
+          <t>BOLAGSVERKET (INTERNET K0135</t>
+        </is>
+      </c>
+      <c r="E1489" t="inlineStr"/>
+      <c r="F1489" t="n">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1490" t="inlineStr">
+        <is>
+          <t>Reko268</t>
+        </is>
+      </c>
+      <c r="C1490" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1490" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703862550</t>
+        </is>
+      </c>
+      <c r="E1490" t="inlineStr"/>
+      <c r="F1490" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1491" t="inlineStr">
+        <is>
+          <t>Reko268</t>
+        </is>
+      </c>
+      <c r="C1491" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1491" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703862550</t>
+        </is>
+      </c>
+      <c r="E1491" t="inlineStr"/>
+      <c r="F1491" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1492" t="inlineStr">
+        <is>
+          <t>Reko268</t>
+        </is>
+      </c>
+      <c r="C1492" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1492" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703862550</t>
+        </is>
+      </c>
+      <c r="E1492" t="n">
+        <v>774</v>
+      </c>
+      <c r="F1492" t="inlineStr"/>
+    </row>
+    <row r="1493">
+      <c r="A1493" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1493" t="inlineStr">
+        <is>
+          <t>Reko269</t>
+        </is>
+      </c>
+      <c r="C1493" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1493" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702087212</t>
+        </is>
+      </c>
+      <c r="E1493" t="inlineStr"/>
+      <c r="F1493" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1494" t="inlineStr">
+        <is>
+          <t>Reko269</t>
+        </is>
+      </c>
+      <c r="C1494" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1494" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702087212</t>
+        </is>
+      </c>
+      <c r="E1494" t="inlineStr"/>
+      <c r="F1494" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1495" t="inlineStr">
+        <is>
+          <t>Reko269</t>
+        </is>
+      </c>
+      <c r="C1495" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1495" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702087212</t>
+        </is>
+      </c>
+      <c r="E1495" t="n">
+        <v>645</v>
+      </c>
+      <c r="F1495" t="inlineStr"/>
+    </row>
+    <row r="1496">
+      <c r="A1496" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1496" t="inlineStr">
+        <is>
+          <t>Reko270</t>
+        </is>
+      </c>
+      <c r="C1496" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1496" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739883614</t>
+        </is>
+      </c>
+      <c r="E1496" t="inlineStr"/>
+      <c r="F1496" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1497" t="inlineStr">
+        <is>
+          <t>Reko270</t>
+        </is>
+      </c>
+      <c r="C1497" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1497" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739883614</t>
+        </is>
+      </c>
+      <c r="E1497" t="inlineStr"/>
+      <c r="F1497" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1498" t="inlineStr">
+        <is>
+          <t>Reko270</t>
+        </is>
+      </c>
+      <c r="C1498" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1498" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739883614</t>
+        </is>
+      </c>
+      <c r="E1498" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1498" t="inlineStr"/>
+    </row>
+    <row r="1499">
+      <c r="A1499" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1499" t="inlineStr">
+        <is>
+          <t>Reko271</t>
+        </is>
+      </c>
+      <c r="C1499" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1499" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704545110</t>
+        </is>
+      </c>
+      <c r="E1499" t="inlineStr"/>
+      <c r="F1499" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1500" t="inlineStr">
+        <is>
+          <t>Reko271</t>
+        </is>
+      </c>
+      <c r="C1500" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1500" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704545110</t>
+        </is>
+      </c>
+      <c r="E1500" t="inlineStr"/>
+      <c r="F1500" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" s="2" t="n">
+        <v>44454</v>
+      </c>
+      <c r="B1501" t="inlineStr">
+        <is>
+          <t>Reko271</t>
+        </is>
+      </c>
+      <c r="C1501" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1501" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704545110</t>
+        </is>
+      </c>
+      <c r="E1501" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1501" t="inlineStr"/>
+    </row>
+    <row r="1502">
+      <c r="A1502" s="2" t="n">
+        <v>44455</v>
+      </c>
+      <c r="B1502" t="inlineStr">
+        <is>
+          <t>5162015</t>
+        </is>
+      </c>
+      <c r="C1502" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1502" t="inlineStr">
+        <is>
+          <t>Order 5162015 Swish +46703895060</t>
+        </is>
+      </c>
+      <c r="E1502" t="inlineStr"/>
+      <c r="F1502" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" s="2" t="n">
+        <v>44455</v>
+      </c>
+      <c r="B1503" t="inlineStr">
+        <is>
+          <t>5162015</t>
+        </is>
+      </c>
+      <c r="C1503" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1503" t="inlineStr">
+        <is>
+          <t>Order 5162015 Swish +46703895060</t>
+        </is>
+      </c>
+      <c r="E1503" t="inlineStr"/>
+      <c r="F1503" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" s="2" t="n">
+        <v>44455</v>
+      </c>
+      <c r="B1504" t="inlineStr">
+        <is>
+          <t>5162015</t>
+        </is>
+      </c>
+      <c r="C1504" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1504" t="inlineStr">
+        <is>
+          <t>Order 5162015 Swish +46703895060</t>
+        </is>
+      </c>
+      <c r="E1504" t="n">
+        <v>645</v>
+      </c>
+      <c r="F1504" t="inlineStr"/>
+    </row>
+    <row r="1505">
+      <c r="A1505" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1505" t="inlineStr"/>
+      <c r="C1505" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1505" t="inlineStr">
+        <is>
+          <t>FACEBK E3RA26XY62 K6885</t>
+        </is>
+      </c>
+      <c r="E1505" t="n">
+        <v>300</v>
+      </c>
+      <c r="F1505" t="inlineStr"/>
+    </row>
+    <row r="1506">
+      <c r="A1506" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1506" t="inlineStr"/>
+      <c r="C1506" t="inlineStr"/>
+      <c r="D1506" t="inlineStr">
+        <is>
+          <t>FACEBK E3RA26XY62 K6885</t>
+        </is>
+      </c>
+      <c r="E1506" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1506" t="inlineStr"/>
+    </row>
+    <row r="1507">
+      <c r="A1507" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1507" t="inlineStr"/>
+      <c r="C1507" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1507" t="inlineStr">
+        <is>
+          <t>FACEBK E3RA26XY62 K6885</t>
+        </is>
+      </c>
+      <c r="E1507" t="inlineStr"/>
+      <c r="F1507" t="n">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1508" t="inlineStr"/>
+      <c r="C1508" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1508" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1508" t="n">
+        <v>478.3</v>
+      </c>
+      <c r="F1508" t="inlineStr"/>
+    </row>
+    <row r="1509">
+      <c r="A1509" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1509" t="inlineStr"/>
+      <c r="C1509" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1509" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1509" t="n">
+        <v>57.4</v>
+      </c>
+      <c r="F1509" t="inlineStr"/>
+    </row>
+    <row r="1510">
+      <c r="A1510" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1510" t="inlineStr"/>
+      <c r="C1510" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1510" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1510" t="inlineStr"/>
+      <c r="F1510" t="n">
+        <v>535.7</v>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1511" t="inlineStr"/>
+      <c r="C1511" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1511" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1511" t="n">
+        <v>794.85</v>
+      </c>
+      <c r="F1511" t="inlineStr"/>
+    </row>
+    <row r="1512">
+      <c r="A1512" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1512" t="inlineStr"/>
+      <c r="C1512" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1512" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1512" t="n">
+        <v>198.71</v>
+      </c>
+      <c r="F1512" t="inlineStr"/>
+    </row>
+    <row r="1513">
+      <c r="A1513" s="2" t="n">
+        <v>44456</v>
+      </c>
+      <c r="B1513" t="inlineStr"/>
+      <c r="C1513" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1513" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1513" t="inlineStr"/>
+      <c r="F1513" t="n">
+        <v>993.5599999999999</v>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" s="2" t="n">
+        <v>44458</v>
+      </c>
+      <c r="B1514" t="inlineStr"/>
+      <c r="C1514" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1514" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1514" t="n">
+        <v>762.96</v>
+      </c>
+      <c r="F1514" t="inlineStr"/>
+    </row>
+    <row r="1515">
+      <c r="A1515" s="2" t="n">
+        <v>44458</v>
+      </c>
+      <c r="B1515" t="inlineStr"/>
+      <c r="C1515" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1515" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1515" t="n">
+        <v>190.74</v>
+      </c>
+      <c r="F1515" t="inlineStr"/>
+    </row>
+    <row r="1516">
+      <c r="A1516" s="2" t="n">
+        <v>44458</v>
+      </c>
+      <c r="B1516" t="inlineStr"/>
+      <c r="C1516" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1516" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1516" t="inlineStr"/>
+      <c r="F1516" t="n">
+        <v>953.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 24 new rows for week ending 2021-09-26 (total 1539 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1516"/>
+  <dimension ref="A1:F1540"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31885,6 +31885,480 @@
         <v>953.7</v>
       </c>
     </row>
+    <row r="1517">
+      <c r="A1517" s="2" t="n">
+        <v>44459</v>
+      </c>
+      <c r="B1517" t="inlineStr">
+        <is>
+          <t>Reko272</t>
+        </is>
+      </c>
+      <c r="C1517" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1517" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733987105</t>
+        </is>
+      </c>
+      <c r="E1517" t="inlineStr"/>
+      <c r="F1517" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" s="2" t="n">
+        <v>44459</v>
+      </c>
+      <c r="B1518" t="inlineStr">
+        <is>
+          <t>Reko272</t>
+        </is>
+      </c>
+      <c r="C1518" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1518" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733987105</t>
+        </is>
+      </c>
+      <c r="E1518" t="inlineStr"/>
+      <c r="F1518" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" s="2" t="n">
+        <v>44459</v>
+      </c>
+      <c r="B1519" t="inlineStr">
+        <is>
+          <t>Reko272</t>
+        </is>
+      </c>
+      <c r="C1519" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1519" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733987105</t>
+        </is>
+      </c>
+      <c r="E1519" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1519" t="inlineStr"/>
+    </row>
+    <row r="1520">
+      <c r="A1520" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1520" t="inlineStr">
+        <is>
+          <t>Reko273</t>
+        </is>
+      </c>
+      <c r="C1520" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1520" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723698764</t>
+        </is>
+      </c>
+      <c r="E1520" t="inlineStr"/>
+      <c r="F1520" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1521" t="inlineStr">
+        <is>
+          <t>Reko273</t>
+        </is>
+      </c>
+      <c r="C1521" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1521" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723698764</t>
+        </is>
+      </c>
+      <c r="E1521" t="inlineStr"/>
+      <c r="F1521" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1522" t="inlineStr">
+        <is>
+          <t>Reko273</t>
+        </is>
+      </c>
+      <c r="C1522" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1522" t="inlineStr">
+        <is>
+          <t>Reko Swish +46723698764</t>
+        </is>
+      </c>
+      <c r="E1522" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1522" t="inlineStr"/>
+    </row>
+    <row r="1523">
+      <c r="A1523" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1523" t="inlineStr">
+        <is>
+          <t>Reko274</t>
+        </is>
+      </c>
+      <c r="C1523" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1523" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E1523" t="inlineStr"/>
+      <c r="F1523" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1524" t="inlineStr">
+        <is>
+          <t>Reko274</t>
+        </is>
+      </c>
+      <c r="C1524" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1524" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E1524" t="inlineStr"/>
+      <c r="F1524" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1525" t="inlineStr">
+        <is>
+          <t>Reko274</t>
+        </is>
+      </c>
+      <c r="C1525" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1525" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E1525" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1525" t="inlineStr"/>
+    </row>
+    <row r="1526">
+      <c r="A1526" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1526" t="inlineStr">
+        <is>
+          <t>Reko275</t>
+        </is>
+      </c>
+      <c r="C1526" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1526" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1526" t="inlineStr"/>
+      <c r="F1526" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1527" t="inlineStr">
+        <is>
+          <t>Reko275</t>
+        </is>
+      </c>
+      <c r="C1527" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1527" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1527" t="inlineStr"/>
+      <c r="F1527" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" s="2" t="n">
+        <v>44461</v>
+      </c>
+      <c r="B1528" t="inlineStr">
+        <is>
+          <t>Reko275</t>
+        </is>
+      </c>
+      <c r="C1528" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1528" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703677212</t>
+        </is>
+      </c>
+      <c r="E1528" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1528" t="inlineStr"/>
+    </row>
+    <row r="1529">
+      <c r="A1529" s="2" t="n">
+        <v>44462</v>
+      </c>
+      <c r="B1529" t="inlineStr"/>
+      <c r="C1529" t="n">
+        <v>6540</v>
+      </c>
+      <c r="D1529" t="inlineStr">
+        <is>
+          <t>Klarna*kamda.se K0135</t>
+        </is>
+      </c>
+      <c r="E1529" t="n">
+        <v>479.2</v>
+      </c>
+      <c r="F1529" t="inlineStr"/>
+    </row>
+    <row r="1530">
+      <c r="A1530" s="2" t="n">
+        <v>44462</v>
+      </c>
+      <c r="B1530" t="inlineStr"/>
+      <c r="C1530" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1530" t="inlineStr">
+        <is>
+          <t>Klarna*kamda.se K0135</t>
+        </is>
+      </c>
+      <c r="E1530" t="n">
+        <v>119.8</v>
+      </c>
+      <c r="F1530" t="inlineStr"/>
+    </row>
+    <row r="1531">
+      <c r="A1531" s="2" t="n">
+        <v>44462</v>
+      </c>
+      <c r="B1531" t="inlineStr"/>
+      <c r="C1531" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1531" t="inlineStr">
+        <is>
+          <t>Klarna*kamda.se K0135</t>
+        </is>
+      </c>
+      <c r="E1531" t="inlineStr"/>
+      <c r="F1531" t="n">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B1532" t="inlineStr"/>
+      <c r="C1532" t="n">
+        <v>7010</v>
+      </c>
+      <c r="D1532" t="inlineStr">
+        <is>
+          <t>Lön September</t>
+        </is>
+      </c>
+      <c r="E1532" t="n">
+        <v>1317</v>
+      </c>
+      <c r="F1532" t="inlineStr"/>
+    </row>
+    <row r="1533">
+      <c r="A1533" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B1533" t="inlineStr"/>
+      <c r="C1533" t="inlineStr"/>
+      <c r="D1533" t="inlineStr">
+        <is>
+          <t>Lön September</t>
+        </is>
+      </c>
+      <c r="E1533" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1533" t="inlineStr"/>
+    </row>
+    <row r="1534">
+      <c r="A1534" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B1534" t="inlineStr"/>
+      <c r="C1534" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1534" t="inlineStr">
+        <is>
+          <t>Lön September</t>
+        </is>
+      </c>
+      <c r="E1534" t="inlineStr"/>
+      <c r="F1534" t="n">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B1535" t="inlineStr"/>
+      <c r="C1535" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1535" t="inlineStr">
+        <is>
+          <t>FACEBK FG24667Z62 K0135</t>
+        </is>
+      </c>
+      <c r="E1535" t="n">
+        <v>100</v>
+      </c>
+      <c r="F1535" t="inlineStr"/>
+    </row>
+    <row r="1536">
+      <c r="A1536" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B1536" t="inlineStr"/>
+      <c r="C1536" t="inlineStr"/>
+      <c r="D1536" t="inlineStr">
+        <is>
+          <t>FACEBK FG24667Z62 K0135</t>
+        </is>
+      </c>
+      <c r="E1536" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1536" t="inlineStr"/>
+    </row>
+    <row r="1537">
+      <c r="A1537" s="2" t="n">
+        <v>44464</v>
+      </c>
+      <c r="B1537" t="inlineStr"/>
+      <c r="C1537" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1537" t="inlineStr">
+        <is>
+          <t>FACEBK FG24667Z62 K0135</t>
+        </is>
+      </c>
+      <c r="E1537" t="inlineStr"/>
+      <c r="F1537" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" s="2" t="n">
+        <v>44465</v>
+      </c>
+      <c r="B1538" t="inlineStr"/>
+      <c r="C1538" t="n">
+        <v>7010</v>
+      </c>
+      <c r="D1538" t="inlineStr">
+        <is>
+          <t>Sinthu lön Septe</t>
+        </is>
+      </c>
+      <c r="E1538" t="n">
+        <v>4584</v>
+      </c>
+      <c r="F1538" t="inlineStr"/>
+    </row>
+    <row r="1539">
+      <c r="A1539" s="2" t="n">
+        <v>44465</v>
+      </c>
+      <c r="B1539" t="inlineStr"/>
+      <c r="C1539" t="inlineStr"/>
+      <c r="D1539" t="inlineStr">
+        <is>
+          <t>Sinthu lön Septe</t>
+        </is>
+      </c>
+      <c r="E1539" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1539" t="inlineStr"/>
+    </row>
+    <row r="1540">
+      <c r="A1540" s="2" t="n">
+        <v>44465</v>
+      </c>
+      <c r="B1540" t="inlineStr"/>
+      <c r="C1540" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1540" t="inlineStr">
+        <is>
+          <t>Sinthu lön Septe</t>
+        </is>
+      </c>
+      <c r="E1540" t="inlineStr"/>
+      <c r="F1540" t="n">
+        <v>4584</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 48 new rows for week ending 2021-10-03 (total 1587 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1540"/>
+  <dimension ref="A1:F1588"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -32359,6 +32359,1036 @@
         <v>4584</v>
       </c>
     </row>
+    <row r="1541">
+      <c r="A1541" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1541" t="inlineStr">
+        <is>
+          <t>Reko276</t>
+        </is>
+      </c>
+      <c r="C1541" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1541" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1541" t="inlineStr"/>
+      <c r="F1541" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1542" t="inlineStr">
+        <is>
+          <t>Reko276</t>
+        </is>
+      </c>
+      <c r="C1542" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1542" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1542" t="inlineStr"/>
+      <c r="F1542" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1543">
+      <c r="A1543" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1543" t="inlineStr">
+        <is>
+          <t>Reko276</t>
+        </is>
+      </c>
+      <c r="C1543" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1543" t="inlineStr">
+        <is>
+          <t>Reko Swish +46768598228</t>
+        </is>
+      </c>
+      <c r="E1543" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1543" t="inlineStr"/>
+    </row>
+    <row r="1544">
+      <c r="A1544" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1544" t="inlineStr">
+        <is>
+          <t>Reko277</t>
+        </is>
+      </c>
+      <c r="C1544" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1544" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705693806</t>
+        </is>
+      </c>
+      <c r="E1544" t="inlineStr"/>
+      <c r="F1544" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1545">
+      <c r="A1545" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1545" t="inlineStr">
+        <is>
+          <t>Reko277</t>
+        </is>
+      </c>
+      <c r="C1545" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1545" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705693806</t>
+        </is>
+      </c>
+      <c r="E1545" t="inlineStr"/>
+      <c r="F1545" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1546">
+      <c r="A1546" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1546" t="inlineStr">
+        <is>
+          <t>Reko277</t>
+        </is>
+      </c>
+      <c r="C1546" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1546" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705693806</t>
+        </is>
+      </c>
+      <c r="E1546" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1546" t="inlineStr"/>
+    </row>
+    <row r="1547">
+      <c r="A1547" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1547" t="inlineStr">
+        <is>
+          <t>Reko278</t>
+        </is>
+      </c>
+      <c r="C1547" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1547" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E1547" t="inlineStr"/>
+      <c r="F1547" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1548" t="inlineStr">
+        <is>
+          <t>Reko278</t>
+        </is>
+      </c>
+      <c r="C1548" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1548" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E1548" t="inlineStr"/>
+      <c r="F1548" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1549" t="inlineStr">
+        <is>
+          <t>Reko278</t>
+        </is>
+      </c>
+      <c r="C1549" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1549" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709528558</t>
+        </is>
+      </c>
+      <c r="E1549" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1549" t="inlineStr"/>
+    </row>
+    <row r="1550">
+      <c r="A1550" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1550" t="inlineStr">
+        <is>
+          <t>Reko279</t>
+        </is>
+      </c>
+      <c r="C1550" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1550" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1550" t="inlineStr"/>
+      <c r="F1550" t="n">
+        <v>70.54000000000001</v>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1551" t="inlineStr">
+        <is>
+          <t>Reko279</t>
+        </is>
+      </c>
+      <c r="C1551" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1551" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1551" t="inlineStr"/>
+      <c r="F1551" t="n">
+        <v>8.460000000000001</v>
+      </c>
+    </row>
+    <row r="1552">
+      <c r="A1552" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1552" t="inlineStr">
+        <is>
+          <t>Reko279</t>
+        </is>
+      </c>
+      <c r="C1552" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1552" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735011685</t>
+        </is>
+      </c>
+      <c r="E1552" t="n">
+        <v>79</v>
+      </c>
+      <c r="F1552" t="inlineStr"/>
+    </row>
+    <row r="1553">
+      <c r="A1553" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1553" t="inlineStr">
+        <is>
+          <t>Reko280</t>
+        </is>
+      </c>
+      <c r="C1553" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1553" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E1553" t="inlineStr"/>
+      <c r="F1553" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1554">
+      <c r="A1554" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1554" t="inlineStr">
+        <is>
+          <t>Reko280</t>
+        </is>
+      </c>
+      <c r="C1554" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1554" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E1554" t="inlineStr"/>
+      <c r="F1554" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1555">
+      <c r="A1555" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1555" t="inlineStr">
+        <is>
+          <t>Reko280</t>
+        </is>
+      </c>
+      <c r="C1555" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1555" t="inlineStr">
+        <is>
+          <t>Reko Swish +46725644740</t>
+        </is>
+      </c>
+      <c r="E1555" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1555" t="inlineStr"/>
+    </row>
+    <row r="1556">
+      <c r="A1556" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1556" t="inlineStr">
+        <is>
+          <t>Reko281</t>
+        </is>
+      </c>
+      <c r="C1556" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1556" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700391434</t>
+        </is>
+      </c>
+      <c r="E1556" t="inlineStr"/>
+      <c r="F1556" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="1557">
+      <c r="A1557" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1557" t="inlineStr">
+        <is>
+          <t>Reko281</t>
+        </is>
+      </c>
+      <c r="C1557" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1557" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700391434</t>
+        </is>
+      </c>
+      <c r="E1557" t="inlineStr"/>
+      <c r="F1557" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="1558">
+      <c r="A1558" s="2" t="n">
+        <v>44466</v>
+      </c>
+      <c r="B1558" t="inlineStr">
+        <is>
+          <t>Reko281</t>
+        </is>
+      </c>
+      <c r="C1558" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1558" t="inlineStr">
+        <is>
+          <t>Reko Swish +46700391434</t>
+        </is>
+      </c>
+      <c r="E1558" t="n">
+        <v>645</v>
+      </c>
+      <c r="F1558" t="inlineStr"/>
+    </row>
+    <row r="1559">
+      <c r="A1559" s="2" t="n">
+        <v>44468</v>
+      </c>
+      <c r="B1559" t="inlineStr">
+        <is>
+          <t>Reko282</t>
+        </is>
+      </c>
+      <c r="C1559" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1559" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760438</t>
+        </is>
+      </c>
+      <c r="E1559" t="inlineStr"/>
+      <c r="F1559" t="n">
+        <v>691.0700000000001</v>
+      </c>
+    </row>
+    <row r="1560">
+      <c r="A1560" s="2" t="n">
+        <v>44468</v>
+      </c>
+      <c r="B1560" t="inlineStr">
+        <is>
+          <t>Reko282</t>
+        </is>
+      </c>
+      <c r="C1560" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1560" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760438</t>
+        </is>
+      </c>
+      <c r="E1560" t="inlineStr"/>
+      <c r="F1560" t="n">
+        <v>82.93000000000001</v>
+      </c>
+    </row>
+    <row r="1561">
+      <c r="A1561" s="2" t="n">
+        <v>44468</v>
+      </c>
+      <c r="B1561" t="inlineStr">
+        <is>
+          <t>Reko282</t>
+        </is>
+      </c>
+      <c r="C1561" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1561" t="inlineStr">
+        <is>
+          <t>Reko Swish +46708760438</t>
+        </is>
+      </c>
+      <c r="E1561" t="n">
+        <v>774</v>
+      </c>
+      <c r="F1561" t="inlineStr"/>
+    </row>
+    <row r="1562">
+      <c r="A1562" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1562" t="inlineStr">
+        <is>
+          <t>6301514</t>
+        </is>
+      </c>
+      <c r="C1562" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1562" t="inlineStr">
+        <is>
+          <t>Order 6301514 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1562" t="inlineStr"/>
+      <c r="F1562" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1563">
+      <c r="A1563" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1563" t="inlineStr">
+        <is>
+          <t>6301514</t>
+        </is>
+      </c>
+      <c r="C1563" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1563" t="inlineStr">
+        <is>
+          <t>Order 6301514 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1563" t="inlineStr"/>
+      <c r="F1563" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1564">
+      <c r="A1564" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1564" t="inlineStr">
+        <is>
+          <t>6301514</t>
+        </is>
+      </c>
+      <c r="C1564" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1564" t="inlineStr">
+        <is>
+          <t>Order 6301514 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1564" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1564" t="inlineStr"/>
+    </row>
+    <row r="1565">
+      <c r="A1565" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1565" t="inlineStr">
+        <is>
+          <t>8301850</t>
+        </is>
+      </c>
+      <c r="C1565" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1565" t="inlineStr">
+        <is>
+          <t>Order 8301850 Swish +46793351577</t>
+        </is>
+      </c>
+      <c r="E1565" t="inlineStr"/>
+      <c r="F1565" t="n">
+        <v>774.11</v>
+      </c>
+    </row>
+    <row r="1566">
+      <c r="A1566" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1566" t="inlineStr">
+        <is>
+          <t>8301850</t>
+        </is>
+      </c>
+      <c r="C1566" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1566" t="inlineStr">
+        <is>
+          <t>Order 8301850 Swish +46793351577</t>
+        </is>
+      </c>
+      <c r="E1566" t="inlineStr"/>
+      <c r="F1566" t="n">
+        <v>92.89</v>
+      </c>
+    </row>
+    <row r="1567">
+      <c r="A1567" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1567" t="inlineStr">
+        <is>
+          <t>8301850</t>
+        </is>
+      </c>
+      <c r="C1567" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1567" t="inlineStr">
+        <is>
+          <t>Order 8301850 Swish +46793351577</t>
+        </is>
+      </c>
+      <c r="E1567" t="n">
+        <v>867</v>
+      </c>
+      <c r="F1567" t="inlineStr"/>
+    </row>
+    <row r="1568">
+      <c r="A1568" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1568" t="inlineStr">
+        <is>
+          <t>0302115</t>
+        </is>
+      </c>
+      <c r="C1568" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1568" t="inlineStr">
+        <is>
+          <t>Order 0302115 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1568" t="inlineStr"/>
+      <c r="F1568" t="n">
+        <v>883.9299999999999</v>
+      </c>
+    </row>
+    <row r="1569">
+      <c r="A1569" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1569" t="inlineStr">
+        <is>
+          <t>0302115</t>
+        </is>
+      </c>
+      <c r="C1569" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1569" t="inlineStr">
+        <is>
+          <t>Order 0302115 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1569" t="inlineStr"/>
+      <c r="F1569" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1570">
+      <c r="A1570" s="2" t="n">
+        <v>44469</v>
+      </c>
+      <c r="B1570" t="inlineStr">
+        <is>
+          <t>0302115</t>
+        </is>
+      </c>
+      <c r="C1570" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1570" t="inlineStr">
+        <is>
+          <t>Order 0302115 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1570" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1570" t="inlineStr"/>
+    </row>
+    <row r="1571">
+      <c r="A1571" s="2" t="n">
+        <v>44470</v>
+      </c>
+      <c r="B1571" t="inlineStr"/>
+      <c r="C1571" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1571" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K6885</t>
+        </is>
+      </c>
+      <c r="E1571" t="n">
+        <v>807.64</v>
+      </c>
+      <c r="F1571" t="inlineStr"/>
+    </row>
+    <row r="1572">
+      <c r="A1572" s="2" t="n">
+        <v>44470</v>
+      </c>
+      <c r="B1572" t="inlineStr"/>
+      <c r="C1572" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1572" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K6885</t>
+        </is>
+      </c>
+      <c r="E1572" t="n">
+        <v>96.92</v>
+      </c>
+      <c r="F1572" t="inlineStr"/>
+    </row>
+    <row r="1573">
+      <c r="A1573" s="2" t="n">
+        <v>44470</v>
+      </c>
+      <c r="B1573" t="inlineStr"/>
+      <c r="C1573" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1573" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K6885</t>
+        </is>
+      </c>
+      <c r="E1573" t="inlineStr"/>
+      <c r="F1573" t="n">
+        <v>904.5599999999999</v>
+      </c>
+    </row>
+    <row r="1574">
+      <c r="A1574" s="2" t="n">
+        <v>44471</v>
+      </c>
+      <c r="B1574" t="inlineStr">
+        <is>
+          <t>2022228</t>
+        </is>
+      </c>
+      <c r="C1574" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1574" t="inlineStr">
+        <is>
+          <t>Order 2022228 Swish +46733425054</t>
+        </is>
+      </c>
+      <c r="E1574" t="inlineStr"/>
+      <c r="F1574" t="n">
+        <v>610.71</v>
+      </c>
+    </row>
+    <row r="1575">
+      <c r="A1575" s="2" t="n">
+        <v>44471</v>
+      </c>
+      <c r="B1575" t="inlineStr">
+        <is>
+          <t>2022228</t>
+        </is>
+      </c>
+      <c r="C1575" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1575" t="inlineStr">
+        <is>
+          <t>Order 2022228 Swish +46733425054</t>
+        </is>
+      </c>
+      <c r="E1575" t="inlineStr"/>
+      <c r="F1575" t="n">
+        <v>73.29000000000001</v>
+      </c>
+    </row>
+    <row r="1576">
+      <c r="A1576" s="2" t="n">
+        <v>44471</v>
+      </c>
+      <c r="B1576" t="inlineStr">
+        <is>
+          <t>2022228</t>
+        </is>
+      </c>
+      <c r="C1576" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1576" t="inlineStr">
+        <is>
+          <t>Order 2022228 Swish +46733425054</t>
+        </is>
+      </c>
+      <c r="E1576" t="n">
+        <v>684</v>
+      </c>
+      <c r="F1576" t="inlineStr"/>
+    </row>
+    <row r="1577">
+      <c r="A1577" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1577" t="inlineStr">
+        <is>
+          <t>6031335</t>
+        </is>
+      </c>
+      <c r="C1577" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1577" t="inlineStr">
+        <is>
+          <t>Order 6031335 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1577" t="inlineStr"/>
+      <c r="F1577" t="n">
+        <v>953.5700000000001</v>
+      </c>
+    </row>
+    <row r="1578">
+      <c r="A1578" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1578" t="inlineStr">
+        <is>
+          <t>6031335</t>
+        </is>
+      </c>
+      <c r="C1578" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1578" t="inlineStr">
+        <is>
+          <t>Order 6031335 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1578" t="inlineStr"/>
+      <c r="F1578" t="n">
+        <v>114.43</v>
+      </c>
+    </row>
+    <row r="1579">
+      <c r="A1579" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1579" t="inlineStr">
+        <is>
+          <t>6031335</t>
+        </is>
+      </c>
+      <c r="C1579" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1579" t="inlineStr">
+        <is>
+          <t>Order 6031335 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1579" t="n">
+        <v>1068</v>
+      </c>
+      <c r="F1579" t="inlineStr"/>
+    </row>
+    <row r="1580">
+      <c r="A1580" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1580" t="inlineStr">
+        <is>
+          <t>6031943</t>
+        </is>
+      </c>
+      <c r="C1580" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1580" t="inlineStr">
+        <is>
+          <t>Order 6031943 Swish +46766346071</t>
+        </is>
+      </c>
+      <c r="E1580" t="inlineStr"/>
+      <c r="F1580" t="n">
+        <v>583.04</v>
+      </c>
+    </row>
+    <row r="1581">
+      <c r="A1581" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1581" t="inlineStr">
+        <is>
+          <t>6031943</t>
+        </is>
+      </c>
+      <c r="C1581" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1581" t="inlineStr">
+        <is>
+          <t>Order 6031943 Swish +46766346071</t>
+        </is>
+      </c>
+      <c r="E1581" t="inlineStr"/>
+      <c r="F1581" t="n">
+        <v>69.95999999999999</v>
+      </c>
+    </row>
+    <row r="1582">
+      <c r="A1582" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1582" t="inlineStr">
+        <is>
+          <t>6031943</t>
+        </is>
+      </c>
+      <c r="C1582" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1582" t="inlineStr">
+        <is>
+          <t>Order 6031943 Swish +46766346071</t>
+        </is>
+      </c>
+      <c r="E1582" t="n">
+        <v>653</v>
+      </c>
+      <c r="F1582" t="inlineStr"/>
+    </row>
+    <row r="1583">
+      <c r="A1583" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1583" t="inlineStr">
+        <is>
+          <t>7032050</t>
+        </is>
+      </c>
+      <c r="C1583" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1583" t="inlineStr">
+        <is>
+          <t>Order 7032050 Swish +46727774946</t>
+        </is>
+      </c>
+      <c r="E1583" t="inlineStr"/>
+      <c r="F1583" t="n">
+        <v>493.75</v>
+      </c>
+    </row>
+    <row r="1584">
+      <c r="A1584" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1584" t="inlineStr">
+        <is>
+          <t>7032050</t>
+        </is>
+      </c>
+      <c r="C1584" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1584" t="inlineStr">
+        <is>
+          <t>Order 7032050 Swish +46727774946</t>
+        </is>
+      </c>
+      <c r="E1584" t="inlineStr"/>
+      <c r="F1584" t="n">
+        <v>59.25</v>
+      </c>
+    </row>
+    <row r="1585">
+      <c r="A1585" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1585" t="inlineStr">
+        <is>
+          <t>7032050</t>
+        </is>
+      </c>
+      <c r="C1585" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1585" t="inlineStr">
+        <is>
+          <t>Order 7032050 Swish +46727774946</t>
+        </is>
+      </c>
+      <c r="E1585" t="n">
+        <v>553</v>
+      </c>
+      <c r="F1585" t="inlineStr"/>
+    </row>
+    <row r="1586">
+      <c r="A1586" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1586" t="inlineStr"/>
+      <c r="C1586" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1586" t="inlineStr">
+        <is>
+          <t>FACEBK 8B6RB63272 K6885</t>
+        </is>
+      </c>
+      <c r="E1586" t="n">
+        <v>440</v>
+      </c>
+      <c r="F1586" t="inlineStr"/>
+    </row>
+    <row r="1587">
+      <c r="A1587" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1587" t="inlineStr"/>
+      <c r="C1587" t="inlineStr"/>
+      <c r="D1587" t="inlineStr">
+        <is>
+          <t>FACEBK 8B6RB63272 K6885</t>
+        </is>
+      </c>
+      <c r="E1587" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1587" t="inlineStr"/>
+    </row>
+    <row r="1588">
+      <c r="A1588" s="2" t="n">
+        <v>44472</v>
+      </c>
+      <c r="B1588" t="inlineStr"/>
+      <c r="C1588" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1588" t="inlineStr">
+        <is>
+          <t>FACEBK 8B6RB63272 K6885</t>
+        </is>
+      </c>
+      <c r="E1588" t="inlineStr"/>
+      <c r="F1588" t="n">
+        <v>440</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 90 new rows for week ending 2021-10-10 (total 1677 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1588"/>
+  <dimension ref="A1:F1678"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33389,6 +33389,1878 @@
         <v>440</v>
       </c>
     </row>
+    <row r="1589">
+      <c r="A1589" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1589" t="inlineStr">
+        <is>
+          <t>0040830</t>
+        </is>
+      </c>
+      <c r="C1589" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1589" t="inlineStr">
+        <is>
+          <t>Order 0040830 Swish +46727815808</t>
+        </is>
+      </c>
+      <c r="E1589" t="inlineStr"/>
+      <c r="F1589" t="n">
+        <v>616.0700000000001</v>
+      </c>
+    </row>
+    <row r="1590">
+      <c r="A1590" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1590" t="inlineStr">
+        <is>
+          <t>0040830</t>
+        </is>
+      </c>
+      <c r="C1590" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1590" t="inlineStr">
+        <is>
+          <t>Order 0040830 Swish +46727815808</t>
+        </is>
+      </c>
+      <c r="E1590" t="inlineStr"/>
+      <c r="F1590" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="1591">
+      <c r="A1591" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1591" t="inlineStr">
+        <is>
+          <t>0040830</t>
+        </is>
+      </c>
+      <c r="C1591" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1591" t="inlineStr">
+        <is>
+          <t>Order 0040830 Swish +46727815808</t>
+        </is>
+      </c>
+      <c r="E1591" t="n">
+        <v>690</v>
+      </c>
+      <c r="F1591" t="inlineStr"/>
+    </row>
+    <row r="1592">
+      <c r="A1592" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1592" t="inlineStr">
+        <is>
+          <t>2041209</t>
+        </is>
+      </c>
+      <c r="C1592" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1592" t="inlineStr">
+        <is>
+          <t>Order 2041209 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1592" t="inlineStr"/>
+      <c r="F1592" t="n">
+        <v>918.75</v>
+      </c>
+    </row>
+    <row r="1593">
+      <c r="A1593" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1593" t="inlineStr">
+        <is>
+          <t>2041209</t>
+        </is>
+      </c>
+      <c r="C1593" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1593" t="inlineStr">
+        <is>
+          <t>Order 2041209 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1593" t="inlineStr"/>
+      <c r="F1593" t="n">
+        <v>110.25</v>
+      </c>
+    </row>
+    <row r="1594">
+      <c r="A1594" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1594" t="inlineStr">
+        <is>
+          <t>2041209</t>
+        </is>
+      </c>
+      <c r="C1594" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1594" t="inlineStr">
+        <is>
+          <t>Order 2041209 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1594" t="n">
+        <v>1029</v>
+      </c>
+      <c r="F1594" t="inlineStr"/>
+    </row>
+    <row r="1595">
+      <c r="A1595" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1595" t="inlineStr">
+        <is>
+          <t>Reko283</t>
+        </is>
+      </c>
+      <c r="C1595" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1595" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703191908</t>
+        </is>
+      </c>
+      <c r="E1595" t="inlineStr"/>
+      <c r="F1595" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1596">
+      <c r="A1596" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1596" t="inlineStr">
+        <is>
+          <t>Reko283</t>
+        </is>
+      </c>
+      <c r="C1596" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1596" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703191908</t>
+        </is>
+      </c>
+      <c r="E1596" t="inlineStr"/>
+      <c r="F1596" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1597">
+      <c r="A1597" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1597" t="inlineStr">
+        <is>
+          <t>Reko283</t>
+        </is>
+      </c>
+      <c r="C1597" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1597" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703191908</t>
+        </is>
+      </c>
+      <c r="E1597" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1597" t="inlineStr"/>
+    </row>
+    <row r="1598">
+      <c r="A1598" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1598" t="inlineStr">
+        <is>
+          <t>Reko284</t>
+        </is>
+      </c>
+      <c r="C1598" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1598" t="inlineStr">
+        <is>
+          <t>Reko Swish +46760844133</t>
+        </is>
+      </c>
+      <c r="E1598" t="inlineStr"/>
+      <c r="F1598" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1599">
+      <c r="A1599" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1599" t="inlineStr">
+        <is>
+          <t>Reko284</t>
+        </is>
+      </c>
+      <c r="C1599" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1599" t="inlineStr">
+        <is>
+          <t>Reko Swish +46760844133</t>
+        </is>
+      </c>
+      <c r="E1599" t="inlineStr"/>
+      <c r="F1599" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1600">
+      <c r="A1600" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1600" t="inlineStr">
+        <is>
+          <t>Reko284</t>
+        </is>
+      </c>
+      <c r="C1600" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1600" t="inlineStr">
+        <is>
+          <t>Reko Swish +46760844133</t>
+        </is>
+      </c>
+      <c r="E1600" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1600" t="inlineStr"/>
+    </row>
+    <row r="1601">
+      <c r="A1601" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1601" t="inlineStr">
+        <is>
+          <t>Reko285</t>
+        </is>
+      </c>
+      <c r="C1601" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1601" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733987105</t>
+        </is>
+      </c>
+      <c r="E1601" t="inlineStr"/>
+      <c r="F1601" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1602">
+      <c r="A1602" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1602" t="inlineStr">
+        <is>
+          <t>Reko285</t>
+        </is>
+      </c>
+      <c r="C1602" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1602" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733987105</t>
+        </is>
+      </c>
+      <c r="E1602" t="inlineStr"/>
+      <c r="F1602" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1603">
+      <c r="A1603" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1603" t="inlineStr">
+        <is>
+          <t>Reko285</t>
+        </is>
+      </c>
+      <c r="C1603" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1603" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733987105</t>
+        </is>
+      </c>
+      <c r="E1603" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1603" t="inlineStr"/>
+    </row>
+    <row r="1604">
+      <c r="A1604" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1604" t="inlineStr">
+        <is>
+          <t>Reko286</t>
+        </is>
+      </c>
+      <c r="C1604" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1604" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733500883</t>
+        </is>
+      </c>
+      <c r="E1604" t="inlineStr"/>
+      <c r="F1604" t="n">
+        <v>345.54</v>
+      </c>
+    </row>
+    <row r="1605">
+      <c r="A1605" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1605" t="inlineStr">
+        <is>
+          <t>Reko286</t>
+        </is>
+      </c>
+      <c r="C1605" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1605" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733500883</t>
+        </is>
+      </c>
+      <c r="E1605" t="inlineStr"/>
+      <c r="F1605" t="n">
+        <v>41.46</v>
+      </c>
+    </row>
+    <row r="1606">
+      <c r="A1606" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1606" t="inlineStr">
+        <is>
+          <t>Reko286</t>
+        </is>
+      </c>
+      <c r="C1606" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1606" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733500883</t>
+        </is>
+      </c>
+      <c r="E1606" t="n">
+        <v>387</v>
+      </c>
+      <c r="F1606" t="inlineStr"/>
+    </row>
+    <row r="1607">
+      <c r="A1607" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1607" t="inlineStr">
+        <is>
+          <t>Reko287</t>
+        </is>
+      </c>
+      <c r="C1607" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1607" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736136907</t>
+        </is>
+      </c>
+      <c r="E1607" t="inlineStr"/>
+      <c r="F1607" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1608">
+      <c r="A1608" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1608" t="inlineStr">
+        <is>
+          <t>Reko287</t>
+        </is>
+      </c>
+      <c r="C1608" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1608" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736136907</t>
+        </is>
+      </c>
+      <c r="E1608" t="inlineStr"/>
+      <c r="F1608" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1609">
+      <c r="A1609" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1609" t="inlineStr">
+        <is>
+          <t>Reko287</t>
+        </is>
+      </c>
+      <c r="C1609" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1609" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736136907</t>
+        </is>
+      </c>
+      <c r="E1609" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1609" t="inlineStr"/>
+    </row>
+    <row r="1610">
+      <c r="A1610" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1610" t="inlineStr">
+        <is>
+          <t>Reko288</t>
+        </is>
+      </c>
+      <c r="C1610" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1610" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737106645</t>
+        </is>
+      </c>
+      <c r="E1610" t="inlineStr"/>
+      <c r="F1610" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1611">
+      <c r="A1611" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1611" t="inlineStr">
+        <is>
+          <t>Reko288</t>
+        </is>
+      </c>
+      <c r="C1611" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1611" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737106645</t>
+        </is>
+      </c>
+      <c r="E1611" t="inlineStr"/>
+      <c r="F1611" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1612">
+      <c r="A1612" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1612" t="inlineStr">
+        <is>
+          <t>Reko288</t>
+        </is>
+      </c>
+      <c r="C1612" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1612" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737106645</t>
+        </is>
+      </c>
+      <c r="E1612" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1612" t="inlineStr"/>
+    </row>
+    <row r="1613">
+      <c r="A1613" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1613" t="inlineStr">
+        <is>
+          <t>Reko289</t>
+        </is>
+      </c>
+      <c r="C1613" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1613" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703841334</t>
+        </is>
+      </c>
+      <c r="E1613" t="inlineStr"/>
+      <c r="F1613" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1614">
+      <c r="A1614" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1614" t="inlineStr">
+        <is>
+          <t>Reko289</t>
+        </is>
+      </c>
+      <c r="C1614" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1614" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703841334</t>
+        </is>
+      </c>
+      <c r="E1614" t="inlineStr"/>
+      <c r="F1614" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1615">
+      <c r="A1615" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1615" t="inlineStr">
+        <is>
+          <t>Reko289</t>
+        </is>
+      </c>
+      <c r="C1615" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1615" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703841334</t>
+        </is>
+      </c>
+      <c r="E1615" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1615" t="inlineStr"/>
+    </row>
+    <row r="1616">
+      <c r="A1616" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1616" t="inlineStr">
+        <is>
+          <t>Reko290</t>
+        </is>
+      </c>
+      <c r="C1616" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1616" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706891114</t>
+        </is>
+      </c>
+      <c r="E1616" t="inlineStr"/>
+      <c r="F1616" t="n">
+        <v>185.71</v>
+      </c>
+    </row>
+    <row r="1617">
+      <c r="A1617" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1617" t="inlineStr">
+        <is>
+          <t>Reko290</t>
+        </is>
+      </c>
+      <c r="C1617" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1617" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706891114</t>
+        </is>
+      </c>
+      <c r="E1617" t="inlineStr"/>
+      <c r="F1617" t="n">
+        <v>22.29</v>
+      </c>
+    </row>
+    <row r="1618">
+      <c r="A1618" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1618" t="inlineStr">
+        <is>
+          <t>Reko290</t>
+        </is>
+      </c>
+      <c r="C1618" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1618" t="inlineStr">
+        <is>
+          <t>Reko Swish +46706891114</t>
+        </is>
+      </c>
+      <c r="E1618" t="n">
+        <v>208</v>
+      </c>
+      <c r="F1618" t="inlineStr"/>
+    </row>
+    <row r="1619">
+      <c r="A1619" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1619" t="inlineStr">
+        <is>
+          <t>Reko291</t>
+        </is>
+      </c>
+      <c r="C1619" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1619" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736634875</t>
+        </is>
+      </c>
+      <c r="E1619" t="inlineStr"/>
+      <c r="F1619" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1620">
+      <c r="A1620" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1620" t="inlineStr">
+        <is>
+          <t>Reko291</t>
+        </is>
+      </c>
+      <c r="C1620" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1620" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736634875</t>
+        </is>
+      </c>
+      <c r="E1620" t="inlineStr"/>
+      <c r="F1620" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1621">
+      <c r="A1621" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1621" t="inlineStr">
+        <is>
+          <t>Reko291</t>
+        </is>
+      </c>
+      <c r="C1621" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1621" t="inlineStr">
+        <is>
+          <t>Reko Swish +46736634875</t>
+        </is>
+      </c>
+      <c r="E1621" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1621" t="inlineStr"/>
+    </row>
+    <row r="1622">
+      <c r="A1622" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1622" t="inlineStr"/>
+      <c r="C1622" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1622" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1622" t="n">
+        <v>1467.92</v>
+      </c>
+      <c r="F1622" t="inlineStr"/>
+    </row>
+    <row r="1623">
+      <c r="A1623" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1623" t="inlineStr"/>
+      <c r="C1623" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1623" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1623" t="n">
+        <v>176.15</v>
+      </c>
+      <c r="F1623" t="inlineStr"/>
+    </row>
+    <row r="1624">
+      <c r="A1624" s="2" t="n">
+        <v>44473</v>
+      </c>
+      <c r="B1624" t="inlineStr"/>
+      <c r="C1624" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1624" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1624" t="inlineStr"/>
+      <c r="F1624" t="n">
+        <v>1644.07</v>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1625" t="inlineStr">
+        <is>
+          <t>Reko292</t>
+        </is>
+      </c>
+      <c r="C1625" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1625" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738941039</t>
+        </is>
+      </c>
+      <c r="E1625" t="inlineStr"/>
+      <c r="F1625" t="n">
+        <v>460.71</v>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1626" t="inlineStr">
+        <is>
+          <t>Reko292</t>
+        </is>
+      </c>
+      <c r="C1626" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1626" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738941039</t>
+        </is>
+      </c>
+      <c r="E1626" t="inlineStr"/>
+      <c r="F1626" t="n">
+        <v>55.29</v>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1627" t="inlineStr">
+        <is>
+          <t>Reko292</t>
+        </is>
+      </c>
+      <c r="C1627" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1627" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738941039</t>
+        </is>
+      </c>
+      <c r="E1627" t="n">
+        <v>516</v>
+      </c>
+      <c r="F1627" t="inlineStr"/>
+    </row>
+    <row r="1628">
+      <c r="A1628" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1628" t="inlineStr">
+        <is>
+          <t>Reko293</t>
+        </is>
+      </c>
+      <c r="C1628" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1628" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735309860</t>
+        </is>
+      </c>
+      <c r="E1628" t="inlineStr"/>
+      <c r="F1628" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1629" t="inlineStr">
+        <is>
+          <t>Reko293</t>
+        </is>
+      </c>
+      <c r="C1629" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1629" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735309860</t>
+        </is>
+      </c>
+      <c r="E1629" t="inlineStr"/>
+      <c r="F1629" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1630" t="inlineStr">
+        <is>
+          <t>Reko293</t>
+        </is>
+      </c>
+      <c r="C1630" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1630" t="inlineStr">
+        <is>
+          <t>Reko Swish +46735309860</t>
+        </is>
+      </c>
+      <c r="E1630" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1630" t="inlineStr"/>
+    </row>
+    <row r="1631">
+      <c r="A1631" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1631" t="inlineStr">
+        <is>
+          <t>Reko294</t>
+        </is>
+      </c>
+      <c r="C1631" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1631" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739065270</t>
+        </is>
+      </c>
+      <c r="E1631" t="inlineStr"/>
+      <c r="F1631" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1632" t="inlineStr">
+        <is>
+          <t>Reko294</t>
+        </is>
+      </c>
+      <c r="C1632" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1632" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739065270</t>
+        </is>
+      </c>
+      <c r="E1632" t="inlineStr"/>
+      <c r="F1632" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1633" t="inlineStr">
+        <is>
+          <t>Reko294</t>
+        </is>
+      </c>
+      <c r="C1633" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1633" t="inlineStr">
+        <is>
+          <t>Reko Swish +46739065270</t>
+        </is>
+      </c>
+      <c r="E1633" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1633" t="inlineStr"/>
+    </row>
+    <row r="1634">
+      <c r="A1634" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1634" t="inlineStr">
+        <is>
+          <t>Reko295</t>
+        </is>
+      </c>
+      <c r="C1634" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1634" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704561477</t>
+        </is>
+      </c>
+      <c r="E1634" t="inlineStr"/>
+      <c r="F1634" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1635" t="inlineStr">
+        <is>
+          <t>Reko295</t>
+        </is>
+      </c>
+      <c r="C1635" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1635" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704561477</t>
+        </is>
+      </c>
+      <c r="E1635" t="inlineStr"/>
+      <c r="F1635" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1636">
+      <c r="A1636" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1636" t="inlineStr">
+        <is>
+          <t>Reko295</t>
+        </is>
+      </c>
+      <c r="C1636" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1636" t="inlineStr">
+        <is>
+          <t>Reko Swish +46704561477</t>
+        </is>
+      </c>
+      <c r="E1636" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1636" t="inlineStr"/>
+    </row>
+    <row r="1637">
+      <c r="A1637" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1637" t="inlineStr">
+        <is>
+          <t>Reko296</t>
+        </is>
+      </c>
+      <c r="C1637" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1637" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733100116</t>
+        </is>
+      </c>
+      <c r="E1637" t="inlineStr"/>
+      <c r="F1637" t="n">
+        <v>230.36</v>
+      </c>
+    </row>
+    <row r="1638">
+      <c r="A1638" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1638" t="inlineStr">
+        <is>
+          <t>Reko296</t>
+        </is>
+      </c>
+      <c r="C1638" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1638" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733100116</t>
+        </is>
+      </c>
+      <c r="E1638" t="inlineStr"/>
+      <c r="F1638" t="n">
+        <v>27.64</v>
+      </c>
+    </row>
+    <row r="1639">
+      <c r="A1639" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1639" t="inlineStr">
+        <is>
+          <t>Reko296</t>
+        </is>
+      </c>
+      <c r="C1639" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1639" t="inlineStr">
+        <is>
+          <t>Reko Swish +46733100116</t>
+        </is>
+      </c>
+      <c r="E1639" t="n">
+        <v>258</v>
+      </c>
+      <c r="F1639" t="inlineStr"/>
+    </row>
+    <row r="1640">
+      <c r="A1640" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1640" t="inlineStr"/>
+      <c r="C1640" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1640" t="inlineStr">
+        <is>
+          <t>Storgrossen i Sverige K6885</t>
+        </is>
+      </c>
+      <c r="E1640" t="n">
+        <v>133.48</v>
+      </c>
+      <c r="F1640" t="inlineStr"/>
+    </row>
+    <row r="1641">
+      <c r="A1641" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1641" t="inlineStr"/>
+      <c r="C1641" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1641" t="inlineStr">
+        <is>
+          <t>Storgrossen i Sverige K6885</t>
+        </is>
+      </c>
+      <c r="E1641" t="n">
+        <v>16.02</v>
+      </c>
+      <c r="F1641" t="inlineStr"/>
+    </row>
+    <row r="1642">
+      <c r="A1642" s="2" t="n">
+        <v>44474</v>
+      </c>
+      <c r="B1642" t="inlineStr"/>
+      <c r="C1642" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1642" t="inlineStr">
+        <is>
+          <t>Storgrossen i Sverige K6885</t>
+        </is>
+      </c>
+      <c r="E1642" t="inlineStr"/>
+      <c r="F1642" t="n">
+        <v>149.5</v>
+      </c>
+    </row>
+    <row r="1643">
+      <c r="A1643" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1643" t="inlineStr">
+        <is>
+          <t>Reko297</t>
+        </is>
+      </c>
+      <c r="C1643" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1643" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E1643" t="inlineStr"/>
+      <c r="F1643" t="n">
+        <v>115.18</v>
+      </c>
+    </row>
+    <row r="1644">
+      <c r="A1644" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1644" t="inlineStr">
+        <is>
+          <t>Reko297</t>
+        </is>
+      </c>
+      <c r="C1644" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1644" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E1644" t="inlineStr"/>
+      <c r="F1644" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="1645">
+      <c r="A1645" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1645" t="inlineStr">
+        <is>
+          <t>Reko297</t>
+        </is>
+      </c>
+      <c r="C1645" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1645" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709906521</t>
+        </is>
+      </c>
+      <c r="E1645" t="n">
+        <v>129</v>
+      </c>
+      <c r="F1645" t="inlineStr"/>
+    </row>
+    <row r="1646">
+      <c r="A1646" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1646" t="inlineStr">
+        <is>
+          <t>0061105</t>
+        </is>
+      </c>
+      <c r="C1646" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1646" t="inlineStr">
+        <is>
+          <t>Order 0061105 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1646" t="inlineStr"/>
+      <c r="F1646" t="n">
+        <v>616.0699999999999</v>
+      </c>
+    </row>
+    <row r="1647">
+      <c r="A1647" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1647" t="inlineStr">
+        <is>
+          <t>0061105</t>
+        </is>
+      </c>
+      <c r="C1647" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1647" t="inlineStr">
+        <is>
+          <t>Order 0061105 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1647" t="inlineStr"/>
+      <c r="F1647" t="n">
+        <v>73.93000000000001</v>
+      </c>
+    </row>
+    <row r="1648">
+      <c r="A1648" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1648" t="inlineStr">
+        <is>
+          <t>0061105</t>
+        </is>
+      </c>
+      <c r="C1648" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1648" t="inlineStr">
+        <is>
+          <t>Order 0061105 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1648" t="n">
+        <v>690</v>
+      </c>
+      <c r="F1648" t="inlineStr"/>
+    </row>
+    <row r="1649">
+      <c r="A1649" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1649" t="inlineStr"/>
+      <c r="C1649" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1649" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E1649" t="n">
+        <v>187.23</v>
+      </c>
+      <c r="F1649" t="inlineStr"/>
+    </row>
+    <row r="1650">
+      <c r="A1650" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1650" t="inlineStr"/>
+      <c r="C1650" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1650" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E1650" t="n">
+        <v>22.47</v>
+      </c>
+      <c r="F1650" t="inlineStr"/>
+    </row>
+    <row r="1651">
+      <c r="A1651" s="2" t="n">
+        <v>44475</v>
+      </c>
+      <c r="B1651" t="inlineStr"/>
+      <c r="C1651" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1651" t="inlineStr">
+        <is>
+          <t>WILLYS STOCKHOLM VINST K0135</t>
+        </is>
+      </c>
+      <c r="E1651" t="inlineStr"/>
+      <c r="F1651" t="n">
+        <v>209.7</v>
+      </c>
+    </row>
+    <row r="1652">
+      <c r="A1652" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B1652" t="inlineStr"/>
+      <c r="C1652" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1652" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1652" t="n">
+        <v>487.47</v>
+      </c>
+      <c r="F1652" t="inlineStr"/>
+    </row>
+    <row r="1653">
+      <c r="A1653" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B1653" t="inlineStr"/>
+      <c r="C1653" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1653" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1653" t="n">
+        <v>58.5</v>
+      </c>
+      <c r="F1653" t="inlineStr"/>
+    </row>
+    <row r="1654">
+      <c r="A1654" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B1654" t="inlineStr"/>
+      <c r="C1654" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1654" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1654" t="inlineStr"/>
+      <c r="F1654" t="n">
+        <v>545.97</v>
+      </c>
+    </row>
+    <row r="1655">
+      <c r="A1655" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B1655" t="inlineStr"/>
+      <c r="C1655" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1655" t="inlineStr">
+        <is>
+          <t>STOCKHOLM NYA VEDDESTA K0135</t>
+        </is>
+      </c>
+      <c r="E1655" t="n">
+        <v>891.0700000000001</v>
+      </c>
+      <c r="F1655" t="inlineStr"/>
+    </row>
+    <row r="1656">
+      <c r="A1656" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B1656" t="inlineStr"/>
+      <c r="C1656" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1656" t="inlineStr">
+        <is>
+          <t>STOCKHOLM NYA VEDDESTA K0135</t>
+        </is>
+      </c>
+      <c r="E1656" t="n">
+        <v>106.93</v>
+      </c>
+      <c r="F1656" t="inlineStr"/>
+    </row>
+    <row r="1657">
+      <c r="A1657" s="2" t="n">
+        <v>44476</v>
+      </c>
+      <c r="B1657" t="inlineStr"/>
+      <c r="C1657" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1657" t="inlineStr">
+        <is>
+          <t>STOCKHOLM NYA VEDDESTA K0135</t>
+        </is>
+      </c>
+      <c r="E1657" t="inlineStr"/>
+      <c r="F1657" t="n">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="1658">
+      <c r="A1658" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="B1658" t="inlineStr">
+        <is>
+          <t>5082329</t>
+        </is>
+      </c>
+      <c r="C1658" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1658" t="inlineStr">
+        <is>
+          <t>Order 5082329 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1658" t="inlineStr"/>
+      <c r="F1658" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1659">
+      <c r="A1659" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="B1659" t="inlineStr">
+        <is>
+          <t>5082329</t>
+        </is>
+      </c>
+      <c r="C1659" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1659" t="inlineStr">
+        <is>
+          <t>Order 5082329 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1659" t="inlineStr"/>
+      <c r="F1659" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1660">
+      <c r="A1660" s="2" t="n">
+        <v>44477</v>
+      </c>
+      <c r="B1660" t="inlineStr">
+        <is>
+          <t>5082329</t>
+        </is>
+      </c>
+      <c r="C1660" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1660" t="inlineStr">
+        <is>
+          <t>Order 5082329 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1660" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1660" t="inlineStr"/>
+    </row>
+    <row r="1661">
+      <c r="A1661" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1661" t="inlineStr"/>
+      <c r="C1661" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1661" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1661" t="n">
+        <v>813.5</v>
+      </c>
+      <c r="F1661" t="inlineStr"/>
+    </row>
+    <row r="1662">
+      <c r="A1662" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1662" t="inlineStr"/>
+      <c r="C1662" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1662" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1662" t="n">
+        <v>97.62</v>
+      </c>
+      <c r="F1662" t="inlineStr"/>
+    </row>
+    <row r="1663">
+      <c r="A1663" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1663" t="inlineStr"/>
+      <c r="C1663" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1663" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1663" t="inlineStr"/>
+      <c r="F1663" t="n">
+        <v>911.12</v>
+      </c>
+    </row>
+    <row r="1664">
+      <c r="A1664" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1664" t="inlineStr"/>
+      <c r="C1664" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1664" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1664" t="n">
+        <v>905.46</v>
+      </c>
+      <c r="F1664" t="inlineStr"/>
+    </row>
+    <row r="1665">
+      <c r="A1665" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1665" t="inlineStr"/>
+      <c r="C1665" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1665" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1665" t="n">
+        <v>108.65</v>
+      </c>
+      <c r="F1665" t="inlineStr"/>
+    </row>
+    <row r="1666">
+      <c r="A1666" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1666" t="inlineStr"/>
+      <c r="C1666" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1666" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1666" t="inlineStr"/>
+      <c r="F1666" t="n">
+        <v>1014.11</v>
+      </c>
+    </row>
+    <row r="1667">
+      <c r="A1667" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1667" t="inlineStr"/>
+      <c r="C1667" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1667" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1667" t="n">
+        <v>408.63</v>
+      </c>
+      <c r="F1667" t="inlineStr"/>
+    </row>
+    <row r="1668">
+      <c r="A1668" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1668" t="inlineStr"/>
+      <c r="C1668" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1668" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1668" t="n">
+        <v>49.04</v>
+      </c>
+      <c r="F1668" t="inlineStr"/>
+    </row>
+    <row r="1669">
+      <c r="A1669" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1669" t="inlineStr"/>
+      <c r="C1669" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1669" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1669" t="inlineStr"/>
+      <c r="F1669" t="n">
+        <v>457.67</v>
+      </c>
+    </row>
+    <row r="1670">
+      <c r="A1670" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1670" t="inlineStr"/>
+      <c r="C1670" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1670" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1670" t="n">
+        <v>960.08</v>
+      </c>
+      <c r="F1670" t="inlineStr"/>
+    </row>
+    <row r="1671">
+      <c r="A1671" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1671" t="inlineStr"/>
+      <c r="C1671" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1671" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1671" t="n">
+        <v>240.02</v>
+      </c>
+      <c r="F1671" t="inlineStr"/>
+    </row>
+    <row r="1672">
+      <c r="A1672" s="2" t="n">
+        <v>44478</v>
+      </c>
+      <c r="B1672" t="inlineStr"/>
+      <c r="C1672" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1672" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1672" t="inlineStr"/>
+      <c r="F1672" t="n">
+        <v>1200.1</v>
+      </c>
+    </row>
+    <row r="1673">
+      <c r="A1673" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B1673" t="inlineStr">
+        <is>
+          <t>1101302</t>
+        </is>
+      </c>
+      <c r="C1673" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1673" t="inlineStr">
+        <is>
+          <t>Order 1101302 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1673" t="inlineStr"/>
+      <c r="F1673" t="n">
+        <v>1023.21</v>
+      </c>
+    </row>
+    <row r="1674">
+      <c r="A1674" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B1674" t="inlineStr">
+        <is>
+          <t>1101302</t>
+        </is>
+      </c>
+      <c r="C1674" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1674" t="inlineStr">
+        <is>
+          <t>Order 1101302 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1674" t="inlineStr"/>
+      <c r="F1674" t="n">
+        <v>122.79</v>
+      </c>
+    </row>
+    <row r="1675">
+      <c r="A1675" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B1675" t="inlineStr">
+        <is>
+          <t>1101302</t>
+        </is>
+      </c>
+      <c r="C1675" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1675" t="inlineStr">
+        <is>
+          <t>Order 1101302 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1675" t="n">
+        <v>1146</v>
+      </c>
+      <c r="F1675" t="inlineStr"/>
+    </row>
+    <row r="1676">
+      <c r="A1676" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B1676" t="inlineStr">
+        <is>
+          <t>5102120</t>
+        </is>
+      </c>
+      <c r="C1676" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1676" t="inlineStr">
+        <is>
+          <t>Order 5102120 Swish +46707445448</t>
+        </is>
+      </c>
+      <c r="E1676" t="inlineStr"/>
+      <c r="F1676" t="n">
+        <v>575.89</v>
+      </c>
+    </row>
+    <row r="1677">
+      <c r="A1677" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B1677" t="inlineStr">
+        <is>
+          <t>5102120</t>
+        </is>
+      </c>
+      <c r="C1677" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1677" t="inlineStr">
+        <is>
+          <t>Order 5102120 Swish +46707445448</t>
+        </is>
+      </c>
+      <c r="E1677" t="inlineStr"/>
+      <c r="F1677" t="n">
+        <v>69.11</v>
+      </c>
+    </row>
+    <row r="1678">
+      <c r="A1678" s="2" t="n">
+        <v>44479</v>
+      </c>
+      <c r="B1678" t="inlineStr">
+        <is>
+          <t>5102120</t>
+        </is>
+      </c>
+      <c r="C1678" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1678" t="inlineStr">
+        <is>
+          <t>Order 5102120 Swish +46707445448</t>
+        </is>
+      </c>
+      <c r="E1678" t="n">
+        <v>645</v>
+      </c>
+      <c r="F1678" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 27 new rows for week ending 2021-10-17 (total 1704 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1678"/>
+  <dimension ref="A1:F1705"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35261,6 +35261,562 @@
       </c>
       <c r="F1678" t="inlineStr"/>
     </row>
+    <row r="1679">
+      <c r="A1679" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1679" t="inlineStr"/>
+      <c r="C1679" t="n">
+        <v>7510</v>
+      </c>
+      <c r="D1679" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1679" t="n">
+        <v>2321</v>
+      </c>
+      <c r="F1679" t="inlineStr"/>
+    </row>
+    <row r="1680">
+      <c r="A1680" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1680" t="inlineStr"/>
+      <c r="C1680" t="inlineStr"/>
+      <c r="D1680" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1680" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1680" t="inlineStr"/>
+    </row>
+    <row r="1681">
+      <c r="A1681" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1681" t="inlineStr"/>
+      <c r="C1681" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1681" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1681" t="inlineStr"/>
+      <c r="F1681" t="n">
+        <v>2321</v>
+      </c>
+    </row>
+    <row r="1682">
+      <c r="A1682" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1682" t="inlineStr">
+        <is>
+          <t>Reko298</t>
+        </is>
+      </c>
+      <c r="C1682" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1682" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E1682" t="inlineStr"/>
+      <c r="F1682" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="1683">
+      <c r="A1683" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1683" t="inlineStr">
+        <is>
+          <t>Reko298</t>
+        </is>
+      </c>
+      <c r="C1683" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1683" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E1683" t="inlineStr"/>
+      <c r="F1683" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="1684">
+      <c r="A1684" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1684" t="inlineStr">
+        <is>
+          <t>Reko298</t>
+        </is>
+      </c>
+      <c r="C1684" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1684" t="inlineStr">
+        <is>
+          <t>Reko Swish +46738070018</t>
+        </is>
+      </c>
+      <c r="E1684" t="n">
+        <v>395</v>
+      </c>
+      <c r="F1684" t="inlineStr"/>
+    </row>
+    <row r="1685">
+      <c r="A1685" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1685" t="inlineStr">
+        <is>
+          <t>Reko299</t>
+        </is>
+      </c>
+      <c r="C1685" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1685" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978347</t>
+        </is>
+      </c>
+      <c r="E1685" t="inlineStr"/>
+      <c r="F1685" t="n">
+        <v>558.04</v>
+      </c>
+    </row>
+    <row r="1686">
+      <c r="A1686" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1686" t="inlineStr">
+        <is>
+          <t>Reko299</t>
+        </is>
+      </c>
+      <c r="C1686" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1686" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978347</t>
+        </is>
+      </c>
+      <c r="E1686" t="inlineStr"/>
+      <c r="F1686" t="n">
+        <v>66.95999999999999</v>
+      </c>
+    </row>
+    <row r="1687">
+      <c r="A1687" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1687" t="inlineStr">
+        <is>
+          <t>Reko299</t>
+        </is>
+      </c>
+      <c r="C1687" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1687" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978347</t>
+        </is>
+      </c>
+      <c r="E1687" t="n">
+        <v>625</v>
+      </c>
+      <c r="F1687" t="inlineStr"/>
+    </row>
+    <row r="1688">
+      <c r="A1688" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1688" t="inlineStr">
+        <is>
+          <t>Reko300</t>
+        </is>
+      </c>
+      <c r="C1688" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1688" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978347 Return</t>
+        </is>
+      </c>
+      <c r="E1688" t="n">
+        <v>558.04</v>
+      </c>
+      <c r="F1688" t="inlineStr"/>
+    </row>
+    <row r="1689">
+      <c r="A1689" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1689" t="inlineStr">
+        <is>
+          <t>Reko300</t>
+        </is>
+      </c>
+      <c r="C1689" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1689" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978347 Return</t>
+        </is>
+      </c>
+      <c r="E1689" t="n">
+        <v>66.95999999999999</v>
+      </c>
+      <c r="F1689" t="inlineStr"/>
+    </row>
+    <row r="1690">
+      <c r="A1690" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1690" t="inlineStr">
+        <is>
+          <t>Reko300</t>
+        </is>
+      </c>
+      <c r="C1690" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1690" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978347 Return</t>
+        </is>
+      </c>
+      <c r="E1690" t="inlineStr"/>
+      <c r="F1690" t="n">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="1691">
+      <c r="A1691" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1691" t="inlineStr">
+        <is>
+          <t>Reko301</t>
+        </is>
+      </c>
+      <c r="C1691" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1691" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737318059</t>
+        </is>
+      </c>
+      <c r="E1691" t="inlineStr"/>
+      <c r="F1691" t="n">
+        <v>141.07</v>
+      </c>
+    </row>
+    <row r="1692">
+      <c r="A1692" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1692" t="inlineStr">
+        <is>
+          <t>Reko301</t>
+        </is>
+      </c>
+      <c r="C1692" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1692" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737318059</t>
+        </is>
+      </c>
+      <c r="E1692" t="inlineStr"/>
+      <c r="F1692" t="n">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="1693">
+      <c r="A1693" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1693" t="inlineStr">
+        <is>
+          <t>Reko301</t>
+        </is>
+      </c>
+      <c r="C1693" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1693" t="inlineStr">
+        <is>
+          <t>Reko Swish +46737318059</t>
+        </is>
+      </c>
+      <c r="E1693" t="n">
+        <v>158</v>
+      </c>
+      <c r="F1693" t="inlineStr"/>
+    </row>
+    <row r="1694">
+      <c r="A1694" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1694" t="inlineStr"/>
+      <c r="C1694" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1694" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1694" t="n">
+        <v>721.4299999999999</v>
+      </c>
+      <c r="F1694" t="inlineStr"/>
+    </row>
+    <row r="1695">
+      <c r="A1695" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1695" t="inlineStr"/>
+      <c r="C1695" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1695" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1695" t="n">
+        <v>86.56999999999999</v>
+      </c>
+      <c r="F1695" t="inlineStr"/>
+    </row>
+    <row r="1696">
+      <c r="A1696" s="2" t="n">
+        <v>44480</v>
+      </c>
+      <c r="B1696" t="inlineStr"/>
+      <c r="C1696" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1696" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1696" t="inlineStr"/>
+      <c r="F1696" t="n">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="1697">
+      <c r="A1697" s="2" t="n">
+        <v>44481</v>
+      </c>
+      <c r="B1697" t="inlineStr"/>
+      <c r="C1697" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1697" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1697" t="n">
+        <v>851.88</v>
+      </c>
+      <c r="F1697" t="inlineStr"/>
+    </row>
+    <row r="1698">
+      <c r="A1698" s="2" t="n">
+        <v>44481</v>
+      </c>
+      <c r="B1698" t="inlineStr"/>
+      <c r="C1698" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1698" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1698" t="n">
+        <v>212.97</v>
+      </c>
+      <c r="F1698" t="inlineStr"/>
+    </row>
+    <row r="1699">
+      <c r="A1699" s="2" t="n">
+        <v>44481</v>
+      </c>
+      <c r="B1699" t="inlineStr"/>
+      <c r="C1699" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1699" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1699" t="inlineStr"/>
+      <c r="F1699" t="n">
+        <v>1064.85</v>
+      </c>
+    </row>
+    <row r="1700">
+      <c r="A1700" s="2" t="n">
+        <v>44483</v>
+      </c>
+      <c r="B1700" t="inlineStr">
+        <is>
+          <t>2141055</t>
+        </is>
+      </c>
+      <c r="C1700" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1700" t="inlineStr">
+        <is>
+          <t>Order 2141055 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1700" t="inlineStr"/>
+      <c r="F1700" t="n">
+        <v>193.75</v>
+      </c>
+    </row>
+    <row r="1701">
+      <c r="A1701" s="2" t="n">
+        <v>44483</v>
+      </c>
+      <c r="B1701" t="inlineStr">
+        <is>
+          <t>2141055</t>
+        </is>
+      </c>
+      <c r="C1701" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1701" t="inlineStr">
+        <is>
+          <t>Order 2141055 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1701" t="inlineStr"/>
+      <c r="F1701" t="n">
+        <v>23.25</v>
+      </c>
+    </row>
+    <row r="1702">
+      <c r="A1702" s="2" t="n">
+        <v>44483</v>
+      </c>
+      <c r="B1702" t="inlineStr">
+        <is>
+          <t>2141055</t>
+        </is>
+      </c>
+      <c r="C1702" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1702" t="inlineStr">
+        <is>
+          <t>Order 2141055 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1702" t="n">
+        <v>217</v>
+      </c>
+      <c r="F1702" t="inlineStr"/>
+    </row>
+    <row r="1703">
+      <c r="A1703" s="2" t="n">
+        <v>44486</v>
+      </c>
+      <c r="B1703" t="inlineStr">
+        <is>
+          <t>5172038</t>
+        </is>
+      </c>
+      <c r="C1703" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1703" t="inlineStr">
+        <is>
+          <t>Order 5172038 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1703" t="inlineStr"/>
+      <c r="F1703" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1704">
+      <c r="A1704" s="2" t="n">
+        <v>44486</v>
+      </c>
+      <c r="B1704" t="inlineStr">
+        <is>
+          <t>5172038</t>
+        </is>
+      </c>
+      <c r="C1704" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1704" t="inlineStr">
+        <is>
+          <t>Order 5172038 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1704" t="inlineStr"/>
+      <c r="F1704" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1705">
+      <c r="A1705" s="2" t="n">
+        <v>44486</v>
+      </c>
+      <c r="B1705" t="inlineStr">
+        <is>
+          <t>5172038</t>
+        </is>
+      </c>
+      <c r="C1705" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1705" t="inlineStr">
+        <is>
+          <t>Order 5172038 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1705" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1705" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 30 new rows for week ending 2021-10-24 (total 1734 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1705"/>
+  <dimension ref="A1:F1735"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35817,6 +35817,602 @@
       </c>
       <c r="F1705" t="inlineStr"/>
     </row>
+    <row r="1706">
+      <c r="A1706" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B1706" t="inlineStr">
+        <is>
+          <t>4182031</t>
+        </is>
+      </c>
+      <c r="C1706" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1706" t="inlineStr">
+        <is>
+          <t>Order 4182031 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1706" t="inlineStr"/>
+      <c r="F1706" t="n">
+        <v>685.71</v>
+      </c>
+    </row>
+    <row r="1707">
+      <c r="A1707" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B1707" t="inlineStr">
+        <is>
+          <t>4182031</t>
+        </is>
+      </c>
+      <c r="C1707" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1707" t="inlineStr">
+        <is>
+          <t>Order 4182031 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1707" t="inlineStr"/>
+      <c r="F1707" t="n">
+        <v>82.29000000000001</v>
+      </c>
+    </row>
+    <row r="1708">
+      <c r="A1708" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B1708" t="inlineStr">
+        <is>
+          <t>4182031</t>
+        </is>
+      </c>
+      <c r="C1708" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1708" t="inlineStr">
+        <is>
+          <t>Order 4182031 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1708" t="n">
+        <v>768</v>
+      </c>
+      <c r="F1708" t="inlineStr"/>
+    </row>
+    <row r="1709">
+      <c r="A1709" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B1709" t="inlineStr"/>
+      <c r="C1709" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1709" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K6885</t>
+        </is>
+      </c>
+      <c r="E1709" t="n">
+        <v>232.23</v>
+      </c>
+      <c r="F1709" t="inlineStr"/>
+    </row>
+    <row r="1710">
+      <c r="A1710" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B1710" t="inlineStr"/>
+      <c r="C1710" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1710" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K6885</t>
+        </is>
+      </c>
+      <c r="E1710" t="n">
+        <v>27.87</v>
+      </c>
+      <c r="F1710" t="inlineStr"/>
+    </row>
+    <row r="1711">
+      <c r="A1711" s="2" t="n">
+        <v>44487</v>
+      </c>
+      <c r="B1711" t="inlineStr"/>
+      <c r="C1711" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1711" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K6885</t>
+        </is>
+      </c>
+      <c r="E1711" t="inlineStr"/>
+      <c r="F1711" t="n">
+        <v>260.1</v>
+      </c>
+    </row>
+    <row r="1712">
+      <c r="A1712" s="2" t="n">
+        <v>44488</v>
+      </c>
+      <c r="B1712" t="inlineStr">
+        <is>
+          <t>7190943</t>
+        </is>
+      </c>
+      <c r="C1712" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1712" t="inlineStr">
+        <is>
+          <t>Order 7190943 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1712" t="inlineStr"/>
+      <c r="F1712" t="n">
+        <v>650.89</v>
+      </c>
+    </row>
+    <row r="1713">
+      <c r="A1713" s="2" t="n">
+        <v>44488</v>
+      </c>
+      <c r="B1713" t="inlineStr">
+        <is>
+          <t>7190943</t>
+        </is>
+      </c>
+      <c r="C1713" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1713" t="inlineStr">
+        <is>
+          <t>Order 7190943 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1713" t="inlineStr"/>
+      <c r="F1713" t="n">
+        <v>78.11</v>
+      </c>
+    </row>
+    <row r="1714">
+      <c r="A1714" s="2" t="n">
+        <v>44488</v>
+      </c>
+      <c r="B1714" t="inlineStr">
+        <is>
+          <t>7190943</t>
+        </is>
+      </c>
+      <c r="C1714" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1714" t="inlineStr">
+        <is>
+          <t>Order 7190943 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1714" t="n">
+        <v>729</v>
+      </c>
+      <c r="F1714" t="inlineStr"/>
+    </row>
+    <row r="1715">
+      <c r="A1715" s="2" t="n">
+        <v>44489</v>
+      </c>
+      <c r="B1715" t="inlineStr"/>
+      <c r="C1715" t="n">
+        <v>6570</v>
+      </c>
+      <c r="D1715" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1715" t="n">
+        <v>64.5</v>
+      </c>
+      <c r="F1715" t="inlineStr"/>
+    </row>
+    <row r="1716">
+      <c r="A1716" s="2" t="n">
+        <v>44489</v>
+      </c>
+      <c r="B1716" t="inlineStr"/>
+      <c r="C1716" t="inlineStr"/>
+      <c r="D1716" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1716" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1716" t="inlineStr"/>
+    </row>
+    <row r="1717">
+      <c r="A1717" s="2" t="n">
+        <v>44489</v>
+      </c>
+      <c r="B1717" t="inlineStr"/>
+      <c r="C1717" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1717" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1717" t="inlineStr"/>
+      <c r="F1717" t="n">
+        <v>64.5</v>
+      </c>
+    </row>
+    <row r="1718">
+      <c r="A1718" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1718" t="inlineStr">
+        <is>
+          <t>3211947</t>
+        </is>
+      </c>
+      <c r="C1718" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1718" t="inlineStr">
+        <is>
+          <t>Order 3211947 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1718" t="inlineStr"/>
+      <c r="F1718" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="1719">
+      <c r="A1719" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1719" t="inlineStr">
+        <is>
+          <t>3211947</t>
+        </is>
+      </c>
+      <c r="C1719" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1719" t="inlineStr">
+        <is>
+          <t>Order 3211947 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1719" t="inlineStr"/>
+      <c r="F1719" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="1720">
+      <c r="A1720" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1720" t="inlineStr">
+        <is>
+          <t>3211947</t>
+        </is>
+      </c>
+      <c r="C1720" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1720" t="inlineStr">
+        <is>
+          <t>Order 3211947 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1720" t="n">
+        <v>474</v>
+      </c>
+      <c r="F1720" t="inlineStr"/>
+    </row>
+    <row r="1721">
+      <c r="A1721" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1721" t="inlineStr"/>
+      <c r="C1721" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1721" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1721" t="n">
+        <v>625.66</v>
+      </c>
+      <c r="F1721" t="inlineStr"/>
+    </row>
+    <row r="1722">
+      <c r="A1722" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1722" t="inlineStr"/>
+      <c r="C1722" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1722" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1722" t="n">
+        <v>75.08</v>
+      </c>
+      <c r="F1722" t="inlineStr"/>
+    </row>
+    <row r="1723">
+      <c r="A1723" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1723" t="inlineStr"/>
+      <c r="C1723" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1723" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1723" t="inlineStr"/>
+      <c r="F1723" t="n">
+        <v>700.74</v>
+      </c>
+    </row>
+    <row r="1724">
+      <c r="A1724" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1724" t="inlineStr"/>
+      <c r="C1724" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1724" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1724" t="n">
+        <v>326.24</v>
+      </c>
+      <c r="F1724" t="inlineStr"/>
+    </row>
+    <row r="1725">
+      <c r="A1725" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1725" t="inlineStr"/>
+      <c r="C1725" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1725" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1725" t="n">
+        <v>39.15</v>
+      </c>
+      <c r="F1725" t="inlineStr"/>
+    </row>
+    <row r="1726">
+      <c r="A1726" s="2" t="n">
+        <v>44490</v>
+      </c>
+      <c r="B1726" t="inlineStr"/>
+      <c r="C1726" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1726" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1726" t="inlineStr"/>
+      <c r="F1726" t="n">
+        <v>365.39</v>
+      </c>
+    </row>
+    <row r="1727">
+      <c r="A1727" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B1727" t="inlineStr">
+        <is>
+          <t>5221941</t>
+        </is>
+      </c>
+      <c r="C1727" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1727" t="inlineStr">
+        <is>
+          <t>Order 5221941 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1727" t="inlineStr"/>
+      <c r="F1727" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1728">
+      <c r="A1728" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B1728" t="inlineStr">
+        <is>
+          <t>5221941</t>
+        </is>
+      </c>
+      <c r="C1728" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1728" t="inlineStr">
+        <is>
+          <t>Order 5221941 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1728" t="inlineStr"/>
+      <c r="F1728" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1729">
+      <c r="A1729" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B1729" t="inlineStr">
+        <is>
+          <t>5221941</t>
+        </is>
+      </c>
+      <c r="C1729" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1729" t="inlineStr">
+        <is>
+          <t>Order 5221941 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1729" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1729" t="inlineStr"/>
+    </row>
+    <row r="1730">
+      <c r="A1730" s="2" t="n">
+        <v>44492</v>
+      </c>
+      <c r="B1730" t="inlineStr">
+        <is>
+          <t>6231033</t>
+        </is>
+      </c>
+      <c r="C1730" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1730" t="inlineStr">
+        <is>
+          <t>Order 6231033 Swish +46769332411</t>
+        </is>
+      </c>
+      <c r="E1730" t="inlineStr"/>
+      <c r="F1730" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="1731">
+      <c r="A1731" s="2" t="n">
+        <v>44492</v>
+      </c>
+      <c r="B1731" t="inlineStr">
+        <is>
+          <t>6231033</t>
+        </is>
+      </c>
+      <c r="C1731" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1731" t="inlineStr">
+        <is>
+          <t>Order 6231033 Swish +46769332411</t>
+        </is>
+      </c>
+      <c r="E1731" t="inlineStr"/>
+      <c r="F1731" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="1732">
+      <c r="A1732" s="2" t="n">
+        <v>44492</v>
+      </c>
+      <c r="B1732" t="inlineStr">
+        <is>
+          <t>6231033</t>
+        </is>
+      </c>
+      <c r="C1732" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1732" t="inlineStr">
+        <is>
+          <t>Order 6231033 Swish +46769332411</t>
+        </is>
+      </c>
+      <c r="E1732" t="n">
+        <v>474</v>
+      </c>
+      <c r="F1732" t="inlineStr"/>
+    </row>
+    <row r="1733">
+      <c r="A1733" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B1733" t="inlineStr"/>
+      <c r="C1733" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1733" t="inlineStr">
+        <is>
+          <t>FACEBK LEWEZ6XY62 K6885</t>
+        </is>
+      </c>
+      <c r="E1733" t="n">
+        <v>430</v>
+      </c>
+      <c r="F1733" t="inlineStr"/>
+    </row>
+    <row r="1734">
+      <c r="A1734" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B1734" t="inlineStr"/>
+      <c r="C1734" t="inlineStr"/>
+      <c r="D1734" t="inlineStr">
+        <is>
+          <t>FACEBK LEWEZ6XY62 K6885</t>
+        </is>
+      </c>
+      <c r="E1734" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1734" t="inlineStr"/>
+    </row>
+    <row r="1735">
+      <c r="A1735" s="2" t="n">
+        <v>44491</v>
+      </c>
+      <c r="B1735" t="inlineStr"/>
+      <c r="C1735" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1735" t="inlineStr">
+        <is>
+          <t>FACEBK LEWEZ6XY62 K6885</t>
+        </is>
+      </c>
+      <c r="E1735" t="inlineStr"/>
+      <c r="F1735" t="n">
+        <v>430</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 33 new rows for week ending 2021-10-31 (total 1767 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1735"/>
+  <dimension ref="A1:F1768"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -36413,6 +36413,654 @@
         <v>430</v>
       </c>
     </row>
+    <row r="1736">
+      <c r="A1736" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B1736" t="inlineStr">
+        <is>
+          <t>8251330</t>
+        </is>
+      </c>
+      <c r="C1736" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1736" t="inlineStr">
+        <is>
+          <t>Order 8251330 Swish +46727815808</t>
+        </is>
+      </c>
+      <c r="E1736" t="inlineStr"/>
+      <c r="F1736" t="n">
+        <v>924.11</v>
+      </c>
+    </row>
+    <row r="1737">
+      <c r="A1737" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B1737" t="inlineStr">
+        <is>
+          <t>8251330</t>
+        </is>
+      </c>
+      <c r="C1737" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1737" t="inlineStr">
+        <is>
+          <t>Order 8251330 Swish +46727815808</t>
+        </is>
+      </c>
+      <c r="E1737" t="inlineStr"/>
+      <c r="F1737" t="n">
+        <v>110.89</v>
+      </c>
+    </row>
+    <row r="1738">
+      <c r="A1738" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B1738" t="inlineStr">
+        <is>
+          <t>8251330</t>
+        </is>
+      </c>
+      <c r="C1738" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1738" t="inlineStr">
+        <is>
+          <t>Order 8251330 Swish +46727815808</t>
+        </is>
+      </c>
+      <c r="E1738" t="n">
+        <v>1035</v>
+      </c>
+      <c r="F1738" t="inlineStr"/>
+    </row>
+    <row r="1739">
+      <c r="A1739" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B1739" t="inlineStr"/>
+      <c r="C1739" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1739" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K6885</t>
+        </is>
+      </c>
+      <c r="E1739" t="n">
+        <v>1023.71</v>
+      </c>
+      <c r="F1739" t="inlineStr"/>
+    </row>
+    <row r="1740">
+      <c r="A1740" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B1740" t="inlineStr"/>
+      <c r="C1740" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1740" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K6885</t>
+        </is>
+      </c>
+      <c r="E1740" t="n">
+        <v>122.85</v>
+      </c>
+      <c r="F1740" t="inlineStr"/>
+    </row>
+    <row r="1741">
+      <c r="A1741" s="2" t="n">
+        <v>44494</v>
+      </c>
+      <c r="B1741" t="inlineStr"/>
+      <c r="C1741" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1741" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K6885</t>
+        </is>
+      </c>
+      <c r="E1741" t="inlineStr"/>
+      <c r="F1741" t="n">
+        <v>1146.56</v>
+      </c>
+    </row>
+    <row r="1742">
+      <c r="A1742" s="2" t="n">
+        <v>44495</v>
+      </c>
+      <c r="B1742" t="inlineStr">
+        <is>
+          <t>0261144</t>
+        </is>
+      </c>
+      <c r="C1742" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1742" t="inlineStr">
+        <is>
+          <t>Order 0261144 Swish +46793351577</t>
+        </is>
+      </c>
+      <c r="E1742" t="inlineStr"/>
+      <c r="F1742" t="n">
+        <v>739.29</v>
+      </c>
+    </row>
+    <row r="1743">
+      <c r="A1743" s="2" t="n">
+        <v>44495</v>
+      </c>
+      <c r="B1743" t="inlineStr">
+        <is>
+          <t>0261144</t>
+        </is>
+      </c>
+      <c r="C1743" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1743" t="inlineStr">
+        <is>
+          <t>Order 0261144 Swish +46793351577</t>
+        </is>
+      </c>
+      <c r="E1743" t="inlineStr"/>
+      <c r="F1743" t="n">
+        <v>88.70999999999999</v>
+      </c>
+    </row>
+    <row r="1744">
+      <c r="A1744" s="2" t="n">
+        <v>44495</v>
+      </c>
+      <c r="B1744" t="inlineStr">
+        <is>
+          <t>0261144</t>
+        </is>
+      </c>
+      <c r="C1744" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1744" t="inlineStr">
+        <is>
+          <t>Order 0261144 Swish +46793351577</t>
+        </is>
+      </c>
+      <c r="E1744" t="n">
+        <v>828</v>
+      </c>
+      <c r="F1744" t="inlineStr"/>
+    </row>
+    <row r="1745">
+      <c r="A1745" s="2" t="n">
+        <v>44496</v>
+      </c>
+      <c r="B1745" t="inlineStr"/>
+      <c r="C1745" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1745" t="inlineStr">
+        <is>
+          <t>Fresh Life</t>
+        </is>
+      </c>
+      <c r="E1745" t="n">
+        <v>133.93</v>
+      </c>
+      <c r="F1745" t="inlineStr"/>
+    </row>
+    <row r="1746">
+      <c r="A1746" s="2" t="n">
+        <v>44496</v>
+      </c>
+      <c r="B1746" t="inlineStr"/>
+      <c r="C1746" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1746" t="inlineStr">
+        <is>
+          <t>Fresh Life</t>
+        </is>
+      </c>
+      <c r="E1746" t="n">
+        <v>16.07</v>
+      </c>
+      <c r="F1746" t="inlineStr"/>
+    </row>
+    <row r="1747">
+      <c r="A1747" s="2" t="n">
+        <v>44496</v>
+      </c>
+      <c r="B1747" t="inlineStr"/>
+      <c r="C1747" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1747" t="inlineStr">
+        <is>
+          <t>Fresh Life</t>
+        </is>
+      </c>
+      <c r="E1747" t="inlineStr"/>
+      <c r="F1747" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="1748">
+      <c r="A1748" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B1748" t="inlineStr">
+        <is>
+          <t>9281259</t>
+        </is>
+      </c>
+      <c r="C1748" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1748" t="inlineStr">
+        <is>
+          <t>Order 9281259 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1748" t="inlineStr"/>
+      <c r="F1748" t="n">
+        <v>883.9299999999999</v>
+      </c>
+    </row>
+    <row r="1749">
+      <c r="A1749" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B1749" t="inlineStr">
+        <is>
+          <t>9281259</t>
+        </is>
+      </c>
+      <c r="C1749" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1749" t="inlineStr">
+        <is>
+          <t>Order 9281259 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1749" t="inlineStr"/>
+      <c r="F1749" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1750">
+      <c r="A1750" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B1750" t="inlineStr">
+        <is>
+          <t>9281259</t>
+        </is>
+      </c>
+      <c r="C1750" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1750" t="inlineStr">
+        <is>
+          <t>Order 9281259 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1750" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1750" t="inlineStr"/>
+    </row>
+    <row r="1751">
+      <c r="A1751" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B1751" t="inlineStr"/>
+      <c r="C1751" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1751" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1751" t="n">
+        <v>180.78</v>
+      </c>
+      <c r="F1751" t="inlineStr"/>
+    </row>
+    <row r="1752">
+      <c r="A1752" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B1752" t="inlineStr"/>
+      <c r="C1752" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1752" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1752" t="n">
+        <v>21.69</v>
+      </c>
+      <c r="F1752" t="inlineStr"/>
+    </row>
+    <row r="1753">
+      <c r="A1753" s="2" t="n">
+        <v>44497</v>
+      </c>
+      <c r="B1753" t="inlineStr"/>
+      <c r="C1753" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1753" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1753" t="inlineStr"/>
+      <c r="F1753" t="n">
+        <v>202.47</v>
+      </c>
+    </row>
+    <row r="1754">
+      <c r="A1754" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B1754" t="inlineStr"/>
+      <c r="C1754" t="n">
+        <v>7010</v>
+      </c>
+      <c r="D1754" t="inlineStr">
+        <is>
+          <t>NEHA OCT LÖN</t>
+        </is>
+      </c>
+      <c r="E1754" t="n">
+        <v>2848</v>
+      </c>
+      <c r="F1754" t="inlineStr"/>
+    </row>
+    <row r="1755">
+      <c r="A1755" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B1755" t="inlineStr"/>
+      <c r="C1755" t="inlineStr"/>
+      <c r="D1755" t="inlineStr">
+        <is>
+          <t>NEHA OCT LÖN</t>
+        </is>
+      </c>
+      <c r="E1755" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1755" t="inlineStr"/>
+    </row>
+    <row r="1756">
+      <c r="A1756" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B1756" t="inlineStr"/>
+      <c r="C1756" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1756" t="inlineStr">
+        <is>
+          <t>NEHA OCT LÖN</t>
+        </is>
+      </c>
+      <c r="E1756" t="inlineStr"/>
+      <c r="F1756" t="n">
+        <v>2848</v>
+      </c>
+    </row>
+    <row r="1757">
+      <c r="A1757" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B1757" t="inlineStr">
+        <is>
+          <t>8291809</t>
+        </is>
+      </c>
+      <c r="C1757" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1757" t="inlineStr">
+        <is>
+          <t>Order 8291809 Swish +46705093344</t>
+        </is>
+      </c>
+      <c r="E1757" t="inlineStr"/>
+      <c r="F1757" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="1758">
+      <c r="A1758" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B1758" t="inlineStr">
+        <is>
+          <t>8291809</t>
+        </is>
+      </c>
+      <c r="C1758" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1758" t="inlineStr">
+        <is>
+          <t>Order 8291809 Swish +46705093344</t>
+        </is>
+      </c>
+      <c r="E1758" t="inlineStr"/>
+      <c r="F1758" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="1759">
+      <c r="A1759" s="2" t="n">
+        <v>44498</v>
+      </c>
+      <c r="B1759" t="inlineStr">
+        <is>
+          <t>8291809</t>
+        </is>
+      </c>
+      <c r="C1759" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1759" t="inlineStr">
+        <is>
+          <t>Order 8291809 Swish +46705093344</t>
+        </is>
+      </c>
+      <c r="E1759" t="n">
+        <v>474</v>
+      </c>
+      <c r="F1759" t="inlineStr"/>
+    </row>
+    <row r="1760">
+      <c r="A1760" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B1760" t="inlineStr"/>
+      <c r="C1760" t="n">
+        <v>7010</v>
+      </c>
+      <c r="D1760" t="inlineStr">
+        <is>
+          <t>Sinthu Lön Octob</t>
+        </is>
+      </c>
+      <c r="E1760" t="n">
+        <v>2757</v>
+      </c>
+      <c r="F1760" t="inlineStr"/>
+    </row>
+    <row r="1761">
+      <c r="A1761" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B1761" t="inlineStr"/>
+      <c r="C1761" t="inlineStr"/>
+      <c r="D1761" t="inlineStr">
+        <is>
+          <t>Sinthu Lön Octob</t>
+        </is>
+      </c>
+      <c r="E1761" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1761" t="inlineStr"/>
+    </row>
+    <row r="1762">
+      <c r="A1762" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B1762" t="inlineStr"/>
+      <c r="C1762" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1762" t="inlineStr">
+        <is>
+          <t>Sinthu Lön Octob</t>
+        </is>
+      </c>
+      <c r="E1762" t="inlineStr"/>
+      <c r="F1762" t="n">
+        <v>2757</v>
+      </c>
+    </row>
+    <row r="1763">
+      <c r="A1763" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B1763" t="inlineStr"/>
+      <c r="C1763" t="n">
+        <v>6540</v>
+      </c>
+      <c r="D1763" t="inlineStr">
+        <is>
+          <t>TWILIO.COM DUBLIN</t>
+        </is>
+      </c>
+      <c r="E1763" t="n">
+        <v>174.89</v>
+      </c>
+      <c r="F1763" t="inlineStr"/>
+    </row>
+    <row r="1764">
+      <c r="A1764" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B1764" t="inlineStr"/>
+      <c r="C1764" t="inlineStr"/>
+      <c r="D1764" t="inlineStr">
+        <is>
+          <t>TWILIO.COM DUBLIN</t>
+        </is>
+      </c>
+      <c r="E1764" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1764" t="inlineStr"/>
+    </row>
+    <row r="1765">
+      <c r="A1765" s="2" t="n">
+        <v>44499</v>
+      </c>
+      <c r="B1765" t="inlineStr"/>
+      <c r="C1765" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1765" t="inlineStr">
+        <is>
+          <t>TWILIO.COM DUBLIN</t>
+        </is>
+      </c>
+      <c r="E1765" t="inlineStr"/>
+      <c r="F1765" t="n">
+        <v>174.89</v>
+      </c>
+    </row>
+    <row r="1766">
+      <c r="A1766" s="2" t="n">
+        <v>44500</v>
+      </c>
+      <c r="B1766" t="inlineStr">
+        <is>
+          <t>8310827</t>
+        </is>
+      </c>
+      <c r="C1766" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1766" t="inlineStr">
+        <is>
+          <t>Order 8310827 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1766" t="inlineStr"/>
+      <c r="F1766" t="n">
+        <v>953.5700000000001</v>
+      </c>
+    </row>
+    <row r="1767">
+      <c r="A1767" s="2" t="n">
+        <v>44500</v>
+      </c>
+      <c r="B1767" t="inlineStr">
+        <is>
+          <t>8310827</t>
+        </is>
+      </c>
+      <c r="C1767" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1767" t="inlineStr">
+        <is>
+          <t>Order 8310827 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1767" t="inlineStr"/>
+      <c r="F1767" t="n">
+        <v>114.43</v>
+      </c>
+    </row>
+    <row r="1768">
+      <c r="A1768" s="2" t="n">
+        <v>44500</v>
+      </c>
+      <c r="B1768" t="inlineStr">
+        <is>
+          <t>8310827</t>
+        </is>
+      </c>
+      <c r="C1768" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1768" t="inlineStr">
+        <is>
+          <t>Order 8310827 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1768" t="n">
+        <v>1068</v>
+      </c>
+      <c r="F1768" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 21 new rows for week ending 2021-11-07 (total 1788 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1768"/>
+  <dimension ref="A1:F1789"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37061,6 +37061,418 @@
       </c>
       <c r="F1768" t="inlineStr"/>
     </row>
+    <row r="1769">
+      <c r="A1769" s="2" t="n">
+        <v>44501</v>
+      </c>
+      <c r="B1769" t="inlineStr">
+        <is>
+          <t>0010821</t>
+        </is>
+      </c>
+      <c r="C1769" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1769" t="inlineStr">
+        <is>
+          <t>Order 0010821 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1769" t="inlineStr"/>
+      <c r="F1769" t="n">
+        <v>988.39</v>
+      </c>
+    </row>
+    <row r="1770">
+      <c r="A1770" s="2" t="n">
+        <v>44501</v>
+      </c>
+      <c r="B1770" t="inlineStr">
+        <is>
+          <t>0010821</t>
+        </is>
+      </c>
+      <c r="C1770" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1770" t="inlineStr">
+        <is>
+          <t>Order 0010821 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1770" t="inlineStr"/>
+      <c r="F1770" t="n">
+        <v>118.61</v>
+      </c>
+    </row>
+    <row r="1771">
+      <c r="A1771" s="2" t="n">
+        <v>44501</v>
+      </c>
+      <c r="B1771" t="inlineStr">
+        <is>
+          <t>0010821</t>
+        </is>
+      </c>
+      <c r="C1771" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1771" t="inlineStr">
+        <is>
+          <t>Order 0010821 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1771" t="n">
+        <v>1107</v>
+      </c>
+      <c r="F1771" t="inlineStr"/>
+    </row>
+    <row r="1772">
+      <c r="A1772" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1772" t="inlineStr">
+        <is>
+          <t>3021432</t>
+        </is>
+      </c>
+      <c r="C1772" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1772" t="inlineStr">
+        <is>
+          <t>Order 3021432 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1772" t="inlineStr"/>
+      <c r="F1772" t="n">
+        <v>954.46</v>
+      </c>
+    </row>
+    <row r="1773">
+      <c r="A1773" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1773" t="inlineStr">
+        <is>
+          <t>3021432</t>
+        </is>
+      </c>
+      <c r="C1773" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1773" t="inlineStr">
+        <is>
+          <t>Order 3021432 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1773" t="inlineStr"/>
+      <c r="F1773" t="n">
+        <v>114.54</v>
+      </c>
+    </row>
+    <row r="1774">
+      <c r="A1774" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1774" t="inlineStr">
+        <is>
+          <t>3021432</t>
+        </is>
+      </c>
+      <c r="C1774" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1774" t="inlineStr">
+        <is>
+          <t>Order 3021432 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1774" t="n">
+        <v>1069</v>
+      </c>
+      <c r="F1774" t="inlineStr"/>
+    </row>
+    <row r="1775">
+      <c r="A1775" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1775" t="inlineStr"/>
+      <c r="C1775" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1775" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1775" t="n">
+        <v>425.89</v>
+      </c>
+      <c r="F1775" t="inlineStr"/>
+    </row>
+    <row r="1776">
+      <c r="A1776" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1776" t="inlineStr"/>
+      <c r="C1776" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1776" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1776" t="n">
+        <v>51.11</v>
+      </c>
+      <c r="F1776" t="inlineStr"/>
+    </row>
+    <row r="1777">
+      <c r="A1777" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1777" t="inlineStr"/>
+      <c r="C1777" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1777" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1777" t="inlineStr"/>
+      <c r="F1777" t="n">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="1778">
+      <c r="A1778" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1778" t="inlineStr"/>
+      <c r="C1778" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1778" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1778" t="n">
+        <v>1003.43</v>
+      </c>
+      <c r="F1778" t="inlineStr"/>
+    </row>
+    <row r="1779">
+      <c r="A1779" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1779" t="inlineStr"/>
+      <c r="C1779" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1779" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1779" t="n">
+        <v>250.86</v>
+      </c>
+      <c r="F1779" t="inlineStr"/>
+    </row>
+    <row r="1780">
+      <c r="A1780" s="2" t="n">
+        <v>44502</v>
+      </c>
+      <c r="B1780" t="inlineStr"/>
+      <c r="C1780" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1780" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1780" t="inlineStr"/>
+      <c r="F1780" t="n">
+        <v>1254.29</v>
+      </c>
+    </row>
+    <row r="1781">
+      <c r="A1781" s="2" t="n">
+        <v>44505</v>
+      </c>
+      <c r="B1781" t="inlineStr">
+        <is>
+          <t>5051209</t>
+        </is>
+      </c>
+      <c r="C1781" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1781" t="inlineStr">
+        <is>
+          <t>Order 5051209 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1781" t="inlineStr"/>
+      <c r="F1781" t="n">
+        <v>1238.39</v>
+      </c>
+    </row>
+    <row r="1782">
+      <c r="A1782" s="2" t="n">
+        <v>44505</v>
+      </c>
+      <c r="B1782" t="inlineStr">
+        <is>
+          <t>5051209</t>
+        </is>
+      </c>
+      <c r="C1782" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1782" t="inlineStr">
+        <is>
+          <t>Order 5051209 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1782" t="inlineStr"/>
+      <c r="F1782" t="n">
+        <v>148.61</v>
+      </c>
+    </row>
+    <row r="1783">
+      <c r="A1783" s="2" t="n">
+        <v>44505</v>
+      </c>
+      <c r="B1783" t="inlineStr">
+        <is>
+          <t>5051209</t>
+        </is>
+      </c>
+      <c r="C1783" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1783" t="inlineStr">
+        <is>
+          <t>Order 5051209 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1783" t="n">
+        <v>1387</v>
+      </c>
+      <c r="F1783" t="inlineStr"/>
+    </row>
+    <row r="1784">
+      <c r="A1784" s="2" t="n">
+        <v>44506</v>
+      </c>
+      <c r="B1784" t="inlineStr"/>
+      <c r="C1784" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1784" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1784" t="n">
+        <v>469.99</v>
+      </c>
+      <c r="F1784" t="inlineStr"/>
+    </row>
+    <row r="1785">
+      <c r="A1785" s="2" t="n">
+        <v>44506</v>
+      </c>
+      <c r="B1785" t="inlineStr"/>
+      <c r="C1785" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1785" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1785" t="n">
+        <v>56.4</v>
+      </c>
+      <c r="F1785" t="inlineStr"/>
+    </row>
+    <row r="1786">
+      <c r="A1786" s="2" t="n">
+        <v>44506</v>
+      </c>
+      <c r="B1786" t="inlineStr"/>
+      <c r="C1786" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1786" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1786" t="inlineStr"/>
+      <c r="F1786" t="n">
+        <v>526.39</v>
+      </c>
+    </row>
+    <row r="1787">
+      <c r="A1787" s="2" t="n">
+        <v>44507</v>
+      </c>
+      <c r="B1787" t="inlineStr"/>
+      <c r="C1787" t="n">
+        <v>6400</v>
+      </c>
+      <c r="D1787" t="inlineStr">
+        <is>
+          <t>GOOGLE *ADS4960863493 K0135</t>
+        </is>
+      </c>
+      <c r="E1787" t="n">
+        <v>162.82</v>
+      </c>
+      <c r="F1787" t="inlineStr"/>
+    </row>
+    <row r="1788">
+      <c r="A1788" s="2" t="n">
+        <v>44507</v>
+      </c>
+      <c r="B1788" t="inlineStr"/>
+      <c r="C1788" t="inlineStr"/>
+      <c r="D1788" t="inlineStr">
+        <is>
+          <t>GOOGLE *ADS4960863493 K0135</t>
+        </is>
+      </c>
+      <c r="E1788" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1788" t="inlineStr"/>
+    </row>
+    <row r="1789">
+      <c r="A1789" s="2" t="n">
+        <v>44507</v>
+      </c>
+      <c r="B1789" t="inlineStr"/>
+      <c r="C1789" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1789" t="inlineStr">
+        <is>
+          <t>GOOGLE *ADS4960863493 K0135</t>
+        </is>
+      </c>
+      <c r="E1789" t="inlineStr"/>
+      <c r="F1789" t="n">
+        <v>162.82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2021-11-14 (total 1794 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1789"/>
+  <dimension ref="A1:F1795"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37473,6 +37473,124 @@
         <v>162.82</v>
       </c>
     </row>
+    <row r="1790">
+      <c r="A1790" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="B1790" t="inlineStr">
+        <is>
+          <t>3121734</t>
+        </is>
+      </c>
+      <c r="C1790" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1790" t="inlineStr">
+        <is>
+          <t>Order 3121734 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1790" t="inlineStr"/>
+      <c r="F1790" t="n">
+        <v>1062.5</v>
+      </c>
+    </row>
+    <row r="1791">
+      <c r="A1791" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="B1791" t="inlineStr">
+        <is>
+          <t>3121734</t>
+        </is>
+      </c>
+      <c r="C1791" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1791" t="inlineStr">
+        <is>
+          <t>Order 3121734 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1791" t="inlineStr"/>
+      <c r="F1791" t="n">
+        <v>127.5</v>
+      </c>
+    </row>
+    <row r="1792">
+      <c r="A1792" s="2" t="n">
+        <v>44512</v>
+      </c>
+      <c r="B1792" t="inlineStr">
+        <is>
+          <t>3121734</t>
+        </is>
+      </c>
+      <c r="C1792" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1792" t="inlineStr">
+        <is>
+          <t>Order 3121734 Swish +46703564388</t>
+        </is>
+      </c>
+      <c r="E1792" t="n">
+        <v>1190</v>
+      </c>
+      <c r="F1792" t="inlineStr"/>
+    </row>
+    <row r="1793">
+      <c r="A1793" s="2" t="n">
+        <v>44514</v>
+      </c>
+      <c r="B1793" t="inlineStr"/>
+      <c r="C1793" t="n">
+        <v>7510</v>
+      </c>
+      <c r="D1793" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1793" t="n">
+        <v>2423</v>
+      </c>
+      <c r="F1793" t="inlineStr"/>
+    </row>
+    <row r="1794">
+      <c r="A1794" s="2" t="n">
+        <v>44514</v>
+      </c>
+      <c r="B1794" t="inlineStr"/>
+      <c r="C1794" t="inlineStr"/>
+      <c r="D1794" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1794" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1794" t="inlineStr"/>
+    </row>
+    <row r="1795">
+      <c r="A1795" s="2" t="n">
+        <v>44514</v>
+      </c>
+      <c r="B1795" t="inlineStr"/>
+      <c r="C1795" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1795" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1795" t="inlineStr"/>
+      <c r="F1795" t="n">
+        <v>2423</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 15 new rows for week ending 2021-11-21 (total 1809 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1795"/>
+  <dimension ref="A1:F1810"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37591,6 +37591,288 @@
         <v>2423</v>
       </c>
     </row>
+    <row r="1796">
+      <c r="A1796" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B1796" t="inlineStr"/>
+      <c r="C1796" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D1796" t="inlineStr">
+        <is>
+          <t>Hyra October</t>
+        </is>
+      </c>
+      <c r="E1796" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F1796" t="inlineStr"/>
+    </row>
+    <row r="1797">
+      <c r="A1797" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B1797" t="inlineStr"/>
+      <c r="C1797" t="inlineStr"/>
+      <c r="D1797" t="inlineStr">
+        <is>
+          <t>Hyra October</t>
+        </is>
+      </c>
+      <c r="E1797" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1797" t="inlineStr"/>
+    </row>
+    <row r="1798">
+      <c r="A1798" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B1798" t="inlineStr"/>
+      <c r="C1798" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1798" t="inlineStr">
+        <is>
+          <t>Hyra October</t>
+        </is>
+      </c>
+      <c r="E1798" t="inlineStr"/>
+      <c r="F1798" t="n">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="1799">
+      <c r="A1799" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B1799" t="inlineStr"/>
+      <c r="C1799" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D1799" t="inlineStr">
+        <is>
+          <t>Hyra September</t>
+        </is>
+      </c>
+      <c r="E1799" t="n">
+        <v>4166</v>
+      </c>
+      <c r="F1799" t="inlineStr"/>
+    </row>
+    <row r="1800">
+      <c r="A1800" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B1800" t="inlineStr"/>
+      <c r="C1800" t="inlineStr"/>
+      <c r="D1800" t="inlineStr">
+        <is>
+          <t>Hyra September</t>
+        </is>
+      </c>
+      <c r="E1800" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1800" t="inlineStr"/>
+    </row>
+    <row r="1801">
+      <c r="A1801" s="2" t="n">
+        <v>44515</v>
+      </c>
+      <c r="B1801" t="inlineStr"/>
+      <c r="C1801" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1801" t="inlineStr">
+        <is>
+          <t>Hyra September</t>
+        </is>
+      </c>
+      <c r="E1801" t="inlineStr"/>
+      <c r="F1801" t="n">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="1802">
+      <c r="A1802" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B1802" t="n">
+        <v>3480325</v>
+      </c>
+      <c r="C1802" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1802" t="inlineStr">
+        <is>
+          <t>Order 3480325</t>
+        </is>
+      </c>
+      <c r="E1802" t="inlineStr"/>
+      <c r="F1802" t="n">
+        <v>714.29</v>
+      </c>
+    </row>
+    <row r="1803">
+      <c r="A1803" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B1803" t="n">
+        <v>3480325</v>
+      </c>
+      <c r="C1803" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1803" t="inlineStr">
+        <is>
+          <t>Order 3480325</t>
+        </is>
+      </c>
+      <c r="E1803" t="inlineStr"/>
+      <c r="F1803" t="n">
+        <v>85.70999999999999</v>
+      </c>
+    </row>
+    <row r="1804">
+      <c r="A1804" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B1804" t="n">
+        <v>3480325</v>
+      </c>
+      <c r="C1804" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1804" t="inlineStr">
+        <is>
+          <t>Order 3480325</t>
+        </is>
+      </c>
+      <c r="E1804" t="n">
+        <v>800</v>
+      </c>
+      <c r="F1804" t="inlineStr"/>
+    </row>
+    <row r="1805">
+      <c r="A1805" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B1805" t="inlineStr"/>
+      <c r="C1805" t="n">
+        <v>7510</v>
+      </c>
+      <c r="D1805" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1805" t="n">
+        <v>2103</v>
+      </c>
+      <c r="F1805" t="inlineStr"/>
+    </row>
+    <row r="1806">
+      <c r="A1806" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B1806" t="inlineStr"/>
+      <c r="C1806" t="inlineStr"/>
+      <c r="D1806" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1806" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1806" t="inlineStr"/>
+    </row>
+    <row r="1807">
+      <c r="A1807" s="2" t="n">
+        <v>44517</v>
+      </c>
+      <c r="B1807" t="inlineStr"/>
+      <c r="C1807" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1807" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1807" t="inlineStr"/>
+      <c r="F1807" t="n">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="1808">
+      <c r="A1808" s="2" t="n">
+        <v>44519</v>
+      </c>
+      <c r="B1808" t="inlineStr">
+        <is>
+          <t>5191648</t>
+        </is>
+      </c>
+      <c r="C1808" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1808" t="inlineStr">
+        <is>
+          <t>Order 5191648 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1808" t="inlineStr"/>
+      <c r="F1808" t="n">
+        <v>562.5</v>
+      </c>
+    </row>
+    <row r="1809">
+      <c r="A1809" s="2" t="n">
+        <v>44519</v>
+      </c>
+      <c r="B1809" t="inlineStr">
+        <is>
+          <t>5191648</t>
+        </is>
+      </c>
+      <c r="C1809" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1809" t="inlineStr">
+        <is>
+          <t>Order 5191648 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1809" t="inlineStr"/>
+      <c r="F1809" t="n">
+        <v>67.5</v>
+      </c>
+    </row>
+    <row r="1810">
+      <c r="A1810" s="2" t="n">
+        <v>44519</v>
+      </c>
+      <c r="B1810" t="inlineStr">
+        <is>
+          <t>5191648</t>
+        </is>
+      </c>
+      <c r="C1810" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1810" t="inlineStr">
+        <is>
+          <t>Order 5191648 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1810" t="n">
+        <v>630</v>
+      </c>
+      <c r="F1810" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2021-11-28 (total 1812 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1810"/>
+  <dimension ref="A1:F1813"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37873,6 +37873,60 @@
       </c>
       <c r="F1810" t="inlineStr"/>
     </row>
+    <row r="1811">
+      <c r="A1811" s="2" t="n">
+        <v>44526</v>
+      </c>
+      <c r="B1811" t="inlineStr"/>
+      <c r="C1811" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1811" t="inlineStr">
+        <is>
+          <t>OKQ8 K0135</t>
+        </is>
+      </c>
+      <c r="E1811" t="n">
+        <v>517.36</v>
+      </c>
+      <c r="F1811" t="inlineStr"/>
+    </row>
+    <row r="1812">
+      <c r="A1812" s="2" t="n">
+        <v>44526</v>
+      </c>
+      <c r="B1812" t="inlineStr"/>
+      <c r="C1812" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1812" t="inlineStr">
+        <is>
+          <t>OKQ8 K0135</t>
+        </is>
+      </c>
+      <c r="E1812" t="n">
+        <v>129.34</v>
+      </c>
+      <c r="F1812" t="inlineStr"/>
+    </row>
+    <row r="1813">
+      <c r="A1813" s="2" t="n">
+        <v>44526</v>
+      </c>
+      <c r="B1813" t="inlineStr"/>
+      <c r="C1813" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1813" t="inlineStr">
+        <is>
+          <t>OKQ8 K0135</t>
+        </is>
+      </c>
+      <c r="E1813" t="inlineStr"/>
+      <c r="F1813" t="n">
+        <v>646.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2021-12-05 (total 1818 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1813"/>
+  <dimension ref="A1:F1819"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37927,6 +37927,138 @@
         <v>646.7</v>
       </c>
     </row>
+    <row r="1814">
+      <c r="A1814" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B1814" t="inlineStr">
+        <is>
+          <t>0301337</t>
+        </is>
+      </c>
+      <c r="C1814" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1814" t="inlineStr">
+        <is>
+          <t>Order 0301337 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1814" t="inlineStr"/>
+      <c r="F1814" t="n">
+        <v>720.54</v>
+      </c>
+    </row>
+    <row r="1815">
+      <c r="A1815" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B1815" t="inlineStr">
+        <is>
+          <t>0301337</t>
+        </is>
+      </c>
+      <c r="C1815" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1815" t="inlineStr">
+        <is>
+          <t>Order 0301337 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1815" t="inlineStr"/>
+      <c r="F1815" t="n">
+        <v>86.45999999999999</v>
+      </c>
+    </row>
+    <row r="1816">
+      <c r="A1816" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B1816" t="inlineStr">
+        <is>
+          <t>0301337</t>
+        </is>
+      </c>
+      <c r="C1816" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1816" t="inlineStr">
+        <is>
+          <t>Order 0301337 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1816" t="n">
+        <v>807</v>
+      </c>
+      <c r="F1816" t="inlineStr"/>
+    </row>
+    <row r="1817">
+      <c r="A1817" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B1817" t="inlineStr">
+        <is>
+          <t>9281260</t>
+        </is>
+      </c>
+      <c r="C1817" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1817" t="inlineStr">
+        <is>
+          <t>Order 9281260 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1817" t="inlineStr"/>
+      <c r="F1817" t="n">
+        <v>441.96</v>
+      </c>
+    </row>
+    <row r="1818">
+      <c r="A1818" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B1818" t="inlineStr">
+        <is>
+          <t>9281260</t>
+        </is>
+      </c>
+      <c r="C1818" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1818" t="inlineStr">
+        <is>
+          <t>Order 9281260 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1818" t="inlineStr"/>
+      <c r="F1818" t="n">
+        <v>53.04</v>
+      </c>
+    </row>
+    <row r="1819">
+      <c r="A1819" s="2" t="n">
+        <v>44530</v>
+      </c>
+      <c r="B1819" t="inlineStr">
+        <is>
+          <t>9281260</t>
+        </is>
+      </c>
+      <c r="C1819" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1819" t="inlineStr">
+        <is>
+          <t>Order 9281260 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1819" t="n">
+        <v>495</v>
+      </c>
+      <c r="F1819" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2021-12-12 (total 1824 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1819"/>
+  <dimension ref="A1:F1825"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38059,6 +38059,138 @@
       </c>
       <c r="F1819" t="inlineStr"/>
     </row>
+    <row r="1820">
+      <c r="A1820" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B1820" t="inlineStr">
+        <is>
+          <t>Reko302</t>
+        </is>
+      </c>
+      <c r="C1820" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1820" t="inlineStr">
+        <is>
+          <t>Reko Swish +46729661281</t>
+        </is>
+      </c>
+      <c r="E1820" t="inlineStr"/>
+      <c r="F1820" t="n">
+        <v>158.93</v>
+      </c>
+    </row>
+    <row r="1821">
+      <c r="A1821" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B1821" t="inlineStr">
+        <is>
+          <t>Reko302</t>
+        </is>
+      </c>
+      <c r="C1821" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1821" t="inlineStr">
+        <is>
+          <t>Reko Swish +46729661281</t>
+        </is>
+      </c>
+      <c r="E1821" t="inlineStr"/>
+      <c r="F1821" t="n">
+        <v>19.07</v>
+      </c>
+    </row>
+    <row r="1822">
+      <c r="A1822" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B1822" t="inlineStr">
+        <is>
+          <t>Reko302</t>
+        </is>
+      </c>
+      <c r="C1822" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1822" t="inlineStr">
+        <is>
+          <t>Reko Swish +46729661281</t>
+        </is>
+      </c>
+      <c r="E1822" t="n">
+        <v>178</v>
+      </c>
+      <c r="F1822" t="inlineStr"/>
+    </row>
+    <row r="1823">
+      <c r="A1823" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B1823" t="inlineStr">
+        <is>
+          <t>Reko303</t>
+        </is>
+      </c>
+      <c r="C1823" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1823" t="inlineStr">
+        <is>
+          <t>Reko Swish +46729661281 Return</t>
+        </is>
+      </c>
+      <c r="E1823" t="n">
+        <v>158.93</v>
+      </c>
+      <c r="F1823" t="inlineStr"/>
+    </row>
+    <row r="1824">
+      <c r="A1824" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B1824" t="inlineStr">
+        <is>
+          <t>Reko303</t>
+        </is>
+      </c>
+      <c r="C1824" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1824" t="inlineStr">
+        <is>
+          <t>Reko Swish +46729661281 Return</t>
+        </is>
+      </c>
+      <c r="E1824" t="n">
+        <v>19.07</v>
+      </c>
+      <c r="F1824" t="inlineStr"/>
+    </row>
+    <row r="1825">
+      <c r="A1825" s="2" t="n">
+        <v>44536</v>
+      </c>
+      <c r="B1825" t="inlineStr">
+        <is>
+          <t>Reko303</t>
+        </is>
+      </c>
+      <c r="C1825" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1825" t="inlineStr">
+        <is>
+          <t>Reko Swish +46729661281 Return</t>
+        </is>
+      </c>
+      <c r="E1825" t="inlineStr"/>
+      <c r="F1825" t="n">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 15 new rows for week ending 2021-12-19 (total 1839 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1825"/>
+  <dimension ref="A1:F1840"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38191,6 +38191,312 @@
         <v>178</v>
       </c>
     </row>
+    <row r="1826">
+      <c r="A1826" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1826" t="inlineStr">
+        <is>
+          <t>6082039</t>
+        </is>
+      </c>
+      <c r="C1826" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1826" t="inlineStr">
+        <is>
+          <t>Order 6082039 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1826" t="inlineStr"/>
+      <c r="F1826" t="n">
+        <v>459.82</v>
+      </c>
+    </row>
+    <row r="1827">
+      <c r="A1827" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1827" t="inlineStr">
+        <is>
+          <t>6082039</t>
+        </is>
+      </c>
+      <c r="C1827" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1827" t="inlineStr">
+        <is>
+          <t>Order 6082039 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1827" t="inlineStr"/>
+      <c r="F1827" t="n">
+        <v>55.18</v>
+      </c>
+    </row>
+    <row r="1828">
+      <c r="A1828" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1828" t="inlineStr">
+        <is>
+          <t>6082039</t>
+        </is>
+      </c>
+      <c r="C1828" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1828" t="inlineStr">
+        <is>
+          <t>Order 6082039 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1828" t="n">
+        <v>515</v>
+      </c>
+      <c r="F1828" t="inlineStr"/>
+    </row>
+    <row r="1829">
+      <c r="A1829" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1829" t="inlineStr">
+        <is>
+          <t>2141045</t>
+        </is>
+      </c>
+      <c r="C1829" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1829" t="inlineStr">
+        <is>
+          <t>Order 2141045 Swish +46704991461</t>
+        </is>
+      </c>
+      <c r="E1829" t="inlineStr"/>
+      <c r="F1829" t="n">
+        <v>265.18</v>
+      </c>
+    </row>
+    <row r="1830">
+      <c r="A1830" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1830" t="inlineStr">
+        <is>
+          <t>2141045</t>
+        </is>
+      </c>
+      <c r="C1830" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1830" t="inlineStr">
+        <is>
+          <t>Order 2141045 Swish +46704991461</t>
+        </is>
+      </c>
+      <c r="E1830" t="inlineStr"/>
+      <c r="F1830" t="n">
+        <v>31.82</v>
+      </c>
+    </row>
+    <row r="1831">
+      <c r="A1831" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1831" t="inlineStr">
+        <is>
+          <t>2141045</t>
+        </is>
+      </c>
+      <c r="C1831" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1831" t="inlineStr">
+        <is>
+          <t>Order 2141045 Swish +46704991461</t>
+        </is>
+      </c>
+      <c r="E1831" t="n">
+        <v>297</v>
+      </c>
+      <c r="F1831" t="inlineStr"/>
+    </row>
+    <row r="1832">
+      <c r="A1832" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1832" t="inlineStr"/>
+      <c r="C1832" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1832" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1832" t="n">
+        <v>417.9</v>
+      </c>
+      <c r="F1832" t="inlineStr"/>
+    </row>
+    <row r="1833">
+      <c r="A1833" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1833" t="inlineStr"/>
+      <c r="C1833" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1833" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1833" t="n">
+        <v>104.47</v>
+      </c>
+      <c r="F1833" t="inlineStr"/>
+    </row>
+    <row r="1834">
+      <c r="A1834" s="2" t="n">
+        <v>44544</v>
+      </c>
+      <c r="B1834" t="inlineStr"/>
+      <c r="C1834" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1834" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1834" t="inlineStr"/>
+      <c r="F1834" t="n">
+        <v>522.37</v>
+      </c>
+    </row>
+    <row r="1835">
+      <c r="A1835" s="2" t="n">
+        <v>44546</v>
+      </c>
+      <c r="B1835" t="inlineStr">
+        <is>
+          <t>3162016</t>
+        </is>
+      </c>
+      <c r="C1835" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1835" t="inlineStr">
+        <is>
+          <t>Order 3162016 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1835" t="inlineStr"/>
+      <c r="F1835" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1836">
+      <c r="A1836" s="2" t="n">
+        <v>44546</v>
+      </c>
+      <c r="B1836" t="inlineStr">
+        <is>
+          <t>3162016</t>
+        </is>
+      </c>
+      <c r="C1836" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1836" t="inlineStr">
+        <is>
+          <t>Order 3162016 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1836" t="inlineStr"/>
+      <c r="F1836" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1837">
+      <c r="A1837" s="2" t="n">
+        <v>44546</v>
+      </c>
+      <c r="B1837" t="inlineStr">
+        <is>
+          <t>3162016</t>
+        </is>
+      </c>
+      <c r="C1837" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1837" t="inlineStr">
+        <is>
+          <t>Order 3162016 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1837" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1837" t="inlineStr"/>
+    </row>
+    <row r="1838">
+      <c r="A1838" s="2" t="n">
+        <v>44548</v>
+      </c>
+      <c r="B1838" t="inlineStr"/>
+      <c r="C1838" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1838" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1838" t="n">
+        <v>465.33</v>
+      </c>
+      <c r="F1838" t="inlineStr"/>
+    </row>
+    <row r="1839">
+      <c r="A1839" s="2" t="n">
+        <v>44548</v>
+      </c>
+      <c r="B1839" t="inlineStr"/>
+      <c r="C1839" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1839" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1839" t="n">
+        <v>55.84</v>
+      </c>
+      <c r="F1839" t="inlineStr"/>
+    </row>
+    <row r="1840">
+      <c r="A1840" s="2" t="n">
+        <v>44548</v>
+      </c>
+      <c r="B1840" t="inlineStr"/>
+      <c r="C1840" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1840" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1840" t="inlineStr"/>
+      <c r="F1840" t="n">
+        <v>521.17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 21 new rows for week ending 2021-12-26 (total 1860 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1840"/>
+  <dimension ref="A1:F1861"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38497,6 +38497,468 @@
         <v>521.17</v>
       </c>
     </row>
+    <row r="1841">
+      <c r="A1841" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1841" t="inlineStr">
+        <is>
+          <t>Reko304</t>
+        </is>
+      </c>
+      <c r="C1841" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1841" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978496</t>
+        </is>
+      </c>
+      <c r="E1841" t="inlineStr"/>
+      <c r="F1841" t="n">
+        <v>193.75</v>
+      </c>
+    </row>
+    <row r="1842">
+      <c r="A1842" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1842" t="inlineStr">
+        <is>
+          <t>Reko304</t>
+        </is>
+      </c>
+      <c r="C1842" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1842" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978496</t>
+        </is>
+      </c>
+      <c r="E1842" t="inlineStr"/>
+      <c r="F1842" t="n">
+        <v>23.25</v>
+      </c>
+    </row>
+    <row r="1843">
+      <c r="A1843" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1843" t="inlineStr">
+        <is>
+          <t>Reko304</t>
+        </is>
+      </c>
+      <c r="C1843" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1843" t="inlineStr">
+        <is>
+          <t>Reko Swish +46705978496</t>
+        </is>
+      </c>
+      <c r="E1843" t="n">
+        <v>217</v>
+      </c>
+      <c r="F1843" t="inlineStr"/>
+    </row>
+    <row r="1844">
+      <c r="A1844" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1844" t="inlineStr">
+        <is>
+          <t>Reko305</t>
+        </is>
+      </c>
+      <c r="C1844" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1844" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E1844" t="inlineStr"/>
+      <c r="F1844" t="n">
+        <v>174.11</v>
+      </c>
+    </row>
+    <row r="1845">
+      <c r="A1845" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1845" t="inlineStr">
+        <is>
+          <t>Reko305</t>
+        </is>
+      </c>
+      <c r="C1845" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1845" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E1845" t="inlineStr"/>
+      <c r="F1845" t="n">
+        <v>20.89</v>
+      </c>
+    </row>
+    <row r="1846">
+      <c r="A1846" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1846" t="inlineStr">
+        <is>
+          <t>Reko305</t>
+        </is>
+      </c>
+      <c r="C1846" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1846" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709941173</t>
+        </is>
+      </c>
+      <c r="E1846" t="n">
+        <v>195</v>
+      </c>
+      <c r="F1846" t="inlineStr"/>
+    </row>
+    <row r="1847">
+      <c r="A1847" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1847" t="inlineStr">
+        <is>
+          <t>Reko306</t>
+        </is>
+      </c>
+      <c r="C1847" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1847" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1847" t="inlineStr"/>
+      <c r="F1847" t="n">
+        <v>176.79</v>
+      </c>
+    </row>
+    <row r="1848">
+      <c r="A1848" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1848" t="inlineStr">
+        <is>
+          <t>Reko306</t>
+        </is>
+      </c>
+      <c r="C1848" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1848" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1848" t="inlineStr"/>
+      <c r="F1848" t="n">
+        <v>21.21</v>
+      </c>
+    </row>
+    <row r="1849">
+      <c r="A1849" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1849" t="inlineStr">
+        <is>
+          <t>Reko306</t>
+        </is>
+      </c>
+      <c r="C1849" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1849" t="inlineStr">
+        <is>
+          <t>Reko Swish +46703533270</t>
+        </is>
+      </c>
+      <c r="E1849" t="n">
+        <v>198</v>
+      </c>
+      <c r="F1849" t="inlineStr"/>
+    </row>
+    <row r="1850">
+      <c r="A1850" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1850" t="inlineStr">
+        <is>
+          <t>Reko307</t>
+        </is>
+      </c>
+      <c r="C1850" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1850" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707532445</t>
+        </is>
+      </c>
+      <c r="E1850" t="inlineStr"/>
+      <c r="F1850" t="n">
+        <v>265.18</v>
+      </c>
+    </row>
+    <row r="1851">
+      <c r="A1851" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1851" t="inlineStr">
+        <is>
+          <t>Reko307</t>
+        </is>
+      </c>
+      <c r="C1851" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1851" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707532445</t>
+        </is>
+      </c>
+      <c r="E1851" t="inlineStr"/>
+      <c r="F1851" t="n">
+        <v>31.82</v>
+      </c>
+    </row>
+    <row r="1852">
+      <c r="A1852" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1852" t="inlineStr">
+        <is>
+          <t>Reko307</t>
+        </is>
+      </c>
+      <c r="C1852" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1852" t="inlineStr">
+        <is>
+          <t>Reko Swish +46707532445</t>
+        </is>
+      </c>
+      <c r="E1852" t="n">
+        <v>297</v>
+      </c>
+      <c r="F1852" t="inlineStr"/>
+    </row>
+    <row r="1853">
+      <c r="A1853" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1853" t="inlineStr">
+        <is>
+          <t>Reko308</t>
+        </is>
+      </c>
+      <c r="C1853" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1853" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E1853" t="inlineStr"/>
+      <c r="F1853" t="n">
+        <v>265.18</v>
+      </c>
+    </row>
+    <row r="1854">
+      <c r="A1854" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1854" t="inlineStr">
+        <is>
+          <t>Reko308</t>
+        </is>
+      </c>
+      <c r="C1854" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1854" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E1854" t="inlineStr"/>
+      <c r="F1854" t="n">
+        <v>31.82</v>
+      </c>
+    </row>
+    <row r="1855">
+      <c r="A1855" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1855" t="inlineStr">
+        <is>
+          <t>Reko308</t>
+        </is>
+      </c>
+      <c r="C1855" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1855" t="inlineStr">
+        <is>
+          <t>Reko Swish +46709927597</t>
+        </is>
+      </c>
+      <c r="E1855" t="n">
+        <v>297</v>
+      </c>
+      <c r="F1855" t="inlineStr"/>
+    </row>
+    <row r="1856">
+      <c r="A1856" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1856" t="inlineStr">
+        <is>
+          <t>Reko309</t>
+        </is>
+      </c>
+      <c r="C1856" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1856" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702390837</t>
+        </is>
+      </c>
+      <c r="E1856" t="inlineStr"/>
+      <c r="F1856" t="n">
+        <v>158.04</v>
+      </c>
+    </row>
+    <row r="1857">
+      <c r="A1857" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1857" t="inlineStr">
+        <is>
+          <t>Reko309</t>
+        </is>
+      </c>
+      <c r="C1857" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1857" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702390837</t>
+        </is>
+      </c>
+      <c r="E1857" t="inlineStr"/>
+      <c r="F1857" t="n">
+        <v>18.96</v>
+      </c>
+    </row>
+    <row r="1858">
+      <c r="A1858" s="2" t="n">
+        <v>44550</v>
+      </c>
+      <c r="B1858" t="inlineStr">
+        <is>
+          <t>Reko309</t>
+        </is>
+      </c>
+      <c r="C1858" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1858" t="inlineStr">
+        <is>
+          <t>Reko Swish +46702390837</t>
+        </is>
+      </c>
+      <c r="E1858" t="n">
+        <v>177</v>
+      </c>
+      <c r="F1858" t="inlineStr"/>
+    </row>
+    <row r="1859">
+      <c r="A1859" s="2" t="n">
+        <v>44551</v>
+      </c>
+      <c r="B1859" t="inlineStr">
+        <is>
+          <t>Reko310</t>
+        </is>
+      </c>
+      <c r="C1859" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1859" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767693959</t>
+        </is>
+      </c>
+      <c r="E1859" t="inlineStr"/>
+      <c r="F1859" t="n">
+        <v>158.04</v>
+      </c>
+    </row>
+    <row r="1860">
+      <c r="A1860" s="2" t="n">
+        <v>44551</v>
+      </c>
+      <c r="B1860" t="inlineStr">
+        <is>
+          <t>Reko310</t>
+        </is>
+      </c>
+      <c r="C1860" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1860" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767693959</t>
+        </is>
+      </c>
+      <c r="E1860" t="inlineStr"/>
+      <c r="F1860" t="n">
+        <v>18.96</v>
+      </c>
+    </row>
+    <row r="1861">
+      <c r="A1861" s="2" t="n">
+        <v>44551</v>
+      </c>
+      <c r="B1861" t="inlineStr">
+        <is>
+          <t>Reko310</t>
+        </is>
+      </c>
+      <c r="C1861" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1861" t="inlineStr">
+        <is>
+          <t>Reko Swish +46767693959</t>
+        </is>
+      </c>
+      <c r="E1861" t="n">
+        <v>177</v>
+      </c>
+      <c r="F1861" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2022-01-02 (total 1866 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1861"/>
+  <dimension ref="A1:F1867"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -38959,6 +38959,138 @@
       </c>
       <c r="F1861" t="inlineStr"/>
     </row>
+    <row r="1862">
+      <c r="A1862" s="2" t="n">
+        <v>44557</v>
+      </c>
+      <c r="B1862" t="inlineStr">
+        <is>
+          <t>7270704</t>
+        </is>
+      </c>
+      <c r="C1862" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1862" t="inlineStr">
+        <is>
+          <t>Order 7270704 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1862" t="inlineStr"/>
+      <c r="F1862" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1863">
+      <c r="A1863" s="2" t="n">
+        <v>44557</v>
+      </c>
+      <c r="B1863" t="inlineStr">
+        <is>
+          <t>7270704</t>
+        </is>
+      </c>
+      <c r="C1863" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1863" t="inlineStr">
+        <is>
+          <t>Order 7270704 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1863" t="inlineStr"/>
+      <c r="F1863" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1864">
+      <c r="A1864" s="2" t="n">
+        <v>44557</v>
+      </c>
+      <c r="B1864" t="inlineStr">
+        <is>
+          <t>7270704</t>
+        </is>
+      </c>
+      <c r="C1864" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1864" t="inlineStr">
+        <is>
+          <t>Order 7270704 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1864" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1864" t="inlineStr"/>
+    </row>
+    <row r="1865">
+      <c r="A1865" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B1865" t="inlineStr">
+        <is>
+          <t>1311614</t>
+        </is>
+      </c>
+      <c r="C1865" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1865" t="inlineStr">
+        <is>
+          <t>Order 1311614 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1865" t="inlineStr"/>
+      <c r="F1865" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1866">
+      <c r="A1866" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B1866" t="inlineStr">
+        <is>
+          <t>1311614</t>
+        </is>
+      </c>
+      <c r="C1866" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1866" t="inlineStr">
+        <is>
+          <t>Order 1311614 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1866" t="inlineStr"/>
+      <c r="F1866" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1867">
+      <c r="A1867" s="2" t="n">
+        <v>44562</v>
+      </c>
+      <c r="B1867" t="inlineStr">
+        <is>
+          <t>1311614</t>
+        </is>
+      </c>
+      <c r="C1867" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1867" t="inlineStr">
+        <is>
+          <t>Order 1311614 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1867" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1867" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2022-01-09 (total 1872 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1867"/>
+  <dimension ref="A1:F1873"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39091,6 +39091,138 @@
       </c>
       <c r="F1867" t="inlineStr"/>
     </row>
+    <row r="1868">
+      <c r="A1868" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="B1868" t="inlineStr">
+        <is>
+          <t>0051833</t>
+        </is>
+      </c>
+      <c r="C1868" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1868" t="inlineStr">
+        <is>
+          <t>Order 0051833 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1868" t="inlineStr"/>
+      <c r="F1868" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1869">
+      <c r="A1869" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="B1869" t="inlineStr">
+        <is>
+          <t>0051833</t>
+        </is>
+      </c>
+      <c r="C1869" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1869" t="inlineStr">
+        <is>
+          <t>Order 0051833 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1869" t="inlineStr"/>
+      <c r="F1869" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1870">
+      <c r="A1870" s="2" t="n">
+        <v>44566</v>
+      </c>
+      <c r="B1870" t="inlineStr">
+        <is>
+          <t>0051833</t>
+        </is>
+      </c>
+      <c r="C1870" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1870" t="inlineStr">
+        <is>
+          <t>Order 0051833 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1870" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1870" t="inlineStr"/>
+    </row>
+    <row r="1871">
+      <c r="A1871" s="2" t="n">
+        <v>44568</v>
+      </c>
+      <c r="B1871" t="inlineStr">
+        <is>
+          <t>2071440</t>
+        </is>
+      </c>
+      <c r="C1871" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1871" t="inlineStr">
+        <is>
+          <t>Order 2071440 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1871" t="inlineStr"/>
+      <c r="F1871" t="n">
+        <v>423.21</v>
+      </c>
+    </row>
+    <row r="1872">
+      <c r="A1872" s="2" t="n">
+        <v>44568</v>
+      </c>
+      <c r="B1872" t="inlineStr">
+        <is>
+          <t>2071440</t>
+        </is>
+      </c>
+      <c r="C1872" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1872" t="inlineStr">
+        <is>
+          <t>Order 2071440 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1872" t="inlineStr"/>
+      <c r="F1872" t="n">
+        <v>50.79</v>
+      </c>
+    </row>
+    <row r="1873">
+      <c r="A1873" s="2" t="n">
+        <v>44568</v>
+      </c>
+      <c r="B1873" t="inlineStr">
+        <is>
+          <t>2071440</t>
+        </is>
+      </c>
+      <c r="C1873" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1873" t="inlineStr">
+        <is>
+          <t>Order 2071440 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1873" t="n">
+        <v>474</v>
+      </c>
+      <c r="F1873" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2022-01-16 (total 1878 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1873"/>
+  <dimension ref="A1:F1879"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39223,6 +39223,126 @@
       </c>
       <c r="F1873" t="inlineStr"/>
     </row>
+    <row r="1874">
+      <c r="A1874" s="2" t="n">
+        <v>44572</v>
+      </c>
+      <c r="B1874" t="inlineStr"/>
+      <c r="C1874" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1874" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1874" t="n">
+        <v>202.41</v>
+      </c>
+      <c r="F1874" t="inlineStr"/>
+    </row>
+    <row r="1875">
+      <c r="A1875" s="2" t="n">
+        <v>44572</v>
+      </c>
+      <c r="B1875" t="inlineStr"/>
+      <c r="C1875" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1875" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1875" t="n">
+        <v>24.29</v>
+      </c>
+      <c r="F1875" t="inlineStr"/>
+    </row>
+    <row r="1876">
+      <c r="A1876" s="2" t="n">
+        <v>44572</v>
+      </c>
+      <c r="B1876" t="inlineStr"/>
+      <c r="C1876" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1876" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1876" t="inlineStr"/>
+      <c r="F1876" t="n">
+        <v>226.7</v>
+      </c>
+    </row>
+    <row r="1877">
+      <c r="A1877" s="2" t="n">
+        <v>44575</v>
+      </c>
+      <c r="B1877" t="inlineStr">
+        <is>
+          <t>9141636</t>
+        </is>
+      </c>
+      <c r="C1877" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1877" t="inlineStr">
+        <is>
+          <t>Order 9141636 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1877" t="inlineStr"/>
+      <c r="F1877" t="n">
+        <v>637.5</v>
+      </c>
+    </row>
+    <row r="1878">
+      <c r="A1878" s="2" t="n">
+        <v>44575</v>
+      </c>
+      <c r="B1878" t="inlineStr">
+        <is>
+          <t>9141636</t>
+        </is>
+      </c>
+      <c r="C1878" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1878" t="inlineStr">
+        <is>
+          <t>Order 9141636 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1878" t="inlineStr"/>
+      <c r="F1878" t="n">
+        <v>76.5</v>
+      </c>
+    </row>
+    <row r="1879">
+      <c r="A1879" s="2" t="n">
+        <v>44575</v>
+      </c>
+      <c r="B1879" t="inlineStr">
+        <is>
+          <t>9141636</t>
+        </is>
+      </c>
+      <c r="C1879" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1879" t="inlineStr">
+        <is>
+          <t>Order 9141636 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1879" t="n">
+        <v>714</v>
+      </c>
+      <c r="F1879" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 12 new rows for week ending 2022-01-23 (total 1890 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1879"/>
+  <dimension ref="A1:F1891"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39343,6 +39343,244 @@
       </c>
       <c r="F1879" t="inlineStr"/>
     </row>
+    <row r="1880">
+      <c r="A1880" s="2" t="n">
+        <v>44581</v>
+      </c>
+      <c r="B1880" t="inlineStr"/>
+      <c r="C1880" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1880" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1880" t="n">
+        <v>1307</v>
+      </c>
+      <c r="F1880" t="inlineStr"/>
+    </row>
+    <row r="1881">
+      <c r="A1881" s="2" t="n">
+        <v>44581</v>
+      </c>
+      <c r="B1881" t="inlineStr"/>
+      <c r="C1881" t="inlineStr"/>
+      <c r="D1881" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1881" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1881" t="inlineStr"/>
+    </row>
+    <row r="1882">
+      <c r="A1882" s="2" t="n">
+        <v>44581</v>
+      </c>
+      <c r="B1882" t="inlineStr"/>
+      <c r="C1882" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1882" t="inlineStr">
+        <is>
+          <t>Pris banktjänster enligt faktura</t>
+        </is>
+      </c>
+      <c r="E1882" t="inlineStr"/>
+      <c r="F1882" t="n">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="1883">
+      <c r="A1883" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1883" t="inlineStr">
+        <is>
+          <t>1131900</t>
+        </is>
+      </c>
+      <c r="C1883" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1883" t="inlineStr">
+        <is>
+          <t>Order 1131900 Swish +46707644450</t>
+        </is>
+      </c>
+      <c r="E1883" t="inlineStr"/>
+      <c r="F1883" t="n">
+        <v>600.89</v>
+      </c>
+    </row>
+    <row r="1884">
+      <c r="A1884" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1884" t="inlineStr">
+        <is>
+          <t>1131900</t>
+        </is>
+      </c>
+      <c r="C1884" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1884" t="inlineStr">
+        <is>
+          <t>Order 1131900 Swish +46707644450</t>
+        </is>
+      </c>
+      <c r="E1884" t="inlineStr"/>
+      <c r="F1884" t="n">
+        <v>72.11</v>
+      </c>
+    </row>
+    <row r="1885">
+      <c r="A1885" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1885" t="inlineStr">
+        <is>
+          <t>1131900</t>
+        </is>
+      </c>
+      <c r="C1885" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1885" t="inlineStr">
+        <is>
+          <t>Order 1131900 Swish +46707644450</t>
+        </is>
+      </c>
+      <c r="E1885" t="n">
+        <v>673</v>
+      </c>
+      <c r="F1885" t="inlineStr"/>
+    </row>
+    <row r="1886">
+      <c r="A1886" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1886" t="inlineStr">
+        <is>
+          <t>5231248</t>
+        </is>
+      </c>
+      <c r="C1886" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1886" t="inlineStr">
+        <is>
+          <t>Order 5231248 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1886" t="inlineStr"/>
+      <c r="F1886" t="n">
+        <v>1601.79</v>
+      </c>
+    </row>
+    <row r="1887">
+      <c r="A1887" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1887" t="inlineStr">
+        <is>
+          <t>5231248</t>
+        </is>
+      </c>
+      <c r="C1887" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1887" t="inlineStr">
+        <is>
+          <t>Order 5231248 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1887" t="inlineStr"/>
+      <c r="F1887" t="n">
+        <v>192.21</v>
+      </c>
+    </row>
+    <row r="1888">
+      <c r="A1888" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1888" t="inlineStr">
+        <is>
+          <t>5231248</t>
+        </is>
+      </c>
+      <c r="C1888" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1888" t="inlineStr">
+        <is>
+          <t>Order 5231248 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1888" t="n">
+        <v>1794</v>
+      </c>
+      <c r="F1888" t="inlineStr"/>
+    </row>
+    <row r="1889">
+      <c r="A1889" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1889" t="inlineStr"/>
+      <c r="C1889" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1889" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1889" t="n">
+        <v>980.37</v>
+      </c>
+      <c r="F1889" t="inlineStr"/>
+    </row>
+    <row r="1890">
+      <c r="A1890" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1890" t="inlineStr"/>
+      <c r="C1890" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1890" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1890" t="n">
+        <v>117.64</v>
+      </c>
+      <c r="F1890" t="inlineStr"/>
+    </row>
+    <row r="1891">
+      <c r="A1891" s="2" t="n">
+        <v>44584</v>
+      </c>
+      <c r="B1891" t="inlineStr"/>
+      <c r="C1891" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1891" t="inlineStr">
+        <is>
+          <t>M&amp;S RB BROMMA K0135</t>
+        </is>
+      </c>
+      <c r="E1891" t="inlineStr"/>
+      <c r="F1891" t="n">
+        <v>1098.01</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 9 new rows for week ending 2022-01-30 (total 1899 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1891"/>
+  <dimension ref="A1:F1900"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39581,6 +39581,192 @@
         <v>1098.01</v>
       </c>
     </row>
+    <row r="1892">
+      <c r="A1892" s="2" t="n">
+        <v>44585</v>
+      </c>
+      <c r="B1892" t="inlineStr"/>
+      <c r="C1892" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1892" t="inlineStr">
+        <is>
+          <t>AMAZONRETAIL*ZP9PZ0VH5 K0135</t>
+        </is>
+      </c>
+      <c r="E1892" t="n">
+        <v>963.1799999999999</v>
+      </c>
+      <c r="F1892" t="inlineStr"/>
+    </row>
+    <row r="1893">
+      <c r="A1893" s="2" t="n">
+        <v>44585</v>
+      </c>
+      <c r="B1893" t="inlineStr"/>
+      <c r="C1893" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1893" t="inlineStr">
+        <is>
+          <t>AMAZONRETAIL*ZP9PZ0VH5 K0135</t>
+        </is>
+      </c>
+      <c r="E1893" t="n">
+        <v>240.79</v>
+      </c>
+      <c r="F1893" t="inlineStr"/>
+    </row>
+    <row r="1894">
+      <c r="A1894" s="2" t="n">
+        <v>44585</v>
+      </c>
+      <c r="B1894" t="inlineStr"/>
+      <c r="C1894" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1894" t="inlineStr">
+        <is>
+          <t>AMAZONRETAIL*ZP9PZ0VH5 K0135</t>
+        </is>
+      </c>
+      <c r="E1894" t="inlineStr"/>
+      <c r="F1894" t="n">
+        <v>1203.97</v>
+      </c>
+    </row>
+    <row r="1895">
+      <c r="A1895" s="2" t="n">
+        <v>44591</v>
+      </c>
+      <c r="B1895" t="inlineStr">
+        <is>
+          <t>9301514</t>
+        </is>
+      </c>
+      <c r="C1895" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1895" t="inlineStr">
+        <is>
+          <t>Order 9301514 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1895" t="inlineStr"/>
+      <c r="F1895" t="n">
+        <v>1025.89</v>
+      </c>
+    </row>
+    <row r="1896">
+      <c r="A1896" s="2" t="n">
+        <v>44591</v>
+      </c>
+      <c r="B1896" t="inlineStr">
+        <is>
+          <t>9301514</t>
+        </is>
+      </c>
+      <c r="C1896" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1896" t="inlineStr">
+        <is>
+          <t>Order 9301514 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1896" t="inlineStr"/>
+      <c r="F1896" t="n">
+        <v>123.11</v>
+      </c>
+    </row>
+    <row r="1897">
+      <c r="A1897" s="2" t="n">
+        <v>44591</v>
+      </c>
+      <c r="B1897" t="inlineStr">
+        <is>
+          <t>9301514</t>
+        </is>
+      </c>
+      <c r="C1897" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1897" t="inlineStr">
+        <is>
+          <t>Order 9301514 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1897" t="n">
+        <v>1149</v>
+      </c>
+      <c r="F1897" t="inlineStr"/>
+    </row>
+    <row r="1898">
+      <c r="A1898" s="2" t="n">
+        <v>44591</v>
+      </c>
+      <c r="B1898" t="inlineStr">
+        <is>
+          <t>2302001</t>
+        </is>
+      </c>
+      <c r="C1898" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1898" t="inlineStr">
+        <is>
+          <t>Order 2302001 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1898" t="inlineStr"/>
+      <c r="F1898" t="n">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="1899">
+      <c r="A1899" s="2" t="n">
+        <v>44591</v>
+      </c>
+      <c r="B1899" t="inlineStr">
+        <is>
+          <t>2302001</t>
+        </is>
+      </c>
+      <c r="C1899" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1899" t="inlineStr">
+        <is>
+          <t>Order 2302001 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1899" t="inlineStr"/>
+      <c r="F1899" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="1900">
+      <c r="A1900" s="2" t="n">
+        <v>44591</v>
+      </c>
+      <c r="B1900" t="inlineStr">
+        <is>
+          <t>2302001</t>
+        </is>
+      </c>
+      <c r="C1900" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1900" t="inlineStr">
+        <is>
+          <t>Order 2302001 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1900" t="n">
+        <v>952</v>
+      </c>
+      <c r="F1900" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 12 new rows for week ending 2022-02-06 (total 1911 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1900"/>
+  <dimension ref="A1:F1912"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -39767,6 +39767,258 @@
       </c>
       <c r="F1900" t="inlineStr"/>
     </row>
+    <row r="1901">
+      <c r="A1901" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B1901" t="inlineStr">
+        <is>
+          <t>5012018</t>
+        </is>
+      </c>
+      <c r="C1901" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1901" t="inlineStr">
+        <is>
+          <t>Order 5012018 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1901" t="inlineStr"/>
+      <c r="F1901" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1902">
+      <c r="A1902" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B1902" t="inlineStr">
+        <is>
+          <t>5012018</t>
+        </is>
+      </c>
+      <c r="C1902" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1902" t="inlineStr">
+        <is>
+          <t>Order 5012018 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1902" t="inlineStr"/>
+      <c r="F1902" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1903">
+      <c r="A1903" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B1903" t="inlineStr">
+        <is>
+          <t>5012018</t>
+        </is>
+      </c>
+      <c r="C1903" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1903" t="inlineStr">
+        <is>
+          <t>Order 5012018 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1903" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1903" t="inlineStr"/>
+    </row>
+    <row r="1904">
+      <c r="A1904" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B1904" t="inlineStr">
+        <is>
+          <t>5012019</t>
+        </is>
+      </c>
+      <c r="C1904" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1904" t="inlineStr">
+        <is>
+          <t>Order 5012019 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1904" t="inlineStr"/>
+      <c r="F1904" t="n">
+        <v>883.9300000000001</v>
+      </c>
+    </row>
+    <row r="1905">
+      <c r="A1905" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B1905" t="inlineStr">
+        <is>
+          <t>5012019</t>
+        </is>
+      </c>
+      <c r="C1905" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1905" t="inlineStr">
+        <is>
+          <t>Order 5012019 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1905" t="inlineStr"/>
+      <c r="F1905" t="n">
+        <v>106.07</v>
+      </c>
+    </row>
+    <row r="1906">
+      <c r="A1906" s="2" t="n">
+        <v>44593</v>
+      </c>
+      <c r="B1906" t="inlineStr">
+        <is>
+          <t>5012019</t>
+        </is>
+      </c>
+      <c r="C1906" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1906" t="inlineStr">
+        <is>
+          <t>Order 5012019 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1906" t="n">
+        <v>990</v>
+      </c>
+      <c r="F1906" t="inlineStr"/>
+    </row>
+    <row r="1907">
+      <c r="A1907" s="2" t="n">
+        <v>44596</v>
+      </c>
+      <c r="B1907" t="inlineStr"/>
+      <c r="C1907" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1907" t="inlineStr">
+        <is>
+          <t>CIRCLE K SUNDBYBERG RI K0135</t>
+        </is>
+      </c>
+      <c r="E1907" t="n">
+        <v>336.55</v>
+      </c>
+      <c r="F1907" t="inlineStr"/>
+    </row>
+    <row r="1908">
+      <c r="A1908" s="2" t="n">
+        <v>44596</v>
+      </c>
+      <c r="B1908" t="inlineStr"/>
+      <c r="C1908" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1908" t="inlineStr">
+        <is>
+          <t>CIRCLE K SUNDBYBERG RI K0135</t>
+        </is>
+      </c>
+      <c r="E1908" t="n">
+        <v>84.14</v>
+      </c>
+      <c r="F1908" t="inlineStr"/>
+    </row>
+    <row r="1909">
+      <c r="A1909" s="2" t="n">
+        <v>44596</v>
+      </c>
+      <c r="B1909" t="inlineStr"/>
+      <c r="C1909" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1909" t="inlineStr">
+        <is>
+          <t>CIRCLE K SUNDBYBERG RI K0135</t>
+        </is>
+      </c>
+      <c r="E1909" t="inlineStr"/>
+      <c r="F1909" t="n">
+        <v>420.69</v>
+      </c>
+    </row>
+    <row r="1910">
+      <c r="A1910" s="2" t="n">
+        <v>44598</v>
+      </c>
+      <c r="B1910" t="inlineStr">
+        <is>
+          <t>0310956</t>
+        </is>
+      </c>
+      <c r="C1910" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1910" t="inlineStr">
+        <is>
+          <t>Order 0310956 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1910" t="inlineStr"/>
+      <c r="F1910" t="n">
+        <v>918.75</v>
+      </c>
+    </row>
+    <row r="1911">
+      <c r="A1911" s="2" t="n">
+        <v>44598</v>
+      </c>
+      <c r="B1911" t="inlineStr">
+        <is>
+          <t>0310956</t>
+        </is>
+      </c>
+      <c r="C1911" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1911" t="inlineStr">
+        <is>
+          <t>Order 0310956 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1911" t="inlineStr"/>
+      <c r="F1911" t="n">
+        <v>110.25</v>
+      </c>
+    </row>
+    <row r="1912">
+      <c r="A1912" s="2" t="n">
+        <v>44598</v>
+      </c>
+      <c r="B1912" t="inlineStr">
+        <is>
+          <t>0310956</t>
+        </is>
+      </c>
+      <c r="C1912" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1912" t="inlineStr">
+        <is>
+          <t>Order 0310956 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1912" t="n">
+        <v>1029</v>
+      </c>
+      <c r="F1912" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2022-02-13 (total 1917 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1912"/>
+  <dimension ref="A1:F1918"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40019,6 +40019,138 @@
       </c>
       <c r="F1912" t="inlineStr"/>
     </row>
+    <row r="1913">
+      <c r="A1913" s="2" t="n">
+        <v>44601</v>
+      </c>
+      <c r="B1913" t="inlineStr">
+        <is>
+          <t>2091750</t>
+        </is>
+      </c>
+      <c r="C1913" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1913" t="inlineStr">
+        <is>
+          <t>Order 2091750 Swish +46760784377</t>
+        </is>
+      </c>
+      <c r="E1913" t="inlineStr"/>
+      <c r="F1913" t="n">
+        <v>352.68</v>
+      </c>
+    </row>
+    <row r="1914">
+      <c r="A1914" s="2" t="n">
+        <v>44601</v>
+      </c>
+      <c r="B1914" t="inlineStr">
+        <is>
+          <t>2091750</t>
+        </is>
+      </c>
+      <c r="C1914" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1914" t="inlineStr">
+        <is>
+          <t>Order 2091750 Swish +46760784377</t>
+        </is>
+      </c>
+      <c r="E1914" t="inlineStr"/>
+      <c r="F1914" t="n">
+        <v>42.32</v>
+      </c>
+    </row>
+    <row r="1915">
+      <c r="A1915" s="2" t="n">
+        <v>44601</v>
+      </c>
+      <c r="B1915" t="inlineStr">
+        <is>
+          <t>2091750</t>
+        </is>
+      </c>
+      <c r="C1915" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1915" t="inlineStr">
+        <is>
+          <t>Order 2091750 Swish +46760784377</t>
+        </is>
+      </c>
+      <c r="E1915" t="n">
+        <v>395</v>
+      </c>
+      <c r="F1915" t="inlineStr"/>
+    </row>
+    <row r="1916">
+      <c r="A1916" s="2" t="n">
+        <v>44605</v>
+      </c>
+      <c r="B1916" t="inlineStr">
+        <is>
+          <t>0131128</t>
+        </is>
+      </c>
+      <c r="C1916" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1916" t="inlineStr">
+        <is>
+          <t>Order 0131128 Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1916" t="inlineStr"/>
+      <c r="F1916" t="n">
+        <v>741.96</v>
+      </c>
+    </row>
+    <row r="1917">
+      <c r="A1917" s="2" t="n">
+        <v>44605</v>
+      </c>
+      <c r="B1917" t="inlineStr">
+        <is>
+          <t>0131128</t>
+        </is>
+      </c>
+      <c r="C1917" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1917" t="inlineStr">
+        <is>
+          <t>Order 0131128 Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1917" t="inlineStr"/>
+      <c r="F1917" t="n">
+        <v>89.04000000000001</v>
+      </c>
+    </row>
+    <row r="1918">
+      <c r="A1918" s="2" t="n">
+        <v>44605</v>
+      </c>
+      <c r="B1918" t="inlineStr">
+        <is>
+          <t>0131128</t>
+        </is>
+      </c>
+      <c r="C1918" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1918" t="inlineStr">
+        <is>
+          <t>Order 0131128 Swish +46739968231</t>
+        </is>
+      </c>
+      <c r="E1918" t="n">
+        <v>831</v>
+      </c>
+      <c r="F1918" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 9 new rows for week ending 2022-02-20 (total 1926 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1918"/>
+  <dimension ref="A1:F1927"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40151,6 +40151,180 @@
       </c>
       <c r="F1918" t="inlineStr"/>
     </row>
+    <row r="1919">
+      <c r="A1919" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B1919" t="inlineStr"/>
+      <c r="C1919" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1919" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1919" t="n">
+        <v>321.34</v>
+      </c>
+      <c r="F1919" t="inlineStr"/>
+    </row>
+    <row r="1920">
+      <c r="A1920" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B1920" t="inlineStr"/>
+      <c r="C1920" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1920" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1920" t="n">
+        <v>38.56</v>
+      </c>
+      <c r="F1920" t="inlineStr"/>
+    </row>
+    <row r="1921">
+      <c r="A1921" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B1921" t="inlineStr"/>
+      <c r="C1921" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1921" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1921" t="inlineStr"/>
+      <c r="F1921" t="n">
+        <v>359.9</v>
+      </c>
+    </row>
+    <row r="1922">
+      <c r="A1922" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B1922" t="inlineStr"/>
+      <c r="C1922" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1922" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1922" t="n">
+        <v>1134.46</v>
+      </c>
+      <c r="F1922" t="inlineStr"/>
+    </row>
+    <row r="1923">
+      <c r="A1923" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B1923" t="inlineStr"/>
+      <c r="C1923" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1923" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1923" t="n">
+        <v>283.62</v>
+      </c>
+      <c r="F1923" t="inlineStr"/>
+    </row>
+    <row r="1924">
+      <c r="A1924" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B1924" t="inlineStr"/>
+      <c r="C1924" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1924" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1924" t="inlineStr"/>
+      <c r="F1924" t="n">
+        <v>1418.08</v>
+      </c>
+    </row>
+    <row r="1925">
+      <c r="A1925" s="2" t="n">
+        <v>44609</v>
+      </c>
+      <c r="B1925" t="inlineStr">
+        <is>
+          <t>4171656</t>
+        </is>
+      </c>
+      <c r="C1925" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1925" t="inlineStr">
+        <is>
+          <t>Order 4171656 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1925" t="inlineStr"/>
+      <c r="F1925" t="n">
+        <v>459.82</v>
+      </c>
+    </row>
+    <row r="1926">
+      <c r="A1926" s="2" t="n">
+        <v>44609</v>
+      </c>
+      <c r="B1926" t="inlineStr">
+        <is>
+          <t>4171656</t>
+        </is>
+      </c>
+      <c r="C1926" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1926" t="inlineStr">
+        <is>
+          <t>Order 4171656 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1926" t="inlineStr"/>
+      <c r="F1926" t="n">
+        <v>55.18</v>
+      </c>
+    </row>
+    <row r="1927">
+      <c r="A1927" s="2" t="n">
+        <v>44609</v>
+      </c>
+      <c r="B1927" t="inlineStr">
+        <is>
+          <t>4171656</t>
+        </is>
+      </c>
+      <c r="C1927" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1927" t="inlineStr">
+        <is>
+          <t>Order 4171656 Swish +46761877260</t>
+        </is>
+      </c>
+      <c r="E1927" t="n">
+        <v>515</v>
+      </c>
+      <c r="F1927" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 15 new rows for week ending 2022-03-06 (total 1941 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1927"/>
+  <dimension ref="A1:F1942"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40325,6 +40325,288 @@
       </c>
       <c r="F1927" t="inlineStr"/>
     </row>
+    <row r="1928">
+      <c r="A1928" s="2" t="n">
+        <v>44620</v>
+      </c>
+      <c r="B1928" t="inlineStr"/>
+      <c r="C1928" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1928" t="inlineStr">
+        <is>
+          <t>Meds Apotek AB</t>
+        </is>
+      </c>
+      <c r="E1928" t="n">
+        <v>473.57</v>
+      </c>
+      <c r="F1928" t="inlineStr"/>
+    </row>
+    <row r="1929">
+      <c r="A1929" s="2" t="n">
+        <v>44620</v>
+      </c>
+      <c r="B1929" t="inlineStr"/>
+      <c r="C1929" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1929" t="inlineStr">
+        <is>
+          <t>Meds Apotek AB</t>
+        </is>
+      </c>
+      <c r="E1929" t="n">
+        <v>56.83</v>
+      </c>
+      <c r="F1929" t="inlineStr"/>
+    </row>
+    <row r="1930">
+      <c r="A1930" s="2" t="n">
+        <v>44620</v>
+      </c>
+      <c r="B1930" t="inlineStr"/>
+      <c r="C1930" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1930" t="inlineStr">
+        <is>
+          <t>Meds Apotek AB</t>
+        </is>
+      </c>
+      <c r="E1930" t="inlineStr"/>
+      <c r="F1930" t="n">
+        <v>530.4</v>
+      </c>
+    </row>
+    <row r="1931">
+      <c r="A1931" s="2" t="n">
+        <v>44622</v>
+      </c>
+      <c r="B1931" t="inlineStr"/>
+      <c r="C1931" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1931" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1931" t="n">
+        <v>357.02</v>
+      </c>
+      <c r="F1931" t="inlineStr"/>
+    </row>
+    <row r="1932">
+      <c r="A1932" s="2" t="n">
+        <v>44622</v>
+      </c>
+      <c r="B1932" t="inlineStr"/>
+      <c r="C1932" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1932" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1932" t="n">
+        <v>42.84</v>
+      </c>
+      <c r="F1932" t="inlineStr"/>
+    </row>
+    <row r="1933">
+      <c r="A1933" s="2" t="n">
+        <v>44622</v>
+      </c>
+      <c r="B1933" t="inlineStr"/>
+      <c r="C1933" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1933" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1933" t="inlineStr"/>
+      <c r="F1933" t="n">
+        <v>399.86</v>
+      </c>
+    </row>
+    <row r="1934">
+      <c r="A1934" s="2" t="n">
+        <v>44623</v>
+      </c>
+      <c r="B1934" t="inlineStr">
+        <is>
+          <t>4030911</t>
+        </is>
+      </c>
+      <c r="C1934" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1934" t="inlineStr">
+        <is>
+          <t>Order 4030911 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1934" t="inlineStr"/>
+      <c r="F1934" t="n">
+        <v>870.54</v>
+      </c>
+    </row>
+    <row r="1935">
+      <c r="A1935" s="2" t="n">
+        <v>44623</v>
+      </c>
+      <c r="B1935" t="inlineStr">
+        <is>
+          <t>4030911</t>
+        </is>
+      </c>
+      <c r="C1935" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1935" t="inlineStr">
+        <is>
+          <t>Order 4030911 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1935" t="inlineStr"/>
+      <c r="F1935" t="n">
+        <v>104.46</v>
+      </c>
+    </row>
+    <row r="1936">
+      <c r="A1936" s="2" t="n">
+        <v>44623</v>
+      </c>
+      <c r="B1936" t="inlineStr">
+        <is>
+          <t>4030911</t>
+        </is>
+      </c>
+      <c r="C1936" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1936" t="inlineStr">
+        <is>
+          <t>Order 4030911 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1936" t="n">
+        <v>975</v>
+      </c>
+      <c r="F1936" t="inlineStr"/>
+    </row>
+    <row r="1937">
+      <c r="A1937" s="2" t="n">
+        <v>44625</v>
+      </c>
+      <c r="B1937" t="inlineStr"/>
+      <c r="C1937" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1937" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1937" t="n">
+        <v>1204.8</v>
+      </c>
+      <c r="F1937" t="inlineStr"/>
+    </row>
+    <row r="1938">
+      <c r="A1938" s="2" t="n">
+        <v>44625</v>
+      </c>
+      <c r="B1938" t="inlineStr"/>
+      <c r="C1938" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1938" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1938" t="n">
+        <v>144.58</v>
+      </c>
+      <c r="F1938" t="inlineStr"/>
+    </row>
+    <row r="1939">
+      <c r="A1939" s="2" t="n">
+        <v>44625</v>
+      </c>
+      <c r="B1939" t="inlineStr"/>
+      <c r="C1939" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1939" t="inlineStr">
+        <is>
+          <t>SNABBGROSS SOLNA K0135</t>
+        </is>
+      </c>
+      <c r="E1939" t="inlineStr"/>
+      <c r="F1939" t="n">
+        <v>1349.38</v>
+      </c>
+    </row>
+    <row r="1940">
+      <c r="A1940" s="2" t="n">
+        <v>44626</v>
+      </c>
+      <c r="B1940" t="inlineStr"/>
+      <c r="C1940" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1940" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1940" t="n">
+        <v>374.5</v>
+      </c>
+      <c r="F1940" t="inlineStr"/>
+    </row>
+    <row r="1941">
+      <c r="A1941" s="2" t="n">
+        <v>44626</v>
+      </c>
+      <c r="B1941" t="inlineStr"/>
+      <c r="C1941" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1941" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1941" t="n">
+        <v>44.94</v>
+      </c>
+      <c r="F1941" t="inlineStr"/>
+    </row>
+    <row r="1942">
+      <c r="A1942" s="2" t="n">
+        <v>44626</v>
+      </c>
+      <c r="B1942" t="inlineStr"/>
+      <c r="C1942" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1942" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1942" t="inlineStr"/>
+      <c r="F1942" t="n">
+        <v>419.44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 9 new rows for week ending 2022-03-13 (total 1950 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1942"/>
+  <dimension ref="A1:F1951"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40607,6 +40607,192 @@
         <v>419.44</v>
       </c>
     </row>
+    <row r="1943">
+      <c r="A1943" s="2" t="n">
+        <v>44627</v>
+      </c>
+      <c r="B1943" t="inlineStr">
+        <is>
+          <t>2211030</t>
+        </is>
+      </c>
+      <c r="C1943" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1943" t="inlineStr">
+        <is>
+          <t>Order 2211030 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1943" t="inlineStr"/>
+      <c r="F1943" t="n">
+        <v>1577.68</v>
+      </c>
+    </row>
+    <row r="1944">
+      <c r="A1944" s="2" t="n">
+        <v>44627</v>
+      </c>
+      <c r="B1944" t="inlineStr">
+        <is>
+          <t>2211030</t>
+        </is>
+      </c>
+      <c r="C1944" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1944" t="inlineStr">
+        <is>
+          <t>Order 2211030 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1944" t="inlineStr"/>
+      <c r="F1944" t="n">
+        <v>189.32</v>
+      </c>
+    </row>
+    <row r="1945">
+      <c r="A1945" s="2" t="n">
+        <v>44627</v>
+      </c>
+      <c r="B1945" t="inlineStr">
+        <is>
+          <t>2211030</t>
+        </is>
+      </c>
+      <c r="C1945" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1945" t="inlineStr">
+        <is>
+          <t>Order 2211030 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1945" t="n">
+        <v>1767</v>
+      </c>
+      <c r="F1945" t="inlineStr"/>
+    </row>
+    <row r="1946">
+      <c r="A1946" s="2" t="n">
+        <v>44629</v>
+      </c>
+      <c r="B1946" t="inlineStr">
+        <is>
+          <t>9091109</t>
+        </is>
+      </c>
+      <c r="C1946" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1946" t="inlineStr">
+        <is>
+          <t>Order 9091109 Swish +46760541746</t>
+        </is>
+      </c>
+      <c r="E1946" t="inlineStr"/>
+      <c r="F1946" t="n">
+        <v>705.36</v>
+      </c>
+    </row>
+    <row r="1947">
+      <c r="A1947" s="2" t="n">
+        <v>44629</v>
+      </c>
+      <c r="B1947" t="inlineStr">
+        <is>
+          <t>9091109</t>
+        </is>
+      </c>
+      <c r="C1947" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1947" t="inlineStr">
+        <is>
+          <t>Order 9091109 Swish +46760541746</t>
+        </is>
+      </c>
+      <c r="E1947" t="inlineStr"/>
+      <c r="F1947" t="n">
+        <v>84.64</v>
+      </c>
+    </row>
+    <row r="1948">
+      <c r="A1948" s="2" t="n">
+        <v>44629</v>
+      </c>
+      <c r="B1948" t="inlineStr">
+        <is>
+          <t>9091109</t>
+        </is>
+      </c>
+      <c r="C1948" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1948" t="inlineStr">
+        <is>
+          <t>Order 9091109 Swish +46760541746</t>
+        </is>
+      </c>
+      <c r="E1948" t="n">
+        <v>790</v>
+      </c>
+      <c r="F1948" t="inlineStr"/>
+    </row>
+    <row r="1949">
+      <c r="A1949" s="2" t="n">
+        <v>44631</v>
+      </c>
+      <c r="B1949" t="inlineStr"/>
+      <c r="C1949" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1949" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1949" t="n">
+        <v>225.45</v>
+      </c>
+      <c r="F1949" t="inlineStr"/>
+    </row>
+    <row r="1950">
+      <c r="A1950" s="2" t="n">
+        <v>44631</v>
+      </c>
+      <c r="B1950" t="inlineStr"/>
+      <c r="C1950" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1950" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1950" t="n">
+        <v>27.05</v>
+      </c>
+      <c r="F1950" t="inlineStr"/>
+    </row>
+    <row r="1951">
+      <c r="A1951" s="2" t="n">
+        <v>44631</v>
+      </c>
+      <c r="B1951" t="inlineStr"/>
+      <c r="C1951" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1951" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1951" t="inlineStr"/>
+      <c r="F1951" t="n">
+        <v>252.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 15 new rows for week ending 2022-03-27 (total 1965 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1951"/>
+  <dimension ref="A1:F1966"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -40793,6 +40793,288 @@
         <v>252.5</v>
       </c>
     </row>
+    <row r="1952">
+      <c r="A1952" s="2" t="n">
+        <v>44642</v>
+      </c>
+      <c r="B1952" t="inlineStr"/>
+      <c r="C1952" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1952" t="inlineStr">
+        <is>
+          <t>HANDLARN URSVIK K6885</t>
+        </is>
+      </c>
+      <c r="E1952" t="n">
+        <v>30.36</v>
+      </c>
+      <c r="F1952" t="inlineStr"/>
+    </row>
+    <row r="1953">
+      <c r="A1953" s="2" t="n">
+        <v>44642</v>
+      </c>
+      <c r="B1953" t="inlineStr"/>
+      <c r="C1953" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1953" t="inlineStr">
+        <is>
+          <t>HANDLARN URSVIK K6885</t>
+        </is>
+      </c>
+      <c r="E1953" t="n">
+        <v>3.64</v>
+      </c>
+      <c r="F1953" t="inlineStr"/>
+    </row>
+    <row r="1954">
+      <c r="A1954" s="2" t="n">
+        <v>44642</v>
+      </c>
+      <c r="B1954" t="inlineStr"/>
+      <c r="C1954" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1954" t="inlineStr">
+        <is>
+          <t>HANDLARN URSVIK K6885</t>
+        </is>
+      </c>
+      <c r="E1954" t="inlineStr"/>
+      <c r="F1954" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="1955">
+      <c r="A1955" s="2" t="n">
+        <v>44644</v>
+      </c>
+      <c r="B1955" t="inlineStr"/>
+      <c r="C1955" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1955" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1955" t="n">
+        <v>829.5</v>
+      </c>
+      <c r="F1955" t="inlineStr"/>
+    </row>
+    <row r="1956">
+      <c r="A1956" s="2" t="n">
+        <v>44644</v>
+      </c>
+      <c r="B1956" t="inlineStr"/>
+      <c r="C1956" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1956" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1956" t="n">
+        <v>207.38</v>
+      </c>
+      <c r="F1956" t="inlineStr"/>
+    </row>
+    <row r="1957">
+      <c r="A1957" s="2" t="n">
+        <v>44644</v>
+      </c>
+      <c r="B1957" t="inlineStr"/>
+      <c r="C1957" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1957" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1957" t="inlineStr"/>
+      <c r="F1957" t="n">
+        <v>1036.88</v>
+      </c>
+    </row>
+    <row r="1958">
+      <c r="A1958" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B1958" t="inlineStr">
+        <is>
+          <t>9251027</t>
+        </is>
+      </c>
+      <c r="C1958" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1958" t="inlineStr">
+        <is>
+          <t>Order 9251027 Swish +46760784377</t>
+        </is>
+      </c>
+      <c r="E1958" t="inlineStr"/>
+      <c r="F1958" t="n">
+        <v>565.1799999999999</v>
+      </c>
+    </row>
+    <row r="1959">
+      <c r="A1959" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B1959" t="inlineStr">
+        <is>
+          <t>9251027</t>
+        </is>
+      </c>
+      <c r="C1959" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1959" t="inlineStr">
+        <is>
+          <t>Order 9251027 Swish +46760784377</t>
+        </is>
+      </c>
+      <c r="E1959" t="inlineStr"/>
+      <c r="F1959" t="n">
+        <v>67.81999999999999</v>
+      </c>
+    </row>
+    <row r="1960">
+      <c r="A1960" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B1960" t="inlineStr">
+        <is>
+          <t>9251027</t>
+        </is>
+      </c>
+      <c r="C1960" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1960" t="inlineStr">
+        <is>
+          <t>Order 9251027 Swish +46760784377</t>
+        </is>
+      </c>
+      <c r="E1960" t="n">
+        <v>633</v>
+      </c>
+      <c r="F1960" t="inlineStr"/>
+    </row>
+    <row r="1961">
+      <c r="A1961" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B1961" t="inlineStr"/>
+      <c r="C1961" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1961" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1961" t="n">
+        <v>522.71</v>
+      </c>
+      <c r="F1961" t="inlineStr"/>
+    </row>
+    <row r="1962">
+      <c r="A1962" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B1962" t="inlineStr"/>
+      <c r="C1962" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1962" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1962" t="n">
+        <v>62.73</v>
+      </c>
+      <c r="F1962" t="inlineStr"/>
+    </row>
+    <row r="1963">
+      <c r="A1963" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B1963" t="inlineStr"/>
+      <c r="C1963" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1963" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1963" t="inlineStr"/>
+      <c r="F1963" t="n">
+        <v>585.4400000000001</v>
+      </c>
+    </row>
+    <row r="1964">
+      <c r="A1964" s="2" t="n">
+        <v>44646</v>
+      </c>
+      <c r="B1964" t="inlineStr"/>
+      <c r="C1964" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1964" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E1964" t="n">
+        <v>93.59999999999999</v>
+      </c>
+      <c r="F1964" t="inlineStr"/>
+    </row>
+    <row r="1965">
+      <c r="A1965" s="2" t="n">
+        <v>44646</v>
+      </c>
+      <c r="B1965" t="inlineStr"/>
+      <c r="C1965" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1965" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E1965" t="n">
+        <v>23.4</v>
+      </c>
+      <c r="F1965" t="inlineStr"/>
+    </row>
+    <row r="1966">
+      <c r="A1966" s="2" t="n">
+        <v>44646</v>
+      </c>
+      <c r="B1966" t="inlineStr"/>
+      <c r="C1966" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1966" t="inlineStr">
+        <is>
+          <t>IKEA BARKARBY K0135</t>
+        </is>
+      </c>
+      <c r="E1966" t="inlineStr"/>
+      <c r="F1966" t="n">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 12 new rows for week ending 2022-04-03 (total 1977 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1966"/>
+  <dimension ref="A1:F1978"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41075,6 +41075,246 @@
         <v>117</v>
       </c>
     </row>
+    <row r="1967">
+      <c r="A1967" s="2" t="n">
+        <v>44651</v>
+      </c>
+      <c r="B1967" t="inlineStr"/>
+      <c r="C1967" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1967" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1967" t="n">
+        <v>475.78</v>
+      </c>
+      <c r="F1967" t="inlineStr"/>
+    </row>
+    <row r="1968">
+      <c r="A1968" s="2" t="n">
+        <v>44651</v>
+      </c>
+      <c r="B1968" t="inlineStr"/>
+      <c r="C1968" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1968" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1968" t="n">
+        <v>57.09</v>
+      </c>
+      <c r="F1968" t="inlineStr"/>
+    </row>
+    <row r="1969">
+      <c r="A1969" s="2" t="n">
+        <v>44651</v>
+      </c>
+      <c r="B1969" t="inlineStr"/>
+      <c r="C1969" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1969" t="inlineStr">
+        <is>
+          <t>NGROCERIES K0135</t>
+        </is>
+      </c>
+      <c r="E1969" t="inlineStr"/>
+      <c r="F1969" t="n">
+        <v>532.87</v>
+      </c>
+    </row>
+    <row r="1970">
+      <c r="A1970" s="2" t="n">
+        <v>44653</v>
+      </c>
+      <c r="B1970" t="inlineStr"/>
+      <c r="C1970" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1970" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1970" t="n">
+        <v>183.48</v>
+      </c>
+      <c r="F1970" t="inlineStr"/>
+    </row>
+    <row r="1971">
+      <c r="A1971" s="2" t="n">
+        <v>44653</v>
+      </c>
+      <c r="B1971" t="inlineStr"/>
+      <c r="C1971" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1971" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1971" t="n">
+        <v>22.02</v>
+      </c>
+      <c r="F1971" t="inlineStr"/>
+    </row>
+    <row r="1972">
+      <c r="A1972" s="2" t="n">
+        <v>44653</v>
+      </c>
+      <c r="B1972" t="inlineStr"/>
+      <c r="C1972" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1972" t="inlineStr">
+        <is>
+          <t>WILLYS RISSNE K0135</t>
+        </is>
+      </c>
+      <c r="E1972" t="inlineStr"/>
+      <c r="F1972" t="n">
+        <v>205.5</v>
+      </c>
+    </row>
+    <row r="1973">
+      <c r="A1973" s="2" t="n">
+        <v>44654</v>
+      </c>
+      <c r="B1973" t="inlineStr">
+        <is>
+          <t>8221822</t>
+        </is>
+      </c>
+      <c r="C1973" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1973" t="inlineStr">
+        <is>
+          <t>Order 8221822 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1973" t="inlineStr"/>
+      <c r="F1973" t="n">
+        <v>1456.25</v>
+      </c>
+    </row>
+    <row r="1974">
+      <c r="A1974" s="2" t="n">
+        <v>44654</v>
+      </c>
+      <c r="B1974" t="inlineStr">
+        <is>
+          <t>8221822</t>
+        </is>
+      </c>
+      <c r="C1974" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1974" t="inlineStr">
+        <is>
+          <t>Order 8221822 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1974" t="inlineStr"/>
+      <c r="F1974" t="n">
+        <v>174.75</v>
+      </c>
+    </row>
+    <row r="1975">
+      <c r="A1975" s="2" t="n">
+        <v>44654</v>
+      </c>
+      <c r="B1975" t="inlineStr">
+        <is>
+          <t>8221822</t>
+        </is>
+      </c>
+      <c r="C1975" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1975" t="inlineStr">
+        <is>
+          <t>Order 8221822 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1975" t="n">
+        <v>1631</v>
+      </c>
+      <c r="F1975" t="inlineStr"/>
+    </row>
+    <row r="1976">
+      <c r="A1976" s="2" t="n">
+        <v>44654</v>
+      </c>
+      <c r="B1976" t="inlineStr">
+        <is>
+          <t>4282347</t>
+        </is>
+      </c>
+      <c r="C1976" t="n">
+        <v>3011</v>
+      </c>
+      <c r="D1976" t="inlineStr">
+        <is>
+          <t>Order 4282347 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1976" t="inlineStr"/>
+      <c r="F1976" t="n">
+        <v>870.54</v>
+      </c>
+    </row>
+    <row r="1977">
+      <c r="A1977" s="2" t="n">
+        <v>44654</v>
+      </c>
+      <c r="B1977" t="inlineStr">
+        <is>
+          <t>4282347</t>
+        </is>
+      </c>
+      <c r="C1977" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D1977" t="inlineStr">
+        <is>
+          <t>Order 4282347 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1977" t="inlineStr"/>
+      <c r="F1977" t="n">
+        <v>104.46</v>
+      </c>
+    </row>
+    <row r="1978">
+      <c r="A1978" s="2" t="n">
+        <v>44654</v>
+      </c>
+      <c r="B1978" t="inlineStr">
+        <is>
+          <t>4282347</t>
+        </is>
+      </c>
+      <c r="C1978" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1978" t="inlineStr">
+        <is>
+          <t>Order 4282347 Card(Stripe)</t>
+        </is>
+      </c>
+      <c r="E1978" t="n">
+        <v>975</v>
+      </c>
+      <c r="F1978" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2022-04-17 (total 1980 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1978"/>
+  <dimension ref="A1:F1981"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41315,6 +41315,60 @@
       </c>
       <c r="F1978" t="inlineStr"/>
     </row>
+    <row r="1979">
+      <c r="A1979" s="2" t="n">
+        <v>44668</v>
+      </c>
+      <c r="B1979" t="inlineStr"/>
+      <c r="C1979" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1979" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1979" t="n">
+        <v>1176.8</v>
+      </c>
+      <c r="F1979" t="inlineStr"/>
+    </row>
+    <row r="1980">
+      <c r="A1980" s="2" t="n">
+        <v>44668</v>
+      </c>
+      <c r="B1980" t="inlineStr"/>
+      <c r="C1980" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1980" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1980" t="n">
+        <v>294.2</v>
+      </c>
+      <c r="F1980" t="inlineStr"/>
+    </row>
+    <row r="1981">
+      <c r="A1981" s="2" t="n">
+        <v>44668</v>
+      </c>
+      <c r="B1981" t="inlineStr"/>
+      <c r="C1981" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1981" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E1981" t="inlineStr"/>
+      <c r="F1981" t="n">
+        <v>1471</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2022-04-24 (total 1986 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1981"/>
+  <dimension ref="A1:F1987"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41369,6 +41369,112 @@
         <v>1471</v>
       </c>
     </row>
+    <row r="1982">
+      <c r="A1982" s="2" t="n">
+        <v>44670</v>
+      </c>
+      <c r="B1982" t="inlineStr"/>
+      <c r="C1982" t="n">
+        <v>4010</v>
+      </c>
+      <c r="D1982" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1982" t="n">
+        <v>178.75</v>
+      </c>
+      <c r="F1982" t="inlineStr"/>
+    </row>
+    <row r="1983">
+      <c r="A1983" s="2" t="n">
+        <v>44670</v>
+      </c>
+      <c r="B1983" t="inlineStr"/>
+      <c r="C1983" t="n">
+        <v>2645</v>
+      </c>
+      <c r="D1983" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1983" t="n">
+        <v>21.45</v>
+      </c>
+      <c r="F1983" t="inlineStr"/>
+    </row>
+    <row r="1984">
+      <c r="A1984" s="2" t="n">
+        <v>44670</v>
+      </c>
+      <c r="B1984" t="inlineStr"/>
+      <c r="C1984" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1984" t="inlineStr">
+        <is>
+          <t>NGROCERIES</t>
+        </is>
+      </c>
+      <c r="E1984" t="inlineStr"/>
+      <c r="F1984" t="n">
+        <v>200.2</v>
+      </c>
+    </row>
+    <row r="1985">
+      <c r="A1985" s="2" t="n">
+        <v>44674</v>
+      </c>
+      <c r="B1985" t="inlineStr"/>
+      <c r="C1985" t="n">
+        <v>6990</v>
+      </c>
+      <c r="D1985" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1985" t="n">
+        <v>625</v>
+      </c>
+      <c r="F1985" t="inlineStr"/>
+    </row>
+    <row r="1986">
+      <c r="A1986" s="2" t="n">
+        <v>44674</v>
+      </c>
+      <c r="B1986" t="inlineStr"/>
+      <c r="C1986" t="inlineStr"/>
+      <c r="D1986" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1986" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1986" t="inlineStr"/>
+    </row>
+    <row r="1987">
+      <c r="A1987" s="2" t="n">
+        <v>44674</v>
+      </c>
+      <c r="B1987" t="inlineStr"/>
+      <c r="C1987" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1987" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1987" t="inlineStr"/>
+      <c r="F1987" t="n">
+        <v>625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2022-05-01 (total 1989 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1987"/>
+  <dimension ref="A1:F1990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41475,6 +41475,58 @@
         <v>625</v>
       </c>
     </row>
+    <row r="1988">
+      <c r="A1988" s="2" t="n">
+        <v>44679</v>
+      </c>
+      <c r="B1988" t="inlineStr"/>
+      <c r="C1988" t="n">
+        <v>6990</v>
+      </c>
+      <c r="D1988" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1988" t="n">
+        <v>625</v>
+      </c>
+      <c r="F1988" t="inlineStr"/>
+    </row>
+    <row r="1989">
+      <c r="A1989" s="2" t="n">
+        <v>44679</v>
+      </c>
+      <c r="B1989" t="inlineStr"/>
+      <c r="C1989" t="inlineStr"/>
+      <c r="D1989" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1989" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1989" t="inlineStr"/>
+    </row>
+    <row r="1990">
+      <c r="A1990" s="2" t="n">
+        <v>44679</v>
+      </c>
+      <c r="B1990" t="inlineStr"/>
+      <c r="C1990" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1990" t="inlineStr">
+        <is>
+          <t>SKATTEVERKET</t>
+        </is>
+      </c>
+      <c r="E1990" t="inlineStr"/>
+      <c r="F1990" t="n">
+        <v>625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 6 new rows for week ending 2022-06-05 (total 1995 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1990"/>
+  <dimension ref="A1:F1996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41527,6 +41527,112 @@
         <v>625</v>
       </c>
     </row>
+    <row r="1991">
+      <c r="A1991" s="2" t="n">
+        <v>44714</v>
+      </c>
+      <c r="B1991" t="inlineStr"/>
+      <c r="C1991" t="n">
+        <v>5010</v>
+      </c>
+      <c r="D1991" t="inlineStr">
+        <is>
+          <t>Hyra April-May</t>
+        </is>
+      </c>
+      <c r="E1991" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F1991" t="inlineStr"/>
+    </row>
+    <row r="1992">
+      <c r="A1992" s="2" t="n">
+        <v>44714</v>
+      </c>
+      <c r="B1992" t="inlineStr"/>
+      <c r="C1992" t="inlineStr"/>
+      <c r="D1992" t="inlineStr">
+        <is>
+          <t>Hyra April-May</t>
+        </is>
+      </c>
+      <c r="E1992" t="n">
+        <v>0</v>
+      </c>
+      <c r="F1992" t="inlineStr"/>
+    </row>
+    <row r="1993">
+      <c r="A1993" s="2" t="n">
+        <v>44714</v>
+      </c>
+      <c r="B1993" t="inlineStr"/>
+      <c r="C1993" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1993" t="inlineStr">
+        <is>
+          <t>Hyra April-May</t>
+        </is>
+      </c>
+      <c r="E1993" t="inlineStr"/>
+      <c r="F1993" t="n">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="1994">
+      <c r="A1994" s="2" t="n">
+        <v>44715</v>
+      </c>
+      <c r="B1994" t="inlineStr"/>
+      <c r="C1994" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1994" t="inlineStr">
+        <is>
+          <t>CIRCLE K SUNDBYBERG RI K0135</t>
+        </is>
+      </c>
+      <c r="E1994" t="n">
+        <v>314.28</v>
+      </c>
+      <c r="F1994" t="inlineStr"/>
+    </row>
+    <row r="1995">
+      <c r="A1995" s="2" t="n">
+        <v>44715</v>
+      </c>
+      <c r="B1995" t="inlineStr"/>
+      <c r="C1995" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1995" t="inlineStr">
+        <is>
+          <t>CIRCLE K SUNDBYBERG RI K0135</t>
+        </is>
+      </c>
+      <c r="E1995" t="n">
+        <v>78.56999999999999</v>
+      </c>
+      <c r="F1995" t="inlineStr"/>
+    </row>
+    <row r="1996">
+      <c r="A1996" s="2" t="n">
+        <v>44715</v>
+      </c>
+      <c r="B1996" t="inlineStr"/>
+      <c r="C1996" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1996" t="inlineStr">
+        <is>
+          <t>CIRCLE K SUNDBYBERG RI K0135</t>
+        </is>
+      </c>
+      <c r="E1996" t="inlineStr"/>
+      <c r="F1996" t="n">
+        <v>392.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2022-06-12 (total 1998 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1996"/>
+  <dimension ref="A1:F1999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41633,6 +41633,60 @@
         <v>392.85</v>
       </c>
     </row>
+    <row r="1997">
+      <c r="A1997" s="2" t="n">
+        <v>44722</v>
+      </c>
+      <c r="B1997" t="inlineStr"/>
+      <c r="C1997" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D1997" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1997" t="n">
+        <v>792.63</v>
+      </c>
+      <c r="F1997" t="inlineStr"/>
+    </row>
+    <row r="1998">
+      <c r="A1998" s="2" t="n">
+        <v>44722</v>
+      </c>
+      <c r="B1998" t="inlineStr"/>
+      <c r="C1998" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D1998" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1998" t="n">
+        <v>198.16</v>
+      </c>
+      <c r="F1998" t="inlineStr"/>
+    </row>
+    <row r="1999">
+      <c r="A1999" s="2" t="n">
+        <v>44722</v>
+      </c>
+      <c r="B1999" t="inlineStr"/>
+      <c r="C1999" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D1999" t="inlineStr">
+        <is>
+          <t>ST1 V#LLINGBY K0135</t>
+        </is>
+      </c>
+      <c r="E1999" t="inlineStr"/>
+      <c r="F1999" t="n">
+        <v>990.79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2022-06-19 (total 2001 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1999"/>
+  <dimension ref="A1:F2002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41687,6 +41687,60 @@
         <v>990.79</v>
       </c>
     </row>
+    <row r="2000">
+      <c r="A2000" s="2" t="n">
+        <v>44729</v>
+      </c>
+      <c r="B2000" t="inlineStr"/>
+      <c r="C2000" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D2000" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E2000" t="n">
+        <v>149</v>
+      </c>
+      <c r="F2000" t="inlineStr"/>
+    </row>
+    <row r="2001">
+      <c r="A2001" s="2" t="n">
+        <v>44729</v>
+      </c>
+      <c r="B2001" t="inlineStr"/>
+      <c r="C2001" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D2001" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E2001" t="n">
+        <v>37.25</v>
+      </c>
+      <c r="F2001" t="inlineStr"/>
+    </row>
+    <row r="2002">
+      <c r="A2002" s="2" t="n">
+        <v>44729</v>
+      </c>
+      <c r="B2002" t="inlineStr"/>
+      <c r="C2002" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D2002" t="inlineStr">
+        <is>
+          <t>MISSHOSTIN* MISS HOSTI K0135</t>
+        </is>
+      </c>
+      <c r="E2002" t="inlineStr"/>
+      <c r="F2002" t="n">
+        <v>186.25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OrderReceipts_Expenses_Konto_Classification.xlsx/OrderReceipts_Expenses_Konto_Classification.csv: Entered 3 new rows for week ending 2022-06-26 (total 2004 rows)
</commit_message>
<xml_diff>
--- a/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
+++ b/finance/OrderReceipts_Expenses_Konto_Classification.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2002"/>
+  <dimension ref="A1:F2005"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -41741,6 +41741,60 @@
         <v>186.25</v>
       </c>
     </row>
+    <row r="2003">
+      <c r="A2003" s="2" t="n">
+        <v>44737</v>
+      </c>
+      <c r="B2003" t="inlineStr"/>
+      <c r="C2003" t="n">
+        <v>5670</v>
+      </c>
+      <c r="D2003" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E2003" t="n">
+        <v>724.58</v>
+      </c>
+      <c r="F2003" t="inlineStr"/>
+    </row>
+    <row r="2004">
+      <c r="A2004" s="2" t="n">
+        <v>44737</v>
+      </c>
+      <c r="B2004" t="inlineStr"/>
+      <c r="C2004" t="n">
+        <v>2641</v>
+      </c>
+      <c r="D2004" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E2004" t="n">
+        <v>181.15</v>
+      </c>
+      <c r="F2004" t="inlineStr"/>
+    </row>
+    <row r="2005">
+      <c r="A2005" s="2" t="n">
+        <v>44737</v>
+      </c>
+      <c r="B2005" t="inlineStr"/>
+      <c r="C2005" t="n">
+        <v>1930</v>
+      </c>
+      <c r="D2005" t="inlineStr">
+        <is>
+          <t>PREEM K0135</t>
+        </is>
+      </c>
+      <c r="E2005" t="inlineStr"/>
+      <c r="F2005" t="n">
+        <v>905.73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>